<commit_message>
refactor: chart name change
</commit_message>
<xml_diff>
--- a/DBLP-OpenAlex-testing/fewshot-DBLP-OpenAlex/few_shot_llama_dblp_openalex_results_comparison.xlsx
+++ b/DBLP-OpenAlex-testing/fewshot-DBLP-OpenAlex/few_shot_llama_dblp_openalex_results_comparison.xlsx
@@ -220,112 +220,112 @@
     <t>What is the average number of co-authors for research papers published by Gustaf S\u00F6derlind?</t>
   </si>
   <si>
-    <t>['https://semopenalex.org/work/W188103252', 'https://semopenalex.org/work/W2799918114', 'https://semopenalex.org/work/W4389476656', 'https://semopenalex.org/work/W2164985294', 'https://semopenalex.org/work/W2133946031', 'https://semopenalex.org/work/W3082909461', 'https://semopenalex.org/work/W2005948381', 'https://semopenalex.org/work/W2883183026', 'https://semopenalex.org/work/W3013847853', 'https://semopenalex.org/work/W1996261192', 'https://semopenalex.org/work/W2557406903', 'https://semopenalex.org/work/W2098589561', 'https://semopenalex.org/work/W2901265490', 'https://semopenalex.org/work/W3030243522', 'https://semopenalex.org/work/W1542429709', 'https://semopenalex.org/work/W2080393976', 'https://semopenalex.org/work/W2182446967', 'https://semopenalex.org/work/W3082121147', 'https://semopenalex.org/work/W2170327195', 'https://semopenalex.org/work/W2137367494', 'https://semopenalex.org/work/W2122784464', 'https://semopenalex.org/work/W2059580911', 'https://semopenalex.org/work/W2277916629', 'https://semopenalex.org/work/W2226738307', 'https://semopenalex.org/work/W2171671453', 'https://semopenalex.org/work/W1755261004', 'https://semopenalex.org/work/W2000850157', 'https://semopenalex.org/work/W2138588147', 'https://semopenalex.org/work/W2234365651', 'https://semopenalex.org/work/W2587222093', 'https://semopenalex.org/work/W1041461969', 'https://semopenalex.org/work/W3081685983', 'https://semopenalex.org/work/W4301447820', 'https://semopenalex.org/work/W54673566', 'https://semopenalex.org/work/W2995567949', 'https://semopenalex.org/work/W4396695389', 'https://semopenalex.org/work/W2150505652', 'https://semopenalex.org/work/W2140243124', 'https://semopenalex.org/work/W2113868440', 'https://semopenalex.org/work/W1929232145', 'https://semopenalex.org/work/W4247737681', 'https://semopenalex.org/work/W2514533441', 'https://semopenalex.org/work/W2112753023', 'https://semopenalex.org/work/W2752026712', 'https://semopenalex.org/work/W2181900851', 'https://semopenalex.org/work/W2757690399', 'https://semopenalex.org/work/W1963759754', 'https://semopenalex.org/work/W2136645836', 'https://semopenalex.org/work/W2736157438', 'https://semopenalex.org/work/W146984990', 'https://semopenalex.org/work/W2073156145', 'https://semopenalex.org/work/W2152670036', 'https://semopenalex.org/work/W2740907063', 'https://semopenalex.org/work/W2138250189', 'https://semopenalex.org/work/W3147662830', 'https://semopenalex.org/work/W2166763164', 'https://semopenalex.org/work/W2959129322', 'https://semopenalex.org/work/W2173102402', 'https://semopenalex.org/work/W4300748512', 'https://semopenalex.org/work/W2055827744', 'https://semopenalex.org/work/W4295779216', 'https://semopenalex.org/work/W171991278', 'https://semopenalex.org/work/W2182785605', 'https://semopenalex.org/work/W3016154199', 'https://semopenalex.org/work/W4210813334', 'https://semopenalex.org/work/W4247029563', 'https://semopenalex.org/work/W1729906464', 'https://semopenalex.org/work/W2274206371', 'https://semopenalex.org/work/W2321428856', 'https://semopenalex.org/work/W2067686570', 'https://semopenalex.org/work/W2605122712', 'https://semopenalex.org/work/W3022514883', 'https://semopenalex.org/work/W2167424492', 'https://semopenalex.org/work/W2125654576', 'https://semopenalex.org/work/W2738446327', 'https://semopenalex.org/work/W47444322', 'https://semopenalex.org/work/W2018708687', 'https://semopenalex.org/work/W3037521446', 'https://semopenalex.org/work/W4248877513', 'https://semopenalex.org/work/W562425896', 'https://semopenalex.org/work/W4281490671', 'https://semopenalex.org/work/W4238264174', 'https://semopenalex.org/work/W2608090064', 'https://semopenalex.org/work/W2069469539', 'https://semopenalex.org/work/W1625275222', 'https://semopenalex.org/work/W4205742677', 'https://semopenalex.org/work/W2023289472', 'https://semopenalex.org/work/W3082574538', 'https://semopenalex.org/work/W2165195120', 'https://semopenalex.org/work/W2103364709', 'https://semopenalex.org/work/W2152754828', 'https://semopenalex.org/work/W2105281328', 'https://semopenalex.org/work/W1702815980', 'https://semopenalex.org/work/W2124921180', 'https://semopenalex.org/work/W4210298342', 'https://semopenalex.org/work/W2892078924', 'https://semopenalex.org/work/W1552374822', 'https://semopenalex.org/work/W4238511116', 'https://semopenalex.org/work/W4384263461', 'https://semopenalex.org/work/W3023079907', 'https://semopenalex.org/work/W653390160', 'https://semopenalex.org/work/W3114823909', 'https://semopenalex.org/work/W2182093612', 'https://semopenalex.org/work/W2113694234', 'https://semopenalex.org/work/W1753483902', 'https://semopenalex.org/work/W2028031999', 'https://semopenalex.org/work/W3096817374', 'https://semopenalex.org/work/W2005357327', 'https://semopenalex.org/work/W2133171495', 'https://semopenalex.org/work/W4247632977', 'https://semopenalex.org/work/W1972362582', 'https://semopenalex.org/work/W3164080097', 'https://semopenalex.org/work/W2044023590', 'https://semopenalex.org/work/W4251349925', 'https://semopenalex.org/work/W2163312800', 'https://semopenalex.org/work/W13024336', 'https://semopenalex.org/work/W2100777852', 'https://semopenalex.org/work/W2122538412', 'https://semopenalex.org/work/W2968697710', 'https://semopenalex.org/work/W2512077429', 'https://semopenalex.org/work/W1990776069', 'https://semopenalex.org/work/W2594497686', 'https://semopenalex.org/work/W1817463943', 'https://semopenalex.org/work/W100499533', 'https://semopenalex.org/work/W4360604687', 'https://semopenalex.org/work/W3037487054', 'https://semopenalex.org/work/W4237274094', 'https://semopenalex.org/work/W202954270', 'https://semopenalex.org/work/W2099077058', 'https://semopenalex.org/work/W2906284509', 'https://semopenalex.org/work/W2804810577', 'https://semopenalex.org/work/W2728862777', 'https://semopenalex.org/work/W1558485007', 'https://semopenalex.org/work/W2792227230', 'https://semopenalex.org/work/W1990740853', 'https://semopenalex.org/work/W2128936252', 'https://semopenalex.org/work/W155674873', 'https://semopenalex.org/work/W2034937923', 'https://semopenalex.org/work/W1912056476', 'https://semopenalex.org/work/W1980476288', 'https://semopenalex.org/work/W2584513564', 'https://semopenalex.org/work/W2003205683', 'https://semopenalex.org/work/W2123134063', 'https://semopenalex.org/work/W128593825', 'https://semopenalex.org/work/W4392979894', 'https://semopenalex.org/work/W2117451136', 'https://semopenalex.org/work/W1533919275', 'https://semopenalex.org/work/W4404250201', 'https://semopenalex.org/work/W2990422891', 'https://semopenalex.org/work/W3081749826', 'https://semopenalex.org/work/W4244775271', 'https://semopenalex.org/work/W2530516535', 'https://semopenalex.org/work/W2753693229', 'https://semopenalex.org/work/W961274400', 'https://semopenalex.org/work/W4220992118', 'https://semopenalex.org/work/W201713607', 'https://semopenalex.org/work/W2023479938', 'https://semopenalex.org/work/W2619174663', 'https://semopenalex.org/work/W4320000513', 'https://semopenalex.org/work/W2804317122', 'https://semopenalex.org/work/W4287815821', 'https://semopenalex.org/work/W4394518676', 'https://semopenalex.org/work/W2104167274', 'https://semopenalex.org/work/W2186313366', 'https://semopenalex.org/work/W49930183', 'https://semopenalex.org/work/W3082938327', 'https://semopenalex.org/work/W2149509417', 'https://semopenalex.org/work/W190600666', 'https://semopenalex.org/work/W2029661605', 'https://semopenalex.org/work/W2038517887', 'https://semopenalex.org/work/W1980799317', 'https://semopenalex.org/work/W2591501322', 'https://semopenalex.org/work/W67844065', 'https://semopenalex.org/work/W4312182041', 'https://semopenalex.org/work/W2077513328', 'https://semopenalex.org/work/W2957946622', 'https://semopenalex.org/work/W3120515165', 'https://semopenalex.org/work/W2001775984', 'https://semopenalex.org/work/W2114791275', 'https://semopenalex.org/work/W2599387809', 'https://semopenalex.org/work/W2151304280', 'https://semopenalex.org/work/W2338530657', 'https://semopenalex.org/work/W2143284629', 'https://semopenalex.org/work/W2135586389', 'https://semopenalex.org/work/W2130391582', 'https://semopenalex.org/work/W4235499751', 'https://semopenalex.org/work/W2141115795', 'https://semopenalex.org/work/W2074682051', 'https://semopenalex.org/work/W2401739586', 'https://semopenalex.org/work/W2620095341', 'https://semopenalex.org/work/W3011781542', 'https://semopenalex.org/work/W3149746193', 'https://semopenalex.org/work/W3012737141', 'https://semopenalex.org/work/W2616948544', 'https://semopenalex.org/work/W2018345398', 'https://semopenalex.org/work/W2898552906', 'https://semopenalex.org/work/W4282914661', 'https://semopenalex.org/work/W1516345628', 'https://semopenalex.org/work/W160337249', 'https://semopenalex.org/work/W4299834590', 'https://semopenalex.org/work/W30482722', 'https://semopenalex.org/work/W2023846135', 'https://semopenalex.org/work/W2775903912', 'https://semopenalex.org/work/W2128135249', 'https://semopenalex.org/work/W2005096286', 'https://semopenalex.org/work/W2154216058', 'https://semopenalex.org/work/W3082943899', 'https://semopenalex.org/work/W2745733921', 'https://semopenalex.org/work/W3081898781', 'https://semopenalex.org/work/W3127482518', 'https://semopenalex.org/work/W1986257701', 'https://semopenalex.org/work/W3024342691', 'https://semopenalex.org/work/W2185694006', 'https://semopenalex.org/work/W4237431914', 'https://semopenalex.org/work/W2320884143', 'https://semopenalex.org/work/W2013165801', 'https://semopenalex.org/work/W2153940791', 'https://semopenalex.org/work/W3081541487', 'https://semopenalex.org/work/W2026960907', 'https://semopenalex.org/work/W2771147402', 'https://semopenalex.org/work/W2039210571', 'https://semopenalex.org/work/W2095908354', 'https://semopenalex.org/work/W3027665269', 'https://semopenalex.org/work/W2151573792', 'https://semopenalex.org/work/W3015578022', 'https://semopenalex.org/work/W4378234403', 'https://semopenalex.org/work/W3013220518', 'https://semopenalex.org/work/W2110324005', 'https://semopenalex.org/work/W2969940663', 'https://semopenalex.org/work/W2766450143', 'https://semopenalex.org/work/W67119066', 'https://semopenalex.org/work/W4302424645', 'https://semopenalex.org/work/W4210257758', 'https://semopenalex.org/work/W2724228083', 'https://semopenalex.org/work/W2133819144', 'https://semopenalex.org/work/W2741748074', 'https://semopenalex.org/work/W2937671906', 'https://semopenalex.org/work/W2085864217', 'https://semopenalex.org/work/W2093352090', 'https://semopenalex.org/work/W2038509977', 'https://semopenalex.org/work/W2999466582', 'https://semopenalex.org/work/W4226457422', 'https://semopenalex.org/work/W2968316987', 'https://semopenalex.org/work/W2970449937', 'https://semopenalex.org/work/W2105424397', 'https://semopenalex.org/work/W2096582083', 'https://semopenalex.org/work/W2166662555', 'https://semopenalex.org/work/W4236983726', 'https://semopenalex.org/work/W73405584', 'https://semopenalex.org/work/W2072049173', 'https://semopenalex.org/work/W2061486817', 'https://semopenalex.org/work/W3036157671', 'https://semopenalex.org/work/W1096039644', 'https://semopenalex.org/work/W2593472651', 'https://semopenalex.org/work/W2922365273', 'https://semopenalex.org/work/W2805444673', 'https://semopenalex.org/work/W2588193771', 'https://semopenalex.org/work/W2952764074', 'https://semopenalex.org/work/W626749138', 'https://semopenalex.org/work/W2605190822', 'https://semopenalex.org/work/W2003148032', 'https://semopenalex.org/work/W1979704442', 'https://semopenalex.org/work/W3082188274', 'https://semopenalex.org/work/W2171958563', 'https://semopenalex.org/work/W3082672072', 'https://semopenalex.org/work/W4386776420', 'https://semopenalex.org/work/W1965117376', 'https://semopenalex.org/work/W2123582261', 'https://semopenalex.org/work/W2162395962', 'https://semopenalex.org/work/W2810861266', 'https://semopenalex.org/work/W2514686722', 'https://semopenalex.org/work/W4387589621', 'https://semopenalex.org/work/W3038115327', 'https://semopenalex.org/work/W4239519246', 'https://semopenalex.org/work/W2399215436', 'https://semopenalex.org/work/W1552561574', 'https://semopenalex.org/work/W4383065806', 'https://semopenalex.org/work/W1527768716', 'https://semopenalex.org/work/W2009658718', 'https://semopenalex.org/work/W200396823', 'https://semopenalex.org/work/W2021648931', 'https://semopenalex.org/work/W2943865318', 'https://semopenalex.org/work/W1990062657', 'https://semopenalex.org/work/W1417422537', 'https://semopenalex.org/work/W2774855312', 'https://semopenalex.org/work/W2123551394', 'https://semopenalex.org/work/W2906330222', 'https://semopenalex.org/work/W2901026025', 'https://semopenalex.org/work/W4386220934', 'https://semopenalex.org/work/W2063989480', 'https://semopenalex.org/work/W4400132771', 'https://semopenalex.org/work/W2035958911', 'https://semopenalex.org/work/W2017767972', 'https://semopenalex.org/work/W1870353999', 'https://semopenalex.org/work/W2122677844', 'https://semopenalex.org/work/W2403047599', 'https://semopenalex.org/work/W1963502684', 'https://semopenalex.org/work/W3082580655', 'https://semopenalex.org/work/W3081531507', 'https://semopenalex.org/work/W2024202481', 'https://semopenalex.org/work/W2004149428', 'https://semopenalex.org/work/W2041337419', 'https://semopenalex.org/work/W2143084783', 'https://semopenalex.org/work/W90104346', 'https://semopenalex.org/work/W4364358025', 'https://semopenalex.org/work/W2016652422', 'https://semopenalex.org/work/W1829136368', 'https://semopenalex.org/work/W3007663200', 'https://semopenalex.org/work/W2116449320', 'https://semopenalex.org/work/W2033918799', 'https://semopenalex.org/work/W3154255967', 'https://semopenalex.org/work/W2626706700', 'https://semopenalex.org/work/W2065302863', 'https://semopenalex.org/work/W2888859618', 'https://semopenalex.org/work/W4249463326', 'https://semopenalex.org/work/W2074444313', 'https://semopenalex.org/work/W2407173971', 'https://semopenalex.org/work/W2901545557', 'https://semopenalex.org/work/W3009745595', 'https://semopenalex.org/work/W2986447659', 'https://semopenalex.org/work/W2051791551', 'https://semopenalex.org/work/W2962540522', 'https://semopenalex.org/work/W3126358682', 'https://semopenalex.org/work/W2054518304', 'https://semopenalex.org/work/W1536091370', 'https://semopenalex.org/work/W2309635847', 'https://semopenalex.org/work/W2094867236', 'https://semopenalex.org/work/W2788844524', 'https://semopenalex.org/work/W3173715284', 'https://semopenalex.org/work/W2988464819', 'https://semopenalex.org/work/W2103430250', 'https://semopenalex.org/work/W2141665828', 'https://semopenalex.org/work/W4404250088', 'https://semopenalex.org/work/W4405944965', 'https://semopenalex.org/work/W2019966888', 'https://semopenalex.org/work/W2507172825', 'https://semopenalex.org/work/W2242995227', 'https://semopenalex.org/work/W3021831361', 'https://semopenalex.org/work/W4251952567', 'https://semopenalex.org/work/W1552001157', 'https://semopenalex.org/work/W2004009311', 'https://semopenalex.org/work/W2729343995', 'https://semopenalex.org/work/W1972453858', 'https://semopenalex.org/work/W2049855663', 'https://semopenalex.org/work/W1735274207', 'https://semopenalex.org/work/W2034235801', 'https://semopenalex.org/work/W4386157387', 'https://semopenalex.org/work/W2003067257']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W3047312767', 'https://semopenalex.org/work/W2784045768', 'https://semopenalex.org/work/W3017267450', 'https://semopenalex.org/work/W2754398119', 'https://semopenalex.org/work/W4319980430', 'https://semopenalex.org/work/W4393424568', 'https://semopenalex.org/work/W2809907824', 'https://semopenalex.org/work/W2598695409', 'https://semopenalex.org/work/W4393821610', 'https://semopenalex.org/work/W2964346923']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2809425916', 'https://semopenalex.org/work/W2967175067', 'https://semopenalex.org/work/W2967526509', 'https://semopenalex.org/work/W4249431654', 'https://semopenalex.org/work/W2549612717', 'https://semopenalex.org/work/W2971173586', 'https://semopenalex.org/work/W4313563578', 'https://semopenalex.org/work/W4287668995', 'https://semopenalex.org/work/W4287392742', 'https://semopenalex.org/work/W3169232032', 'https://semopenalex.org/work/W4293065025', 'https://semopenalex.org/work/W3206231781', 'https://semopenalex.org/work/W4321796319', 'https://semopenalex.org/work/W2330908417', 'https://semopenalex.org/work/W3014769903', 'https://semopenalex.org/work/W3127585016', 'https://semopenalex.org/work/W2059943739', 'https://semopenalex.org/work/W2889555883', 'https://semopenalex.org/work/W2967719799', 'https://semopenalex.org/work/W2044633418', 'https://semopenalex.org/work/W2345531317', 'https://semopenalex.org/work/W4213248384', 'https://semopenalex.org/work/W4363671915', 'https://semopenalex.org/work/W4402426748', 'https://semopenalex.org/work/W4240535267', 'https://semopenalex.org/work/W4288261968', 'https://semopenalex.org/work/W2899596954', 'https://semopenalex.org/work/W3209991164', 'https://semopenalex.org/work/W2110499608', 'https://semopenalex.org/work/W2272844336', 'https://semopenalex.org/work/W3121391869', 'https://semopenalex.org/work/W2049381173', 'https://semopenalex.org/work/W3084859057', 'https://semopenalex.org/work/W2293962294', 'https://semopenalex.org/work/W4287235540', 'https://semopenalex.org/work/W2142174774', 'https://semopenalex.org/work/W4280592120', 'https://semopenalex.org/work/W2905847388', 'https://semopenalex.org/work/W4312667018', 'https://semopenalex.org/work/W2119804349', 'https://semopenalex.org/work/W4406157430', 'https://semopenalex.org/work/W3121852636', 'https://semopenalex.org/work/W4400675898', 'https://semopenalex.org/work/W2900603753', 'https://semopenalex.org/work/W3153041448', 'https://semopenalex.org/work/W2077664520', 'https://semopenalex.org/work/W3174473101', 'https://semopenalex.org/work/W2158735282', 'https://semopenalex.org/work/W4283641599', 'https://semopenalex.org/work/W4235240618', 'https://semopenalex.org/work/W4287668646', 'https://semopenalex.org/work/W2340333180', 'https://semopenalex.org/work/W2211800868', 'https://semopenalex.org/work/W1517398235', 'https://semopenalex.org/work/W2530456191', 'https://semopenalex.org/work/W4251429682', 'https://semopenalex.org/work/W3043915370', 'https://semopenalex.org/work/W3033737646', 'https://semopenalex.org/work/W2293309991', 'https://semopenalex.org/work/W4319653723', 'https://semopenalex.org/work/W4367628070', 'https://semopenalex.org/work/W4318159625', 'https://semopenalex.org/work/W3145532460', 'https://semopenalex.org/work/W2055489377', 'https://semopenalex.org/work/W2788992245', 'https://semopenalex.org/work/W2171240869', 'https://semopenalex.org/work/W4320896439', 'https://semopenalex.org/work/W2093284392', 'https://semopenalex.org/work/W4319264802', 'https://semopenalex.org/work/W2893263830', 'https://semopenalex.org/work/W2062032381', 'https://semopenalex.org/work/W3085432304', 'https://semopenalex.org/work/W1908449836', 'https://semopenalex.org/work/W4381713892', 'https://semopenalex.org/work/W3126838471', 'https://semopenalex.org/work/W1810972023', 'https://semopenalex.org/work/W1851000371', 'https://semopenalex.org/work/W3110545566', 'https://semopenalex.org/work/W1593690673', 'https://semopenalex.org/work/W4387737248', 'https://semopenalex.org/work/W4287667875', 'https://semopenalex.org/work/W4225781798', 'https://semopenalex.org/work/W2145330693', 'https://semopenalex.org/work/W4399872440', 'https://semopenalex.org/work/W1568212182', 'https://semopenalex.org/work/W2898811429', 'https://semopenalex.org/work/W2901106555', 'https://semopenalex.org/work/W4312757941', 'https://semopenalex.org/work/W3010403426', 'https://semopenalex.org/work/W4229517606', 'https://semopenalex.org/work/W3119454628', 'https://semopenalex.org/work/W4301582020', 'https://semopenalex.org/work/W3084710058', 'https://semopenalex.org/work/W2272672851', 'https://semopenalex.org/work/W2333194490', 'https://semopenalex.org/work/W3130260207', 'https://semopenalex.org/work/W2135584970']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W4390737683', 'https://semopenalex.org/work/W2996971450', 'https://semopenalex.org/work/W2772966323', 'https://semopenalex.org/work/W4396568545', 'https://semopenalex.org/work/W4206136166', 'https://semopenalex.org/work/W2957110867', 'https://semopenalex.org/work/W4238294234', 'https://semopenalex.org/work/W3134422373', 'https://semopenalex.org/work/W2996342798', 'https://semopenalex.org/work/W3205075200', 'https://semopenalex.org/work/W2897762537', 'https://semopenalex.org/work/W2979701877', 'https://semopenalex.org/work/W2100407406', 'https://semopenalex.org/work/W1999760195', 'https://semopenalex.org/work/W4367671449', 'https://semopenalex.org/work/W2788968669', 'https://semopenalex.org/work/W2974444355', 'https://semopenalex.org/work/W3048792033', 'https://semopenalex.org/work/W2844810377', 'https://semopenalex.org/work/W2903944530', 'https://semopenalex.org/work/W4406267825', 'https://semopenalex.org/work/W2805460435', 'https://semopenalex.org/work/W3202715770', 'https://semopenalex.org/work/W2780277126', 'https://semopenalex.org/work/W2792290921', 'https://semopenalex.org/work/W2948196949', 'https://semopenalex.org/work/W2397277866', 'https://semopenalex.org/work/W4293863370', 'https://semopenalex.org/work/W3158463786', 'https://semopenalex.org/work/W2226359063']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2941573428', 'https://semopenalex.org/work/W3160945783', 'https://semopenalex.org/work/W3168652588', 'https://semopenalex.org/work/W294448757', 'https://semopenalex.org/work/W2162555816', 'https://semopenalex.org/work/W3048770428', 'https://semopenalex.org/work/W2343779160', 'https://semopenalex.org/work/W3201845268', 'https://semopenalex.org/work/W4292798214', 'https://semopenalex.org/work/W1966445952', 'https://semopenalex.org/work/W2022832873', 'https://semopenalex.org/work/W2546536770', 'https://semopenalex.org/work/W1977295820', 'https://semopenalex.org/work/W3131298139', 'https://semopenalex.org/work/W2014168043', 'https://semopenalex.org/work/W4287900890', 'https://semopenalex.org/work/W2473751517', 'https://semopenalex.org/work/W2462370865', 'https://semopenalex.org/work/W4393911083', 'https://semopenalex.org/work/W2073791116', 'https://semopenalex.org/work/W2905242827', 'https://semopenalex.org/work/W4398157632', 'https://semopenalex.org/work/W4221159459', 'https://semopenalex.org/work/W4308083526', 'https://semopenalex.org/work/W4367297631', 'https://semopenalex.org/work/W4233099794', 'https://semopenalex.org/work/W3008746569', 'https://semopenalex.org/work/W4368353176', 'https://semopenalex.org/work/W4379933304', 'https://semopenalex.org/work/W2945856475', 'https://semopenalex.org/work/W4287691869', 'https://semopenalex.org/work/W4210597606', 'https://semopenalex.org/work/W4284892042', 'https://semopenalex.org/work/W1965596253', 'https://semopenalex.org/work/W3194018690', 'https://semopenalex.org/work/W4287241484', 'https://semopenalex.org/work/W3128506819', 'https://semopenalex.org/work/W4287690348', 'https://semopenalex.org/work/W4385292569', 'https://semopenalex.org/work/W3210446150', 'https://semopenalex.org/work/W2244659594', 'https://semopenalex.org/work/W2509887407', 'https://semopenalex.org/work/W2559181347', 'https://semopenalex.org/work/W4288364801', 'https://semopenalex.org/work/W3004806403', 'https://semopenalex.org/work/W2954507353', 'https://semopenalex.org/work/W2525851376', 'https://semopenalex.org/work/W3210764291', 'https://semopenalex.org/work/W2606709877', 'https://semopenalex.org/work/W4287726151', 'https://semopenalex.org/work/W1972302881', 'https://semopenalex.org/work/W4323038447', 'https://semopenalex.org/work/W3156189202', 'https://semopenalex.org/work/W4226302796', 'https://semopenalex.org/work/W97884251', 'https://semopenalex.org/work/W2214980064', 'https://semopenalex.org/work/W4396243491', 'https://semopenalex.org/work/W3027839759', 'https://semopenalex.org/work/W4287776928', 'https://semopenalex.org/work/W3003928672', 'https://semopenalex.org/work/W4404395434', 'https://semopenalex.org/work/W4231137968', 'https://semopenalex.org/work/W2343495200', 'https://semopenalex.org/work/W2184966923', 'https://semopenalex.org/work/W3211048833', 'https://semopenalex.org/work/W2163036976', 'https://semopenalex.org/work/W4406193279', 'https://semopenalex.org/work/W4287746776', 'https://semopenalex.org/work/W2997497769', 'https://semopenalex.org/work/W4230850676', 'https://semopenalex.org/work/W2929118134', 'https://semopenalex.org/work/W2137100320', 'https://semopenalex.org/work/W2467368527', 'https://semopenalex.org/work/W2472426210', 'https://semopenalex.org/work/W3018835489', 'https://semopenalex.org/work/W4287123914', 'https://semopenalex.org/work/W2316889284', 'https://semopenalex.org/work/W2145997469', 'https://semopenalex.org/work/W2297325673', 'https://semopenalex.org/work/W3093436911', 'https://semopenalex.org/work/W2739601332', 'https://semopenalex.org/work/W4387799594', 'https://semopenalex.org/work/W2754395205', 'https://semopenalex.org/work/W1572192454', 'https://semopenalex.org/work/W3049640275', 'https://semopenalex.org/work/W2804309962', 'https://semopenalex.org/work/W4320341944', 'https://semopenalex.org/work/W4389261110', 'https://semopenalex.org/work/W2123140882', 'https://semopenalex.org/work/W2460754307', 'https://semopenalex.org/work/W3043093753', 'https://semopenalex.org/work/W2558974524', 'https://semopenalex.org/work/W2979711838', 'https://semopenalex.org/work/W3101755570', 'https://semopenalex.org/work/W3091415435', 'https://semopenalex.org/work/W2084071117', 'https://semopenalex.org/work/W4377298398', 'https://semopenalex.org/work/W4286953522', 'https://semopenalex.org/work/W3177180018', 'https://semopenalex.org/work/W2900566525', 'https://semopenalex.org/work/W2059743020', 'https://semopenalex.org/work/W2973151896', 'https://semopenalex.org/work/W3096308497', 'https://semopenalex.org/work/W4280611212', 'https://semopenalex.org/work/W3207608819', 'https://semopenalex.org/work/W3034646170', 'https://semopenalex.org/work/W4399986811', 'https://semopenalex.org/work/W1982467666', 'https://semopenalex.org/work/W3174807969', 'https://semopenalex.org/work/W2464529301', 'https://semopenalex.org/work/W3201319033', 'https://semopenalex.org/work/W2995556886', 'https://semopenalex.org/work/W4306703516', 'https://semopenalex.org/work/W2552048974', 'https://semopenalex.org/work/W144502943', 'https://semopenalex.org/work/W3093421867', 'https://semopenalex.org/work/W1805881796', 'https://semopenalex.org/work/W2625157458', 'https://semopenalex.org/work/W4320341743', 'https://semopenalex.org/work/W2039557327', 'https://semopenalex.org/work/W2548547123', 'https://semopenalex.org/work/W3048856089', 'https://semopenalex.org/work/W2572480678', 'https://semopenalex.org/work/W3106951738', 'https://semopenalex.org/work/W4226041925', 'https://semopenalex.org/work/W2914677765', 'https://semopenalex.org/work/W2004314166', 'https://semopenalex.org/work/W4200081143', 'https://semopenalex.org/work/W2038323322', 'https://semopenalex.org/work/W4297060365', 'https://semopenalex.org/work/W2469325223', 'https://semopenalex.org/work/W2784298189', 'https://semopenalex.org/work/W2911439292', 'https://semopenalex.org/work/W4245299688', 'https://semopenalex.org/work/W4390872486', 'https://semopenalex.org/work/W2059502067', 'https://semopenalex.org/work/W2090465764', 'https://semopenalex.org/work/W3041585044', 'https://semopenalex.org/work/W3101164610', 'https://semopenalex.org/work/W169568933', 'https://semopenalex.org/work/W2519804223', 'https://semopenalex.org/work/W4284710143', 'https://semopenalex.org/work/W3104328743', 'https://semopenalex.org/work/W2905715248', 'https://semopenalex.org/work/W4319862456', 'https://semopenalex.org/work/W4296070200', 'https://semopenalex.org/work/W4210756135', 'https://semopenalex.org/work/W3007493000', 'https://semopenalex.org/work/W4283823243', 'https://semopenalex.org/work/W3030459553', 'https://semopenalex.org/work/W3134509799', 'https://semopenalex.org/work/W4378942243', 'https://semopenalex.org/work/W3183881674', 'https://semopenalex.org/work/W2122005484', 'https://semopenalex.org/work/W4324116704', 'https://semopenalex.org/work/W1587612576', 'https://semopenalex.org/work/W4221120919', 'https://semopenalex.org/work/W4286902665', 'https://semopenalex.org/work/W3202872895', 'https://semopenalex.org/work/W4311007713', 'https://semopenalex.org/work/W4287279053', 'https://semopenalex.org/work/W2991253882', 'https://semopenalex.org/work/W3145938895', 'https://semopenalex.org/work/W3008634715', 'https://semopenalex.org/work/W2999276659', 'https://semopenalex.org/work/W1966530006', 'https://semopenalex.org/work/W2939129451', 'https://semopenalex.org/work/W2820922764', 'https://semopenalex.org/work/W1980119762', 'https://semopenalex.org/work/W2043475427', 'https://semopenalex.org/work/W2825911140', 'https://semopenalex.org/work/W2114925746', 'https://semopenalex.org/work/W4287023576', 'https://semopenalex.org/work/W1579732497', 'https://semopenalex.org/work/W2038134612', 'https://semopenalex.org/work/W3173111918', 'https://semopenalex.org/work/W3216699651', 'https://semopenalex.org/work/W4398809881', 'https://semopenalex.org/work/W2142857396', 'https://semopenalex.org/work/W3212849404', 'https://semopenalex.org/work/W2131147042', 'https://semopenalex.org/work/W4400266996', 'https://semopenalex.org/work/W3126679255', 'https://semopenalex.org/work/W4287391921', 'https://semopenalex.org/work/W2972736078', 'https://semopenalex.org/work/W2951433015', 'https://semopenalex.org/work/W2026124805', 'https://semopenalex.org/work/W4406482035', 'https://semopenalex.org/work/W2108950108', 'https://semopenalex.org/work/W2626549485', 'https://semopenalex.org/work/W2972760949', 'https://semopenalex.org/work/W2899181049', 'https://semopenalex.org/work/W2132391423', 'https://semopenalex.org/work/W3096998353', 'https://semopenalex.org/work/W4384919669', 'https://semopenalex.org/work/W3046183292', 'https://semopenalex.org/work/W3210294081', 'https://semopenalex.org/work/W4312473456', 'https://semopenalex.org/work/W2798926091', 'https://semopenalex.org/work/W4385584193', 'https://semopenalex.org/work/W3097384956', 'https://semopenalex.org/work/W4387321281', 'https://semopenalex.org/work/W1997430507', 'https://semopenalex.org/work/W4323038488', 'https://semopenalex.org/work/W1991539813', 'https://semopenalex.org/work/W2041454412', 'https://semopenalex.org/work/W3085924585', 'https://semopenalex.org/work/W3093453792', 'https://semopenalex.org/work/W2898907473', 'https://semopenalex.org/work/W3015838662', 'https://semopenalex.org/work/W4236853429', 'https://semopenalex.org/work/W2150882603', 'https://semopenalex.org/work/W4206707377', 'https://semopenalex.org/work/W4297060071', 'https://semopenalex.org/work/W3028984135', 'https://semopenalex.org/work/W4391766346', 'https://semopenalex.org/work/W4383046641', 'https://semopenalex.org/work/W2027952077', 'https://semopenalex.org/work/W4391901288', 'https://semopenalex.org/work/W2924522543', 'https://semopenalex.org/work/W4283024182', 'https://semopenalex.org/work/W4287902355', 'https://semopenalex.org/work/W4384392951', 'https://semopenalex.org/work/W2060122457', 'https://semopenalex.org/work/W2971872524', 'https://semopenalex.org/work/W2916044424', 'https://semopenalex.org/work/W4403635745', 'https://semopenalex.org/work/W3110875274', 'https://semopenalex.org/work/W3007227736', 'https://semopenalex.org/work/W3203846187', 'https://semopenalex.org/work/W2156740813', 'https://semopenalex.org/work/W3047893908', 'https://semopenalex.org/work/W816337693', 'https://semopenalex.org/work/W3147053158', 'https://semopenalex.org/work/W3095459301', 'https://semopenalex.org/work/W3176114075', 'https://semopenalex.org/work/W2972393922', 'https://semopenalex.org/work/W4310562517', 'https://semopenalex.org/work/W3001208429', 'https://semopenalex.org/work/W3133606938', 'https://semopenalex.org/work/W3038185437', 'https://semopenalex.org/work/W1975771789', 'https://semopenalex.org/work/W75304744', 'https://semopenalex.org/work/W4287123862', 'https://semopenalex.org/work/W3107781032', 'https://semopenalex.org/work/W3121327306', 'https://semopenalex.org/work/W2898863929', 'https://semopenalex.org/work/W2760871008', 'https://semopenalex.org/work/W1753084818', 'https://semopenalex.org/work/W4296596641', 'https://semopenalex.org/work/W2403591241', 'https://semopenalex.org/work/W2732107624', 'https://semopenalex.org/work/W2086755418', 'https://semopenalex.org/work/W4400447326', 'https://semopenalex.org/work/W4403964510', 'https://semopenalex.org/work/W3124523586', 'https://semopenalex.org/work/W3209796046', 'https://semopenalex.org/work/W2154718966', 'https://semopenalex.org/work/W1494996644', 'https://semopenalex.org/work/W3129635911', 'https://semopenalex.org/work/W2337546824', 'https://semopenalex.org/work/W3083323811', 'https://semopenalex.org/work/W2786460214', 'https://semopenalex.org/work/W4392617501', 'https://semopenalex.org/work/W3128789131', 'https://semopenalex.org/work/W3167824842', 'https://semopenalex.org/work/W4394931310', 'https://semopenalex.org/work/W4399317854', 'https://semopenalex.org/work/W4255912054', 'https://semopenalex.org/work/W4406676443', 'https://semopenalex.org/work/W2157747589', 'https://semopenalex.org/work/W4322099461', 'https://semopenalex.org/work/W2996860607', 'https://semopenalex.org/work/W2808145095', 'https://semopenalex.org/work/W2466191378', 'https://semopenalex.org/work/W2164297046', 'https://semopenalex.org/work/W3025540705', 'https://semopenalex.org/work/W2096948221', 'https://semopenalex.org/work/W4385804769', 'https://semopenalex.org/work/W3005828390', 'https://semopenalex.org/work/W2152423878', 'https://semopenalex.org/work/W4366342364', 'https://semopenalex.org/work/W3203181771', 'https://semopenalex.org/work/W4384615920', 'https://semopenalex.org/work/W2969671163', 'https://semopenalex.org/work/W4403786771', 'https://semopenalex.org/work/W2777460464', 'https://semopenalex.org/work/W2117788706', 'https://semopenalex.org/work/W3092216346', 'https://semopenalex.org/work/W2463050926', 'https://semopenalex.org/work/W3106656598', 'https://semopenalex.org/work/W3171100434', 'https://semopenalex.org/work/W1246540336', 'https://semopenalex.org/work/W4384561507', 'https://semopenalex.org/work/W4295253548', 'https://semopenalex.org/work/W2056591916', 'https://semopenalex.org/work/W3198808971', 'https://semopenalex.org/work/W3096783252', 'https://semopenalex.org/work/W3127829048', 'https://semopenalex.org/work/W3099785009', 'https://semopenalex.org/work/W4386082512', 'https://semopenalex.org/work/W4290059224', 'https://semopenalex.org/work/W3207505502', 'https://semopenalex.org/work/W2879029702', 'https://semopenalex.org/work/W2171559681', 'https://semopenalex.org/work/W2120761625', 'https://semopenalex.org/work/W4285827783', 'https://semopenalex.org/work/W4382464396', 'https://semopenalex.org/work/W3001949026', 'https://semopenalex.org/work/W87063158', 'https://semopenalex.org/work/W3176780274', 'https://semopenalex.org/work/W3110177420', 'https://semopenalex.org/work/W3121924028', 'https://semopenalex.org/work/W2087611087']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2202885265', 'https://semopenalex.org/work/W2604384156', 'https://semopenalex.org/work/W176895944', 'https://semopenalex.org/work/W4360907566', 'https://semopenalex.org/work/W2169103252', 'https://semopenalex.org/work/W3020423550', 'https://semopenalex.org/work/W3014966924', 'https://semopenalex.org/work/W2077753966', 'https://semopenalex.org/work/W3090262174', 'https://semopenalex.org/work/W4285207151', 'https://semopenalex.org/work/W2109392297', 'https://semopenalex.org/work/W2210737596', 'https://semopenalex.org/work/W2907905966', 'https://semopenalex.org/work/W2901482574', 'https://semopenalex.org/work/W4200533036', 'https://semopenalex.org/work/W2383025629', 'https://semopenalex.org/work/W1989814488', 'https://semopenalex.org/work/W4386919989', 'https://semopenalex.org/work/W2964541684', 'https://semopenalex.org/work/W2996592540', 'https://semopenalex.org/work/W2330731982', 'https://semopenalex.org/work/W2624719059', 'https://semopenalex.org/work/W2168189713', 'https://semopenalex.org/work/W3005571193', 'https://semopenalex.org/work/W1986594812', 'https://semopenalex.org/work/W2013087313', 'https://semopenalex.org/work/W4404480496', 'https://semopenalex.org/work/W2804263862', 'https://semopenalex.org/work/W2058599944', 'https://semopenalex.org/work/W3199993893', 'https://semopenalex.org/work/W4404459004', 'https://semopenalex.org/work/W4386249920', 'https://semopenalex.org/work/W2947280819', 'https://semopenalex.org/work/W1972504394', 'https://semopenalex.org/work/W4389879531', 'https://semopenalex.org/work/W4386572358', 'https://semopenalex.org/work/W3210281673', 'https://semopenalex.org/work/W3134664381', 'https://semopenalex.org/work/W4404576824', 'https://semopenalex.org/work/W2783829353', 'https://semopenalex.org/work/W2149743901', 'https://semopenalex.org/work/W2058842944', 'https://semopenalex.org/work/W2909902231', 'https://semopenalex.org/work/W2038007991', 'https://semopenalex.org/work/W3145628585', 'https://semopenalex.org/work/W2904413102', 'https://semopenalex.org/work/W2794180747', 'https://semopenalex.org/work/W282835794', 'https://semopenalex.org/work/W2969688740', 'https://semopenalex.org/work/W2528857590', 'https://semopenalex.org/work/W4323663048', 'https://semopenalex.org/work/W4385826750', 'https://semopenalex.org/work/W4402835717', 'https://semopenalex.org/work/W3176567159', 'https://semopenalex.org/work/W4386307089', 'https://semopenalex.org/work/W2037720083', 'https://semopenalex.org/work/W4376142881', 'https://semopenalex.org/work/W3094268044', 'https://semopenalex.org/work/W2476848331', 'https://semopenalex.org/work/W4388675409', 'https://semopenalex.org/work/W3133842302', 'https://semopenalex.org/work/W4367147910', 'https://semopenalex.org/work/W4401990766', 'https://semopenalex.org/work/W2072045292', 'https://semopenalex.org/work/W4387869863', 'https://semopenalex.org/work/W4308342707', 'https://semopenalex.org/work/W2559992739', 'https://semopenalex.org/work/W2556195709', 'https://semopenalex.org/work/W2055657753', 'https://semopenalex.org/work/W4213068964', 'https://semopenalex.org/work/W4312385873', 'https://semopenalex.org/work/W4285211669', 'https://semopenalex.org/work/W4282826154', 'https://semopenalex.org/work/W2151517333', 'https://semopenalex.org/work/W2804348493', 'https://semopenalex.org/work/W4398152845', 'https://semopenalex.org/work/W2912634456', 'https://semopenalex.org/work/W2530101013', 'https://semopenalex.org/work/W4206824496', 'https://semopenalex.org/work/W4288391286', 'https://semopenalex.org/work/W2130027208', 'https://semopenalex.org/work/W4401210873', 'https://semopenalex.org/work/W2805010740', 'https://semopenalex.org/work/W4391429213', 'https://semopenalex.org/work/W4318603270', 'https://semopenalex.org/work/W2965197902', 'https://semopenalex.org/work/W2077093994', 'https://semopenalex.org/work/W2804501132', 'https://semopenalex.org/work/W2292837460', 'https://semopenalex.org/work/W2109565528', 'https://semopenalex.org/work/W4312235824', 'https://semopenalex.org/work/W4399910027', 'https://semopenalex.org/work/W4379983689', 'https://semopenalex.org/work/W4392460796', 'https://semopenalex.org/work/W2789498674', 'https://semopenalex.org/work/W4367148405', 'https://semopenalex.org/work/W3012171841', 'https://semopenalex.org/work/W2269062875', 'https://semopenalex.org/work/W4388213914', 'https://semopenalex.org/work/W4401548819', 'https://semopenalex.org/work/W4387886204', 'https://semopenalex.org/work/W1991496323', 'https://semopenalex.org/work/W4213097356', 'https://semopenalex.org/work/W2988764224', 'https://semopenalex.org/work/W2911885303', 'https://semopenalex.org/work/W3213340154', 'https://semopenalex.org/work/W4313291203', 'https://semopenalex.org/work/W1980855612', 'https://semopenalex.org/work/W3005715390', 'https://semopenalex.org/work/W1489929835', 'https://semopenalex.org/work/W4318601869', 'https://semopenalex.org/work/W4389471415', 'https://semopenalex.org/work/W2052206457', 'https://semopenalex.org/work/W4403646133', 'https://semopenalex.org/work/W976487463', 'https://semopenalex.org/work/W4391326572', 'https://semopenalex.org/work/W4289203223', 'https://semopenalex.org/work/W2068489330', 'https://semopenalex.org/work/W2066271829', 'https://semopenalex.org/work/W4396505344', 'https://semopenalex.org/work/W4386920758', 'https://semopenalex.org/work/W2763111898', 'https://semopenalex.org/work/W2990735505', 'https://semopenalex.org/work/W2047610380', 'https://semopenalex.org/work/W2891934018', 'https://semopenalex.org/work/W2118051735', 'https://semopenalex.org/work/W2052995625', 'https://semopenalex.org/work/W131277285', 'https://semopenalex.org/work/W2012087113', 'https://semopenalex.org/work/W4382119833', 'https://semopenalex.org/work/W2903850618', 'https://semopenalex.org/work/W2912046801', 'https://semopenalex.org/work/W3001204101', 'https://semopenalex.org/work/W2096177399', 'https://semopenalex.org/work/W2073648968', 'https://semopenalex.org/work/W2085023162', 'https://semopenalex.org/work/W4386918403', 'https://semopenalex.org/work/W2139900006', 'https://semopenalex.org/work/W2291494764', 'https://semopenalex.org/work/W4388519971', 'https://semopenalex.org/work/W4282836627', 'https://semopenalex.org/work/W2024504253', 'https://semopenalex.org/work/W4392573792', 'https://semopenalex.org/work/W1967335608', 'https://semopenalex.org/work/W4388666963', 'https://semopenalex.org/work/W2551664773', 'https://semopenalex.org/work/W2095857057', 'https://semopenalex.org/work/W2137422967', 'https://semopenalex.org/work/W2017065682', 'https://semopenalex.org/work/W4403233403', 'https://semopenalex.org/work/W3139325069', 'https://semopenalex.org/work/W4304203349', 'https://semopenalex.org/work/W3129170312', 'https://semopenalex.org/work/W2784259369', 'https://semopenalex.org/work/W2958283264', 'https://semopenalex.org/work/W2313795635', 'https://semopenalex.org/work/W1904270298', 'https://semopenalex.org/work/W2554849750', 'https://semopenalex.org/work/W4394858588', 'https://semopenalex.org/work/W2018860951', 'https://semopenalex.org/work/W4380451175', 'https://semopenalex.org/work/W4306793569', 'https://semopenalex.org/work/W4387714873', 'https://semopenalex.org/work/W3040063675', 'https://semopenalex.org/work/W2171432711', 'https://semopenalex.org/work/W2076890843', 'https://semopenalex.org/work/W4400112330', 'https://semopenalex.org/work/W2566656454', 'https://semopenalex.org/work/W2389323797', 'https://semopenalex.org/work/W2792380105', 'https://semopenalex.org/work/W4388953015', 'https://semopenalex.org/work/W2042556111', 'https://semopenalex.org/work/W3133466818', 'https://semopenalex.org/work/W2520653549', 'https://semopenalex.org/work/W2891734979', 'https://semopenalex.org/work/W4402834678', 'https://semopenalex.org/work/W2727836510', 'https://semopenalex.org/work/W3104724617', 'https://semopenalex.org/work/W4391878166', 'https://semopenalex.org/work/W2793708954', 'https://semopenalex.org/work/W3213939512', 'https://semopenalex.org/work/W2797561181', 'https://semopenalex.org/work/W2085741604', 'https://semopenalex.org/work/W2892268308', 'https://semopenalex.org/work/W2113578263', 'https://semopenalex.org/work/W4296270284', 'https://semopenalex.org/work/W4388145646', 'https://semopenalex.org/work/W2012725729', 'https://semopenalex.org/work/W4388133782', 'https://semopenalex.org/work/W4389076217', 'https://semopenalex.org/work/W4379034010', 'https://semopenalex.org/work/W2971778528', 'https://semopenalex.org/work/W3006413083', 'https://semopenalex.org/work/W2753440200', 'https://semopenalex.org/work/W2101911810', 'https://semopenalex.org/work/W2570577251', 'https://semopenalex.org/work/W2334282167', 'https://semopenalex.org/work/W4387714613', 'https://semopenalex.org/work/W2036764408', 'https://semopenalex.org/work/W2167929182', 'https://semopenalex.org/work/W2175711660', 'https://semopenalex.org/work/W2967954306', 'https://semopenalex.org/work/W2982613775', 'https://semopenalex.org/work/W2100586747', 'https://semopenalex.org/work/W2038570675', 'https://semopenalex.org/work/W4390758153', 'https://semopenalex.org/work/W2573269249', 'https://semopenalex.org/work/W3147589610', 'https://semopenalex.org/work/W2011087369', 'https://semopenalex.org/work/W3196284684', 'https://semopenalex.org/work/W1485445045', 'https://semopenalex.org/work/W4391770026', 'https://semopenalex.org/work/W3156877779', 'https://semopenalex.org/work/W2473242321', 'https://semopenalex.org/work/W3006046181', 'https://semopenalex.org/work/W4402836042', 'https://semopenalex.org/work/W2473454588', 'https://semopenalex.org/work/W4224994268', 'https://semopenalex.org/work/W2768420153', 'https://semopenalex.org/work/W4393252675', 'https://semopenalex.org/work/W3141789341', 'https://semopenalex.org/work/W2143818732', 'https://semopenalex.org/work/W2759469946', 'https://semopenalex.org/work/W4225826211', 'https://semopenalex.org/work/W2695892072', 'https://semopenalex.org/work/W2327416585', 'https://semopenalex.org/work/W4399463135', 'https://semopenalex.org/work/W2785923962', 'https://semopenalex.org/work/W2115198688', 'https://semopenalex.org/work/W2095378229', 'https://semopenalex.org/work/W2903985815', 'https://semopenalex.org/work/W2335568438', 'https://semopenalex.org/work/W2951051768', 'https://semopenalex.org/work/W2783173327', 'https://semopenalex.org/work/W2964463995', 'https://semopenalex.org/work/W2393603173', 'https://semopenalex.org/work/W2089235671', 'https://semopenalex.org/work/W2533270794', 'https://semopenalex.org/work/W1781921775', 'https://semopenalex.org/work/W4386249995', 'https://semopenalex.org/work/W4387319244', 'https://semopenalex.org/work/W2522766745', 'https://semopenalex.org/work/W4402125734', 'https://semopenalex.org/work/W4317555541', 'https://semopenalex.org/work/W2920325736', 'https://semopenalex.org/work/W4390204058', 'https://semopenalex.org/work/W3210031557', 'https://semopenalex.org/work/W2519882343', 'https://semopenalex.org/work/W2045885650', 'https://semopenalex.org/work/W4399341408', 'https://semopenalex.org/work/W3156800857', 'https://semopenalex.org/work/W4385832244', 'https://semopenalex.org/work/W2990794959', 'https://semopenalex.org/work/W4386920013', 'https://semopenalex.org/work/W4403182200', 'https://semopenalex.org/work/W3197793222', 'https://semopenalex.org/work/W4282825011', 'https://semopenalex.org/work/W2557139677', 'https://semopenalex.org/work/W3013399598', 'https://semopenalex.org/work/W3160686564', 'https://semopenalex.org/work/W3004954023', 'https://semopenalex.org/work/W2797953332', 'https://semopenalex.org/work/W4403724277', 'https://semopenalex.org/work/W3152943384', 'https://semopenalex.org/work/W4229028795', 'https://semopenalex.org/work/W2511146638', 'https://semopenalex.org/work/W4213077479', 'https://semopenalex.org/work/W2966498804', 'https://semopenalex.org/work/W2022326160', 'https://semopenalex.org/work/W2341987404', 'https://semopenalex.org/work/W4225497412', 'https://semopenalex.org/work/W4390778221', 'https://semopenalex.org/work/W3143148447', 'https://semopenalex.org/work/W2023637192', 'https://semopenalex.org/work/W3080639911', 'https://semopenalex.org/work/W1991274348', 'https://semopenalex.org/work/W4212902180', 'https://semopenalex.org/work/W2383377836', 'https://semopenalex.org/work/W1990457279', 'https://semopenalex.org/work/W4387715010', 'https://semopenalex.org/work/W2277015358', 'https://semopenalex.org/work/W4386918818', 'https://semopenalex.org/work/W2605870759', 'https://semopenalex.org/work/W2063160426', 'https://semopenalex.org/work/W1492042394', 'https://semopenalex.org/work/W2271825901', 'https://semopenalex.org/work/W2037815363', 'https://semopenalex.org/work/W2076438760', 'https://semopenalex.org/work/W2792002389', 'https://semopenalex.org/work/W2137563824', 'https://semopenalex.org/work/W2518984475', 'https://semopenalex.org/work/W3140868540', 'https://semopenalex.org/work/W4390763328', 'https://semopenalex.org/work/W4391895094', 'https://semopenalex.org/work/W4285251260', 'https://semopenalex.org/work/W2046114048', 'https://semopenalex.org/work/W3152870376', 'https://semopenalex.org/work/W2029284131', 'https://semopenalex.org/work/W2621374881', 'https://semopenalex.org/work/W2144892219', 'https://semopenalex.org/work/W2023195652', 'https://semopenalex.org/work/W2804609139', 'https://semopenalex.org/work/W2712995990', 'https://semopenalex.org/work/W4386260739', 'https://semopenalex.org/work/W2887601228', 'https://semopenalex.org/work/W4289821472', 'https://semopenalex.org/work/W2121795575', 'https://semopenalex.org/work/W2349466730', 'https://semopenalex.org/work/W4367663134', 'https://semopenalex.org/work/W4313244937', 'https://semopenalex.org/work/W2932650350', 'https://semopenalex.org/work/W2535549373', 'https://semopenalex.org/work/W1978699422', 'https://semopenalex.org/work/W4367148109', 'https://semopenalex.org/work/W2116800013', 'https://semopenalex.org/work/W4312427776', 'https://semopenalex.org/work/W2056907372', 'https://semopenalex.org/work/W4396783549', 'https://semopenalex.org/work/W2373453410', 'https://semopenalex.org/work/W2972948959', 'https://semopenalex.org/work/W4367148398', 'https://semopenalex.org/work/W4401806242', 'https://semopenalex.org/work/W43217051', 'https://semopenalex.org/work/W4389961028', 'https://semopenalex.org/work/W2114540871', 'https://semopenalex.org/work/W4405937034', 'https://semopenalex.org/work/W2326531986', 'https://semopenalex.org/work/W2800408116', 'https://semopenalex.org/work/W2078714953', 'https://semopenalex.org/work/W2119212601', 'https://semopenalex.org/work/W4205838995', 'https://semopenalex.org/work/W2810470829', 'https://semopenalex.org/work/W4399339526', 'https://semopenalex.org/work/W2966346292', 'https://semopenalex.org/work/W4405270053', 'https://semopenalex.org/work/W3089077757', 'https://semopenalex.org/work/W2921446145', 'https://semopenalex.org/work/W4312837885', 'https://semopenalex.org/work/W2290066430', 'https://semopenalex.org/work/W2803338056', 'https://semopenalex.org/work/W3176436409', 'https://semopenalex.org/work/W2156848415', 'https://semopenalex.org/work/W4390602383', 'https://semopenalex.org/work/W1991497382', 'https://semopenalex.org/work/W2757377912', 'https://semopenalex.org/work/W3115725655', 'https://semopenalex.org/work/W4388551259', 'https://semopenalex.org/work/W1981489703', 'https://semopenalex.org/work/W3193875369', 'https://semopenalex.org/work/W2122864277', 'https://semopenalex.org/work/W4403124399', 'https://semopenalex.org/work/W4386736850', 'https://semopenalex.org/work/W2055837742', 'https://semopenalex.org/work/W4385214694', 'https://semopenalex.org/work/W2561275332', 'https://semopenalex.org/work/W4312466007', 'https://semopenalex.org/work/W4328027566', 'https://semopenalex.org/work/W2887358166', 'https://semopenalex.org/work/W1556213926', 'https://semopenalex.org/work/W4389303997', 'https://semopenalex.org/work/W3040766658', 'https://semopenalex.org/work/W4404670877', 'https://semopenalex.org/work/W2589296175', 'https://semopenalex.org/work/W4392096060', 'https://semopenalex.org/work/W4396817519', 'https://semopenalex.org/work/W4402978247', 'https://semopenalex.org/work/W2624040609', 'https://semopenalex.org/work/W3186776699', 'https://semopenalex.org/work/W4226107162', 'https://semopenalex.org/work/W4401069975', 'https://semopenalex.org/work/W2986174999', 'https://semopenalex.org/work/W1993621621', 'https://semopenalex.org/work/W2547271336', 'https://semopenalex.org/work/W4390777144', 'https://semopenalex.org/work/W2152003934', 'https://semopenalex.org/work/W4296912939', 'https://semopenalex.org/work/W4391877334', 'https://semopenalex.org/work/W4213143207', 'https://semopenalex.org/work/W2085645466', 'https://semopenalex.org/work/W1984984026', 'https://semopenalex.org/work/W2419608502', 'https://semopenalex.org/work/W4387714561', 'https://semopenalex.org/work/W2495190596', 'https://semopenalex.org/work/W2298711843', 'https://semopenalex.org/work/W3206648460', 'https://semopenalex.org/work/W2010955203', 'https://semopenalex.org/work/W4405179870', 'https://semopenalex.org/work/W2104385531', 'https://semopenalex.org/work/W2769916035', 'https://semopenalex.org/work/W2613801228', 'https://semopenalex.org/work/W4389317944', 'https://semopenalex.org/work/W2535129896', 'https://semopenalex.org/work/W2549420274', 'https://semopenalex.org/work/W4392024074', 'https://semopenalex.org/work/W2538882601', 'https://semopenalex.org/work/W3199970339', 'https://semopenalex.org/work/W3197269278', 'https://semopenalex.org/work/W2518181354', 'https://semopenalex.org/work/W3088595531', 'https://semopenalex.org/work/W2395017188', 'https://semopenalex.org/work/W4213429388', 'https://semopenalex.org/work/W2332928857', 'https://semopenalex.org/work/W4210569910', 'https://semopenalex.org/work/W2143110402', 'https://semopenalex.org/work/W2027931215', 'https://semopenalex.org/work/W4400515993', 'https://semopenalex.org/work/W2977054173', 'https://semopenalex.org/work/W4387322936', 'https://semopenalex.org/work/W2539966993', 'https://semopenalex.org/work/W2540006586', 'https://semopenalex.org/work/W1990148059', 'https://semopenalex.org/work/W2804410540', 'https://semopenalex.org/work/W2066280901', 'https://semopenalex.org/work/W2999941952', 'https://semopenalex.org/work/W2983906786', 'https://semopenalex.org/work/W4312614504', 'https://semopenalex.org/work/W3083528472', 'https://semopenalex.org/work/W2912334744', 'https://semopenalex.org/work/W2620634483', 'https://semopenalex.org/work/W3205428400', 'https://semopenalex.org/work/W4396604650', 'https://semopenalex.org/work/W3133565115', 'https://semopenalex.org/work/W2784241930', 'https://semopenalex.org/work/W2154039139', 'https://semopenalex.org/work/W2064850826', 'https://semopenalex.org/work/W2782998407', 'https://semopenalex.org/work/W2799485966', 'https://semopenalex.org/work/W2118701267', 'https://semopenalex.org/work/W2344052410', 'https://semopenalex.org/work/W3085844533', 'https://semopenalex.org/work/W2039365023', 'https://semopenalex.org/work/W2779973510', 'https://semopenalex.org/work/W3144172827', 'https://semopenalex.org/work/W4367147664', 'https://semopenalex.org/work/W2916900328', 'https://semopenalex.org/work/W2010049933', 'https://semopenalex.org/work/W2949306598', 'https://semopenalex.org/work/W2321042880', 'https://semopenalex.org/work/W4296916443', 'https://semopenalex.org/work/W2946047926', 'https://semopenalex.org/work/W2100819606', 'https://semopenalex.org/work/W2004984354', 'https://semopenalex.org/work/W2905616463', 'https://semopenalex.org/work/W4393033575', 'https://semopenalex.org/work/W2964765424', 'https://semopenalex.org/work/W2900379070', 'https://semopenalex.org/work/W4390778218', 'https://semopenalex.org/work/W2906372377', 'https://semopenalex.org/work/W2129096944', 'https://semopenalex.org/work/W3181963703', 'https://semopenalex.org/work/W1972594074', 'https://semopenalex.org/work/W2737405495', 'https://semopenalex.org/work/W4205522738', 'https://semopenalex.org/work/W2017487069', 'https://semopenalex.org/work/W4328028090', 'https://semopenalex.org/work/W3142830832', 'https://semopenalex.org/work/W2528623020', 'https://semopenalex.org/work/W4392207726', 'https://semopenalex.org/work/W3135039935', 'https://semopenalex.org/work/W2051784811', 'https://semopenalex.org/work/W2145101624', 'https://semopenalex.org/work/W4313306257', 'https://semopenalex.org/work/W2786607830', 'https://semopenalex.org/work/W2036128771', 'https://semopenalex.org/work/W4288039534', 'https://semopenalex.org/work/W4393034258', 'https://semopenalex.org/work/W2883689704', 'https://semopenalex.org/work/W4378805022', 'https://semopenalex.org/work/W2808159133', 'https://semopenalex.org/work/W4365808277', 'https://semopenalex.org/work/W4285548139', 'https://semopenalex.org/work/W2158244986', 'https://semopenalex.org/work/W2016629668', 'https://semopenalex.org/work/W3117499383', 'https://semopenalex.org/work/W4328012044', 'https://semopenalex.org/work/W4293211890', 'https://semopenalex.org/work/W4282837228', 'https://semopenalex.org/work/W2564919106', 'https://semopenalex.org/work/W4285055114', 'https://semopenalex.org/work/W2128477511', 'https://semopenalex.org/work/W4296441394', 'https://semopenalex.org/work/W4206221314', 'https://semopenalex.org/work/W2737288996', 'https://semopenalex.org/work/W2137121156', 'https://semopenalex.org/work/W3200805258', 'https://semopenalex.org/work/W1968665462', 'https://semopenalex.org/work/W2141441280', 'https://semopenalex.org/work/W4388837994', 'https://semopenalex.org/work/W3086256320', 'https://semopenalex.org/work/W2031326270', 'https://semopenalex.org/work/W4393174751', 'https://semopenalex.org/work/W2116843437', 'https://semopenalex.org/work/W1971957085', 'https://semopenalex.org/work/W2028756273', 'https://semopenalex.org/work/W2188557470', 'https://semopenalex.org/work/W2995016007', 'https://semopenalex.org/work/W2928810931', 'https://semopenalex.org/work/W4312265249', 'https://semopenalex.org/work/W3167125565', 'https://semopenalex.org/work/W4387023949', 'https://semopenalex.org/work/W2034325389', 'https://semopenalex.org/work/W2167210003', 'https://semopenalex.org/work/W4384917079', 'https://semopenalex.org/work/W4406355769', 'https://semopenalex.org/work/W2095529201', 'https://semopenalex.org/work/W4224321673', 'https://semopenalex.org/work/W2051236310', 'https://semopenalex.org/work/W2289776346', 'https://semopenalex.org/work/W1968455523', 'https://semopenalex.org/work/W4392513104', 'https://semopenalex.org/work/W1990178810', 'https://semopenalex.org/work/W2991588661', 'https://semopenalex.org/work/W4367146924', 'https://semopenalex.org/work/W4295127425', 'https://semopenalex.org/work/W2548217541', 'https://semopenalex.org/work/W2289770078', 'https://semopenalex.org/work/W2174090751', 'https://semopenalex.org/work/W2905349707', 'https://semopenalex.org/work/W2103606916', 'https://semopenalex.org/work/W2533548130', 'https://semopenalex.org/work/W2145337100', 'https://semopenalex.org/work/W4213269113', 'https://semopenalex.org/work/W4210326058', 'https://semopenalex.org/work/W3112944858', 'https://semopenalex.org/work/W4307405043', 'https://semopenalex.org/work/W4385267612', 'https://semopenalex.org/work/W4404958656', 'https://semopenalex.org/work/W4386528085', 'https://semopenalex.org/work/W4386790563', 'https://semopenalex.org/work/W4391072497', 'https://semopenalex.org/work/W2466861718', 'https://semopenalex.org/work/W2081488658', 'https://semopenalex.org/work/W2124863572', 'https://semopenalex.org/work/W3139378559', 'https://semopenalex.org/work/W2181697561', 'https://semopenalex.org/work/W4313534837', 'https://semopenalex.org/work/W4226219986', 'https://semopenalex.org/work/W3005600351', 'https://semopenalex.org/work/W4387697022', 'https://semopenalex.org/work/W2566503827', 'https://semopenalex.org/work/W4328011761', 'https://semopenalex.org/work/W2473050328', 'https://semopenalex.org/work/W4212865190', 'https://semopenalex.org/work/W4387714660', 'https://semopenalex.org/work/W2887046167', 'https://semopenalex.org/work/W2547677547', 'https://semopenalex.org/work/W2529348703', 'https://semopenalex.org/work/W2401510428', 'https://semopenalex.org/work/W4400904607', 'https://semopenalex.org/work/W2151584377', 'https://semopenalex.org/work/W2796524784', 'https://semopenalex.org/work/W4390938914', 'https://semopenalex.org/work/W2120904939', 'https://semopenalex.org/work/W3040466764', 'https://semopenalex.org/work/W1978499995', 'https://semopenalex.org/work/W2118451262', 'https://semopenalex.org/work/W2800613805', 'https://semopenalex.org/work/W2060045560', 'https://semopenalex.org/work/W2605389968', 'https://semopenalex.org/work/W2258995161', 'https://semopenalex.org/work/W4389888434', 'https://semopenalex.org/work/W2562454548', 'https://semopenalex.org/work/W4295046603', 'https://semopenalex.org/work/W3125270863', 'https://semopenalex.org/work/W1525424336', 'https://semopenalex.org/work/W2591061174', 'https://semopenalex.org/work/W2138141935', 'https://semopenalex.org/work/W4402264038', 'https://semopenalex.org/work/W2768917932', 'https://semopenalex.org/work/W2889572683', 'https://semopenalex.org/work/W4297989904', 'https://semopenalex.org/work/W2551309437', 'https://semopenalex.org/work/W3004718696', 'https://semopenalex.org/work/W3110950550', 'https://semopenalex.org/work/W4389692495', 'https://semopenalex.org/work/W2059373588', 'https://semopenalex.org/work/W3016347687', 'https://semopenalex.org/work/W4402466985', 'https://semopenalex.org/work/W2413354569', 'https://semopenalex.org/work/W2292434057', 'https://semopenalex.org/work/W3143088633', 'https://semopenalex.org/work/W2001792450', 'https://semopenalex.org/work/W2002064143', 'https://semopenalex.org/work/W3214254401', 'https://semopenalex.org/work/W2966881022', 'https://semopenalex.org/work/W4404210445', 'https://semopenalex.org/work/W4366987396', 'https://semopenalex.org/work/W4226250318', 'https://semopenalex.org/work/W2000486418', 'https://semopenalex.org/work/W4224245749', 'https://semopenalex.org/work/W4285122724', 'https://semopenalex.org/work/W2997612014', 'https://semopenalex.org/work/W2154565949', 'https://semopenalex.org/work/W4323644072', 'https://semopenalex.org/work/W4318603823', 'https://semopenalex.org/work/W2910852288', 'https://semopenalex.org/work/W4294690843', 'https://semopenalex.org/work/W4312643037', 'https://semopenalex.org/work/W2967537836', 'https://semopenalex.org/work/W2520379429', 'https://semopenalex.org/work/W4386494434', 'https://semopenalex.org/work/W4386352842', 'https://semopenalex.org/work/W4386361261', 'https://semopenalex.org/work/W4367148069', 'https://semopenalex.org/work/W1966645219', 'https://semopenalex.org/work/W2035601794', 'https://semopenalex.org/work/W1857828242', 'https://semopenalex.org/work/W1971616362', 'https://semopenalex.org/work/W2919497189', 'https://semopenalex.org/work/W2964505054', 'https://semopenalex.org/work/W4389161163', 'https://semopenalex.org/work/W2351972364', 'https://semopenalex.org/work/W2139368697', 'https://semopenalex.org/work/W2743477693', 'https://semopenalex.org/work/W4367147772', 'https://semopenalex.org/work/W4392939659', 'https://semopenalex.org/work/W3076344446', 'https://semopenalex.org/work/W2135168342', 'https://semopenalex.org/work/W4220782062', 'https://semopenalex.org/work/W2115497161', 'https://semopenalex.org/work/W2391301195', 'https://semopenalex.org/work/W4205304527', 'https://semopenalex.org/work/W1035642985', 'https://semopenalex.org/work/W2069882645', 'https://semopenalex.org/work/W3215103574', 'https://semopenalex.org/work/W2901820813', 'https://semopenalex.org/work/W2593161952', 'https://semopenalex.org/work/W4387714810', 'https://semopenalex.org/work/W2535770837', 'https://semopenalex.org/work/W4312161546', 'https://semopenalex.org/work/W2538847865', 'https://semopenalex.org/work/W2905049939', 'https://semopenalex.org/work/W2289803878', 'https://semopenalex.org/work/W3134544950', 'https://semopenalex.org/work/W4403635673', 'https://semopenalex.org/work/W3127926476', 'https://semopenalex.org/work/W3163178830', 'https://semopenalex.org/work/W4388286311', 'https://semopenalex.org/work/W4360901644', 'https://semopenalex.org/work/W2168624747', 'https://semopenalex.org/work/W2060658651', 'https://semopenalex.org/work/W3105144424', 'https://semopenalex.org/work/W2557492665', 'https://semopenalex.org/work/W1964959731', 'https://semopenalex.org/work/W4392607874', 'https://semopenalex.org/work/W2887838626', 'https://semopenalex.org/work/W4386766558', 'https://semopenalex.org/work/W4311533450', 'https://semopenalex.org/work/W3184809481', 'https://semopenalex.org/work/W4393034150', 'https://semopenalex.org/work/W4367148117', 'https://semopenalex.org/work/W2291553515', 'https://semopenalex.org/work/W2765287619', 'https://semopenalex.org/work/W3192507507', 'https://semopenalex.org/work/W2110460866', 'https://semopenalex.org/work/W4395684973', 'https://semopenalex.org/work/W2898562797', 'https://semopenalex.org/work/W2941782253', 'https://semopenalex.org/work/W2556760577', 'https://semopenalex.org/work/W4392175577', 'https://semopenalex.org/work/W2115836030', 'https://semopenalex.org/work/W1497963603', 'https://semopenalex.org/work/W2561915240', 'https://semopenalex.org/work/W2120547457', 'https://semopenalex.org/work/W2134725794', 'https://semopenalex.org/work/W2289787480', 'https://semopenalex.org/work/W2901539986', 'https://semopenalex.org/work/W3017282193', 'https://semopenalex.org/work/W4404979988', 'https://semopenalex.org/work/W4320068529', 'https://semopenalex.org/work/W2920565953', 'https://semopenalex.org/work/W1963528679', 'https://semopenalex.org/work/W3201511537', 'https://semopenalex.org/work/W2291708615', 'https://semopenalex.org/work/W4282831232', 'https://semopenalex.org/work/W3018428182', 'https://semopenalex.org/work/W3033096606', 'https://semopenalex.org/work/W3047065943', 'https://semopenalex.org/work/W2970760542', 'https://semopenalex.org/work/W2782853409', 'https://semopenalex.org/work/W4402834371', 'https://semopenalex.org/work/W1505692277', 'https://semopenalex.org/work/W2517312722', 'https://semopenalex.org/work/W2915318915', 'https://semopenalex.org/work/W2904825736', 'https://semopenalex.org/work/W4399881765', 'https://semopenalex.org/work/W2782839007', 'https://semopenalex.org/work/W3216386918', 'https://semopenalex.org/work/W4312363564', 'https://semopenalex.org/work/W4213124543', 'https://semopenalex.org/work/W2729083427', 'https://semopenalex.org/work/W3023366540', 'https://semopenalex.org/work/W3041302202', 'https://semopenalex.org/work/W3196195396', 'https://semopenalex.org/work/W2029634930', 'https://semopenalex.org/work/W2888258411', 'https://semopenalex.org/work/W4312387367', 'https://semopenalex.org/work/W3034006897', 'https://semopenalex.org/work/W2719102196', 'https://semopenalex.org/work/W2566566708', 'https://semopenalex.org/work/W2998591860', 'https://semopenalex.org/work/W2168645783']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2787117880', 'https://semopenalex.org/work/W3114189270', 'https://semopenalex.org/work/W4400527808', 'https://semopenalex.org/work/W4221162127', 'https://semopenalex.org/work/W2888163892', 'https://semopenalex.org/work/W4385489024', 'https://semopenalex.org/work/W3188528620', 'https://semopenalex.org/work/W4386044088', 'https://semopenalex.org/work/W3014613652', 'https://semopenalex.org/work/W2986822919', 'https://semopenalex.org/work/W3101597364', 'https://semopenalex.org/work/W4404988180', 'https://semopenalex.org/work/W2997573805', 'https://semopenalex.org/work/W2972424355', 'https://semopenalex.org/work/W3035684383', 'https://semopenalex.org/work/W3022437633', 'https://semopenalex.org/work/W4320009753', 'https://semopenalex.org/work/W2913466142', 'https://semopenalex.org/work/W3137123492', 'https://semopenalex.org/work/W4224014834', 'https://semopenalex.org/work/W3136579074', 'https://semopenalex.org/work/W3126451397', 'https://semopenalex.org/work/W3007894033', 'https://semopenalex.org/work/W3139499926', 'https://semopenalex.org/work/W3195437714', 'https://semopenalex.org/work/W2996574577', 'https://semopenalex.org/work/W4394948067', 'https://semopenalex.org/work/W3212725128', 'https://semopenalex.org/work/W3209110530', 'https://semopenalex.org/work/W4252150734', 'https://semopenalex.org/work/W3088160891', 'https://semopenalex.org/work/W2969182950', 'https://semopenalex.org/work/W4293585133', 'https://semopenalex.org/work/W3207776446', 'https://semopenalex.org/work/W4312293932', 'https://semopenalex.org/work/W4287068220', 'https://semopenalex.org/work/W4395687580', 'https://semopenalex.org/work/W4200628991', 'https://semopenalex.org/work/W3156185860', 'https://semopenalex.org/work/W4398156585', 'https://semopenalex.org/work/W4391980038', 'https://semopenalex.org/work/W4402904139', 'https://semopenalex.org/work/W4200560875', 'https://semopenalex.org/work/W3182129567', 'https://semopenalex.org/work/W3215869014', 'https://semopenalex.org/work/W3158615621', 'https://semopenalex.org/work/W3185989052', 'https://semopenalex.org/work/W4287822968', 'https://semopenalex.org/work/W3184989806', 'https://semopenalex.org/work/W4400527492', 'https://semopenalex.org/work/W3187413453', 'https://semopenalex.org/work/W4298544123', 'https://semopenalex.org/work/W4389519214', 'https://semopenalex.org/work/W4390874790', 'https://semopenalex.org/work/W4312262410', 'https://semopenalex.org/work/W4200338016', 'https://semopenalex.org/work/W4251566388', 'https://semopenalex.org/work/W3008209689', 'https://semopenalex.org/work/W4301131967', 'https://semopenalex.org/work/W3178180605', 'https://semopenalex.org/work/W4293161686', 'https://semopenalex.org/work/W3170528657', 'https://semopenalex.org/work/W4394647969', 'https://semopenalex.org/work/W3203158837', 'https://semopenalex.org/work/W4385764233', 'https://semopenalex.org/work/W3034765865', 'https://semopenalex.org/work/W4312705355', 'https://semopenalex.org/work/W3158336705', 'https://semopenalex.org/work/W4287081849', 'https://semopenalex.org/work/W4396913892', 'https://semopenalex.org/work/W3046138787', 'https://semopenalex.org/work/W4287822736', 'https://semopenalex.org/work/W4286783899', 'https://semopenalex.org/work/W4312541592', 'https://semopenalex.org/work/W3126473778', 'https://semopenalex.org/work/W4288864169', 'https://semopenalex.org/work/W4312987540', 'https://semopenalex.org/work/W4221139182', 'https://semopenalex.org/work/W4384807954', 'https://semopenalex.org/work/W3100717519', 'https://semopenalex.org/work/W3013080309', 'https://semopenalex.org/work/W4392933323', 'https://semopenalex.org/work/W4289785280', 'https://semopenalex.org/work/W4283695942', 'https://semopenalex.org/work/W3204322065', 'https://semopenalex.org/work/W4394948053', 'https://semopenalex.org/work/W4287141413', 'https://semopenalex.org/work/W3181073899', 'https://semopenalex.org/work/W3161716357', 'https://semopenalex.org/work/W3175370919', 'https://semopenalex.org/work/W3153883354', 'https://semopenalex.org/work/W3021881370', 'https://semopenalex.org/work/W4288853838', 'https://semopenalex.org/work/W4386044022', 'https://semopenalex.org/work/W3015075688', 'https://semopenalex.org/work/W3089582082', 'https://semopenalex.org/work/W4230527737', 'https://semopenalex.org/work/W3013092573', 'https://semopenalex.org/work/W4287822940', 'https://semopenalex.org/work/W4287990567', 'https://semopenalex.org/work/W4287263991', 'https://semopenalex.org/work/W4400527591', 'https://semopenalex.org/work/W3195626503', 'https://semopenalex.org/work/W4292829106', 'https://semopenalex.org/work/W4306178227', 'https://semopenalex.org/work/W3209714413', 'https://semopenalex.org/work/W4386069017', 'https://semopenalex.org/work/W2941870244', 'https://semopenalex.org/work/W2799020610', 'https://semopenalex.org/work/W4287208746', 'https://semopenalex.org/work/W4297823196', 'https://semopenalex.org/work/W4385002722', 'https://semopenalex.org/work/W4288897652', 'https://semopenalex.org/work/W4400527813', 'https://semopenalex.org/work/W4319336332', 'https://semopenalex.org/work/W4237531552', 'https://semopenalex.org/work/W4385484931', 'https://semopenalex.org/work/W3128169604', 'https://semopenalex.org/work/W4285563099', 'https://semopenalex.org/work/W4391630218', 'https://semopenalex.org/work/W4392488099', 'https://semopenalex.org/work/W2976881356', 'https://semopenalex.org/work/W3120808211', 'https://semopenalex.org/work/W4287070342', 'https://semopenalex.org/work/W4402502660', 'https://semopenalex.org/work/W2972050850', 'https://semopenalex.org/work/W4312903731', 'https://semopenalex.org/work/W4289550833', 'https://semopenalex.org/work/W2937532208', 'https://semopenalex.org/work/W4309873272', 'https://semopenalex.org/work/W4406524575', 'https://semopenalex.org/work/W3120604548', 'https://semopenalex.org/work/W4390190325', 'https://semopenalex.org/work/W4287271714', 'https://semopenalex.org/work/W4302012844', 'https://semopenalex.org/work/W3161569725', 'https://semopenalex.org/work/W4390189793', 'https://semopenalex.org/work/W3139116348', 'https://semopenalex.org/work/W4226484154', 'https://semopenalex.org/work/W3103017991', 'https://semopenalex.org/work/W4390190222', 'https://semopenalex.org/work/W3081562204', 'https://semopenalex.org/work/W4361807104', 'https://semopenalex.org/work/W2781902187', 'https://semopenalex.org/work/W3193694068', 'https://semopenalex.org/work/W3133932964', 'https://semopenalex.org/work/W4366198559', 'https://semopenalex.org/work/W2962689474', 'https://semopenalex.org/work/W3034875137', 'https://semopenalex.org/work/W4287864395', 'https://semopenalex.org/work/W4287854900', 'https://semopenalex.org/work/W4287659757', 'https://semopenalex.org/work/W4287679359', 'https://semopenalex.org/work/W4390874573', 'https://semopenalex.org/work/W2983383098', 'https://semopenalex.org/work/W4392971989', 'https://semopenalex.org/work/W4385714105', 'https://semopenalex.org/work/W3000280594', 'https://semopenalex.org/work/W4396814528', 'https://semopenalex.org/work/W4297748315', 'https://semopenalex.org/work/W3035434014', 'https://semopenalex.org/work/W4385801394', 'https://semopenalex.org/work/W4288854368', 'https://semopenalex.org/work/W2895638065', 'https://semopenalex.org/work/W4226112052', 'https://semopenalex.org/work/W4287205368', 'https://semopenalex.org/work/W2995697759', 'https://semopenalex.org/work/W3205150709', 'https://semopenalex.org/work/W3013912585', 'https://semopenalex.org/work/W3107972479', 'https://semopenalex.org/work/W4287081323', 'https://semopenalex.org/work/W3136988982', 'https://semopenalex.org/work/W4288023982', 'https://semopenalex.org/work/W4401415202', 'https://semopenalex.org/work/W4200024628', 'https://semopenalex.org/work/W4320036968', 'https://semopenalex.org/work/W4224928639', 'https://semopenalex.org/work/W4386114434', 'https://semopenalex.org/work/W3185096436', 'https://semopenalex.org/work/W3210107892', 'https://semopenalex.org/work/W4286911846']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W4224295260', 'https://semopenalex.org/work/W4399991068', 'https://semopenalex.org/work/W4213455810', 'https://semopenalex.org/work/W4392473011', 'https://semopenalex.org/work/W4200494113', 'https://semopenalex.org/work/W4281670064', 'https://semopenalex.org/work/W3158973558', 'https://semopenalex.org/work/W3172648176']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W4390604119', 'https://semopenalex.org/work/W4403094633', 'https://semopenalex.org/work/W4312804251', 'https://semopenalex.org/work/W4386065896']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W4406802119', 'https://semopenalex.org/work/W4392180008', 'https://semopenalex.org/work/W4406620652', 'https://semopenalex.org/work/W4405564152', 'https://semopenalex.org/work/W4391680987', 'https://semopenalex.org/work/W4401879044', 'https://semopenalex.org/work/W4405643736', 'https://semopenalex.org/work/W4396509789', 'https://semopenalex.org/work/W4404839780', 'https://semopenalex.org/work/W4404849982', 'https://semopenalex.org/work/W4405718129', 'https://semopenalex.org/work/W4391903798']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W4400410445', 'https://semopenalex.org/work/W4399070942', 'https://semopenalex.org/work/W4391010236', 'https://semopenalex.org/work/W4400410989', 'https://semopenalex.org/work/W4396787938', 'https://semopenalex.org/work/W4391928869']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W4283322066', 'https://semopenalex.org/work/W4376171783', 'https://semopenalex.org/work/W4376210033', 'https://semopenalex.org/work/W3108935870', 'https://semopenalex.org/work/W3008842679', 'https://semopenalex.org/work/W3140085153', 'https://semopenalex.org/work/W3095401597', 'https://semopenalex.org/work/W4283320724', 'https://semopenalex.org/work/W4362502510', 'https://semopenalex.org/work/W4321503169', 'https://semopenalex.org/work/W4362464651', 'https://semopenalex.org/work/W4362464600', 'https://semopenalex.org/work/W4321230650']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/source/S101949793', 'https://semopenalex.org/source/S4210184905', 'https://semopenalex.org/source/S4210177502', 'https://semopenalex.org/source/S1250476', 'https://semopenalex.org/source/S4306402641', 'https://semopenalex.org/source/S4306417563', 'https://semopenalex.org/source/S4210219776', 'https://semopenalex.org/source/S34838331', 'https://semopenalex.org/source/S4306418564', 'https://semopenalex.org/source/S4306402512', 'https://semopenalex.org/source/S30128005', 'https://semopenalex.org/source/S85375271', 'https://semopenalex.org/source/S153984684', 'https://semopenalex.org/source/S106296714', 'https://semopenalex.org/source/S4210233398', 'https://semopenalex.org/source/S37879656', 'https://semopenalex.org/source/S2764455111', 'https://semopenalex.org/source/S4210177346', 'https://semopenalex.org/source/S4210187232', 'https://semopenalex.org/source/S86192639', 'https://semopenalex.org/source/S4210191760', 'https://semopenalex.org/source/S4306418113', 'https://semopenalex.org/source/S2738664114', 'https://semopenalex.org/source/S4306401280', 'https://semopenalex.org/source/S4306400562', 'https://semopenalex.org/source/S4306400194', 'https://semopenalex.org/source/S4363608934', 'https://semopenalex.org/source/S63392143', 'https://semopenalex.org/source/S4210170441', 'https://semopenalex.org/source/S52395412', 'https://semopenalex.org/source/S116972989', 'https://semopenalex.org/source/S136993123', 'https://semopenalex.org/source/S120348307', 'https://semopenalex.org/source/S4306525036', 'https://semopenalex.org/source/S11065456', 'https://semopenalex.org/source/S4210187899', 'https://semopenalex.org/source/S4306421096', 'https://semopenalex.org/source/S4210197804', 'https://semopenalex.org/source/S4306417857', 'https://semopenalex.org/source/S4306402450', 'https://semopenalex.org/source/S60711021', 'https://semopenalex.org/source/S140982614', 'https://semopenalex.org/source/S4306463937', 'https://semopenalex.org/source/S4306400483', 'https://semopenalex.org/source/S4306419550', 'https://semopenalex.org/source/S4210175514', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S186357190', 'https://semopenalex.org/source/S157921468', 'https://semopenalex.org/source/S4210174798', 'https://semopenalex.org/source/S4306400349', 'https://semopenalex.org/source/S157146593', 'https://semopenalex.org/source/S4363605881', 'https://semopenalex.org/source/S4210175912', 'https://semopenalex.org/source/S4210177528', 'https://semopenalex.org/source/S4306524001', 'https://semopenalex.org/source/S2485537415', 'https://semopenalex.org/source/S158797327', 'https://semopenalex.org/source/S129236917', 'https://semopenalex.org/source/S157670870', 'https://semopenalex.org/source/S4306420911', 'https://semopenalex.org/source/S4306419875', 'https://semopenalex.org/source/S64245694', 'https://semopenalex.org/source/S207090427', 'https://semopenalex.org/source/S96783963', 'https://semopenalex.org/source/S2764435056', 'https://semopenalex.org/source/S115004586', 'https://semopenalex.org/source/S4306419921', 'https://semopenalex.org/source/S4306421051', 'https://semopenalex.org/source/S97833917', 'https://semopenalex.org/source/S58563349', 'https://semopenalex.org/source/S126644992', 'https://semopenalex.org/source/S4210194901', 'https://semopenalex.org/source/S36560696', 'https://semopenalex.org/source/S106148199', 'https://semopenalex.org/source/S147790641']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/source/S4306420436', 'https://semopenalex.org/source/S4210235676', 'https://semopenalex.org/source/S4210239725', 'https://semopenalex.org/source/S2764696622', 'https://semopenalex.org/source/S4210173311', 'https://semopenalex.org/source/S4306420780', 'https://semopenalex.org/source/S2764905038', 'https://semopenalex.org/source/S4306419152', 'https://semopenalex.org/source/S4306532718', 'https://semopenalex.org/source/S4306400662', 'https://semopenalex.org/source/S4306400562', 'https://semopenalex.org/source/S4210226000', 'https://semopenalex.org/source/S4306400194', 'https://semopenalex.org/source/S139930977', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S4306535130', 'https://semopenalex.org/source/S4306530687', 'https://semopenalex.org/source/S4210185096', 'https://semopenalex.org/source/S4306402512', 'https://semopenalex.org/source/S4377196258', 'https://semopenalex.org/source/S18088403', 'https://semopenalex.org/source/S4306418416', 'https://semopenalex.org/source/S106296714']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/source/S4210212400', 'https://semopenalex.org/source/S4363608614', 'https://semopenalex.org/source/S4363607711', 'https://semopenalex.org/source/S2495878607', 'https://semopenalex.org/source/S975621743', 'https://semopenalex.org/source/S4363608918', 'https://semopenalex.org/source/S4210214825', 'https://semopenalex.org/source/S4210213674', 'https://semopenalex.org/source/S21313077', 'https://semopenalex.org/source/S177430994', 'https://semopenalex.org/source/S4363607705', 'https://semopenalex.org/source/S68719679', 'https://semopenalex.org/source/S4210226272', 'https://semopenalex.org/source/S4363607712', 'https://semopenalex.org/source/S106296714', 'https://semopenalex.org/source/S178916657', 'https://semopenalex.org/source/S4210195248', 'https://semopenalex.org/source/S2595095599', 'https://semopenalex.org/source/S4210171255', 'https://semopenalex.org/source/S4306497580', 'https://semopenalex.org/source/S4210211936', 'https://semopenalex.org/source/S2764455111', 'https://semopenalex.org/source/S91329792', 'https://semopenalex.org/source/S56112914', 'https://semopenalex.org/source/S4363608116', 'https://semopenalex.org/source/S4306401722', 'https://semopenalex.org/source/S92163612', 'https://semopenalex.org/source/S131921510', 'https://semopenalex.org/source/S2764900261', 'https://semopenalex.org/source/S4210169774', 'https://semopenalex.org/source/S2764905038', 'https://semopenalex.org/source/S4306401280', 'https://semopenalex.org/source/S4363608034', 'https://semopenalex.org/source/S4306464320', 'https://semopenalex.org/source/S4363607702', 'https://semopenalex.org/source/S4306400194', 'https://semopenalex.org/source/S4363608199', 'https://semopenalex.org/source/S45696439', 'https://semopenalex.org/source/S4306400806', 'https://semopenalex.org/source/S76152103', 'https://semopenalex.org/source/S131145815', 'https://semopenalex.org/source/S41486457', 'https://semopenalex.org/source/S4210233094', 'https://semopenalex.org/source/S58778951', 'https://semopenalex.org/source/S2764763012', 'https://semopenalex.org/source/S4210212235', 'https://semopenalex.org/source/S124503262', 'https://semopenalex.org/source/S15952048', 'https://semopenalex.org/source/S144091109', 'https://semopenalex.org/source/S111927887', 'https://semopenalex.org/source/S4306525036', 'https://semopenalex.org/source/S4363608837', 'https://semopenalex.org/source/S52732750', 'https://semopenalex.org/source/S179591353', 'https://semopenalex.org/source/S45281609', 'https://semopenalex.org/source/S4306402118', 'https://semopenalex.org/source/S195488530', 'https://semopenalex.org/source/S4210191458', 'https://semopenalex.org/source/S4306400385', 'https://semopenalex.org/source/S133768115', 'https://semopenalex.org/source/S4210211086', 'https://semopenalex.org/source/S34730769', 'https://semopenalex.org/source/S4306462788', 'https://semopenalex.org/source/S62507282', 'https://semopenalex.org/source/S4306463937', 'https://semopenalex.org/source/S4363607828', 'https://semopenalex.org/source/S4306463409', 'https://semopenalex.org/source/S4363607759', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S4306463687', 'https://semopenalex.org/source/S137468011', 'https://semopenalex.org/source/S201921491', 'https://semopenalex.org/source/S116420536', 'https://semopenalex.org/source/S4210240769', 'https://semopenalex.org/source/S183492911', 'https://semopenalex.org/source/S157664362', 'https://semopenalex.org/source/S4306402651', 'https://semopenalex.org/source/S4306419999', 'https://semopenalex.org/source/S4306400349', 'https://semopenalex.org/source/S4306419250', 'https://semopenalex.org/source/S202381698', 'https://semopenalex.org/source/S11296630', 'https://semopenalex.org/source/S4210224236', 'https://semopenalex.org/source/S4363607734', 'https://semopenalex.org/source/S4306462995', 'https://semopenalex.org/source/S2764696622', 'https://semopenalex.org/source/S84339699', 'https://semopenalex.org/source/S4210179954', 'https://semopenalex.org/source/S4306417879', 'https://semopenalex.org/source/S104717114', 'https://semopenalex.org/source/S4210212310', 'https://semopenalex.org/source/S4306533995', 'https://semopenalex.org/source/S4306463708', 'https://semopenalex.org/source/S170217976', 'https://semopenalex.org/source/S185008460', 'https://semopenalex.org/source/S107964287', 'https://semopenalex.org/source/S4210205812']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2952648029', 'https://semopenalex.org/work/W2535846100', 'https://semopenalex.org/work/W3037554454', 'https://semopenalex.org/work/W2797304630', 'https://semopenalex.org/work/W2770068518', 'https://semopenalex.org/work/W2973574727', 'https://semopenalex.org/work/W2917509290', 'https://semopenalex.org/work/W2579543964', 'https://semopenalex.org/work/W2793980407', 'https://semopenalex.org/work/W2901496061', 'https://semopenalex.org/work/W4230018104', 'https://semopenalex.org/work/W3022089151', 'https://semopenalex.org/work/W2903327589', 'https://semopenalex.org/work/W2789779636']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2056596857', 'https://semopenalex.org/work/W2100356383', 'https://semopenalex.org/work/W1971453213', 'https://semopenalex.org/work/W2146830885', 'https://semopenalex.org/work/W2155878381', 'https://semopenalex.org/work/W4292013335', 'https://semopenalex.org/work/W1584905179', 'https://semopenalex.org/work/W2087682696', 'https://semopenalex.org/work/W2322381474', 'https://semopenalex.org/work/W1536752040', 'https://semopenalex.org/work/W2023461062', 'https://semopenalex.org/work/W2497935614', 'https://semopenalex.org/work/W1575176919', 'https://semopenalex.org/work/W1576645054', 'https://semopenalex.org/work/W1481479141', 'https://semopenalex.org/work/W2402284853', 'https://semopenalex.org/work/W2113401317', 'https://semopenalex.org/work/W1510701494', 'https://semopenalex.org/work/W1815020819', 'https://semopenalex.org/work/W1533819156', 'https://semopenalex.org/work/W2398987174', 'https://semopenalex.org/work/W2768865949', 'https://semopenalex.org/work/W61308258', 'https://semopenalex.org/work/W2055897235', 'https://semopenalex.org/work/W2501927875', 'https://semopenalex.org/work/W2159677278', 'https://semopenalex.org/work/W1575252762', 'https://semopenalex.org/work/W1591196343', 'https://semopenalex.org/work/W1582766542', 'https://semopenalex.org/work/W1504849558', 'https://semopenalex.org/work/W2157877717', 'https://semopenalex.org/work/W2126729622', 'https://semopenalex.org/work/W2274048031', 'https://semopenalex.org/work/W2912169901', 'https://semopenalex.org/work/W2241306549', 'https://semopenalex.org/work/W1482090313', 'https://semopenalex.org/work/W1489802521', 'https://semopenalex.org/work/W2258785380', 'https://semopenalex.org/work/W2001181659', 'https://semopenalex.org/work/W1528198126', 'https://semopenalex.org/work/W1555904986', 'https://semopenalex.org/work/W177260087', 'https://semopenalex.org/work/W1976471311', 'https://semopenalex.org/work/W4236474819', 'https://semopenalex.org/work/W116884602']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W1984905848', 'https://semopenalex.org/work/W2077395955', 'https://semopenalex.org/work/W1912917402', 'https://semopenalex.org/work/W2114233612', 'https://semopenalex.org/work/W1500154637', 'https://semopenalex.org/work/W2102195169', 'https://semopenalex.org/work/W2147427359', 'https://semopenalex.org/work/W2057938070', 'https://semopenalex.org/work/W2084452057', 'https://semopenalex.org/work/W1983778833', 'https://semopenalex.org/work/W1967044695', 'https://semopenalex.org/work/W2146661121', 'https://semopenalex.org/work/W3146442409', 'https://semopenalex.org/work/W1978468648', 'https://semopenalex.org/work/W2058758829', 'https://semopenalex.org/work/W2029593259', 'https://semopenalex.org/work/W2014659753', 'https://semopenalex.org/work/W2005155776', 'https://semopenalex.org/work/W1522292253', 'https://semopenalex.org/work/W2032444227']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/author/A5051221846', 'https://semopenalex.org/author/A5075061218', 'https://semopenalex.org/author/A5062261441', 'https://semopenalex.org/author/A5069922587', 'https://semopenalex.org/author/A5091453565', 'https://semopenalex.org/author/A5064622877', 'https://semopenalex.org/author/A5015356632', 'https://semopenalex.org/author/A5038581932', 'https://semopenalex.org/author/A5023645490', 'https://semopenalex.org/author/A5012375687', 'https://semopenalex.org/author/A5078555911', 'https://semopenalex.org/author/A5086346640', 'https://semopenalex.org/author/A5064387363', 'https://semopenalex.org/author/A5024584252', 'https://semopenalex.org/author/A5034037954', 'https://semopenalex.org/author/A5020939308', 'https://semopenalex.org/author/A5089362779', 'https://semopenalex.org/author/A5042413456', 'https://semopenalex.org/author/A5074486298', 'https://semopenalex.org/author/A5089914165', 'https://semopenalex.org/author/A5093413149', 'https://semopenalex.org/author/A5102720885', 'https://semopenalex.org/author/A5061675674', 'https://semopenalex.org/author/A5112900377', 'https://semopenalex.org/author/A5031601776', 'https://semopenalex.org/author/A5004507308', 'https://semopenalex.org/author/A5093415912', 'https://semopenalex.org/author/A5025632720', 'https://semopenalex.org/author/A5078921853', 'https://semopenalex.org/author/A5093495936', 'https://semopenalex.org/author/A5078461261', 'https://semopenalex.org/author/A5017353478', 'https://semopenalex.org/author/A5028395580', 'https://semopenalex.org/author/A5089983554', 'https://semopenalex.org/author/A5108988435', 'https://semopenalex.org/author/A5044578275', 'https://semopenalex.org/author/A5112907430', 'https://semopenalex.org/author/A5101845418', 'https://semopenalex.org/author/A5092276801', 'https://semopenalex.org/author/A5074393288', 'https://semopenalex.org/author/A5001454735', 'https://semopenalex.org/author/A5043204400', 'https://semopenalex.org/author/A5090529701', 'https://semopenalex.org/author/A5091298748', 'https://semopenalex.org/author/A5082863339', 'https://semopenalex.org/author/A5060768396', 'https://semopenalex.org/author/A5015144665', 'https://semopenalex.org/author/A5101619735', 'https://semopenalex.org/author/A5106808077', 'https://semopenalex.org/author/A5013421545', 'https://semopenalex.org/author/A5112596472', 'https://semopenalex.org/author/A5092106609', 'https://semopenalex.org/author/A5024581040', 'https://semopenalex.org/author/A5111252081', 'https://semopenalex.org/author/A5025631312', 'https://semopenalex.org/author/A5028750310', 'https://semopenalex.org/author/A5051642217', 'https://semopenalex.org/author/A5084373522', 'https://semopenalex.org/author/A5112387040', 'https://semopenalex.org/author/A5084631861', 'https://semopenalex.org/author/A5062553581', 'https://semopenalex.org/author/A5014205279', 'https://semopenalex.org/author/A5074316484', 'https://semopenalex.org/author/A5035247809', 'https://semopenalex.org/author/A5048521450', 'https://semopenalex.org/author/A5114057383', 'https://semopenalex.org/author/A5092276800', 'https://semopenalex.org/author/A5027096307', 'https://semopenalex.org/author/A5071109276', 'https://semopenalex.org/author/A5086787573', 'https://semopenalex.org/author/A5040925885', 'https://semopenalex.org/author/A5080374319', 'https://semopenalex.org/author/A5006430488']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/author/A5083965446', 'https://semopenalex.org/author/A5100329846', 'https://semopenalex.org/author/A5009296051', 'https://semopenalex.org/author/A5065892913', 'https://semopenalex.org/author/A5113994806', 'https://semopenalex.org/author/A5041317074', 'https://semopenalex.org/author/A5104016331', 'https://semopenalex.org/author/A5026731126', 'https://semopenalex.org/author/A5009158005', 'https://semopenalex.org/author/A5059675637', 'https://semopenalex.org/author/A5052745480', 'https://semopenalex.org/author/A5079749382', 'https://semopenalex.org/author/A5074596026', 'https://semopenalex.org/author/A5038114517', 'https://semopenalex.org/author/A5059726739', 'https://semopenalex.org/author/A5073803240', 'https://semopenalex.org/author/A5090679545', 'https://semopenalex.org/author/A5074598788', 'https://semopenalex.org/author/A5100421943', 'https://semopenalex.org/author/A5058321053', 'https://semopenalex.org/author/A5055129023', 'https://semopenalex.org/author/A5112770923', 'https://semopenalex.org/author/A5052423481', 'https://semopenalex.org/author/A5084014359', 'https://semopenalex.org/author/A5030785463', 'https://semopenalex.org/author/A5022617975', 'https://semopenalex.org/author/A5086959491', 'https://semopenalex.org/author/A5003399501', 'https://semopenalex.org/author/A5114257544', 'https://semopenalex.org/author/A5032959229', 'https://semopenalex.org/author/A5062356522', 'https://semopenalex.org/author/A5016341376', 'https://semopenalex.org/author/A5051357966', 'https://semopenalex.org/author/A5018309977', 'https://semopenalex.org/author/A5024594245', 'https://semopenalex.org/author/A5091752605', 'https://semopenalex.org/author/A5109557603', 'https://semopenalex.org/author/A5041359027', 'https://semopenalex.org/author/A5003775830', 'https://semopenalex.org/author/A5070127492', 'https://semopenalex.org/author/A5064864099', 'https://semopenalex.org/author/A5043857690', 'https://semopenalex.org/author/A5109550726', 'https://semopenalex.org/author/A5021047347', 'https://semopenalex.org/author/A5023277983', 'https://semopenalex.org/author/A5074082047', 'https://semopenalex.org/author/A5074308388', 'https://semopenalex.org/author/A5111957985', 'https://semopenalex.org/author/A5005835278', 'https://semopenalex.org/author/A5113653050', 'https://semopenalex.org/author/A5054255632', 'https://semopenalex.org/author/A5088742299', 'https://semopenalex.org/author/A5042981767', 'https://semopenalex.org/author/A5051949776', 'https://semopenalex.org/author/A5084114117', 'https://semopenalex.org/author/A5057228007', 'https://semopenalex.org/author/A5039019367', 'https://semopenalex.org/author/A5024942519', 'https://semopenalex.org/author/A5089722845', 'https://semopenalex.org/author/A5019114258', 'https://semopenalex.org/author/A5103256649', 'https://semopenalex.org/author/A5109557605', 'https://semopenalex.org/author/A5113537073', 'https://semopenalex.org/author/A5102756198', 'https://semopenalex.org/author/A5031002895', 'https://semopenalex.org/author/A5070309508', 'https://semopenalex.org/author/A5040682720', 'https://semopenalex.org/author/A5091510633', 'https://semopenalex.org/author/A5110866135', 'https://semopenalex.org/author/A5110468084', 'https://semopenalex.org/author/A5101223282', 'https://semopenalex.org/author/A5046291387', 'https://semopenalex.org/author/A5025298438', 'https://semopenalex.org/author/A5069142363', 'https://semopenalex.org/author/A5006986556', 'https://semopenalex.org/author/A5040540194', 'https://semopenalex.org/author/A5094850556', 'https://semopenalex.org/author/A5106121692', 'https://semopenalex.org/author/A5026925615', 'https://semopenalex.org/author/A5085424530', 'https://semopenalex.org/author/A5039203221', 'https://semopenalex.org/author/A5016070230', 'https://semopenalex.org/author/A5016460678', 'https://semopenalex.org/author/A5011271066', 'https://semopenalex.org/author/A5108795666', 'https://semopenalex.org/author/A5057173697', 'https://semopenalex.org/author/A5077501197', 'https://semopenalex.org/author/A5100678452', 'https://semopenalex.org/author/A5074735289', 'https://semopenalex.org/author/A5070045696', 'https://semopenalex.org/author/A5042175742', 'https://semopenalex.org/author/A5062087243', 'https://semopenalex.org/author/A5068502658', 'https://semopenalex.org/author/A5044086454', 'https://semopenalex.org/author/A5094966955', 'https://semopenalex.org/author/A5020691490', 'https://semopenalex.org/author/A5026504154', 'https://semopenalex.org/author/A5113750346', 'https://semopenalex.org/author/A5082559019', 'https://semopenalex.org/author/A5061625295', 'https://semopenalex.org/author/A5061791546', 'https://semopenalex.org/author/A5050603750', 'https://semopenalex.org/author/A5035713595', 'https://semopenalex.org/author/A5047323924', 'https://semopenalex.org/author/A5077182059', 'https://semopenalex.org/author/A5056796690', 'https://semopenalex.org/author/A5035328623', 'https://semopenalex.org/author/A5046521916', 'https://semopenalex.org/author/A5013290328', 'https://semopenalex.org/author/A5009095435', 'https://semopenalex.org/author/A5034482692', 'https://semopenalex.org/author/A5101159423', 'https://semopenalex.org/author/A5079894695', 'https://semopenalex.org/author/A5101815353', 'https://semopenalex.org/author/A5002874750', 'https://semopenalex.org/author/A5072916330', 'https://semopenalex.org/author/A5112789076', 'https://semopenalex.org/author/A5018301889', 'https://semopenalex.org/author/A5052057125', 'https://semopenalex.org/author/A5015881314', 'https://semopenalex.org/author/A5029701178', 'https://semopenalex.org/author/A5026800235', 'https://semopenalex.org/author/A5002400587', 'https://semopenalex.org/author/A5066279170', 'https://semopenalex.org/author/A5086794491', 'https://semopenalex.org/author/A5010063800', 'https://semopenalex.org/author/A5100434965', 'https://semopenalex.org/author/A5109056620', 'https://semopenalex.org/author/A5003817085', 'https://semopenalex.org/author/A5070025348', 'https://semopenalex.org/author/A5068131388', 'https://semopenalex.org/author/A5021385837', 'https://semopenalex.org/author/A5079760641', 'https://semopenalex.org/author/A5051259649', 'https://semopenalex.org/author/A5102461997', 'https://semopenalex.org/author/A5075931954', 'https://semopenalex.org/author/A5075602267', 'https://semopenalex.org/author/A5016479362', 'https://semopenalex.org/author/A5033142925', 'https://semopenalex.org/author/A5069695344', 'https://semopenalex.org/author/A5100613030', 'https://semopenalex.org/author/A5110866137', 'https://semopenalex.org/author/A5009982918', 'https://semopenalex.org/author/A5074589032', 'https://semopenalex.org/author/A5112307831', 'https://semopenalex.org/author/A5087123689', 'https://semopenalex.org/author/A5065844089', 'https://semopenalex.org/author/A5052097686', 'https://semopenalex.org/author/A5046366918', 'https://semopenalex.org/author/A5057833118', 'https://semopenalex.org/author/A5007832994', 'https://semopenalex.org/author/A5104053257', 'https://semopenalex.org/author/A5087538704', 'https://semopenalex.org/author/A5043740841', 'https://semopenalex.org/author/A5076209207', 'https://semopenalex.org/author/A5113723639', 'https://semopenalex.org/author/A5047735602', 'https://semopenalex.org/author/A5100458893', 'https://semopenalex.org/author/A5016245222', 'https://semopenalex.org/author/A5088731092', 'https://semopenalex.org/author/A5030988174', 'https://semopenalex.org/author/A5073410087', 'https://semopenalex.org/author/A5109550729', 'https://semopenalex.org/author/A5071699360', 'https://semopenalex.org/author/A5072837074', 'https://semopenalex.org/author/A5110867527', 'https://semopenalex.org/author/A5082724929', 'https://semopenalex.org/author/A5058644115', 'https://semopenalex.org/author/A5103622490', 'https://semopenalex.org/author/A5033256132', 'https://semopenalex.org/author/A5037435544', 'https://semopenalex.org/author/A5030803226', 'https://semopenalex.org/author/A5039816605', 'https://semopenalex.org/author/A5078631705', 'https://semopenalex.org/author/A5100425978', 'https://semopenalex.org/author/A5108112356', 'https://semopenalex.org/author/A5046114637', 'https://semopenalex.org/author/A5069616469', 'https://semopenalex.org/author/A5014845685', 'https://semopenalex.org/author/A5056986371', 'https://semopenalex.org/author/A5059350239', 'https://semopenalex.org/author/A5049348869', 'https://semopenalex.org/author/A5034996813', 'https://semopenalex.org/author/A5111965782', 'https://semopenalex.org/author/A5108795667', 'https://semopenalex.org/author/A5058422878', 'https://semopenalex.org/author/A5109401743', 'https://semopenalex.org/author/A5038398097', 'https://semopenalex.org/author/A5052558062', 'https://semopenalex.org/author/A5044500644', 'https://semopenalex.org/author/A5086046410', 'https://semopenalex.org/author/A5034690905', 'https://semopenalex.org/author/A5094966956', 'https://semopenalex.org/author/A5110126701', 'https://semopenalex.org/author/A5029808771', 'https://semopenalex.org/author/A5017704096', 'https://semopenalex.org/author/A5090065459', 'https://semopenalex.org/author/A5012514876', 'https://semopenalex.org/author/A5083689259', 'https://semopenalex.org/author/A5094850564', 'https://semopenalex.org/author/A5100307045', 'https://semopenalex.org/author/A5072902302', 'https://semopenalex.org/author/A5083067976', 'https://semopenalex.org/author/A5000810401', 'https://semopenalex.org/author/A5025747170', 'https://semopenalex.org/author/A5053913249', 'https://semopenalex.org/author/A5082861248', 'https://semopenalex.org/author/A5061090738', 'https://semopenalex.org/author/A5001078030', 'https://semopenalex.org/author/A5058288079', 'https://semopenalex.org/author/A5035052603', 'https://semopenalex.org/author/A5031522111', 'https://semopenalex.org/author/A5100729482', 'https://semopenalex.org/author/A5100866986', 'https://semopenalex.org/author/A5085024439', 'https://semopenalex.org/author/A5044696172', 'https://semopenalex.org/author/A5021741380', 'https://semopenalex.org/author/A5005357612', 'https://semopenalex.org/author/A5108609396', 'https://semopenalex.org/author/A5035241917', 'https://semopenalex.org/author/A5063043381', 'https://semopenalex.org/author/A5101159425', 'https://semopenalex.org/author/A5021976057', 'https://semopenalex.org/author/A5006412870', 'https://semopenalex.org/author/A5058048101', 'https://semopenalex.org/author/A5060428445', 'https://semopenalex.org/author/A5089032178', 'https://semopenalex.org/author/A5106691602', 'https://semopenalex.org/author/A5081082953', 'https://semopenalex.org/author/A5102836787', 'https://semopenalex.org/author/A5010873632', 'https://semopenalex.org/author/A5055397205', 'https://semopenalex.org/author/A5083460317', 'https://semopenalex.org/author/A5042185262', 'https://semopenalex.org/author/A5048205587', 'https://semopenalex.org/author/A5061146101', 'https://semopenalex.org/author/A5011958240', 'https://semopenalex.org/author/A5041758250', 'https://semopenalex.org/author/A5055281326', 'https://semopenalex.org/author/A5027703220', 'https://semopenalex.org/author/A5094634113', 'https://semopenalex.org/author/A5094850562', 'https://semopenalex.org/author/A5008144788', 'https://semopenalex.org/author/A5080362727', 'https://semopenalex.org/author/A5011287069', 'https://semopenalex.org/author/A5030807574', 'https://semopenalex.org/author/A5081588858', 'https://semopenalex.org/author/A5050944699', 'https://semopenalex.org/author/A5088694364', 'https://semopenalex.org/author/A5094966959', 'https://semopenalex.org/author/A5020453572', 'https://semopenalex.org/author/A5094850550', 'https://semopenalex.org/author/A5072330498', 'https://semopenalex.org/author/A5076724937', 'https://semopenalex.org/author/A5075748306', 'https://semopenalex.org/author/A5109550727', 'https://semopenalex.org/author/A5032100463', 'https://semopenalex.org/author/A5088083982', 'https://semopenalex.org/author/A5101159427', 'https://semopenalex.org/author/A5070430119', 'https://semopenalex.org/author/A5062934322', 'https://semopenalex.org/author/A5054624012', 'https://semopenalex.org/author/A5033517451', 'https://semopenalex.org/author/A5028602300', 'https://semopenalex.org/author/A5028142123', 'https://semopenalex.org/author/A5013993834', 'https://semopenalex.org/author/A5103141604', 'https://semopenalex.org/author/A5046196600', 'https://semopenalex.org/author/A5100698896', 'https://semopenalex.org/author/A5112845086', 'https://semopenalex.org/author/A5045518977', 'https://semopenalex.org/author/A5067664620', 'https://semopenalex.org/author/A5009425558', 'https://semopenalex.org/author/A5031841696', 'https://semopenalex.org/author/A5034384834', 'https://semopenalex.org/author/A5046423444', 'https://semopenalex.org/author/A5100681023', 'https://semopenalex.org/author/A5100353457', 'https://semopenalex.org/author/A5100436760', 'https://semopenalex.org/author/A5013759413', 'https://semopenalex.org/author/A5072570670', 'https://semopenalex.org/author/A5090735746', 'https://semopenalex.org/author/A5094850558', 'https://semopenalex.org/author/A5086297102', 'https://semopenalex.org/author/A5088202063', 'https://semopenalex.org/author/A5021964111', 'https://semopenalex.org/author/A5045348077', 'https://semopenalex.org/author/A5054687162', 'https://semopenalex.org/author/A5015400278', 'https://semopenalex.org/author/A5112770924', 'https://semopenalex.org/author/A5057579122', 'https://semopenalex.org/author/A5042204813', 'https://semopenalex.org/author/A5076828229', 'https://semopenalex.org/author/A5101843778', 'https://semopenalex.org/author/A5087025037', 'https://semopenalex.org/author/A5094850549', 'https://semopenalex.org/author/A5042669324', 'https://semopenalex.org/author/A5041033177', 'https://semopenalex.org/author/A5113619301', 'https://semopenalex.org/author/A5047487369', 'https://semopenalex.org/author/A5087961115', 'https://semopenalex.org/author/A5050785938', 'https://semopenalex.org/author/A5074969316', 'https://semopenalex.org/author/A5052771319', 'https://semopenalex.org/author/A5054904146', 'https://semopenalex.org/author/A5042070270', 'https://semopenalex.org/author/A5101080554', 'https://semopenalex.org/author/A5033806544', 'https://semopenalex.org/author/A5082652832', 'https://semopenalex.org/author/A5019634121', 'https://semopenalex.org/author/A5030697774', 'https://semopenalex.org/author/A5012951140', 'https://semopenalex.org/author/A5047335465', 'https://semopenalex.org/author/A5102455066', 'https://semopenalex.org/author/A5094850559', 'https://semopenalex.org/author/A5110866136', 'https://semopenalex.org/author/A5093323202', 'https://semopenalex.org/author/A5030954130', 'https://semopenalex.org/author/A5074074791', 'https://semopenalex.org/author/A5005192499', 'https://semopenalex.org/author/A5089085275', 'https://semopenalex.org/author/A5001294898', 'https://semopenalex.org/author/A5013031003', 'https://semopenalex.org/author/A5008094693', 'https://semopenalex.org/author/A5102864970', 'https://semopenalex.org/author/A5079962386', 'https://semopenalex.org/author/A5090533480', 'https://semopenalex.org/author/A5101159424', 'https://semopenalex.org/author/A5094850554', 'https://semopenalex.org/author/A5088803193', 'https://semopenalex.org/author/A5014706612', 'https://semopenalex.org/author/A5015977158', 'https://semopenalex.org/author/A5112789075', 'https://semopenalex.org/author/A5052127146', 'https://semopenalex.org/author/A5031092968', 'https://semopenalex.org/author/A5069815943', 'https://semopenalex.org/author/A5102146502', 'https://semopenalex.org/author/A5091888698', 'https://semopenalex.org/author/A5025998224', 'https://semopenalex.org/author/A5033607252', 'https://semopenalex.org/author/A5017841368', 'https://semopenalex.org/author/A5112194416', 'https://semopenalex.org/author/A5031901931', 'https://semopenalex.org/author/A5009102574', 'https://semopenalex.org/author/A5094966947', 'https://semopenalex.org/author/A5001699131', 'https://semopenalex.org/author/A5057083638', 'https://semopenalex.org/author/A5113667088', 'https://semopenalex.org/author/A5007943091', 'https://semopenalex.org/author/A5080195917', 'https://semopenalex.org/author/A5020565600', 'https://semopenalex.org/author/A5063124631', 'https://semopenalex.org/author/A5035030619', 'https://semopenalex.org/author/A5083759644', 'https://semopenalex.org/author/A5075544010', 'https://semopenalex.org/author/A5068682897', 'https://semopenalex.org/author/A5021496374', 'https://semopenalex.org/author/A5020549462', 'https://semopenalex.org/author/A5094966960', 'https://semopenalex.org/author/A5110879810', 'https://semopenalex.org/author/A5102676712', 'https://semopenalex.org/author/A5049244926', 'https://semopenalex.org/author/A5110432474', 'https://semopenalex.org/author/A5044848288', 'https://semopenalex.org/author/A5109550728', 'https://semopenalex.org/author/A5049803081', 'https://semopenalex.org/author/A5094850563', 'https://semopenalex.org/author/A5004978878', 'https://semopenalex.org/author/A5011092157', 'https://semopenalex.org/author/A5035602018', 'https://semopenalex.org/author/A5065215412', 'https://semopenalex.org/author/A5100563292', 'https://semopenalex.org/author/A5089044044', 'https://semopenalex.org/author/A5019863108', 'https://semopenalex.org/author/A5081380385', 'https://semopenalex.org/author/A5017945484', 'https://semopenalex.org/author/A5094850557', 'https://semopenalex.org/author/A5088120976', 'https://semopenalex.org/author/A5065662869', 'https://semopenalex.org/author/A5092591629', 'https://semopenalex.org/author/A5012057735', 'https://semopenalex.org/author/A5100531979', 'https://semopenalex.org/author/A5058506527', 'https://semopenalex.org/author/A5072385590', 'https://semopenalex.org/author/A5102185302', 'https://semopenalex.org/author/A5006842195', 'https://semopenalex.org/author/A5101725214', 'https://semopenalex.org/author/A5058473639', 'https://semopenalex.org/author/A5109232422', 'https://semopenalex.org/author/A5033778949', 'https://semopenalex.org/author/A5004095672', 'https://semopenalex.org/author/A5054875158', 'https://semopenalex.org/author/A5094966951', 'https://semopenalex.org/author/A5003036713', 'https://semopenalex.org/author/A5001888075', 'https://semopenalex.org/author/A5108854968', 'https://semopenalex.org/author/A5100308761', 'https://semopenalex.org/author/A5059112151', 'https://semopenalex.org/author/A5044990862', 'https://semopenalex.org/author/A5100516401', 'https://semopenalex.org/author/A5111299292', 'https://semopenalex.org/author/A5113164291', 'https://semopenalex.org/author/A5089058942', 'https://semopenalex.org/author/A5022809952', 'https://semopenalex.org/author/A5044628664', 'https://semopenalex.org/author/A5044367354', 'https://semopenalex.org/author/A5108754601', 'https://semopenalex.org/author/A5112718452', 'https://semopenalex.org/author/A5028489255', 'https://semopenalex.org/author/A5035708783', 'https://semopenalex.org/author/A5002964350', 'https://semopenalex.org/author/A5112770926', 'https://semopenalex.org/author/A5047576640', 'https://semopenalex.org/author/A5063434943', 'https://semopenalex.org/author/A5040481275', 'https://semopenalex.org/author/A5104356809', 'https://semopenalex.org/author/A5026923870', 'https://semopenalex.org/author/A5089866956', 'https://semopenalex.org/author/A5057180938', 'https://semopenalex.org/author/A5061880585', 'https://semopenalex.org/author/A5011383988', 'https://semopenalex.org/author/A5100976850', 'https://semopenalex.org/author/A5026707758', 'https://semopenalex.org/author/A5059663464', 'https://semopenalex.org/author/A5017310857', 'https://semopenalex.org/author/A5075449266', 'https://semopenalex.org/author/A5070478103', 'https://semopenalex.org/author/A5061668006', 'https://semopenalex.org/author/A5089148668', 'https://semopenalex.org/author/A5073513391', 'https://semopenalex.org/author/A5000203614', 'https://semopenalex.org/author/A5094850561', 'https://semopenalex.org/author/A5094966946', 'https://semopenalex.org/author/A5059992565', 'https://semopenalex.org/author/A5049158387', 'https://semopenalex.org/author/A5073780213', 'https://semopenalex.org/author/A5041111821', 'https://semopenalex.org/author/A5101505215', 'https://semopenalex.org/author/A5060375005', 'https://semopenalex.org/author/A5087402200', 'https://semopenalex.org/author/A5039368373', 'https://semopenalex.org/author/A5101729519', 'https://semopenalex.org/author/A5027345703', 'https://semopenalex.org/author/A5100732392', 'https://semopenalex.org/author/A5111874391', 'https://semopenalex.org/author/A5113721167', 'https://semopenalex.org/author/A5026576007', 'https://semopenalex.org/author/A5011208990', 'https://semopenalex.org/author/A5067291755', 'https://semopenalex.org/author/A5094966952', 'https://semopenalex.org/author/A5079309664', 'https://semopenalex.org/author/A5112770925', 'https://semopenalex.org/author/A5020293284', 'https://semopenalex.org/author/A5040457891', 'https://semopenalex.org/author/A5103267619', 'https://semopenalex.org/author/A5111747866', 'https://semopenalex.org/author/A5020701887', 'https://semopenalex.org/author/A5040926780', 'https://semopenalex.org/author/A5032586796', 'https://semopenalex.org/author/A5111745917', 'https://semopenalex.org/author/A5042189562', 'https://semopenalex.org/author/A5019071895', 'https://semopenalex.org/author/A5057129019', 'https://semopenalex.org/author/A5113555750', 'https://semopenalex.org/author/A5062953965', 'https://semopenalex.org/author/A5021564301', 'https://semopenalex.org/author/A5072296738', 'https://semopenalex.org/author/A5094966945', 'https://semopenalex.org/author/A5077839667', 'https://semopenalex.org/author/A5012860343', 'https://semopenalex.org/author/A5100439502', 'https://semopenalex.org/author/A5112796516', 'https://semopenalex.org/author/A5006284497', 'https://semopenalex.org/author/A5103447072', 'https://semopenalex.org/author/A5064540278', 'https://semopenalex.org/author/A5048999390', 'https://semopenalex.org/author/A5028655113', 'https://semopenalex.org/author/A5015192494', 'https://semopenalex.org/author/A5027348774', 'https://semopenalex.org/author/A5102845298', 'https://semopenalex.org/author/A5101754929', 'https://semopenalex.org/author/A5080079347', 'https://semopenalex.org/author/A5006074944', 'https://semopenalex.org/author/A5020890252', 'https://semopenalex.org/author/A5088560930', 'https://semopenalex.org/author/A5080136207', 'https://semopenalex.org/author/A5112789074', 'https://semopenalex.org/author/A5109040569', 'https://semopenalex.org/author/A5111920218', 'https://semopenalex.org/author/A5103726315', 'https://semopenalex.org/author/A5013796744', 'https://semopenalex.org/author/A5054694688', 'https://semopenalex.org/author/A5109894548', 'https://semopenalex.org/author/A5027694435', 'https://semopenalex.org/author/A5035044634', 'https://semopenalex.org/author/A5100390687', 'https://semopenalex.org/author/A5076222775', 'https://semopenalex.org/author/A5073739308', 'https://semopenalex.org/author/A5017193950', 'https://semopenalex.org/author/A5069829960', 'https://semopenalex.org/author/A5100695007', 'https://semopenalex.org/author/A5054677861', 'https://semopenalex.org/author/A5040341362', 'https://semopenalex.org/author/A5035731144', 'https://semopenalex.org/author/A5003335464', 'https://semopenalex.org/author/A5061493594', 'https://semopenalex.org/author/A5017549278', 'https://semopenalex.org/author/A5112895504', 'https://semopenalex.org/author/A5088935199', 'https://semopenalex.org/author/A5065938167', 'https://semopenalex.org/author/A5000563459', 'https://semopenalex.org/author/A5006214623', 'https://semopenalex.org/author/A5088805136', 'https://semopenalex.org/author/A5088969714', 'https://semopenalex.org/author/A5050409448', 'https://semopenalex.org/author/A5087781429', 'https://semopenalex.org/author/A5010169168', 'https://semopenalex.org/author/A5070309541', 'https://semopenalex.org/author/A5112770922', 'https://semopenalex.org/author/A5065946530', 'https://semopenalex.org/author/A5108322148', 'https://semopenalex.org/author/A5011886931', 'https://semopenalex.org/author/A5007728844', 'https://semopenalex.org/author/A5035879340', 'https://semopenalex.org/author/A5021519204', 'https://semopenalex.org/author/A5057416433', 'https://semopenalex.org/author/A5086630717', 'https://semopenalex.org/author/A5094966953', 'https://semopenalex.org/author/A5057391353', 'https://semopenalex.org/author/A5083932343', 'https://semopenalex.org/author/A5054944358', 'https://semopenalex.org/author/A5022916875', 'https://semopenalex.org/author/A5058021734', 'https://semopenalex.org/author/A5054239026', 'https://semopenalex.org/author/A5003443602', 'https://semopenalex.org/author/A5090198878', 'https://semopenalex.org/author/A5002366144', 'https://semopenalex.org/author/A5112014544', 'https://semopenalex.org/author/A5015181699', 'https://semopenalex.org/author/A5000889165', 'https://semopenalex.org/author/A5004548068', 'https://semopenalex.org/author/A5013975143', 'https://semopenalex.org/author/A5107204848', 'https://semopenalex.org/author/A5002266542', 'https://semopenalex.org/author/A5000045142', 'https://semopenalex.org/author/A5005503619', 'https://semopenalex.org/author/A5065466432', 'https://semopenalex.org/author/A5054833334', 'https://semopenalex.org/author/A5100437036', 'https://semopenalex.org/author/A5080481085', 'https://semopenalex.org/author/A5101558388', 'https://semopenalex.org/author/A5035534381', 'https://semopenalex.org/author/A5101525412', 'https://semopenalex.org/author/A5065213427', 'https://semopenalex.org/author/A5094966948', 'https://semopenalex.org/author/A5110244736', 'https://semopenalex.org/author/A5014584767', 'https://semopenalex.org/author/A5094850551', 'https://semopenalex.org/author/A5019810478', 'https://semopenalex.org/author/A5110866138', 'https://semopenalex.org/author/A5001283900', 'https://semopenalex.org/author/A5007690829', 'https://semopenalex.org/author/A5016680661', 'https://semopenalex.org/author/A5018934854', 'https://semopenalex.org/author/A5071892402', 'https://semopenalex.org/author/A5009940583', 'https://semopenalex.org/author/A5100382191', 'https://semopenalex.org/author/A5075283583', 'https://semopenalex.org/author/A5110225216', 'https://semopenalex.org/author/A5083755757', 'https://semopenalex.org/author/A5075050367', 'https://semopenalex.org/author/A5100350849', 'https://semopenalex.org/author/A5066794150', 'https://semopenalex.org/author/A5048567127', 'https://semopenalex.org/author/A5025851255', 'https://semopenalex.org/author/A5053876673', 'https://semopenalex.org/author/A5072728622', 'https://semopenalex.org/author/A5020223949', 'https://semopenalex.org/author/A5061937018', 'https://semopenalex.org/author/A5048006075', 'https://semopenalex.org/author/A5040920032', 'https://semopenalex.org/author/A5075085355', 'https://semopenalex.org/author/A5094966944', 'https://semopenalex.org/author/A5090185743', 'https://semopenalex.org/author/A5045614803', 'https://semopenalex.org/author/A5049314735', 'https://semopenalex.org/author/A5013806560', 'https://semopenalex.org/author/A5100426981', 'https://semopenalex.org/author/A5025012438', 'https://semopenalex.org/author/A5058899219', 'https://semopenalex.org/author/A5103860234', 'https://semopenalex.org/author/A5101164166', 'https://semopenalex.org/author/A5001240699', 'https://semopenalex.org/author/A5087315126', 'https://semopenalex.org/author/A5030396947', 'https://semopenalex.org/author/A5100610161', 'https://semopenalex.org/author/A5034842369', 'https://semopenalex.org/author/A5010667155', 'https://semopenalex.org/author/A5084544975', 'https://semopenalex.org/author/A5085413987', 'https://semopenalex.org/author/A5039190016', 'https://semopenalex.org/author/A5112770927', 'https://semopenalex.org/author/A5089847337', 'https://semopenalex.org/author/A5087206674', 'https://semopenalex.org/author/A5029732249', 'https://semopenalex.org/author/A5094966950', 'https://semopenalex.org/author/A5029995660', 'https://semopenalex.org/author/A5110970351', 'https://semopenalex.org/author/A5100386180', 'https://semopenalex.org/author/A5069815367', 'https://semopenalex.org/author/A5100428572', 'https://semopenalex.org/author/A5032948315', 'https://semopenalex.org/author/A5059045306', 'https://semopenalex.org/author/A5039301079', 'https://semopenalex.org/author/A5009197679', 'https://semopenalex.org/author/A5076181565', 'https://semopenalex.org/author/A5111246205', 'https://semopenalex.org/author/A5017534073', 'https://semopenalex.org/author/A5004693243', 'https://semopenalex.org/author/A5026946838', 'https://semopenalex.org/author/A5017257513', 'https://semopenalex.org/author/A5001839757', 'https://semopenalex.org/author/A5033358586', 'https://semopenalex.org/author/A5022655755', 'https://semopenalex.org/author/A5025759507', 'https://semopenalex.org/author/A5104053258', 'https://semopenalex.org/author/A5067111142', 'https://semopenalex.org/author/A5114085404', 'https://semopenalex.org/author/A5032040667', 'https://semopenalex.org/author/A5013152760', 'https://semopenalex.org/author/A5009578658', 'https://semopenalex.org/author/A5082932410', 'https://semopenalex.org/author/A5058732387', 'https://semopenalex.org/author/A5021090586', 'https://semopenalex.org/author/A5040530849', 'https://semopenalex.org/author/A5021792918', 'https://semopenalex.org/author/A5077149145', 'https://semopenalex.org/author/A5090437811', 'https://semopenalex.org/author/A5025025481', 'https://semopenalex.org/author/A5039281963', 'https://semopenalex.org/author/A5062058930', 'https://semopenalex.org/author/A5062066146', 'https://semopenalex.org/author/A5082373681', 'https://semopenalex.org/author/A5102775803', 'https://semopenalex.org/author/A5067334214', 'https://semopenalex.org/author/A5072028806', 'https://semopenalex.org/author/A5108134868', 'https://semopenalex.org/author/A5065638410', 'https://semopenalex.org/author/A5005290550', 'https://semopenalex.org/author/A5038742643', 'https://semopenalex.org/author/A5058940849', 'https://semopenalex.org/author/A5058771477', 'https://semopenalex.org/author/A5011092296', 'https://semopenalex.org/author/A5102722569', 'https://semopenalex.org/author/A5038024446', 'https://semopenalex.org/author/A5106680720', 'https://semopenalex.org/author/A5108866418', 'https://semopenalex.org/author/A5088241324', 'https://semopenalex.org/author/A5023770864', 'https://semopenalex.org/author/A5090890994', 'https://semopenalex.org/author/A5023532428', 'https://semopenalex.org/author/A5074788841', 'https://semopenalex.org/author/A5062882537', 'https://semopenalex.org/author/A5094850552', 'https://semopenalex.org/author/A5041661688', 'https://semopenalex.org/author/A5112705691', 'https://semopenalex.org/author/A5041069081', 'https://semopenalex.org/author/A5035006986', 'https://semopenalex.org/author/A5070589510', 'https://semopenalex.org/author/A5100641783', 'https://semopenalex.org/author/A5081846222', 'https://semopenalex.org/author/A5039061395', 'https://semopenalex.org/author/A5083053651', 'https://semopenalex.org/author/A5029196810', 'https://semopenalex.org/author/A5016330520', 'https://semopenalex.org/author/A5112433524', 'https://semopenalex.org/author/A5100418957', 'https://semopenalex.org/author/A5110568866', 'https://semopenalex.org/author/A5015415192', 'https://semopenalex.org/author/A5088485570', 'https://semopenalex.org/author/A5069481232', 'https://semopenalex.org/author/A5036018560', 'https://semopenalex.org/author/A5081627591', 'https://semopenalex.org/author/A5080019669', 'https://semopenalex.org/author/A5013828217', 'https://semopenalex.org/author/A5080593862', 'https://semopenalex.org/author/A5052396894', 'https://semopenalex.org/author/A5110695897', 'https://semopenalex.org/author/A5101941642', 'https://semopenalex.org/author/A5053715191', 'https://semopenalex.org/author/A5066368261', 'https://semopenalex.org/author/A5010466931', 'https://semopenalex.org/author/A5077494978', 'https://semopenalex.org/author/A5027495637', 'https://semopenalex.org/author/A5064932423', 'https://semopenalex.org/author/A5111408885', 'https://semopenalex.org/author/A5016900185', 'https://semopenalex.org/author/A5101466236', 'https://semopenalex.org/author/A5083509514', 'https://semopenalex.org/author/A5067216808', 'https://semopenalex.org/author/A5105408906', 'https://semopenalex.org/author/A5038743559', 'https://semopenalex.org/author/A5087685351', 'https://semopenalex.org/author/A5047925616', 'https://semopenalex.org/author/A5110293736', 'https://semopenalex.org/author/A5032060363', 'https://semopenalex.org/author/A5035676027', 'https://semopenalex.org/author/A5101535147', 'https://semopenalex.org/author/A5046907740', 'https://semopenalex.org/author/A5037590981', 'https://semopenalex.org/author/A5113926166', 'https://semopenalex.org/author/A5005645577', 'https://semop</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/author/A5074307489', 'https://semopenalex.org/author/A5052249316', 'https://semopenalex.org/author/A5100638997', 'https://semopenalex.org/author/A5101601497', 'https://semopenalex.org/author/A5070152860', 'https://semopenalex.org/author/A5050308989', 'https://semopenalex.org/author/A5102928967', 'https://semopenalex.org/author/A5041073042', 'https://semopenalex.org/author/A5018128809', 'https://semopenalex.org/author/A5101617703', 'https://semopenalex.org/author/A5040987266', 'https://semopenalex.org/author/A5002594574', 'https://semopenalex.org/author/A5010181158', 'https://semopenalex.org/author/A5073947585', 'https://semopenalex.org/author/A5101637945', 'https://semopenalex.org/author/A5101812436', 'https://semopenalex.org/author/A5100412598', 'https://semopenalex.org/author/A5005639930', 'https://semopenalex.org/author/A5024456332', 'https://semopenalex.org/author/A5021631329', 'https://semopenalex.org/author/A5101558050', 'https://semopenalex.org/author/A5013325392', 'https://semopenalex.org/author/A5072002680', 'https://semopenalex.org/author/A5058828089', 'https://semopenalex.org/author/A5012621594', 'https://semopenalex.org/author/A5033163346', 'https://semopenalex.org/author/A5068340305', 'https://semopenalex.org/author/A5100375823', 'https://semopenalex.org/author/A5115595561', 'https://semopenalex.org/author/A5077138780', 'https://semopenalex.org/author/A5065848808', 'https://semopenalex.org/author/A5100409885', 'https://semopenalex.org/author/A5103205468', 'https://semopenalex.org/author/A5081145634', 'https://semopenalex.org/author/A5019525050', 'https://semopenalex.org/author/A5081420063', 'https://semopenalex.org/author/A5051192643', 'https://semopenalex.org/author/A5044689090', 'https://semopenalex.org/author/A5030997313', 'https://semopenalex.org/author/A5005007374', 'https://semopenalex.org/author/A5047271595', 'https://semopenalex.org/author/A5100408010', 'https://semopenalex.org/author/A5103047914', 'https://semopenalex.org/author/A5100738980', 'https://semopenalex.org/author/A5025839857', 'https://semopenalex.org/author/A5101468661', 'https://semopenalex.org/author/A5100439996', 'https://semopenalex.org/author/A5100386104', 'https://semopenalex.org/author/A5101264794', 'https://semopenalex.org/author/A5100440010', 'https://semopenalex.org/author/A5107006112', 'https://semopenalex.org/author/A5049142567', 'https://semopenalex.org/author/A5017334961', 'https://semopenalex.org/author/A5026927053', 'https://semopenalex.org/author/A5088725475', 'https://semopenalex.org/author/A5049076146', 'https://semopenalex.org/author/A5103205784', 'https://semopenalex.org/author/A5069596903', 'https://semopenalex.org/author/A5109297018', 'https://semopenalex.org/author/A5050080938', 'https://semopenalex.org/author/A5101660937', 'https://semopenalex.org/author/A5110172698', 'https://semopenalex.org/author/A5033542967', 'https://semopenalex.org/author/A5100301259', 'https://semopenalex.org/author/A5007043113', 'https://semopenalex.org/author/A5102717988', 'https://semopenalex.org/author/A5052199638', 'https://semopenalex.org/author/A5000845080', 'https://semopenalex.org/author/A5100772234', 'https://semopenalex.org/author/A5100349343', 'https://semopenalex.org/author/A5000645139', 'https://semopenalex.org/author/A5032068969', 'https://semopenalex.org/author/A5103761162', 'https://semopenalex.org/author/A5067163535', 'https://semopenalex.org/author/A5100385498', 'https://semopenalex.org/author/A5100758675', 'https://semopenalex.org/author/A5103286574', 'https://semopenalex.org/author/A5103073505', 'https://semopenalex.org/author/A5101636662', 'https://semopenalex.org/author/A5101261545', 'https://semopenalex.org/author/A5077610917', 'https://semopenalex.org/author/A5043798385', 'https://semopenalex.org/author/A5086338440', 'https://semopenalex.org/author/A5081036622', 'https://semopenalex.org/author/A5046237164', 'https://semopenalex.org/author/A5100429004', 'https://semopenalex.org/author/A5084735407', 'https://semopenalex.org/author/A5058738211', 'https://semopenalex.org/author/A5011367069', 'https://semopenalex.org/author/A5101289775', 'https://semopenalex.org/author/A5114778131', 'https://semopenalex.org/author/A5100639062', 'https://semopenalex.org/author/A5033111691', 'https://semopenalex.org/author/A5024821632', 'https://semopenalex.org/author/A5100405159', 'https://semopenalex.org/author/A5015967363', 'https://semopenalex.org/author/A5022677467', 'https://semopenalex.org/author/A5032062525', 'https://semopenalex.org/author/A5103233342', 'https://semopenalex.org/author/A5012561478', 'https://semopenalex.org/author/A5039037722', 'https://semopenalex.org/author/A5060115298', 'https://semopenalex.org/author/A5113160035', 'https://semopenalex.org/author/A5026939932', 'https://semopenalex.org/author/A5101983121', 'https://semopenalex.org/author/A5101655978', 'https://semopenalex.org/author/A5009435651', 'https://semopenalex.org/author/A5087492388', 'https://semopenalex.org/author/A5100365555', 'https://semopenalex.org/author/A5067467896', 'https://semopenalex.org/author/A5077984014', 'https://semopenalex.org/author/A5107864790', 'https://semopenalex.org/author/A5058164381', 'https://semopenalex.org/author/A5069621751', 'https://semopenalex.org/author/A5043801432', 'https://semopenalex.org/author/A5100610450', 'https://semopenalex.org/author/A5049100391', 'https://semopenalex.org/author/A5101556258', 'https://semopenalex.org/author/A5102900280', 'https://semopenalex.org/author/A5100349346', 'https://semopenalex.org/author/A5108459503', 'https://semopenalex.org/author/A5085666756', 'https://semopenalex.org/author/A5072432956', 'https://semopenalex.org/author/A5015836405', 'https://semopenalex.org/author/A5058258996', 'https://semopenalex.org/author/A5100388597', 'https://semopenalex.org/author/A5100401412', 'https://semopenalex.org/author/A5114213934', 'https://semopenalex.org/author/A5000019783', 'https://semopenalex.org/author/A5040272202', 'https://semopenalex.org/author/A5075929099', 'https://semopenalex.org/author/A5022905724', 'https://semopenalex.org/author/A5076516205', 'https://semopenalex.org/author/A5077658936', 'https://semopenalex.org/author/A5100388576', 'https://semopenalex.org/author/A5100426931', 'https://semopenalex.org/author/A5100676331', 'https://semopenalex.org/author/A5101011726', 'https://semopenalex.org/author/A5025292884', 'https://semopenalex.org/author/A5009487151', 'https://semopenalex.org/author/A5100385507', 'https://semopenalex.org/author/A5000381434', 'https://semopenalex.org/author/A5084874990', 'https://semopenalex.org/author/A5100447691', 'https://semopenalex.org/author/A5013438083', 'https://semopenalex.org/author/A5056526226', 'https://semopenalex.org/author/A5100633784', 'https://semopenalex.org/author/A5091706559', 'https://semopenalex.org/author/A5065293581', 'https://semopenalex.org/author/A5102222159', 'https://semopenalex.org/author/A5101555891', 'https://semopenalex.org/author/A5023155310', 'https://semopenalex.org/author/A5100361984', 'https://semopenalex.org/author/A5035359666', 'https://semopenalex.org/author/A5035089987', 'https://semopenalex.org/author/A5027206285', 'https://semopenalex.org/author/A5009455568', 'https://semopenalex.org/author/A5075273130', 'https://semopenalex.org/author/A5040203716', 'https://semopenalex.org/author/A5055422837', 'https://semopenalex.org/author/A5036120394', 'https://semopenalex.org/author/A5002289161', 'https://semopenalex.org/author/A5034057959', 'https://semopenalex.org/author/A5064776947', 'https://semopenalex.org/author/A5090671359', 'https://semopenalex.org/author/A5073965511', 'https://semopenalex.org/author/A5077008083', 'https://semopenalex.org/author/A5047965752', 'https://semopenalex.org/author/A5045087569', 'https://semopenalex.org/author/A5100299966', 'https://semopenalex.org/author/A5048118068', 'https://semopenalex.org/author/A5100388609', 'https://semopenalex.org/author/A5027084532', 'https://semopenalex.org/author/A5100458045', 'https://semopenalex.org/author/A5023035566', 'https://semopenalex.org/author/A5023093639', 'https://semopenalex.org/author/A5100779597', 'https://semopenalex.org/author/A5055149708', 'https://semopenalex.org/author/A5049622460', 'https://semopenalex.org/author/A5110161847', 'https://semopenalex.org/author/A5054115813', 'https://semopenalex.org/author/A5065120715', 'https://semopenalex.org/author/A5100367825', 'https://semopenalex.org/author/A5032194564', 'https://semopenalex.org/author/A5000582109', 'https://semopenalex.org/author/A5090627608', 'https://semopenalex.org/author/A5100523187', 'https://semopenalex.org/author/A5081340873', 'https://semopenalex.org/author/A5053084752', 'https://semopenalex.org/author/A5088708850', 'https://semopenalex.org/author/A5033164669', 'https://semopenalex.org/author/A5102858698', 'https://semopenalex.org/author/A5039326697', 'https://semopenalex.org/author/A5100388581', 'https://semopenalex.org/author/A5024073253', 'https://semopenalex.org/author/A5058257080', 'https://semopenalex.org/author/A5038017715', 'https://semopenalex.org/author/A5052404451', 'https://semopenalex.org/author/A5056980315', 'https://semopenalex.org/author/A5025977354', 'https://semopenalex.org/author/A5009071576', 'https://semopenalex.org/author/A5050748634', 'https://semopenalex.org/author/A5100608460', 'https://semopenalex.org/author/A5077424533', 'https://semopenalex.org/author/A5102014459', 'https://semopenalex.org/author/A5003031253', 'https://semopenalex.org/author/A5101614814', 'https://semopenalex.org/author/A5102859232', 'https://semopenalex.org/author/A5059065212', 'https://semopenalex.org/author/A5079431306', 'https://semopenalex.org/author/A5042235813', 'https://semopenalex.org/author/A5011086593', 'https://semopenalex.org/author/A5103234102', 'https://semopenalex.org/author/A5074540830', 'https://semopenalex.org/author/A5048041198', 'https://semopenalex.org/author/A5089294104', 'https://semopenalex.org/author/A5102987690', 'https://semopenalex.org/author/A5085247180', 'https://semopenalex.org/author/A5101966381', 'https://semopenalex.org/author/A5088498790', 'https://semopenalex.org/author/A5004490190', 'https://semopenalex.org/author/A5100388599', 'https://semopenalex.org/author/A5100447531', 'https://semopenalex.org/author/A5081650066', 'https://semopenalex.org/author/A5100738977', 'https://semopenalex.org/author/A5100408160', 'https://semopenalex.org/author/A5021179945', 'https://semopenalex.org/author/A5100665833', 'https://semopenalex.org/author/A5030490896', 'https://semopenalex.org/author/A5100388617', 'https://semopenalex.org/author/A5042986574', 'https://semopenalex.org/author/A5100458090', 'https://semopenalex.org/author/A5088646345', 'https://semopenalex.org/author/A5006357713', 'https://semopenalex.org/author/A5019450472', 'https://semopenalex.org/author/A5028716858', 'https://semopenalex.org/author/A5069809962', 'https://semopenalex.org/author/A5100443727', 'https://semopenalex.org/author/A5100331488', 'https://semopenalex.org/author/A5100367807', 'https://semopenalex.org/author/A5101308414', 'https://semopenalex.org/author/A5079729956', 'https://semopenalex.org/author/A5059555100', 'https://semopenalex.org/author/A5034794084', 'https://semopenalex.org/author/A5100388627', 'https://semopenalex.org/author/A5102204689', 'https://semopenalex.org/author/A5052981404', 'https://semopenalex.org/author/A5043476448', 'https://semopenalex.org/author/A5100322125', 'https://semopenalex.org/author/A5100394129', 'https://semopenalex.org/author/A5100753041', 'https://semopenalex.org/author/A5100445622', 'https://semopenalex.org/author/A5100447682', 'https://semopenalex.org/author/A5030626281', 'https://semopenalex.org/author/A5101194950', 'https://semopenalex.org/author/A5040850915', 'https://semopenalex.org/author/A5074075949', 'https://semopenalex.org/author/A5102020713', 'https://semopenalex.org/author/A5100459874', 'https://semopenalex.org/author/A5103223639', 'https://semopenalex.org/author/A5100677820', 'https://semopenalex.org/author/A5085393851', 'https://semopenalex.org/author/A5012469172', 'https://semopenalex.org/author/A5100438174', 'https://semopenalex.org/author/A5101540631', 'https://semopenalex.org/author/A5056755949', 'https://semopenalex.org/author/A5100376204', 'https://semopenalex.org/author/A5068122240', 'https://semopenalex.org/author/A5025099559', 'https://semopenalex.org/author/A5010958113', 'https://semopenalex.org/author/A5100753039', 'https://semopenalex.org/author/A5100697624', 'https://semopenalex.org/author/A5016401353', 'https://semopenalex.org/author/A5072456187', 'https://semopenalex.org/author/A5100388716', 'https://semopenalex.org/author/A5101852647', 'https://semopenalex.org/author/A5081886276', 'https://semopenalex.org/author/A5005604635', 'https://semopenalex.org/author/A5067395122', 'https://semopenalex.org/author/A5054753279', 'https://semopenalex.org/author/A5076444296', 'https://semopenalex.org/author/A5021222755', 'https://semopenalex.org/author/A5101612059', 'https://semopenalex.org/author/A5059396373', 'https://semopenalex.org/author/A5045500611', 'https://semopenalex.org/author/A5036986396', 'https://semopenalex.org/author/A5100327487', 'https://semopenalex.org/author/A5061863093', 'https://semopenalex.org/author/A5041961808', 'https://semopenalex.org/author/A5113115887', 'https://semopenalex.org/author/A5100361632', 'https://semopenalex.org/author/A5111956187', 'https://semopenalex.org/author/A5060364305', 'https://semopenalex.org/author/A5115590096', 'https://semopenalex.org/author/A5085611398', 'https://semopenalex.org/author/A5036039721', 'https://semopenalex.org/author/A5011667547', 'https://semopenalex.org/author/A5081449581', 'https://semopenalex.org/author/A5006669765', 'https://semopenalex.org/author/A5066916130', 'https://semopenalex.org/author/A5084868951', 'https://semopenalex.org/author/A5100388644', 'https://semopenalex.org/author/A5100738974', 'https://semopenalex.org/author/A5002503342', 'https://semopenalex.org/author/A5018031899', 'https://semopenalex.org/author/A5043546718', 'https://semopenalex.org/author/A5013103539', 'https://semopenalex.org/author/A5087587101']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2980909386', 'https://semopenalex.org/work/W2108772193', 'https://semopenalex.org/work/W3183223328', 'https://semopenalex.org/work/W2080778070', '2010', 'https://semopenalex.org/work/W3094530900', 'https://semopenalex.org/work/W2768867910', 'https://semopenalex.org/work/W2013683587', 'https://semopenalex.org/work/W4283727356', '2014', '2011', 'https://semopenalex.org/work/W577437274', 'https://semopenalex.org/work/W4229332766', 'https://semopenalex.org/work/W2139123718', 'https://semopenalex.org/work/W4402111012', '2016', '2022', 'https://semopenalex.org/work/W4396774950', 'https://semopenalex.org/work/W2102571324', 'https://semopenalex.org/work/W2898517899', 'https://semopenalex.org/work/W12409091', 'https://semopenalex.org/work/W4200300839', 'https://semopenalex.org/work/W2259681201', 'https://semopenalex.org/work/W3196969850', 'https://semopenalex.org/work/W2979306097', 'https://semopenalex.org/work/W2066079643', 'https://semopenalex.org/work/W2767279489', 'https://semopenalex.org/work/W3042971551', 'https://semopenalex.org/work/W2773748254', 'https://semopenalex.org/work/W3081722247', 'https://semopenalex.org/work/W4283719869', 'https://semopenalex.org/work/W4388442457', 'https://semopenalex.org/work/W2509319904', 'https://semopenalex.org/work/W1992481796', 'https://semopenalex.org/work/W2460327056', 'https://semopenalex.org/work/W1970969056', 'https://semopenalex.org/work/W2166474382', 'https://semopenalex.org/work/W2132176043', 'https://semopenalex.org/work/W4200171350', 'https://semopenalex.org/work/W1997556505', 'https://semopenalex.org/work/W2948301006', 'https://semopenalex.org/work/W1500793049', 'https://semopenalex.org/work/W2948842040', 'https://semopenalex.org/work/W2064795090', '2019', 'https://semopenalex.org/work/W1497260915', 'https://semopenalex.org/work/W4386658225', '2015', '2021', 'https://semopenalex.org/work/W4389542639', 'https://semopenalex.org/work/W2898652465', '2013', 'https://semopenalex.org/work/W2056938644', 'https://semopenalex.org/work/W2883605426', 'https://semopenalex.org/work/W2140663815', 'https://semopenalex.org/work/W2905245385', 'https://semopenalex.org/work/W2810777165', 'https://semopenalex.org/work/W1642534804', 'https://semopenalex.org/work/W3216430907', 'https://semopenalex.org/work/W2469358968', 'https://semopenalex.org/work/W1966638294', 'https://semopenalex.org/work/W4312342218', 'https://semopenalex.org/work/W4405721239', 'https://semopenalex.org/work/W4312466951', '2023', 'https://semopenalex.org/work/W2895960982', 'https://semopenalex.org/work/W2984980523', 'https://semopenalex.org/work/W4225665789', 'https://semopenalex.org/work/W2912718446', 'https://semopenalex.org/work/W2525447956', 'https://semopenalex.org/work/W2137973352', 'https://semopenalex.org/work/W2781983165', '2024', 'https://semopenalex.org/work/W2614777946', 'https://semopenalex.org/work/W2916024294', 'https://semopenalex.org/work/W2062582789', 'https://semopenalex.org/work/W2160324252', 'https://semopenalex.org/work/W2742357289', 'https://semopenalex.org/work/W2574426197', 'https://semopenalex.org/work/W2729358317', 'https://semopenalex.org/work/W2948077456', '2012', 'https://semopenalex.org/work/W4200567986', 'https://semopenalex.org/work/W1517780295', '2008', 'https://semopenalex.org/work/W2040041660', 'https://semopenalex.org/work/W3003315047', 'https://semopenalex.org/work/W2201795542', 'https://semopenalex.org/work/W2943023300', 'https://semopenalex.org/work/W4389542588', 'https://semopenalex.org/work/W3020102474', 'https://semopenalex.org/work/W2146499289', 'https://semopenalex.org/work/W2974391363', 'https://semopenalex.org/work/W2080816360', 'https://semopenalex.org/work/W2103141465', 'https://semopenalex.org/work/W3146074607', 'https://semopenalex.org/work/W2002565472', '2009', 'https://semopenalex.org/work/W2786699184', 'https://semopenalex.org/work/W2056876297', 'https://semopenalex.org/work/W2600317709', 'https://semopenalex.org/work/W1538014482', '2007', 'https://semopenalex.org/work/W2188075483', 'https://semopenalex.org/work/W1524855866', 'https://semopenalex.org/work/W4394843643', 'https://semopenalex.org/work/W1990881389', '2018', 'https://semopenalex.org/work/W2066797554', '2020', '2017', 'https://semopenalex.org/work/W3119942460', 'https://semopenalex.org/work/W2906936538', 'https://semopenalex.org/work/W2559459321', 'https://semopenalex.org/work/W2198531583', 'https://semopenalex.org/work/W1975460851', 'https://semopenalex.org/work/W2517469201', 'https://semopenalex.org/work/W4205142910']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W4220866607', '1983', 'https://semopenalex.org/work/W2794552363', 'https://semopenalex.org/work/W2996424405', '2010', 'https://semopenalex.org/work/W1986447757', 'https://semopenalex.org/work/W333159667', 'https://semopenalex.org/work/W4376878797', 'https://semopenalex.org/work/W3001208788', '2014', '2006', '2011', 'https://semopenalex.org/work/W3003870406', '2016', '2022', 'https://semopenalex.org/work/W2069403900', 'https://semopenalex.org/work/W4300809016', 'https://semopenalex.org/work/W4213054152', 'https://semopenalex.org/work/W2586196676', 'https://semopenalex.org/work/W4239059882', 'https://semopenalex.org/work/W2894658205', 'https://semopenalex.org/work/W2086291403', 'https://semopenalex.org/work/W4390951576', 'https://semopenalex.org/work/W2124884294', 'https://semopenalex.org/work/W2058003955', 'https://semopenalex.org/work/W2997254714', 'https://semopenalex.org/work/W2980431486', 'https://semopenalex.org/work/W3170390068', 'https://semopenalex.org/work/W2067220443', 'https://semopenalex.org/work/W4285149163', 'https://semopenalex.org/work/W4321792691', 'https://semopenalex.org/work/W3009651427', 'https://semopenalex.org/work/W4403148167', 'https://semopenalex.org/work/W103992416', 'https://semopenalex.org/work/W2550600565', 'https://semopenalex.org/work/W3018966866', 'https://semopenalex.org/work/W3205969438', 'https://semopenalex.org/work/W1527780249', 'https://semopenalex.org/work/W3129198752', 'https://semopenalex.org/work/W4200295656', 'https://semopenalex.org/work/W3207358793', 'https://semopenalex.org/work/W4232171693', '2019', 'https://semopenalex.org/work/W2970509049', 'https://semopenalex.org/work/W4292378819', '2015', '2021', 'https://semopenalex.org/work/W2171009049', '2004', '2013', 'https://semopenalex.org/work/W2151014511', 'https://semopenalex.org/work/W2004860585', 'https://semopenalex.org/work/W3007487359', 'https://semopenalex.org/work/W2947887973', 'https://semopenalex.org/work/W3120867123', 'https://semopenalex.org/work/W2794346483', 'https://semopenalex.org/work/W3047226873', 'https://semopenalex.org/work/W2610903992', 'https://semopenalex.org/work/W2734683486', 'https://semopenalex.org/work/W3187488983', '2023', 'https://semopenalex.org/work/W84099738', '2024', 'https://semopenalex.org/work/W2246115839', 'https://semopenalex.org/work/W4285585511', 'https://semopenalex.org/work/W3010786249', 'https://semopenalex.org/work/W2010105821', '2012', '2008', 'https://semopenalex.org/work/W644371662', 'https://semopenalex.org/work/W2258710106', 'https://semopenalex.org/work/W1971349525', 'https://semopenalex.org/work/W3069035240', 'https://semopenalex.org/work/W2737958970', 'https://semopenalex.org/work/W1109050', 'https://semopenalex.org/work/W2955996770', 'https://semopenalex.org/work/W1549914272', 'https://semopenalex.org/work/W4214922121', 'https://semopenalex.org/work/W2319667788', 'https://semopenalex.org/work/W3113261051', 'https://semopenalex.org/work/W2004089424', 'https://semopenalex.org/work/W4400851484', 'https://semopenalex.org/work/W2130875118', 'https://semopenalex.org/work/W4287876838', 'https://semopenalex.org/work/W2122737845', 'https://semopenalex.org/work/W2072306533', 'https://semopenalex.org/work/W4239020865', 'https://semopenalex.org/work/W579278758', '2025', 'https://semopenalex.org/work/W4300970433', 'https://semopenalex.org/work/W4221004647', 'https://semopenalex.org/work/W1961387618', '2005', '2009', 'https://semopenalex.org/work/W2140290607', 'https://semopenalex.org/work/W2142335546', 'https://semopenalex.org/work/W2623352630', 'https://semopenalex.org/work/W1756002337', 'https://semopenalex.org/work/W4229334755', 'https://semopenalex.org/work/W2761369579', 'https://semopenalex.org/work/W3123633695', '2007', 'https://semopenalex.org/work/W2165467091', 'https://semopenalex.org/work/W4321105981', 'https://semopenalex.org/work/W3036594918', 'https://semopenalex.org/work/W3111209168', 'https://semopenalex.org/work/W3193926349', '1994', 'https://semopenalex.org/work/W4394351286', '2018', 'https://semopenalex.org/work/W4406613231', '2020', 'https://semopenalex.org/work/W2783561900', 'https://semopenalex.org/work/W4292377875', '2017', 'https://semopenalex.org/work/W2118255469', 'https://semopenalex.org/work/W4229365934', 'https://semopenalex.org/work/W4245961146', 'https://semopenalex.org/work/W1842188952', 'https://semopenalex.org/work/W2059263765', 'https://semopenalex.org/work/W2754831193', 'https://semopenalex.org/work/W2923244310', 'https://semopenalex.org/work/W2893305614', 'https://semopenalex.org/work/W2790216340', 'https://semopenalex.org/work/W2343633423', '1991']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2734345462', 'https://semopenalex.org/work/W4399991973', 'https://semopenalex.org/work/W4287199679', '2010', 'https://semopenalex.org/work/W2990368351', 'https://semopenalex.org/work/W4386439320', 'https://semopenalex.org/work/W2921556996', 'https://semopenalex.org/work/W3005127776', 'https://semopenalex.org/work/W1616031638', '2014', '2006', 'https://semopenalex.org/work/W4401978390', 'https://semopenalex.org/work/W2622265924', 'https://semopenalex.org/work/W2205191101', '2011', 'https://semopenalex.org/work/W4206891293', '2016', '2022', 'https://semopenalex.org/work/W4399985329', 'https://semopenalex.org/work/W2621391193', 'https://semopenalex.org/work/W110984805', 'https://semopenalex.org/work/W2097450352', 'https://semopenalex.org/work/W2498298891', 'https://semopenalex.org/work/W1729130926', 'https://semopenalex.org/work/W4385822382', 'https://semopenalex.org/work/W2171302802', 'https://semopenalex.org/work/W4312690141', 'https://semopenalex.org/work/W3037369523', 'https://semopenalex.org/work/W4206844749', 'https://semopenalex.org/work/W2922616702', 'https://semopenalex.org/work/W2617659622', 'https://semopenalex.org/work/W2396037699', 'https://semopenalex.org/work/W4282823283', 'https://semopenalex.org/work/W4391589175', 'https://semopenalex.org/work/W844598165', 'https://semopenalex.org/work/W4200635145', 'https://semopenalex.org/work/W176670434', 'https://semopenalex.org/work/W2980624012', 'https://semopenalex.org/work/W201066287', 'https://semopenalex.org/work/W4392188516', 'https://semopenalex.org/work/W3135916968', 'https://semopenalex.org/work/W2400864908', 'https://semopenalex.org/work/W4392903219', 'https://semopenalex.org/work/W57476147', '2019', '2002', '2015', 'https://semopenalex.org/work/W2508726376', 'https://semopenalex.org/work/W4400169194', '2021', '2004', 'https://semopenalex.org/work/W1984877205', '2013', 'https://semopenalex.org/work/W4322732827', 'https://semopenalex.org/work/W4361193366', 'https://semopenalex.org/work/W4317487766', 'https://semopenalex.org/work/W4255342101', 'https://semopenalex.org/work/W4391011167', 'https://semopenalex.org/work/W4404609477', 'https://semopenalex.org/work/W2002383345', 'https://semopenalex.org/work/W4205871850', 'https://semopenalex.org/work/W2340829226', 'https://semopenalex.org/work/W4206887950', 'https://semopenalex.org/work/W4319776757', 'https://semopenalex.org/work/W4396819389', 'https://semopenalex.org/work/W2786772600', 'https://semopenalex.org/work/W1603914949', 'https://semopenalex.org/work/W3168497289', 'https://semopenalex.org/work/W4292536319', '2023', 'https://semopenalex.org/work/W2282010801', 'https://semopenalex.org/work/W65353647', 'https://semopenalex.org/work/W3037451085', 'https://semopenalex.org/work/W3031195982', '2024', 'https://semopenalex.org/work/W4399992019', 'https://semopenalex.org/work/W4293229595', 'https://semopenalex.org/work/W2918054698', 'https://semopenalex.org/work/W4402548755', 'https://semopenalex.org/work/W2538817717', 'https://semopenalex.org/work/W4375869296', 'https://semopenalex.org/work/W4309564724', '2001', 'https://semopenalex.org/work/W341170223', 'https://semopenalex.org/work/W4280542824', 'https://semopenalex.org/work/W4386096501', 'https://semopenalex.org/work/W4391940378', 'https://semopenalex.org/work/W2021438034', '2012', 'https://semopenalex.org/work/W2127936745', 'https://semopenalex.org/work/W4253642683', '2008', 'https://semopenalex.org/work/W2787015518', 'https://semopenalex.org/work/W4401568144', 'https://semopenalex.org/work/W4402148308', 'https://semopenalex.org/work/W3088081769', 'https://semopenalex.org/work/W3089124902', 'https://semopenalex.org/work/W2098962393', 'https://semopenalex.org/work/W3049587051', 'https://semopenalex.org/work/W2246393841', 'https://semopenalex.org/work/W2136188588', 'https://semopenalex.org/work/W2613217108', 'https://semopenalex.org/work/W2791275386', 'https://semopenalex.org/work/W4406492175', 'https://semopenalex.org/work/W172033102', 'https://semopenalex.org/work/W2261240196', 'https://semopenalex.org/work/W2735097653', 'https://semopenalex.org/work/W1964676816', 'https://semopenalex.org/work/W2987987546', 'https://semopenalex.org/work/W3048280215', 'https://semopenalex.org/work/W4392931449', 'https://semopenalex.org/work/W2736540096', 'https://semopenalex.org/work/W4296902974', '2005', 'https://semopenalex.org/work/W4400169339', 'https://semopenalex.org/work/W3198527244', 'https://semopenalex.org/work/W4302377316', 'https://semopenalex.org/work/W2056981644', 'https://semopenalex.org/work/W4399991937', '2007', 'https://semopenalex.org/work/W2736149122', 'https://semopenalex.org/work/W2123872165', 'https://semopenalex.org/work/W4360764206', '2018', 'https://semopenalex.org/work/W4311721661', '2020', '2017', 'https://semopenalex.org/work/W2481729578', 'https://semopenalex.org/work/W4404569657', 'https://semopenalex.org/work/W2141047835', 'https://semopenalex.org/work/W3026162943', 'https://semopenalex.org/work/W4400165275', 'https://semopenalex.org/work/W4386406820', 'https://semopenalex.org/work/W2402441967', 'https://semopenalex.org/work/W3006009898', 'https://semopenalex.org/work/W4298259748', 'https://semopenalex.org/work/W3009280029', 'https://semopenalex.org/work/W4280560758', '2003', 'https://semopenalex.org/work/W2095962821', 'https://semopenalex.org/work/W3200101073']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2132574120', 'https://semopenalex.org/work/W2915009967', 'https://semopenalex.org/work/W173156922', 'https://semopenalex.org/work/W2011170798', '2010', 'https://semopenalex.org/work/W1991332789', 'https://semopenalex.org/work/W1997210046', '2006', 'https://semopenalex.org/work/W2154282221', 'https://semopenalex.org/work/W2806131721', 'https://semopenalex.org/work/W2129825950', 'https://semopenalex.org/work/W4398191656', '2022', 'https://semopenalex.org/work/W2915030750', 'https://semopenalex.org/work/W1574950491', 'https://semopenalex.org/work/W3138989164', 'https://semopenalex.org/work/W1579677221', 'https://semopenalex.org/work/W1550675824', '2000', 'https://semopenalex.org/work/W4384155490', 'https://semopenalex.org/work/W4400939550', 'https://semopenalex.org/work/W3216444132', 'https://semopenalex.org/work/W1475955015', 'https://semopenalex.org/work/W2921648886', 'https://semopenalex.org/work/W1679509962', 'https://semopenalex.org/work/W2008620714', 'https://semopenalex.org/work/W2012114748', 'https://semopenalex.org/work/W2400762887', 'https://semopenalex.org/work/W4324007121', 'https://semopenalex.org/work/W4394555057', 'https://semopenalex.org/work/W2189085557', 'https://semopenalex.org/work/W2014199531', 'https://semopenalex.org/work/W1560854026', 'https://semopenalex.org/work/W4393474997', 'https://semopenalex.org/work/W2949504704', 'https://semopenalex.org/work/W991450633', 'https://semopenalex.org/work/W2123904236', 'https://semopenalex.org/work/W2103704182', 'https://semopenalex.org/work/W2206340513', 'https://semopenalex.org/work/W2953255159', 'https://semopenalex.org/work/W4406859981', 'https://semopenalex.org/work/W4253646682', '1998', '2015', '1993', '2021', 'https://semopenalex.org/work/W2754252703', 'https://semopenalex.org/work/W2779900466', '2013', 'https://semopenalex.org/work/W2522928308', 'https://semopenalex.org/work/W4298063358', 'https://semopenalex.org/work/W1579914521', 'https://semopenalex.org/work/W1792464322', 'https://semopenalex.org/work/W2739356170', 'https://semopenalex.org/work/W2055963247', 'https://semopenalex.org/work/W2044926733', 'https://semopenalex.org/work/W2125383988', 'https://semopenalex.org/work/W3033698111', 'https://semopenalex.org/work/W2523177018', '1995', 'https://semopenalex.org/work/W2008732772', 'https://semopenalex.org/work/W2103982927', 'https://semopenalex.org/work/W1811359278', 'https://semopenalex.org/work/W1994977110', 'https://semopenalex.org/work/W2085609918', 'https://semopenalex.org/work/W4393943425', 'https://semopenalex.org/work/W1595752763', '1999', 'https://semopenalex.org/work/W4400976691', 'https://semopenalex.org/work/W2525118715', '2024', 'https://semopenalex.org/work/W2078770126', 'https://semopenalex.org/work/W2915945450', 'https://semopenalex.org/work/W52260594', 'https://semopenalex.org/work/W2632860668', '2001', 'https://semopenalex.org/work/W4282576055', 'https://semopenalex.org/work/W1719093023', 'https://semopenalex.org/work/W2008606555', '2012', 'https://semopenalex.org/work/W2008078972', 'https://semopenalex.org/work/W1710751537', 'https://semopenalex.org/work/W1978847709', 'https://semopenalex.org/work/W2520217242', 'https://semopenalex.org/work/W1572167134', 'https://semopenalex.org/work/W2747419197', 'https://semopenalex.org/work/W2166938786', 'https://semopenalex.org/work/W1573454147', 'https://semopenalex.org/work/W3158293305', 'https://semopenalex.org/work/W2747898780', 'https://semopenalex.org/work/W1588734579', 'https://semopenalex.org/work/W2061236588', 'https://semopenalex.org/work/W3116695505', 'https://semopenalex.org/work/W36371468', 'https://semopenalex.org/work/W1987557201', 'https://semopenalex.org/work/W2139525797', 'https://semopenalex.org/work/W1975908943', 'https://semopenalex.org/work/W2118889869', 'https://semopenalex.org/work/W1253240651', 'https://semopenalex.org/work/W2612371455', 'https://semopenalex.org/work/W2527377534', 'https://semopenalex.org/work/W2899402023', 'https://semopenalex.org/work/W2400182190', 'https://semopenalex.org/work/W2123344956', 'https://semopenalex.org/work/W2912433096', '1800', 'https://semopenalex.org/work/W89291972', 'https://semopenalex.org/work/W4282583221', 'https://semopenalex.org/work/W2041544991', '2009', 'https://semopenalex.org/work/W2612962685', 'https://semopenalex.org/work/W4385473607', 'https://semopenalex.org/work/W1537902892', 'https://semopenalex.org/work/W2958694015', 'https://semopenalex.org/work/W115310691', 'https://semopenalex.org/work/W2515946176', 'https://semopenalex.org/work/W2128127301', 'https://semopenalex.org/work/W2525395252', 'https://semopenalex.org/work/W2401057219', 'https://semopenalex.org/work/W1978640117', 'https://semopenalex.org/work/W3137115172', '2020', '2017', 'https://semopenalex.org/work/W1570916159', 'https://semopenalex.org/work/W2963855145', 'https://semopenalex.org/work/W1517590008', 'https://semopenalex.org/work/W2115447277', 'https://semopenalex.org/work/W1975513208', 'https://semopenalex.org/work/W2171326679', 'https://semopenalex.org/work/W1556803451', 'https://semopenalex.org/work/W2155935413', 'https://semopenalex.org/work/W1511466363', 'https://semopenalex.org/work/W205920923', 'https://semopenalex.org/work/W4249900482', 'https://semopenalex.org/work/W1908231796', 'https://semopenalex.org/work/W2098211566', '2014', 'https://semopenalex.org/work/W3108668383', '2011', 'https://semopenalex.org/work/W4242436304', 'https://semopenalex.org/work/W1520649080', 'https://semopenalex.org/work/W2127281178', 'https://semopenalex.org/work/W4242041539', 'https://semopenalex.org/work/W2520300422', '2016', 'https://semopenalex.org/work/W1971941065', 'https://semopenalex.org/work/W2091478774', 'https://semopenalex.org/work/W2039085252', 'https://semopenalex.org/work/W2466104094', 'https://semopenalex.org/work/W4391272934', 'https://semopenalex.org/work/W2047400318', 'https://semopenalex.org/work/W2794546965', 'https://semopenalex.org/work/W2778029444', 'https://semopenalex.org/work/W2153339030', 'https://semopenalex.org/work/W2181042156', 'https://semopenalex.org/work/W1588297513', 'https://semopenalex.org/work/W2015180219', 'https://semopenalex.org/work/W2980176182', 'https://semopenalex.org/work/W1495962746', 'https://semopenalex.org/work/W2152544235', 'https://semopenalex.org/work/W2122811495', 'https://semopenalex.org/work/W139130934', 'https://semopenalex.org/work/W4238210800', 'https://semopenalex.org/work/W1595761884', 'https://semopenalex.org/work/W2123889292', '2019', '2002', '2004', 'https://semopenalex.org/work/W2087840232', 'https://semopenalex.org/work/W2017269495', 'https://semopenalex.org/work/W2949106240', 'https://semopenalex.org/work/W4404057326', 'https://semopenalex.org/work/W2751928463', 'https://semopenalex.org/work/W4296041368', 'https://semopenalex.org/work/W2071433880', 'https://semopenalex.org/work/W3136236837', 'https://semopenalex.org/work/W2094034408', 'https://semopenalex.org/work/W2112609211', '2023', 'https://semopenalex.org/work/W2734788368', 'https://semopenalex.org/work/W4387755431', 'https://semopenalex.org/work/W2104421582', 'https://semopenalex.org/work/W3195402331', 'https://semopenalex.org/work/W4402442861', 'https://semopenalex.org/work/W48558007', 'https://semopenalex.org/work/W1593317697', 'https://semopenalex.org/work/W2592423893', '1996', 'https://semopenalex.org/work/W2109952361', '2008', 'https://semopenalex.org/work/W2132155852', 'https://semopenalex.org/work/W2952092732', 'https://semopenalex.org/work/W1798073562', 'https://semopenalex.org/work/W4237909807', 'https://semopenalex.org/work/W156157953', 'https://semopenalex.org/work/W1592700375', 'https://semopenalex.org/work/W1775494561', 'https://semopenalex.org/work/W2088263927', 'https://semopenalex.org/work/W4313563519', 'https://semopenalex.org/work/W2077394967', 'https://semopenalex.org/work/W147488175', 'https://semopenalex.org/work/W1633377437', 'https://semopenalex.org/work/W2173733616', 'https://semopenalex.org/work/W2734789924', 'https://semopenalex.org/work/W4403628532', 'https://semopenalex.org/work/W2130495724', '2005', 'https://semopenalex.org/work/W4292761028', 'https://semopenalex.org/work/W2145761885', 'https://semopenalex.org/work/W4393670548', 'https://semopenalex.org/work/W2028893723', 'https://semopenalex.org/work/W371525118', '2007', 'https://semopenalex.org/work/W3009455989', 'https://semopenalex.org/work/W2928532935', 'https://semopenalex.org/work/W3092639686', 'https://semopenalex.org/work/W1996454760', 'https://semopenalex.org/work/W1501840263', '1994', 'https://semopenalex.org/work/W2049801349', '2018', 'https://semopenalex.org/work/W2609404595', 'https://semopenalex.org/work/W3183165251', 'https://semopenalex.org/work/W3028360334', 'https://semopenalex.org/work/W144935353', 'https://semopenalex.org/work/W2809114684', 'https://semopenalex.org/work/W2778798134', 'https://semopenalex.org/work/W4312240104', 'https://semopenalex.org/work/W1531484838', '1997', 'https://semopenalex.org/work/W2101874499', '2003', 'https://semopenalex.org/work/W2581324891', 'https://semopenalex.org/work/W1774324140']</t>
-  </si>
-  <si>
-    <t>['On the Use of Reciprocal Filter Against WiFi Packets for Passive Radar', 'Using real data for the implementation of multistatic passive radar geometry optimization procedure', 'Detection performance assessment of the FM-based AULOS® Passive Radar for air surveillance applications', 'A spectral slope-based approach for mitigating bistatic STAP clutter dispersion', 'Lagrange-Polynomial-Interpolation-Based Keystone Transform for a Passive Radar', 'https://semopenalex.org/source/S10936095', 'https://semopenalex.org/source/S4306418573', 'Cramér‐Rao lower bound with &lt;i&gt;P&lt;/i&gt; &lt;sub&gt;d&lt;/sub&gt; &amp;lt; 1 for target localisation accuracy in multistatic passive radar', 'Maritime surveillance via multi-frequency DVB-T based passive radar', 'Passive Radar: A Challenge Where Resourcefulness Is the Key to Success', 'VHF Cross-Range Profiling of Aerial Targets Via Passive ISAR: Signal Processing Schemes and Experimental Results', 'A fast disturbance cancellation scheme for orthogonal frequency division multiplexing‐based passive radar exploiting reciprocal filter', 'https://semopenalex.org/source/S4210172892', 'WiFi-based passive ISAR for high resolution cross-range profiling of moving targets', 'Non-linear and adaptive two-dimensional FIR filters for STAP theory and experimental results', 'Supervised Reciprocal Filter for OFDM Radar Signal Processing', 'https://semopenalex.org/source/S4306402512', 'https://semopenalex.org/source/S4404663355', 'Loaded Reciprocal Filter for OFDM-based Passive Radar Signal Processing', 'WiFi-Based Passive ISAR for High-Resolution Cross-Range Profiling of Moving Targets', 'Optimization of multistatic passive radar geometry based on CRLB with uncertain observations', 'Localization and tracking of moving targets with WiFi-based passive radar', 'Dual adaptive channel STAP: Theory and experimental results', 'Security enhancement in small private airports through active and passive radar sensors', 'https://semopenalex.org/source/S141761900', 'Enhanced WiFi-based passive ISAR for indoor and outdoor surveillance', 'https://semopenalex.org/source/S4306400024', 'https://semopenalex.org/source/S161080992', 'Efficient Detection and Imaging of Moving Targets in SAR Images Based on Chirp Scaling', 'An apodization approach for passive GMTI Radar with Non-Uniform Linear Arrays', 'A new approach for DVB-T Cross-Ambiguity Function evaluation', 'Polarimetric Detection Scheme for Passive Radar based on a 2D Auto-Regressive Disturbance Model', 'https://semopenalex.org/source/S4306498246', 'Passive Bistatic Radar based on mixed DSSS and OFDM WiFi transmissions', 'Effect of Apodization on SAR Image Understanding', 'Supervised DPCA Scheme Based on Reciprocal Filter for Clutter Cancellation From Moving OFDM Radar', 'Experimental results for passive bistatic radar based on DVB-T signals', 'Exploiting long coherent integration times in DVB-T based passive radar systems', 'Passive radar detection of drones with staring illuminators of opportunity', 'Exploitation of Long Coherent Integration Times to Improve Drone Detection in DVB-S based Passive Radar', 'Target DoA estimation in passive radar using non-uniform linear arrays and multiple frequency channels', 'https://semopenalex.org/source/S23688054', 'Parasitic Surveillance Potentialities Based on a GEO-SAR Illuminator', 'Multiband passive radar for drones detection and localization', 'Exploiting polarimetric diversity in FM-based PCL', 'Reference-free Amplitude-based WiFi Passive Sensing', 'https://semopenalex.org/source/S4306400806', 'https://semopenalex.org/source/S4306418371', 'Exploiting polarimetric diversity to mitigate the effect of interferences in FM-based passive radar', 'Preliminary experimental results of polarimetric detection schemes for DVB-T based passive radar', 'A Multistage Processing Algorithm for Disturbance Removal and Target Detection in Passive Bistatic Radar', 'Conclusion', 'Computationally effective range migration compensation in PCL systems for maritime surveillance', 'DVB-T-Based Passive Forward Scatter Radar: Inherent Limitations and Enabling Solutions', 'Automatic vehicles classification approaches for WiFi-based Passive Forward Scatter Radar', 'https://semopenalex.org/source/S4306463440', 'Performance analysis of a multi-frequency FM based Passive Bistatic Radar', 'Threshold Region Performance of Multicarrier Maximum Likelihood Direction of Arrival Estimator', 'Dual Channel Adaptive Antenna Nulling with Auxiliary Selection for Spaceborne Radar', 'https://semopenalex.org/source/S3569471', 'Multi-carrier Adaptive Detection in Polarimetric Passive Radars', 'WiFi emission-based vs passive radar localization of human targets', 'Adaptive beamforming for high-frequency over-the-horizon passive radar', 'https://semopenalex.org/source/S4306402478', 'From the expected scientific applications to the functional specifications, products and performance of the SABRINA missions', 'Foreword to the Special Section on Fully Digital Arrays for Radar', 'Low-cost solutions for mobile passive radar based on multichannel DPCA and NULA configurations', 'A reduced order jammer cancellation scheme based on double adaptivity', 'Facing channel calibration issues affecting passive radar DPCA and STAP for GMTI', 'A Three-Stage Inter-Channel Calibration Approach for Passive Radar on Moving Platforms Exploiting the Minimum Variance Power Spectrum', 'https://semopenalex.org/source/S4306420045', 'Comparison of Clutter and Multipath Cancellation Techniques for Passive Radar', 'Passive Radar DPCA Schemes With Adaptive Channel Calibration', '&amp;lt;title&amp;gt;Passive radar prototypes for multifrequency target detection&amp;lt;/title&amp;gt;', 'Passive Radar: Past, Present, and Future Challenges', 'High resolution cross-range profiling with Passive Radar via ISAR processing', 'A two-stage approach for direct signal and clutter cancellation in passive radar on moving platforms', 'Multi-Frequency Target Detection Techniques for DVB-T Based Passive Radar Sensors', 'https://semopenalex.org/source/S4210171417', 'Parasitic Exploitation of Wi-Fi Signals for Indoor Radar Surveillance', 'Foreword to the Special section on Advances in Radar Imaging', 'Polarimetric passive coherent location', 'Exploiting the Properties of Reciprocal Filter in Low-Complexity OFDM Radar Signal Processing Architectures', 'Multistatic passive radar geometry optimization for target 3D positioning accuracy', 'https://semopenalex.org/source/S4210193624', 'PBR activity at INFOCOM: Adaptive processing techniques and experimental results', 'Antenna Array for Passive Radar: Configuration Design and Adaptive Approaches to Disturbance Cancellation', 'Polarimetric diversity in reference-free amplitude-based Wi-Fi sensing', 'EuMW 2022 Special Issue', 'https://semopenalex.org/source/S189694085', 'WiFi-Based Passive Bistatic Radar: Data Processing Schemes and Experimental Results', 'Comparing phase-locked and non-phase-locked architectures for dual-channel DVB-S passive radar', 'Two‐dimensional location of moving targets within local areas using WiFi‐based multistatic passive radar', 'https://semopenalex.org/source/S111326731', 'Passive Radar STAP Detection and DoA Estimation Under Antenna Calibration Errors', 'Reciprocal-Filter-Based STAP for Passive Radar on Moving Platforms', 'Passive radar concept for automotive applications', 'Passive radar for GMTI', 'https://semopenalex.org/source/S153101029', 'Impact of synchronization on the ambiguity function shape for PBR based on DVB-T signals', 'Quasi-Monostatic Versus Near Forward Scatter Geometry in WiFi-Based Passive Radar Sensors', 'Polarimetric Passive Radar: A Practical Approach to Parametric Adaptive Detection', 'https://semopenalex.org/source/S101949793', 'A procedure for effective receiver positioning in multistatic passive radar', 'Impact of Beacon Interval on the performance of WiFi-based passive radar against human targets', 'Sliding extensive cancellation algorithm for disturbance removal in passive radar', 'DVB-T Signal Ambiguity Function Control for Passive Radars', 'Performance Prediction of the Loaded Reciprocal Filter for OFDM-based Passive Radar', 'DVB-T based Passive Bistatic Radar for maritime surveillance', 'Monitoring and surveillance potentialities obtained by splitting the antenna of the COSMO-SkyMed SAR into multiple sub-apertures', 'Multi‐carrier and multi‐polarimetric model based adaptive target detector for passive radar systems', 'Clutter Suppression Using Thresholded Reciprocal Filter in OFDM Radar', 'IEEE aerospace &amp;amp; electronic systems society organization 2019', 'https://semopenalex.org/source/S4363608562', '2D Localization with WiFi Passive Radar and Device-Based Techniques: An Analysis of Target Measurements Accuracy', 'Short-range passive radar for small private airports surveillance', 'Reducing the computational complexity of WiFi-based passive radar processing', 'Disturbance removal in passive radar via sliding extensive cancellation algorithm (ECA-S)', 'A simple clutter suppression approach for OFDM-based passive radar exploiting reciprocal filter', 'Reduced Order Jammer Cancellation Scheme Based on Double Adaptivity', 'Multi-frequency polarimetric target detection in FM-based passive radar', 'Autoregressive Model Based Polarimetric Adaptive Detection Scheme Part II: Performance Assessment Under Spectral Model Mismatch', 'A practical approach to polarimetric adaptive target detection in Passive Radar', 'WiFi-based PCL for monitoring private airfields', 'https://semopenalex.org/source/S153794155', 'Tackling the different target dynamics issues in counter drone operations using passive radar', 'Advanced Processing Methods for Passive Bistatic Radar Systems', 'Potentialities and challenges of WiFi-based passive radar', 'First experimental results for a WiFi-based passive forward scatter radar', 'https://semopenalex.org/source/S2764455111', 'A Survey on Fundamental Limits of Integrated Sensing and Communication', 'Forward-Looking Passive Radar With Non-Uniform Linear Array for Automotive Applications', 'Inside front cover', '[Front matter]', 'Enabling DPCA via Supervised Reciprocal Filter in OFDM Radar Onboard Moving Platforms', 'Autoregressive Model Based Polarimetric Adaptive Detection Scheme Part I: Theoretical Derivation and Performance Analysis', 'https://semopenalex.org/source/S4377196107', 'Short-range passive radar potentialities', 'https://semopenalex.org/source/S4306401280', 'Experimental evaluation of Supervised Reciprocal Filter Strategies for OFDM-radar signal processing', 'https://semopenalex.org/source/S4210215198', 'Multifrequency integration in FM radio-based passive bistatic radar. Part I: Target detection', 'https://semopenalex.org/source/S4306400194', 'DVB-S based Passive Radar for Short Range Security Application', 'A Study for a Space-Based Passive Multi-Channel SAR', 'https://semopenalex.org/source/S193624734', 'Direction of arrival estimation performance comparison of dual cancelled channels space–time adaptive processing techniques', 'Simultaneous short and long range surveillance of drones and aircrafts with DVB-T based Passive Radar', 'Foreword to the Special Section on Innovations in Radar Spectrum', 'Fusing Measurements from Wi-Fi Emission-Based and Passive Radar Sensors for Short-Range Surveillance', 'DVB-T based Forward Scatter Radar for Small Target Surveillance', 'https://semopenalex.org/source/S4363608355', 'https://semopenalex.org/source/S4306525036', 'Passive Detection Using a Staring Radar Illuminator of Opportunity', 'Ambiguity Function analysis of WiMAX transmissions for passive radar', 'Microphone array based classification for security monitoring in unstructured environments', 'Multifrequency integration in FM radio-based passive bistatic radar. Part II: Direction of arrival estimation', 'Comparing reference‐free WiFi radar sensing approaches for monitoring people and drones', 'Exploiting polarimetric diversity in passive radar', 'A simple NULA design strategy for target detection and DoA estimation in mobile passive radar', 'Ambiguity Function Analysis of Wireless LAN Transmissions for Passive Radar', 'https://semopenalex.org/source/S4306531480', 'Space–time constant modulus algorithm for multipath removal on the reference signal exploited by passive bistatic radar', 'Experimental results of polarimetric detection schemes for DVB‐T‐based passive radar', 'https://semopenalex.org/source/S4363608006', 'Eco-friendly dual-band AULOS® passive radar for air and maritime surveillance applications', 'OFDM based WiFi Passive Sensing: a reference-free non-coherent approach', 'https://semopenalex.org/source/S4377196266', 'Non‐coherent adaptive detection in passive radar exploiting polarimetric and frequency diversity', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S4306418812', 'Analysis and Emulation of FM Radio Signals for Passive Radar', 'https://semopenalex.org/source/S183492911', 'Space-based passive radar enabled by the new generation of geostationary broadcast satellites', 'Minimum variance power spectrum based calibration for improved clutter suppression in PCL on moving platforms', 'Experimental results for OFDM WiFi-based passive bistatic radar', 'Integrated clutter cancellation and high-resolution imaging of moving targets in Multi-channel SAR', 'DVB-T-based passive radar for silent surveillance of drones', 'Dual Cancelled Channel STAP for Target Detection and DOA Estimation in Passive Radar', 'https://semopenalex.org/source/S4306420046', 'Passive radar components of ARGUS 3D', 'Stand-alone WiFi-based Passive Forward Scatter Radar sensor for vehicles classification', 'Exploiting the joint distribution of amplitude and monopulse ratio for chi-square fluctuating targets for target DOA estimation', 'Detection and 3D localization of ultralight aircrafts and drones with a WiFi-based Passive Radar', 'DVB‐T based passive radar for simultaneous counter‐drone operations and civil air traffic surveillance', 'From the EiC: The IEEE Radar Journal is Born', 'https://semopenalex.org/source/S43295729', 'Antenna Sidelobes Level Control in Transmit Subaperturing MIMO Radar', "This Month's Covers....", 'Range sidelobes reduction filters for WiFi-based passive bistatic radar', 'Outlier Rejection Approach for Direction of Arrival Estimation in Low SNR Conditions', 'Passive radar in the high frequency band', 'A Flexible Design Strategy for Three-Element Non-Uniform Linear Arrays', 'Spectral slope-based approach for mitigating bistatic space-time adaptive processing clutter dispersion', 'Exploiting Polarization together with Space-Time Adaptive Processing for GMTI in high resolution SAR images', 'https://semopenalex.org/source/S4387286330', 'Passive STAP approaches for GMTI']</t>
-  </si>
-  <si>
-    <t>['Reliable Communications Over Dependent Fading Wireless Channels.', 'On the Set of Joint Rayleigh Fading Distributions Achieving Positive Zero-Outage Capacities', 'https://semopenalex.org/source/S61310614', 'https://semopenalex.org/source/S4363607711', 'https://semopenalex.org/source/S168680287', 'Frequency Diversity for Ultra-Reliable and Secure Communications in Sub-THz Two-Ray Scenarios', 'Measurements of Wiretap Encoded Image Transmissions over Multi-Mode Fibers', 'On Fading Channel Dependency Structures with a Positive Zero-Outage Capacity', 'https://semopenalex.org/source/S63459445', 'https://semopenalex.org/source/S147316732', 'Deep Learning Based Resource Allocation: How Much Training Data is Needed?', 'https://semopenalex.org/source/S4363607705', 'https://semopenalex.org/source/S4306534978', 'Multi-User Frequency Assignment for Ultra-Reliable mmWave Two-Ray Channels', 'Neural Network Wiretap Code Design for Multi-Mode Fiber Optical Channels', 'On the Zero-Outage Secrecy-Capacity of Dependent Fading Wiretap Channels', 'https://semopenalex.org/source/S2764455111', 'A Simple Frequency Diversity Scheme for Ultra-Reliable Communications in Ground Reflection Scenarios', 'https://semopenalex.org/source/S4363608593', 'Calculation of Bounds on the Ergodic Capacity for Fading Channels with Dependency Uncertainty', 'https://semopenalex.org/source/S4306401280', 'https://semopenalex.org/source/S195231649', 'Learning Based Dynamic Cluster Reconfiguration for UAV Mobility Management with 3D Beamforming', 'https://semopenalex.org/source/S4306400562', 'https://semopenalex.org/source/S4363607702', 'https://semopenalex.org/source/S4306400194', 'Reinforcement Learning Based Dynamic Power Control for UAV Mobility Management', 'RISnet: A Domain-Knowledge Driven Neural Network Architecture for RIS  Optimization with Mutual Coupling and Partial CSI', 'Copula-Based Bounds for Multi-User Communications–Part II: Outage Performance', 'https://semopenalex.org/source/S4210214273', 'Learning Based Dynamic Cluster Reconfiguration for UAV Mobility  Management with 3D Beamforming', 'https://semopenalex.org/source/S4306525036', 'A Globally Optimal Energy-Efficient Power Control Framework and Its Efficient Implementation in Wireless Interference Networks', 'Bounds on the Secrecy Outage Probability for Dependent Fading Channels', 'Securing Data in Multimode Fibers by Exploiting Mode-Dependent Light Propagation Effects', 'Machine Learning Assisted Wiretapping', 'Bounds on the Outage Probability in Dependent Rayleigh Fading Channels', 'Building Resilience in Wireless Communication Systems With a Secret-Key  Budget', 'Wiretap Code Design by Neural Network Autoencoders', 'RISnet: A Scalable Approach for Reconfigurable Intelligent Surface Optimization with Partial CSI', 'Reinforcement Learning-Based Global Programming for Energy Efficiency in Multi-Cell Interference Networks', 'An efficient frequency diversity scheme for ultra-reliable communications in two-path fading channels', 'https://semopenalex.org/source/S4306402617', 'https://semopenalex.org/source/S4393179698', 'Copula-Based Bounds for Multi-User Communications–Part I: Average Performance', 'Achievable Physical-Layer Secrecy in Multi-Mode Fiber Channels using Artificial Noise', 'Reliability and Latency Analysis for Wireless Communication Systems with a Secret-Key Budget', 'https://semopenalex.org/source/S196647941', 'Reliability Bounds for Dependent Fading Wireless Channels', 'Flexible Design of Finite Blocklength Wiretap Codes by Autoencoders', 'Optimal Resource Allocation for Loss-Tolerant Multicast Video Streaming', 'Distributed Combinatorial Optimization of Downlink User Assignment in  mmWave Cell-free Massive MIMO Using Graph Neural Networks', 'Outage Probability Calculation for Two-Ray Ground Reflection Scenarios with Frequency Diversity', 'Reliability and Latency Analysis for Wireless Communication Systems With a Secret-Key Budget', 'Approaching Globally Optimal Energy Efficiency in Interference Networks via Machine Learning', 'Bounds on the Ergodic Secret-Key Capacity for Dependent Fading Channels.', 'On Fading Channel Dependency Structures With a Positive Zero-Outage Capacity', 'https://semopenalex.org/source/S4363608623', 'Non-Convex Optimization of Energy Efficient Power Control in Interference Networks via Machine Learning', 'https://semopenalex.org/source/S173102057', 'https://semopenalex.org/source/S4306402636', 'Artificial Fast Fading from Reconfigurable Surfaces Enables Ultra-Reliable Communications', 'https://semopenalex.org/source/S4210218516', 'Reconfigurable Intelligent Surface Phase Hopping for Ultra-Reliable Communications', 'Reliability and Latency of Wireless Communication Systems with a Secret-Key Budget', 'QMKPy: A Python Testbed for the Quadratic Multiple Knapsack Problem', 'Hierarchical Multi-Agent DRL Based Dynamic Cluster Reconfiguration for  UAV Mobility Management']</t>
-  </si>
-  <si>
-    <t>['Probabilistic Analysis of MULTIPLE QUICK SELECT', 'A multivariate view of random bucket digital search trees', 'Distributions in a class of Poissonized urns with an application to Apollonian networks', 'https://semopenalex.org/source/S44643521', 'https://semopenalex.org/source/S4210182901', 'Polya Urn Models and Connections to Ran- dom Trees: A Review', 'Insertion depth in power-weight trees', 'The degree Gini index of several classes of random trees and their poissonized counterparts---an evidence for a duality theory', 'Analysis of Boyer-Moore-Horspool string-matching heuristic', 'Perpetuities in Fair Leader Election Algorithms', 'On Nodes of Small Degrees and Degree Profile in Preferential Dynamic Attachment Circuits', 'Exactly Solvable Balanced Tenable Urns with Random Entries via the Analytic Methodology', 'Winning a Tournament According to Bradley-Terry Probability Model', 'Some empirical and theoretical attributes of random multi-hooking networks', 'A model for the spreading of fake news', 'One-sided variations on binary search trees', 'Degrees in random $m$-ary hooking networks', 'Asymptotic Properties of a Leader Election Algorithm', 'Random multi-hooking networks', 'Exact Covariances and Refined Asymptotics in Dichromatic Tenable Balanced Polya Urn Schemes', 'https://semopenalex.org/source/S200334879', 'Corrigendum', 'https://semopenalex.org/source/S4306402512', 'The class of tenable zero-balanced Pólya urn schemes: characterization and Gaussian phases', 'https://semopenalex.org/source/S2764412775', 'Affine Diminishing Urns', 'Asymptotic Properties of Protected Nodes in Random Recursive Trees', 'On the structure of random plane‐oriented recursive trees and their branches', 'On the Joint Behavior of Types of Coupons in Generalized Coupon Collection', 'A stochastic model for solitons', 'https://semopenalex.org/source/S147953040', 'Analysis of swaps in radix selection', 'https://semopenalex.org/source/S4306418406', 'Degrees in random &lt;mml:math xmlns:mml=http://www.w3.org/1998/Math/MathML&gt;&lt;mml:mi&gt;m&lt;/mml:mi&gt;&lt;/mml:math&gt;-ary hooking networks', 'https://semopenalex.org/source/S2765029694', 'Balancing m-ary search trees with compressions on the fringe', 'https://semopenalex.org/source/S150892397', 'Probabilistic analysis of bucket recursive trees', 'https://semopenalex.org/source/S4377196372', 'https://semopenalex.org/source/S156280010', 'On the variety of shapes in digital trees', 'https://semopenalex.org/source/S4210224136', 'A Strong Law for the Height of Random Binary Pyramids', 'One-sided Variations on Tries: Path Imbalance, Climbing, and Key Sampling', 'Random networks grown by fusing edges via urns', 'Distributional analysis of swaps in Quick Select', 'On the Distribution of Leaves in Rooted Subtrees of Recursive Trees', 'SOME NODE DEGREE PROPERTIES OF SERIES–PARALLEL GRAPHS EVOLVING UNDER A STOCHASTIC GROWTH MODEL', 'https://semopenalex.org/source/S160779208', 'Affine diminishing urns', 'The class of tenable zero-balanced Pólya urns with an initially dominant subset of colors', 'Polya-Type Urn Models with Multiple Drawings', 'Distribution of the size of random hash trees, pebbled hash trees and N-trees', 'Limiting Distributions for Path Lengths in Recursive Trees', 'Statistical Inequalities', 'https://semopenalex.org/source/S84409463', 'https://semopenalex.org/source/S18902827', 'Survivors in leader election algorithms', 'https://semopenalex.org/source/S164906323', 'Toward a Formal Derivation of the Expected Behavior of Prefix &lt;i&gt;B&lt;/i&gt;-Trees', 'Asymptotic Joint Normality of Counts of Uncorrelated Motifs in Recursive Trees', 'https://semopenalex.org/source/S7571225', 'Limit laws for the Randić index of random binary tree models', 'On nodes of small degrees and degree profile in preferential dynamic attachment circuits', 'The Sackin index and depth of leaves in generalized Schröder trees', 'Oツリー,Bツリー,接頭Bツリーのストレージのオーバーヘッド 比較分析', 'Age statistics in the Moran population model', 'https://semopenalex.org/source/S90727058', 'Analysis of a generalized Friedman’s urn with multiple drawings', 'Asymptotic Joint Normality of Outdegrees of Nodes in Random Recursive Trees', 'Two-color balanced affine urn models with multiple drawings II: large-index and triangular urns', 'The degree profile and weight in Apollonian networks and &lt;i&gt;k&lt;/i&gt;-trees', "Mixed distributions in Sattolo's algorithm for cyclic permutations via randomization and derandomization", 'On rotations in fringe-balanced binary trees', 'Limit laws for terminal nodes in random circuits with restricted fan-out: a family of graphs generalizing binary search trees', 'Distributions in the Ehrenfest process', 'The Expected Distribution of Degrees in Random Binary Search Trees', 'Bivariate Issues in Leader Election Algorithms with Marshall-Olkin Limit Distribution', 'The containment profile of hyper-recursive trees', 'Analysis of Quickselect Under Yaroslavskiy’s Dual-Pivoting Algorithm', 'The Joint Distribution of Elastic Buckets in Multiway Search Trees', 'https://semopenalex.org/source/S128350725', 'https://semopenalex.org/source/S193011845', 'A SPECTRUM OF SERIES–PARALLEL GRAPHS WITH MULTIPLE EDGE EVOLUTION', 'Two-colour balanced affine urn models with multiple drawings I: central limit theorems', 'Estimating the Pólya process', 'مدلهای آوند پولیاگونه با برداشتهای چندگانه', 'https://semopenalex.org/source/S4306400744', 'On the Variety of Shapes in Digital Trees', 'The continuous-time triangular Pólya process', 'Explicit characterization of moments of balanced triangular Pólya urns by an elementary approach', 'Average-case analysis of multiple Quickselect: An algorithm for finding order statistics', 'Exact and Limiting Distributions in Diagonal Pólya Processes', 'The Power of Choice in the Construction of Recursive Trees', 'On affine multicolor urns grown under multiple drawing', 'Problems and Solutions', 'On the average internal path length of m-ary search trees', 'Profile of Random Exponential Recursive Trees', 'JISC: Adaptive stream processing using just-in-time state completion?', 'https://semopenalex.org/source/S4306463230', 'https://semopenalex.org/source/S171741597', 'https://semopenalex.org/source/S4306536558', 'Probabilistic analysis of maximal gap and total accumulated length in interval division', 'The continuum Pólya-like random walk', 'Distances in random digital search trees', 'Exact and limiting distributions in diagonal Pólya processes', 'On the internal structure of random recursive circuits', 'https://semopenalex.org/source/S180803011', 'An index for betting with examples from games and sports', 'Analysis of an Algorithm for Random Sampling', 'Average-Case Analysis of Cousins in m-ary Tries', 'Polya Urn Models', 'A self-equilibrium Friedman-like urn via stochastic approximation', 'ON CLIMBING TRIES', 'An Efficiency Robust Nonparametric Test for Scale Change for Data from a Gamma Distribution', 'https://semopenalex.org/source/S989097277', 'Analysis of the space of search trees under the random insertion algorithm', 'https://semopenalex.org/source/S2530642067', 'Depths in hooking networks', 'https://semopenalex.org/source/S4210191297', 'https://semopenalex.org/source/S89324355', 'https://semopenalex.org/source/S9093621', 'Average measures in polymer graphs', 'https://semopenalex.org/source/S2764830807', 'https://semopenalex.org/source/S4210186879', 'https://semopenalex.org/source/S4306463075', 'https://semopenalex.org/source/S4306402042', 'STORAGE OVERHEAD OF O-TREES, B-TREES AND PREFIX B-TREES: A COMPARATIVE ANALYSIS', 'https://semopenalex.org/source/S59667848', 'https://semopenalex.org/source/S153560523', 'Phase Changes in Subtree Varieties in Random Recursive and Binary Search Trees', 'Analytic variations on bucket selection and sorting', 'https://semopenalex.org/source/S170765028', 'Dynamic Pólya–Eggenberger urns', 'https://semopenalex.org/source/S4210215866', 'Imbalance in Random Digital Trees', 'A Limit Law for Outputs in Random Recursive Circuits', 'On the distribution for the duration of a randomized leader election algorithm', 'Bar Bets and Generating Functions: The Distribution of the Separation of Two Distinct Card Ranks', 'The oscillatory distribution of distances in random tries', 'On generalized Pólya urn models', 'https://semopenalex.org/source/S165473669', 'The joint distribution of the three types of nodes in uniform binary trees', 'Correction to: Egorychev Method: A Hidden Treasure', 'On tree-growing search strategies', 'https://semopenalex.org/source/S4306401280', 'Degrees in random self-similar bipolar networks', 'https://semopenalex.org/source/S23873141', 'https://semopenalex.org/source/S4306400194', 'Local and global degree profiles of randomly grown self-similar hooking networks under uniform and preferential attachment', 'On the joint distribution of the insertion path length and the number of comparisons in search trees', 'Trees grown under young-age preferential attachment', 'https://semopenalex.org/source/S68047077', 'Distribution of distances in random binary search trees', 'Analysis of quickselect : an algorithm for order statistics', 'SOME PROPERTIES OF BINARY SERIES-PARALLEL GRAPHS', 'ON THE COMBINATORICS OF BINARY SERIES-PARALLEL GRAPHS', 'DEGREE PROFILE OF HIERARCHICAL LATTICE NETWORKS', 'Random sprouts as internet models, and P�lya processes', 'https://semopenalex.org/source/S4210234901', 'Limit distribution of distances in biased random tries', 'EXTREMAL WEIGHTED PATH LENGTHS IN RANDOM BINARY SEARCH TREES', 'The size of random bucket trees via urn models', 'The Department of Statistics at The George Washington University', 'https://semopenalex.org/source/S985303', 'The Degree Profile in Some Classes of Random Graphs that Generalize Recursive Trees', 'DRAWING MULTISETS OF BALLS FROM TENABLE BALANCED LINEAR URNS', 'https://semopenalex.org/source/S4306463937', 'Egorychev Method: A Hidden Treasure', 'https://semopenalex.org/source/S4210172589', 'On the Most Probable Shape of a Search Tree Grown from a Random Permutation', 'On affine multi-color urns grown under multiple drawing', 'Some properties of exponential trees', 'https://semopenalex.org/source/S203441484', 'https://semopenalex.org/source/S4393179698', 'DEGREE-BASED GINI INDEX FOR GRAPHS', 'Distances in random plane-oriented recursive trees', 'Paths in &lt;mml:math xmlns:mml=http://www.w3.org/1998/Math/MathML altimg=si2.gif overflow=scroll&gt;&lt;mml:mi&gt;m&lt;/mml:mi&gt;&lt;/mml:math&gt;-ary interval trees', 'Covariances in Pólya urn schemes', 'https://semopenalex.org/source/S4306400349', 'The Gini index of random trees with an application to caterpillars', 'Exact Covariances and Refined Asymptotics in Dichromatic Tenable Balanced Pólya Urn Schemes', 'The Degree Gini Index of Several Classes of Random Trees and Their Poissonized Counterparts�Evidence for Duality', 'Distributions in the constant-differentials Pólya process', 'On the Variety of Shapes on the Fringe of a Random Recursive Tree', 'An Efficiency Robust Nonparametric Test for Scale Change for Data From a Gamma Distribution', 'DEGREE PROFILE OF &lt;i&gt;m&lt;/i&gt;-ARY SEARCH TREES: A VEHICLE FOR DATA STRUCTURE COMPRESSION', 'Gaussian phases in generalized coupon collection', 'Pólya urns: Probabilistic analysis and statistical questions', 'BUILDING RANDOM TREES FROM BLOCKS', 'Profile of Random Exponential Binary Trees', 'Asymptotic distribution of two-protected nodes in random binary search trees', 'https://semopenalex.org/source/S4306417669', 'https://semopenalex.org/source/S6941720', 'The Class of Tenable Zero-Balanced Pólya Urn Schemes: Characterization and Gaussian Phases', 'https://semopenalex.org/source/S4306402264', 'Phases in the Diffusion of Gases via the Ehrenfest URN Modelx', 'https://semopenalex.org/source/S9424914', 'An Urn Model for Population Mixing and the Phases Within', 'Algorithmics of Nonuniformity', 'Throughput analysis in wireless networks with multiple users and multiple channels', 'https://semopenalex.org/source/S4306402441', 'Distribution of inter-node distances in digital trees', 'https://semopenalex.org/source/S4306463019', 'https://semopenalex.org/source/S117679221', 'The containment profile of hyperrecursive trees', 'Two-color balanced affine urn models with multiple drawings', 'One-sided variations on interval trees', 'https://semopenalex.org/source/S94688346', 'BERNOULLI CONVOLUTION OF THE DEPTH OF NODES IN RECURSIVE TREES WITH GENERAL AFFINITIES', 'Phases in the two-color tenable zero-balanced Pólya process', 'https://semopenalex.org/source/S4386872458', 'https://semopenalex.org/source/S177771411', 'Sorting 1-away permutations with underlying Fibonacci convolutions', 'Characterization and Enumeration of Certain Classes of Tenable Pólya Urns Grown by Drawing Multisets of Balls', 'https://semopenalex.org/source/S110520077']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/source/S4210212400', 'Technology for societal change: Evaluating a mobile app addressing the emotional needs of people experiencing homelessness', 'Brainstorm', 'https://semopenalex.org/source/S4306401600', 'Weisst Du wieviel Sternlein stehen? – Building older adults’ confidence in technology use through co-designing digital storytelling', 'https://semopenalex.org/source/S112414500', 'Emotional Factors for Teleaudiology', 'Designing Meaningful, Beneficial and Positive Human Robot Interactions with Older Adults for Increased Wellbeing During Care Activities', 'Using a digital personal recovery resource in routine mental health practice: feasibility, acceptability and outcomes', 'https://semopenalex.org/source/S4210211086', 'Motivational models for validating agile requirements in Software Engineering subjects', 'https://semopenalex.org/source/S4306463409', 'https://semopenalex.org/source/S89276529', 'Evaluating Engagement in Technology-Supported Social Interaction by People Living with Dementia in Residential Care', 'https://semopenalex.org/source/S4306400194', 'Editorial: Designing Technology for Emotions to Improve Mental Health and Wellbeing', 'https://semopenalex.org/source/S4210179225', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S34944277', 'https://semopenalex.org/source/S4306402621', 'A Co-design Approach for Developing and Implementing Smart Health Technologies and Services', 'https://semopenalex.org/source/S201800618', 'Adding Emotions to Models in a Viewpoint Modelling Framework From Agent-Oriented Software Engineering', 'Using Motivational Modelling With an App Designed to Increase Student Performance and Retention', 'https://semopenalex.org/source/S4306525036', 'Interdisciplinary Design Teams Translating Ethnographic Field Data Into Design Models', 'https://semopenalex.org/source/S4306400572', 'Understanding Confidence of Older Adults for Embracing Mobile Technologies']</t>
-  </si>
-  <si>
-    <t>['Promoting Diversity in the Evolution of Biological Sequence Data', 'https://semopenalex.org/source/S4363604921', 'Dungeons, Dragons, and Data Breaches: Analyzing AI Attacks on Various Network Configurations', 'Network Induction Issues', 'All lockdowns are not equal: Reducing epidemic impact through evolutionary computation', 'Vaccine Distribution', 'https://semopenalex.org/source/S99347777', 'What Drives Evolution of Self-Driving Automata?', 'https://semopenalex.org/source/S4210216571', 'AI Versus Epidemics', 'Freezing of gait in Parkinson’s disease: Classification using computational intelligence', 'Conference Report on 2022 IEEE Conference on Computational Intelligence in Bioinformatics and Computational Biology (IEEE CIBCB 2022) [Conference Report]', 'https://semopenalex.org/source/S140556538', 'https://semopenalex.org/source/S4363605353', '2022 IEEE conference on computational intelligence in bioinformatics and computational biology (IEEE CIBCB, 2022)', 'Evolutionary Computation', 'Introduction', 'A multi-objective genetic algorithm for compression of weighted graphs to simplify epidemic analysis', 'Graph Compression', 'Network Induction', 'https://semopenalex.org/source/S4306525036', 'https://semopenalex.org/source/S4210218191', 'https://semopenalex.org/source/S104797584']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/source/S2737955091', 'Augmentation of Additional Arabic Dataset for Jawi Writing and Classification Using Deep Learning', 'Utilizing Edge Device and Streamlit for Comparative Evaluation of CLAHE-Based Underwater Image Enhancement Techniques', 'Performance evaluation of hyper-parameter tuning automation in YOLOV8 and YOLO-NAS for corn leaf disease detection', 'https://semopenalex.org/source/S4306417765', 'Performance Evaluation of Binary Classification of Diabetic Retinopathy through Deep Learning Techniques using Texture Feature', 'https://semopenalex.org/source/S4306401629', 'Pendeteksian Septoria pada Tanaman Tomat dengan Metode Deep Learning berbasis Raspberry Pi', 'https://semopenalex.org/source/S4363607800', 'Impact of CLAHE-based image enhancement for diabetic retinopathy classification through deep learning', 'Performance Evaluation of Coffee Bean Binary Classification Through Deep Learning Techniques', 'Performance Evaluation And Analysis of LBP Utilization In Face Spoofing Detection With Deep Learning', 'Streamlit Application for Helmet Detection Based on YOLOS: Case Study Indonesia', 'Comparative Study of Deep Learning Methods through Improvement of Skin Image Quality of Basal Cell Carcinoma', 'Rancang Bangun Purwarupa Pemilah Sampah Pintar Berbasis Deep Learning', 'https://semopenalex.org/source/S4210183703', 'https://semopenalex.org/source/S4210223945', 'https://semopenalex.org/source/S4363606538', 'Performance Evaluation of Binary Classification of Tuberculosis through Unsharp Masking and Deep Learning Technique', 'Lightweight Pedestrian Detection through Guided Filtering and Deep Learning', 'An Edge AI-Powered Defect Coffee Detector Using Streamlit Web App', 'Students’ emotion classification system through an ensemble approach', 'https://semopenalex.org/source/S4210198570', 'Substraksi Latar Menggunakan Nilai Mean Untuk Klasifikasi Kendaraan Bergerak Berbasis Deep Learning', 'Comparative analysis of deep learning models for detecting face mask', 'Perbandingan Kinerja Deep Learning Dalam Pendeteksian Kerusakan Biji Kopi', 'https://semopenalex.org/source/S4210178035', 'Moving Pedestrian Localization and Detection With Guided Filtering', 'https://semopenalex.org/source/S2485537415', 'https://semopenalex.org/source/S4210187594', 'https://semopenalex.org/source/S2764455111', 'Image Enhancement for Tuberculosis Detection Using Deep Learning', 'https://semopenalex.org/source/S30680879', 'Moving Object Detection for Complex Scenes by Merging BG Modeling and Deep Learning Method', 'Identification of male and female nutmeg seeds based on the shape and texture features of leaf images using the learning vector quantization (LVQ)', 'A Low-cost Raspberry Pi and Deep Learning System for Customer Analysis', 'Web-App based Melanoma Skin Cancer Classification through Streamlit and Deep Learning', 'https://semopenalex.org/source/S4306401280', 'https://semopenalex.org/source/S4210179954', 'https://semopenalex.org/source/S4306498607', 'Hybrid Models for Emotion Classification and Sentiment Analysis in Indonesian Language', 'Embedded-based Tomato Septoria Leaf Detection with Intel Movidius Neural Compute Stick', 'https://semopenalex.org/source/S4210196574', 'Improved Classification of Handwritten Jawi Script Based on Main Part of Script Body', 'Impact of Image Pre-Processing on Skin Cancer Classification Melanoma Through Deep Learning', 'A Deep Learning Method for Early Detection of Diabetic Foot Using Decision Fusion and Thermal Images', 'https://semopenalex.org/source/S4210230916', 'Convolutional Network and Moving Object Analysis for Vehicle Detection in Highway Surveillance Videos', 'Comparison Study of Corn Leaf Disease Detection based on Deep Learning YOLO-v5 and YOLO-v8', 'https://semopenalex.org/source/S2764607890', 'https://semopenalex.org/source/S120348307', 'Effect of CLAHE-based Enhancement on Bean Leaf Disease Classification through Explainable AI', 'Performance Evaluation of Hardhat Image Classification Using Deep Learning and Grad-CAM', 'https://semopenalex.org/source/S4363607821', 'https://semopenalex.org/source/S4306525036', 'Deep anomaly detection through visual attention in surveillance videos', 'https://semopenalex.org/source/S4210205812']</t>
-  </si>
-  <si>
-    <t>['Rotten Green Tests in Java, Pharo and Python', 'https://semopenalex.org/source/S4210192127', 'W. R. Owens, Stuart Sim, and David Walker, eds. Bunyan Studies: A Journal of Reformation and Nonconformist Culture', 'https://semopenalex.org/source/S4377196300', 'W. R. OWENS, STUART SIM, AND DAVID WALKER, EDS. BUNYAN STUDIES: A JOURNAL OF REFORMATION AND NONCONFORMIST CULTURE. NUMBER 22. NORTHUMBRIA UNIVERSITY, 2018. PP. 164.', 'Rotten green tests in Java, Pharo and Python', 'https://semopenalex.org/source/S4363604151', 'The Secret History of HB-2: Bathroom Safety in the Eighteenth Century and Beyond', 'https://semopenalex.org/source/S4306402203', 'https://semopenalex.org/source/S109852484', 'https://semopenalex.org/source/S4306402512', 'https://semopenalex.org/source/S4306463865', 'Pope and the Reformation of the Oral: The Iliad in the History of Mediation', 'Advances in monitoring carbon dioxide exchange between the atmosphere and mine waste derived from ultramafic-hosted mineral deposits; a pilot study at Cassiar, B.C.', 'https://semopenalex.org/source/S73505065', 'https://semopenalex.org/source/S4306462979']</t>
+    <t>['https://semopenalex.org/work/W2000850157', 'https://semopenalex.org/work/W2154216058', 'https://semopenalex.org/work/W2962540522', 'https://semopenalex.org/work/W2039210571', 'https://semopenalex.org/work/W3021831361', 'https://semopenalex.org/work/W171991278', 'https://semopenalex.org/work/W3009745595', 'https://semopenalex.org/work/W2957946622', 'https://semopenalex.org/work/W2738446327', 'https://semopenalex.org/work/W1625275222', 'https://semopenalex.org/work/W2013165801', 'https://semopenalex.org/work/W1963502684', 'https://semopenalex.org/work/W1516345628', 'https://semopenalex.org/work/W2140243124', 'https://semopenalex.org/work/W3082672072', 'https://semopenalex.org/work/W3037521446', 'https://semopenalex.org/work/W3022514883', 'https://semopenalex.org/work/W128593825', 'https://semopenalex.org/work/W2063989480', 'https://semopenalex.org/work/W2937671906', 'https://semopenalex.org/work/W2099077058', 'https://semopenalex.org/work/W2309635847', 'https://semopenalex.org/work/W2114791275', 'https://semopenalex.org/work/W2530516535', 'https://semopenalex.org/work/W2103364709', 'https://semopenalex.org/work/W2110324005', 'https://semopenalex.org/work/W2055827744', 'https://semopenalex.org/work/W2399215436', 'https://semopenalex.org/work/W4205742677', 'https://semopenalex.org/work/W4299834590', 'https://semopenalex.org/work/W2729343995', 'https://semopenalex.org/work/W961274400', 'https://semopenalex.org/work/W3096817374', 'https://semopenalex.org/work/W67119066', 'https://semopenalex.org/work/W2724228083', 'https://semopenalex.org/work/W2166763164', 'https://semopenalex.org/work/W2514533441', 'https://semopenalex.org/work/W2507172825', 'https://semopenalex.org/work/W2005096286', 'https://semopenalex.org/work/W2588193771', 'https://semopenalex.org/work/W1753483902', 'https://semopenalex.org/work/W3081749826', 'https://semopenalex.org/work/W3012737141', 'https://semopenalex.org/work/W3081541487', 'https://semopenalex.org/work/W3082188274', 'https://semopenalex.org/work/W4386220934', 'https://semopenalex.org/work/W2003205683', 'https://semopenalex.org/work/W3114823909', 'https://semopenalex.org/work/W4378234403', 'https://semopenalex.org/work/W2181900851', 'https://semopenalex.org/work/W2143284629', 'https://semopenalex.org/work/W2128135249', 'https://semopenalex.org/work/W2123134063', 'https://semopenalex.org/work/W3126358682', 'https://semopenalex.org/work/W1536091370', 'https://semopenalex.org/work/W2401739586', 'https://semopenalex.org/work/W4394518676', 'https://semopenalex.org/work/W2164985294', 'https://semopenalex.org/work/W3015578022', 'https://semopenalex.org/work/W146984990', 'https://semopenalex.org/work/W2051791551', 'https://semopenalex.org/work/W4251349925', 'https://semopenalex.org/work/W4247737681', 'https://semopenalex.org/work/W2514686722', 'https://semopenalex.org/work/W2163312800', 'https://semopenalex.org/work/W160337249', 'https://semopenalex.org/work/W30482722', 'https://semopenalex.org/work/W2792227230', 'https://semopenalex.org/work/W4400132771', 'https://semopenalex.org/work/W1965117376', 'https://semopenalex.org/work/W2171958563', 'https://semopenalex.org/work/W2122784464', 'https://semopenalex.org/work/W1870353999', 'https://semopenalex.org/work/W3081531507', 'https://semopenalex.org/work/W2003067257', 'https://semopenalex.org/work/W2999466582', 'https://semopenalex.org/work/W188103252', 'https://semopenalex.org/work/W1702815980', 'https://semopenalex.org/work/W4236983726', 'https://semopenalex.org/work/W2143084783', 'https://semopenalex.org/work/W2892078924', 'https://semopenalex.org/work/W4387589621', 'https://semopenalex.org/work/W3024342691', 'https://semopenalex.org/work/W2321428856', 'https://semopenalex.org/work/W3007663200', 'https://semopenalex.org/work/W2033918799', 'https://semopenalex.org/work/W2403047599', 'https://semopenalex.org/work/W1980799317', 'https://semopenalex.org/work/W4237431914', 'https://semopenalex.org/work/W2242995227', 'https://semopenalex.org/work/W3147662830', 'https://semopenalex.org/work/W2968316987', 'https://semopenalex.org/work/W2898552906', 'https://semopenalex.org/work/W2151304280', 'https://semopenalex.org/work/W1817463943', 'https://semopenalex.org/work/W4301447820', 'https://semopenalex.org/work/W1735274207', 'https://semopenalex.org/work/W4226457422', 'https://semopenalex.org/work/W2182446967', 'https://semopenalex.org/work/W2123551394', 'https://semopenalex.org/work/W2072049173', 'https://semopenalex.org/work/W2005357327', 'https://semopenalex.org/work/W2338530657', 'https://semopenalex.org/work/W2149509417', 'https://semopenalex.org/work/W1972453858', 'https://semopenalex.org/work/W2018345398', 'https://semopenalex.org/work/W2766450143', 'https://semopenalex.org/work/W2970449937', 'https://semopenalex.org/work/W2041337419', 'https://semopenalex.org/work/W653390160', 'https://semopenalex.org/work/W202954270', 'https://semopenalex.org/work/W2753693229', 'https://semopenalex.org/work/W2226738307', 'https://semopenalex.org/work/W2591501322', 'https://semopenalex.org/work/W2112753023', 'https://semopenalex.org/work/W4220992118', 'https://semopenalex.org/work/W2095908354', 'https://semopenalex.org/work/W2883183026', 'https://semopenalex.org/work/W562425896', 'https://semopenalex.org/work/W2133946031', 'https://semopenalex.org/work/W4247029563', 'https://semopenalex.org/work/W3011781542', 'https://semopenalex.org/work/W13024336', 'https://semopenalex.org/work/W4312182041', 'https://semopenalex.org/work/W1990740853', 'https://semopenalex.org/work/W4383065806', 'https://semopenalex.org/work/W2018708687', 'https://semopenalex.org/work/W2557406903', 'https://semopenalex.org/work/W2103430250', 'https://semopenalex.org/work/W2141665828', 'https://semopenalex.org/work/W3081685983', 'https://semopenalex.org/work/W2113694234', 'https://semopenalex.org/work/W2138250189', 'https://semopenalex.org/work/W2888859618', 'https://semopenalex.org/work/W3030243522', 'https://semopenalex.org/work/W4281490671', 'https://semopenalex.org/work/W2599387809', 'https://semopenalex.org/work/W2774855312', 'https://semopenalex.org/work/W2004149428', 'https://semopenalex.org/work/W4404250088', 'https://semopenalex.org/work/W2952764074', 'https://semopenalex.org/work/W2741748074', 'https://semopenalex.org/work/W3013847853', 'https://semopenalex.org/work/W3082938327', 'https://semopenalex.org/work/W200396823', 'https://semopenalex.org/work/W2028031999', 'https://semopenalex.org/work/W2096582083', 'https://semopenalex.org/work/W2771147402', 'https://semopenalex.org/work/W2152754828', 'https://semopenalex.org/work/W2044023590', 'https://semopenalex.org/work/W2587222093', 'https://semopenalex.org/work/W2059580911', 'https://semopenalex.org/work/W2166662555', 'https://semopenalex.org/work/W2165195120', 'https://semopenalex.org/work/W3027665269', 'https://semopenalex.org/work/W4300748512', 'https://semopenalex.org/work/W1986257701', 'https://semopenalex.org/work/W1552001157', 'https://semopenalex.org/work/W2922365273', 'https://semopenalex.org/work/W2234365651', 'https://semopenalex.org/work/W2906284509', 'https://semopenalex.org/work/W1527768716', 'https://semopenalex.org/work/W2805444673', 'https://semopenalex.org/work/W73405584', 'https://semopenalex.org/work/W1552561574', 'https://semopenalex.org/work/W3173715284', 'https://semopenalex.org/work/W1729906464', 'https://semopenalex.org/work/W2067686570', 'https://semopenalex.org/work/W2901545557', 'https://semopenalex.org/work/W2023846135', 'https://semopenalex.org/work/W1417422537', 'https://semopenalex.org/work/W54673566', 'https://semopenalex.org/work/W2150505652', 'https://semopenalex.org/work/W3037487054', 'https://semopenalex.org/work/W2113868440', 'https://semopenalex.org/work/W2901026025', 'https://semopenalex.org/work/W2061486817', 'https://semopenalex.org/work/W2034937923', 'https://semopenalex.org/work/W2023479938', 'https://semopenalex.org/work/W2122677844', 'https://semopenalex.org/work/W4210298342', 'https://semopenalex.org/work/W626749138', 'https://semopenalex.org/work/W2105424397', 'https://semopenalex.org/work/W2035958911', 'https://semopenalex.org/work/W4247632977', 'https://semopenalex.org/work/W1912056476', 'https://semopenalex.org/work/W2065302863', 'https://semopenalex.org/work/W1533919275', 'https://semopenalex.org/work/W1979704442', 'https://semopenalex.org/work/W2100777852', 'https://semopenalex.org/work/W2122538412', 'https://semopenalex.org/work/W4360604687', 'https://semopenalex.org/work/W1552374822', 'https://semopenalex.org/work/W2320884143', 'https://semopenalex.org/work/W2124921180', 'https://semopenalex.org/work/W3036157671', 'https://semopenalex.org/work/W49930183', 'https://semopenalex.org/work/W3082943899', 'https://semopenalex.org/work/W2080393976', 'https://semopenalex.org/work/W2073156145', 'https://semopenalex.org/work/W3149746193', 'https://semopenalex.org/work/W1829136368', 'https://semopenalex.org/work/W2968697710', 'https://semopenalex.org/work/W2004009311', 'https://semopenalex.org/work/W2135586389', 'https://semopenalex.org/work/W4364358025', 'https://semopenalex.org/work/W2130391582', 'https://semopenalex.org/work/W2990422891', 'https://semopenalex.org/work/W4392979894', 'https://semopenalex.org/work/W90104346', 'https://semopenalex.org/work/W2901265490', 'https://semopenalex.org/work/W3016154199', 'https://semopenalex.org/work/W2186313366', 'https://semopenalex.org/work/W2029661605', 'https://semopenalex.org/work/W4249463326', 'https://semopenalex.org/work/W4386157387', 'https://semopenalex.org/work/W1041461969', 'https://semopenalex.org/work/W2728862777', 'https://semopenalex.org/work/W2128936252', 'https://semopenalex.org/work/W2049855663', 'https://semopenalex.org/work/W2162395962', 'https://semopenalex.org/work/W2074682051', 'https://semopenalex.org/work/W2593472651', 'https://semopenalex.org/work/W3082574538', 'https://semopenalex.org/work/W1929232145', 'https://semopenalex.org/work/W2001775984', 'https://semopenalex.org/work/W67844065', 'https://semopenalex.org/work/W2619174663', 'https://semopenalex.org/work/W2141115795', 'https://semopenalex.org/work/W3023079907', 'https://semopenalex.org/work/W2093352090', 'https://semopenalex.org/work/W2775903912', 'https://semopenalex.org/work/W2620095341', 'https://semopenalex.org/work/W155674873', 'https://semopenalex.org/work/W1990062657', 'https://semopenalex.org/work/W2173102402', 'https://semopenalex.org/work/W2512077429', 'https://semopenalex.org/work/W2125654576', 'https://semopenalex.org/work/W2274206371', 'https://semopenalex.org/work/W2185694006', 'https://semopenalex.org/work/W4386776420', 'https://semopenalex.org/work/W2752026712', 'https://semopenalex.org/work/W2098589561', 'https://semopenalex.org/work/W4237274094', 'https://semopenalex.org/work/W2959129322', 'https://semopenalex.org/work/W2136645836', 'https://semopenalex.org/work/W2123582261', 'https://semopenalex.org/work/W1990776069', 'https://semopenalex.org/work/W4287815821', 'https://semopenalex.org/work/W2138588147', 'https://semopenalex.org/work/W2017767972', 'https://semopenalex.org/work/W1542429709', 'https://semopenalex.org/work/W3082580655', 'https://semopenalex.org/work/W2074444313', 'https://semopenalex.org/work/W1755261004', 'https://semopenalex.org/work/W2021648931', 'https://semopenalex.org/work/W2799918114', 'https://semopenalex.org/work/W1096039644', 'https://semopenalex.org/work/W2626706700', 'https://semopenalex.org/work/W1972362582', 'https://semopenalex.org/work/W4404250201', 'https://semopenalex.org/work/W2943865318', 'https://semopenalex.org/work/W2736157438', 'https://semopenalex.org/work/W2152670036', 'https://semopenalex.org/work/W2137367494', 'https://semopenalex.org/work/W4244775271', 'https://semopenalex.org/work/W3038115327', 'https://semopenalex.org/work/W2608090064', 'https://semopenalex.org/work/W2009658718', 'https://semopenalex.org/work/W2969940663', 'https://semopenalex.org/work/W4282914661', 'https://semopenalex.org/work/W3127482518', 'https://semopenalex.org/work/W1963759754', 'https://semopenalex.org/work/W2133819144', 'https://semopenalex.org/work/W2407173971', 'https://semopenalex.org/work/W4251952567', 'https://semopenalex.org/work/W4302424645', 'https://semopenalex.org/work/W2804317122', 'https://semopenalex.org/work/W2906330222', 'https://semopenalex.org/work/W2605190822', 'https://semopenalex.org/work/W2038509977', 'https://semopenalex.org/work/W1996261192', 'https://semopenalex.org/work/W2810861266', 'https://semopenalex.org/work/W2117451136', 'https://semopenalex.org/work/W3120515165', 'https://semopenalex.org/work/W2594497686', 'https://semopenalex.org/work/W4295779216', 'https://semopenalex.org/work/W190600666', 'https://semopenalex.org/work/W2085864217', 'https://semopenalex.org/work/W1980476288', 'https://semopenalex.org/work/W2182785605', 'https://semopenalex.org/work/W2038517887', 'https://semopenalex.org/work/W4210813334', 'https://semopenalex.org/work/W2034235801', 'https://semopenalex.org/work/W4320000513', 'https://semopenalex.org/work/W2077513328', 'https://semopenalex.org/work/W1558485007', 'https://semopenalex.org/work/W2023289472', 'https://semopenalex.org/work/W4210257758', 'https://semopenalex.org/work/W3013220518', 'https://semopenalex.org/work/W2745733921', 'https://semopenalex.org/work/W2003148032', 'https://semopenalex.org/work/W2788844524', 'https://semopenalex.org/work/W2026960907', 'https://semopenalex.org/work/W100499533', 'https://semopenalex.org/work/W2804810577', 'https://semopenalex.org/work/W4239519246', 'https://semopenalex.org/work/W3164080097', 'https://semopenalex.org/work/W2740907063', 'https://semopenalex.org/work/W47444322', 'https://semopenalex.org/work/W2182093612', 'https://semopenalex.org/work/W4396695389', 'https://semopenalex.org/work/W201713607', 'https://semopenalex.org/work/W2153940791', 'https://semopenalex.org/work/W2005948381', 'https://semopenalex.org/work/W4235499751', 'https://semopenalex.org/work/W2151573792', 'https://semopenalex.org/work/W2988464819', 'https://semopenalex.org/work/W2584513564', 'https://semopenalex.org/work/W4384263461', 'https://semopenalex.org/work/W3081898781', 'https://semopenalex.org/work/W2104167274', 'https://semopenalex.org/work/W2171671453', 'https://semopenalex.org/work/W2105281328', 'https://semopenalex.org/work/W2024202481', 'https://semopenalex.org/work/W4389476656', 'https://semopenalex.org/work/W3154255967', 'https://semopenalex.org/work/W2616948544', 'https://semopenalex.org/work/W2995567949', 'https://semopenalex.org/work/W2986447659', 'https://semopenalex.org/work/W4238511116', 'https://semopenalex.org/work/W2116449320', 'https://semopenalex.org/work/W3082909461', 'https://semopenalex.org/work/W2019966888', 'https://semopenalex.org/work/W2094867236', 'https://semopenalex.org/work/W2757690399', 'https://semopenalex.org/work/W2133171495', 'https://semopenalex.org/work/W2605122712', 'https://semopenalex.org/work/W2167424492', 'https://semopenalex.org/work/W4405944965', 'https://semopenalex.org/work/W2069469539', 'https://semopenalex.org/work/W2054518304', 'https://semopenalex.org/work/W2016652422', 'https://semopenalex.org/work/W3082121147', 'https://semopenalex.org/work/W2170327195', 'https://semopenalex.org/work/W4248877513', 'https://semopenalex.org/work/W2277916629', 'https://semopenalex.org/work/W4238264174']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W4319980430', 'https://semopenalex.org/work/W2809907824', 'https://semopenalex.org/work/W2754398119', 'https://semopenalex.org/work/W4393424568', 'https://semopenalex.org/work/W3017267450', 'https://semopenalex.org/work/W4393821610', 'https://semopenalex.org/work/W3047312767', 'https://semopenalex.org/work/W2598695409', 'https://semopenalex.org/work/W2784045768', 'https://semopenalex.org/work/W2964346923']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W2898811429', 'https://semopenalex.org/work/W4320896439', 'https://semopenalex.org/work/W4400675898', 'https://semopenalex.org/work/W4367628070', 'https://semopenalex.org/work/W3145532460', 'https://semopenalex.org/work/W2158735282', 'https://semopenalex.org/work/W1517398235', 'https://semopenalex.org/work/W4293065025', 'https://semopenalex.org/work/W2145330693', 'https://semopenalex.org/work/W1568212182', 'https://semopenalex.org/work/W1810972023', 'https://semopenalex.org/work/W2044633418', 'https://semopenalex.org/work/W4280592120', 'https://semopenalex.org/work/W4283641599', 'https://semopenalex.org/work/W4287668646', 'https://semopenalex.org/work/W2062032381', 'https://semopenalex.org/work/W1908449836', 'https://semopenalex.org/work/W4213248384', 'https://semopenalex.org/work/W4402426748', 'https://semopenalex.org/work/W3010403426', 'https://semopenalex.org/work/W4312667018', 'https://semopenalex.org/work/W4301582020', 'https://semopenalex.org/work/W3153041448', 'https://semopenalex.org/work/W2119804349', 'https://semopenalex.org/work/W4381713892', 'https://semopenalex.org/work/W2971173586', 'https://semopenalex.org/work/W2171240869', 'https://semopenalex.org/work/W3209991164', 'https://semopenalex.org/work/W2549612717', 'https://semopenalex.org/work/W1851000371', 'https://semopenalex.org/work/W3033737646', 'https://semopenalex.org/work/W3127585016', 'https://semopenalex.org/work/W4229517606', 'https://semopenalex.org/work/W4313563578', 'https://semopenalex.org/work/W2135584970', 'https://semopenalex.org/work/W2340333180', 'https://semopenalex.org/work/W4287667875', 'https://semopenalex.org/work/W3126838471', 'https://semopenalex.org/work/W3119454628', 'https://semopenalex.org/work/W2905847388', 'https://semopenalex.org/work/W2049381173', 'https://semopenalex.org/work/W4406157430', 'https://semopenalex.org/work/W2901106555', 'https://semopenalex.org/work/W2333194490', 'https://semopenalex.org/work/W1593690673', 'https://semopenalex.org/work/W2889555883', 'https://semopenalex.org/work/W3085432304', 'https://semopenalex.org/work/W2330908417', 'https://semopenalex.org/work/W4225781798', 'https://semopenalex.org/work/W4319653723', 'https://semopenalex.org/work/W2967719799', 'https://semopenalex.org/work/W3130260207', 'https://semopenalex.org/work/W4387737248', 'https://semopenalex.org/work/W2293962294', 'https://semopenalex.org/work/W4251429682', 'https://semopenalex.org/work/W2110499608', 'https://semopenalex.org/work/W4240535267', 'https://semopenalex.org/work/W2345531317', 'https://semopenalex.org/work/W2059943739', 'https://semopenalex.org/work/W2900603753', 'https://semopenalex.org/work/W3174473101', 'https://semopenalex.org/work/W3084710058', 'https://semopenalex.org/work/W4287668995', 'https://semopenalex.org/work/W4235240618', 'https://semopenalex.org/work/W2077664520', 'https://semopenalex.org/work/W2967526509', 'https://semopenalex.org/work/W3206231781', 'https://semopenalex.org/work/W2788992245', 'https://semopenalex.org/work/W2142174774', 'https://semopenalex.org/work/W3043915370', 'https://semopenalex.org/work/W4363671915', 'https://semopenalex.org/work/W4249431654', 'https://semopenalex.org/work/W2809425916', 'https://semopenalex.org/work/W3169232032', 'https://semopenalex.org/work/W4288261968', 'https://semopenalex.org/work/W2211800868', 'https://semopenalex.org/work/W2293309991', 'https://semopenalex.org/work/W2530456191', 'https://semopenalex.org/work/W4287235540', 'https://semopenalex.org/work/W3084859057', 'https://semopenalex.org/work/W4287392742', 'https://semopenalex.org/work/W4319264802', 'https://semopenalex.org/work/W3121391869', 'https://semopenalex.org/work/W2055489377', 'https://semopenalex.org/work/W2899596954', 'https://semopenalex.org/work/W4399872440', 'https://semopenalex.org/work/W4318159625', 'https://semopenalex.org/work/W4321796319', 'https://semopenalex.org/work/W3014769903', 'https://semopenalex.org/work/W2272844336', 'https://semopenalex.org/work/W3121852636', 'https://semopenalex.org/work/W2893263830', 'https://semopenalex.org/work/W3110545566', 'https://semopenalex.org/work/W2272672851', 'https://semopenalex.org/work/W2967175067', 'https://semopenalex.org/work/W4312757941', 'https://semopenalex.org/work/W2093284392']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W1999760195', 'https://semopenalex.org/work/W2903944530', 'https://semopenalex.org/work/W3134422373', 'https://semopenalex.org/work/W2897762537', 'https://semopenalex.org/work/W4396568545', 'https://semopenalex.org/work/W2844810377', 'https://semopenalex.org/work/W4367671449', 'https://semopenalex.org/work/W3048792033', 'https://semopenalex.org/work/W4238294234', 'https://semopenalex.org/work/W2996342798', 'https://semopenalex.org/work/W2100407406', 'https://semopenalex.org/work/W2974444355', 'https://semopenalex.org/work/W2996971450', 'https://semopenalex.org/work/W4390737683', 'https://semopenalex.org/work/W2780277126', 'https://semopenalex.org/work/W2979701877', 'https://semopenalex.org/work/W2957110867', 'https://semopenalex.org/work/W2792290921', 'https://semopenalex.org/work/W4206136166', 'https://semopenalex.org/work/W2772966323', 'https://semopenalex.org/work/W2788968669', 'https://semopenalex.org/work/W3202715770', 'https://semopenalex.org/work/W3158463786', 'https://semopenalex.org/work/W2226359063', 'https://semopenalex.org/work/W3205075200', 'https://semopenalex.org/work/W2948196949', 'https://semopenalex.org/work/W2805460435', 'https://semopenalex.org/work/W4406267825', 'https://semopenalex.org/work/W4293863370', 'https://semopenalex.org/work/W2397277866']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W2150882603', 'https://semopenalex.org/work/W4206707377', 'https://semopenalex.org/work/W2073791116', 'https://semopenalex.org/work/W4386082512', 'https://semopenalex.org/work/W2469325223', 'https://semopenalex.org/work/W1980119762', 'https://semopenalex.org/work/W3110875274', 'https://semopenalex.org/work/W4287391921', 'https://semopenalex.org/work/W2995556886', 'https://semopenalex.org/work/W4378942243', 'https://semopenalex.org/work/W2972760949', 'https://semopenalex.org/work/W4322099461', 'https://semopenalex.org/work/W4406676443', 'https://semopenalex.org/work/W3083323811', 'https://semopenalex.org/work/W3207608819', 'https://semopenalex.org/work/W4400266996', 'https://semopenalex.org/work/W3203181771', 'https://semopenalex.org/work/W3168652588', 'https://semopenalex.org/work/W4393911083', 'https://semopenalex.org/work/W4290059224', 'https://semopenalex.org/work/W2879029702', 'https://semopenalex.org/work/W4288364801', 'https://semopenalex.org/work/W4210756135', 'https://semopenalex.org/work/W2184966923', 'https://semopenalex.org/work/W4245299688', 'https://semopenalex.org/work/W3202872895', 'https://semopenalex.org/work/W1977295820', 'https://semopenalex.org/work/W4391901288', 'https://semopenalex.org/work/W2038323322', 'https://semopenalex.org/work/W2784298189', 'https://semopenalex.org/work/W4295253548', 'https://semopenalex.org/work/W4284710143', 'https://semopenalex.org/work/W4394931310', 'https://semopenalex.org/work/W294448757', 'https://semopenalex.org/work/W3099785009', 'https://semopenalex.org/work/W4312473456', 'https://semopenalex.org/work/W2022832873', 'https://semopenalex.org/work/W3091415435', 'https://semopenalex.org/work/W4398157632', 'https://semopenalex.org/work/W2039557327', 'https://semopenalex.org/work/W2467368527', 'https://semopenalex.org/work/W3183881674', 'https://semopenalex.org/work/W4398809881', 'https://semopenalex.org/work/W1805881796', 'https://semopenalex.org/work/W3046183292', 'https://semopenalex.org/work/W2090465764', 'https://semopenalex.org/work/W4255912054', 'https://semopenalex.org/work/W2027952077', 'https://semopenalex.org/work/W4285827783', 'https://semopenalex.org/work/W4392617501', 'https://semopenalex.org/work/W1966530006', 'https://semopenalex.org/work/W3176114075', 'https://semopenalex.org/work/W4383046641', 'https://semopenalex.org/work/W3003928672', 'https://semopenalex.org/work/W4287900890', 'https://semopenalex.org/work/W2929118134', 'https://semopenalex.org/work/W2145997469', 'https://semopenalex.org/work/W4399986811', 'https://semopenalex.org/work/W3126679255', 'https://semopenalex.org/work/W2548547123', 'https://semopenalex.org/work/W2898907473', 'https://semopenalex.org/work/W3095459301', 'https://semopenalex.org/work/W3121327306', 'https://semopenalex.org/work/W3004806403', 'https://semopenalex.org/work/W1494996644', 'https://semopenalex.org/work/W4385292569', 'https://semopenalex.org/work/W2464529301', 'https://semopenalex.org/work/W4406193279', 'https://semopenalex.org/work/W816337693', 'https://semopenalex.org/work/W4385804769', 'https://semopenalex.org/work/W4379933304', 'https://semopenalex.org/work/W2552048974', 'https://semopenalex.org/work/W4287776928', 'https://semopenalex.org/work/W2519804223', 'https://semopenalex.org/work/W2996860607', 'https://semopenalex.org/work/W2137100320', 'https://semopenalex.org/work/W3047893908', 'https://semopenalex.org/work/W3110177420', 'https://semopenalex.org/work/W2914677765', 'https://semopenalex.org/work/W2244659594', 'https://semopenalex.org/work/W4200081143', 'https://semopenalex.org/work/W2337546824', 'https://semopenalex.org/work/W2162555816', 'https://semopenalex.org/work/W4368353176', 'https://semopenalex.org/work/W2114925746', 'https://semopenalex.org/work/W4384561507', 'https://semopenalex.org/work/W1997430507', 'https://semopenalex.org/work/W3025540705', 'https://semopenalex.org/work/W3093436911', 'https://semopenalex.org/work/W1753084818', 'https://semopenalex.org/work/W3212849404', 'https://semopenalex.org/work/W3048856089', 'https://semopenalex.org/work/W2171559681', 'https://semopenalex.org/work/W4292798214', 'https://semopenalex.org/work/W4320341743', 'https://semopenalex.org/work/W75304744', 'https://semopenalex.org/work/W3096998353', 'https://semopenalex.org/work/W2760871008', 'https://semopenalex.org/work/W3007227736', 'https://semopenalex.org/work/W2131147042', 'https://semopenalex.org/work/W2157747589', 'https://semopenalex.org/work/W2059502067', 'https://semopenalex.org/work/W2525851376', 'https://semopenalex.org/work/W2466191378', 'https://semopenalex.org/work/W3127829048', 'https://semopenalex.org/work/W3171100434', 'https://semopenalex.org/work/W3156189202', 'https://semopenalex.org/work/W97884251', 'https://semopenalex.org/work/W3034646170', 'https://semopenalex.org/work/W2625157458', 'https://semopenalex.org/work/W4400447326', 'https://semopenalex.org/work/W2086755418', 'https://semopenalex.org/work/W3167824842', 'https://semopenalex.org/work/W4323038488', 'https://semopenalex.org/work/W2786460214', 'https://semopenalex.org/work/W4311007713', 'https://semopenalex.org/work/W3001208429', 'https://semopenalex.org/work/W3096783252', 'https://semopenalex.org/work/W3001949026', 'https://semopenalex.org/work/W169568933', 'https://semopenalex.org/work/W4221159459', 'https://semopenalex.org/work/W4231137968', 'https://semopenalex.org/work/W3174807969', 'https://semopenalex.org/work/W3048770428', 'https://semopenalex.org/work/W4210597606', 'https://semopenalex.org/work/W3210446150', 'https://semopenalex.org/work/W3207505502', 'https://semopenalex.org/work/W3129635911', 'https://semopenalex.org/work/W4406482035', 'https://semopenalex.org/work/W2606709877', 'https://semopenalex.org/work/W4385584193', 'https://semopenalex.org/work/W1972302881', 'https://semopenalex.org/work/W2945856475', 'https://semopenalex.org/work/W3211048833', 'https://semopenalex.org/work/W4287691869', 'https://semopenalex.org/work/W3145938895', 'https://semopenalex.org/work/W2059743020', 'https://semopenalex.org/work/W3008746569', 'https://semopenalex.org/work/W3096308497', 'https://semopenalex.org/work/W4297060365', 'https://semopenalex.org/work/W3015838662', 'https://semopenalex.org/work/W2969671163', 'https://semopenalex.org/work/W2108950108', 'https://semopenalex.org/work/W2152423878', 'https://semopenalex.org/work/W4367297631', 'https://semopenalex.org/work/W4387321281', 'https://semopenalex.org/work/W2122005484', 'https://semopenalex.org/work/W2014168043', 'https://semopenalex.org/work/W3198808971', 'https://semopenalex.org/work/W2898863929', 'https://semopenalex.org/work/W2999276659', 'https://semopenalex.org/work/W3104328743', 'https://semopenalex.org/work/W3173111918', 'https://semopenalex.org/work/W2462370865', 'https://semopenalex.org/work/W2820922764', 'https://semopenalex.org/work/W4286953522', 'https://semopenalex.org/work/W4287123914', 'https://semopenalex.org/work/W1991539813', 'https://semopenalex.org/work/W1587612576', 'https://semopenalex.org/work/W4230850676', 'https://semopenalex.org/work/W3131298139', 'https://semopenalex.org/work/W4283823243', 'https://semopenalex.org/work/W4366342364', 'https://semopenalex.org/work/W2939129451', 'https://semopenalex.org/work/W4284892042', 'https://semopenalex.org/work/W2924522543', 'https://semopenalex.org/work/W1579732497', 'https://semopenalex.org/work/W2403591241', 'https://semopenalex.org/work/W2732107624', 'https://semopenalex.org/work/W2460754307', 'https://semopenalex.org/work/W4324116704', 'https://semopenalex.org/work/W3106951738', 'https://semopenalex.org/work/W2808145095', 'https://semopenalex.org/work/W4287023576', 'https://semopenalex.org/work/W2905242827', 'https://semopenalex.org/work/W3092216346', 'https://semopenalex.org/work/W3007493000', 'https://semopenalex.org/work/W4296070200', 'https://semopenalex.org/work/W2972736078', 'https://semopenalex.org/work/W2004314166', 'https://semopenalex.org/work/W2087611087', 'https://semopenalex.org/work/W2154718966', 'https://semopenalex.org/work/W2804309962', 'https://semopenalex.org/work/W4403635745', 'https://semopenalex.org/work/W2060122457', 'https://semopenalex.org/work/W2117788706', 'https://semopenalex.org/work/W2316889284', 'https://semopenalex.org/work/W1975771789', 'https://semopenalex.org/work/W2899181049', 'https://semopenalex.org/work/W2971872524', 'https://semopenalex.org/work/W3041585044', 'https://semopenalex.org/work/W4384392951', 'https://semopenalex.org/work/W3203846187', 'https://semopenalex.org/work/W3028984135', 'https://semopenalex.org/work/W4384919669', 'https://semopenalex.org/work/W2056591916', 'https://semopenalex.org/work/W2156740813', 'https://semopenalex.org/work/W4384615920', 'https://semopenalex.org/work/W4387799594', 'https://semopenalex.org/work/W1246540336', 'https://semopenalex.org/work/W87063158', 'https://semopenalex.org/work/W4221120919', 'https://semopenalex.org/work/W4287690348', 'https://semopenalex.org/work/W4236853429', 'https://semopenalex.org/work/W2038134612', 'https://semopenalex.org/work/W4323038447', 'https://semopenalex.org/work/W2979711838', 'https://semopenalex.org/work/W4287279053', 'https://semopenalex.org/work/W4297060071', 'https://semopenalex.org/work/W2084071117', 'https://semopenalex.org/work/W2343779160', 'https://semopenalex.org/work/W3008634715', 'https://semopenalex.org/work/W2972393922', 'https://semopenalex.org/work/W2905715248', 'https://semopenalex.org/work/W2297325673', 'https://semopenalex.org/work/W3038185437', 'https://semopenalex.org/work/W4233099794', 'https://semopenalex.org/work/W3049640275', 'https://semopenalex.org/work/W2132391423', 'https://semopenalex.org/work/W4287241484', 'https://semopenalex.org/work/W1982467666', 'https://semopenalex.org/work/W2558974524', 'https://semopenalex.org/work/W3018835489', 'https://semopenalex.org/work/W2546536770', 'https://semopenalex.org/work/W4310562517', 'https://semopenalex.org/work/W2214980064', 'https://semopenalex.org/work/W2096948221', 'https://semopenalex.org/work/W3043093753', 'https://semopenalex.org/work/W3093421867', 'https://semopenalex.org/work/W2463050926', 'https://semopenalex.org/work/W3121924028', 'https://semopenalex.org/work/W3134509799', 'https://semopenalex.org/work/W3210294081', 'https://semopenalex.org/work/W4287746776', 'https://semopenalex.org/work/W3133606938', 'https://semopenalex.org/work/W1965596253', 'https://semopenalex.org/work/W2991253882', 'https://semopenalex.org/work/W4287123862', 'https://semopenalex.org/work/W3005828390', 'https://semopenalex.org/work/W4306703516', 'https://semopenalex.org/work/W2973151896', 'https://semopenalex.org/work/W4403786771', 'https://semopenalex.org/work/W3093453792', 'https://semopenalex.org/work/W4390872486', 'https://semopenalex.org/work/W4403964510', 'https://semopenalex.org/work/W2343495200', 'https://semopenalex.org/work/W2559181347', 'https://semopenalex.org/work/W4283024182', 'https://semopenalex.org/work/W4308083526', 'https://semopenalex.org/work/W4286902665', 'https://semopenalex.org/work/W3106656598', 'https://semopenalex.org/work/W3201845268', 'https://semopenalex.org/work/W1572192454', 'https://semopenalex.org/work/W4287902355', 'https://semopenalex.org/work/W3101755570', 'https://semopenalex.org/work/W3085924585', 'https://semopenalex.org/work/W2472426210', 'https://semopenalex.org/work/W2509887407', 'https://semopenalex.org/work/W4226041925', 'https://semopenalex.org/work/W2739601332', 'https://semopenalex.org/work/W4320341944', 'https://semopenalex.org/work/W2142857396', 'https://semopenalex.org/work/W1966445952', 'https://semopenalex.org/work/W2041454412', 'https://semopenalex.org/work/W3030459553', 'https://semopenalex.org/work/W3216699651', 'https://semopenalex.org/work/W4396243491', 'https://semopenalex.org/work/W2626549485', 'https://semopenalex.org/work/W2911439292', 'https://semopenalex.org/work/W3128789131', 'https://semopenalex.org/work/W4389261110', 'https://semopenalex.org/work/W2572480678', 'https://semopenalex.org/work/W4296596641', 'https://semopenalex.org/work/W2120761625', 'https://semopenalex.org/work/W4377298398', 'https://semopenalex.org/work/W4280611212', 'https://semopenalex.org/work/W2798926091', 'https://semopenalex.org/work/W4226302796', 'https://semopenalex.org/work/W3027839759', 'https://semopenalex.org/work/W3124523586', 'https://semopenalex.org/work/W2123140882', 'https://semopenalex.org/work/W3194018690', 'https://semopenalex.org/work/W4319862456', 'https://semopenalex.org/work/W4382464396', 'https://semopenalex.org/work/W3176780274', 'https://semopenalex.org/work/W144502943', 'https://semopenalex.org/work/W2043475427', 'https://semopenalex.org/work/W3147053158', 'https://semopenalex.org/work/W3097384956', 'https://semopenalex.org/work/W2916044424', 'https://semopenalex.org/work/W4399317854', 'https://semopenalex.org/work/W4391766346', 'https://semopenalex.org/work/W2997497769', 'https://semopenalex.org/work/W2754395205', 'https://semopenalex.org/work/W2941573428', 'https://semopenalex.org/work/W2900566525', 'https://semopenalex.org/work/W4287726151', 'https://semopenalex.org/work/W2951433015', 'https://semopenalex.org/work/W2954507353', 'https://semopenalex.org/work/W2777460464', 'https://semopenalex.org/work/W2473751517', 'https://semopenalex.org/work/W4404395434', 'https://semopenalex.org/work/W3177180018', 'https://semopenalex.org/work/W3128506819', 'https://semopenalex.org/work/W3107781032', 'https://semopenalex.org/work/W3160945783', 'https://semopenalex.org/work/W2163036976', 'https://semopenalex.org/work/W3209796046', 'https://semopenalex.org/work/W3201319033', 'https://semopenalex.org/work/W3101164610', 'https://semopenalex.org/work/W2164297046', 'https://semopenalex.org/work/W3210764291', 'https://semopenalex.org/work/W2026124805', 'https://semopenalex.org/work/W2825911140']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W4386572358', 'https://semopenalex.org/work/W2037815363', 'https://semopenalex.org/work/W4312385873', 'https://semopenalex.org/work/W2012725729', 'https://semopenalex.org/work/W4387714873', 'https://semopenalex.org/work/W4403635673', 'https://semopenalex.org/work/W2335568438', 'https://semopenalex.org/work/W2964765424', 'https://semopenalex.org/work/W2202885265', 'https://semopenalex.org/work/W2889572683', 'https://semopenalex.org/work/W2120547457', 'https://semopenalex.org/work/W3184809481', 'https://semopenalex.org/work/W2970760542', 'https://semopenalex.org/work/W2695892072', 'https://semopenalex.org/work/W4400112330', 'https://semopenalex.org/work/W2158244986', 'https://semopenalex.org/work/W2063160426', 'https://semopenalex.org/work/W3143148447', 'https://semopenalex.org/work/W4399339526', 'https://semopenalex.org/work/W2116800013', 'https://semopenalex.org/work/W2958283264', 'https://semopenalex.org/work/W2110460866', 'https://semopenalex.org/work/W2002064143', 'https://semopenalex.org/work/W2966346292', 'https://semopenalex.org/work/W2907905966', 'https://semopenalex.org/work/W4297989904', 'https://semopenalex.org/work/W4395684973', 'https://semopenalex.org/work/W1989814488', 'https://semopenalex.org/work/W2784241930', 'https://semopenalex.org/work/W2326531986', 'https://semopenalex.org/work/W4387869863', 'https://semopenalex.org/work/W4386528085', 'https://semopenalex.org/work/W4386919989', 'https://semopenalex.org/work/W3210031557', 'https://semopenalex.org/work/W3014966924', 'https://semopenalex.org/work/W4213077479', 'https://semopenalex.org/work/W2466861718', 'https://semopenalex.org/work/W2116843437', 'https://semopenalex.org/work/W1990148059', 'https://semopenalex.org/work/W2046114048', 'https://semopenalex.org/work/W4389961028', 'https://semopenalex.org/work/W2763111898', 'https://semopenalex.org/work/W4296270284', 'https://semopenalex.org/work/W4390938914', 'https://semopenalex.org/work/W4400904607', 'https://semopenalex.org/work/W4205522738', 'https://semopenalex.org/work/W2990794959', 'https://semopenalex.org/work/W2932650350', 'https://semopenalex.org/work/W3139378559', 'https://semopenalex.org/work/W2269062875', 'https://semopenalex.org/work/W4404210445', 'https://semopenalex.org/work/W2916900328', 'https://semopenalex.org/work/W2154565949', 'https://semopenalex.org/work/W2535770837', 'https://semopenalex.org/work/W4403124399', 'https://semopenalex.org/work/W1993621621', 'https://semopenalex.org/work/W2564919106', 'https://semopenalex.org/work/W2966498804', 'https://semopenalex.org/work/W2912046801', 'https://semopenalex.org/work/W3181963703', 'https://semopenalex.org/work/W2143110402', 'https://semopenalex.org/work/W2765287619', 'https://semopenalex.org/work/W4390602383', 'https://semopenalex.org/work/W3196284684', 'https://semopenalex.org/work/W2965197902', 'https://semopenalex.org/work/W4384917079', 'https://semopenalex.org/work/W4367147910', 'https://semopenalex.org/work/W1991496323', 'https://semopenalex.org/work/W1986594812', 'https://semopenalex.org/work/W2988764224', 'https://semopenalex.org/work/W4392513104', 'https://semopenalex.org/work/W2941782253', 'https://semopenalex.org/work/W2557139677', 'https://semopenalex.org/work/W1990178810', 'https://semopenalex.org/work/W1972504394', 'https://semopenalex.org/work/W3160686564', 'https://semopenalex.org/work/W2056907372', 'https://semopenalex.org/work/W4386918818', 'https://semopenalex.org/work/W4389888434', 'https://semopenalex.org/work/W2535549373', 'https://semopenalex.org/work/W2010049933', 'https://semopenalex.org/work/W4399341408', 'https://semopenalex.org/work/W2797953332', 'https://semopenalex.org/work/W3192507507', 'https://semopenalex.org/work/W2557492665', 'https://semopenalex.org/work/W2964505054', 'https://semopenalex.org/work/W4404670877', 'https://semopenalex.org/work/W1556213926', 'https://semopenalex.org/work/W2341987404', 'https://semopenalex.org/work/W4224245749', 'https://semopenalex.org/work/W2804501132', 'https://semopenalex.org/work/W4206824496', 'https://semopenalex.org/work/W4390758153', 'https://semopenalex.org/work/W4388286311', 'https://semopenalex.org/work/W2769916035', 'https://semopenalex.org/work/W3083528472', 'https://semopenalex.org/work/W3013399598', 'https://semopenalex.org/work/W2401510428', 'https://semopenalex.org/work/W2175711660', 'https://semopenalex.org/work/W4385267612', 'https://semopenalex.org/work/W3139325069', 'https://semopenalex.org/work/W2620634483', 'https://semopenalex.org/work/W4293211890', 'https://semopenalex.org/work/W2905349707', 'https://semopenalex.org/work/W3104724617', 'https://semopenalex.org/work/W2058599944', 'https://semopenalex.org/work/W2010955203', 'https://semopenalex.org/work/W4391878166', 'https://semopenalex.org/work/W2951051768', 'https://semopenalex.org/work/W4226250318', 'https://semopenalex.org/work/W2520653549', 'https://semopenalex.org/work/W2562454548', 'https://semopenalex.org/work/W2912334744', 'https://semopenalex.org/work/W4391895094', 'https://semopenalex.org/work/W2036764408', 'https://semopenalex.org/work/W2038007991', 'https://semopenalex.org/work/W3216386918', 'https://semopenalex.org/work/W4380451175', 'https://semopenalex.org/work/W2712995990', 'https://semopenalex.org/work/W2095378229', 'https://semopenalex.org/work/W2121795575', 'https://semopenalex.org/work/W4367148117', 'https://semopenalex.org/work/W3163178830', 'https://semopenalex.org/work/W4402125734', 'https://semopenalex.org/work/W1904270298', 'https://semopenalex.org/work/W4328028090', 'https://semopenalex.org/work/W4389303997', 'https://semopenalex.org/work/W2064850826', 'https://semopenalex.org/work/W4386736850', 'https://semopenalex.org/work/W2383377836', 'https://semopenalex.org/work/W2017065682', 'https://semopenalex.org/work/W4402264038', 'https://semopenalex.org/work/W2038570675', 'https://semopenalex.org/work/W1971616362', 'https://semopenalex.org/work/W1497963603', 'https://semopenalex.org/work/W4390778221', 'https://semopenalex.org/work/W2031326270', 'https://semopenalex.org/work/W2621374881', 'https://semopenalex.org/work/W2887601228', 'https://semopenalex.org/work/W2122864277', 'https://semopenalex.org/work/W2036128771', 'https://semopenalex.org/work/W2391301195', 'https://semopenalex.org/work/W2796524784', 'https://semopenalex.org/work/W2983906786', 'https://semopenalex.org/work/W2589296175', 'https://semopenalex.org/work/W4205304527', 'https://semopenalex.org/work/W2784259369', 'https://semopenalex.org/work/W3117499383', 'https://semopenalex.org/work/W4391429213', 'https://semopenalex.org/work/W2029634930', 'https://semopenalex.org/work/W4225497412', 'https://semopenalex.org/work/W3133466818', 'https://semopenalex.org/work/W1984984026', 'https://semopenalex.org/work/W2605870759', 'https://semopenalex.org/work/W2012087113', 'https://semopenalex.org/work/W2169103252', 'https://semopenalex.org/work/W2168189713', 'https://semopenalex.org/work/W4206221314', 'https://semopenalex.org/work/W4405179870', 'https://semopenalex.org/work/W2066280901', 'https://semopenalex.org/work/W2804609139', 'https://semopenalex.org/work/W2946047926', 'https://semopenalex.org/work/W1492042394', 'https://semopenalex.org/work/W1857828242', 'https://semopenalex.org/work/W2058842944', 'https://semopenalex.org/work/W4367147772', 'https://semopenalex.org/work/W3004718696', 'https://semopenalex.org/work/W2561915240', 'https://semopenalex.org/work/W3012171841', 'https://semopenalex.org/work/W4398152845', 'https://semopenalex.org/work/W4403182200', 'https://semopenalex.org/work/W2982613775', 'https://semopenalex.org/work/W4328011761', 'https://semopenalex.org/work/W4367148069', 'https://semopenalex.org/work/W3206648460', 'https://semopenalex.org/work/W2789498674', 'https://semopenalex.org/work/W2330731982', 'https://semopenalex.org/work/W4389161163', 'https://semopenalex.org/work/W282835794', 'https://semopenalex.org/work/W4399463135', 'https://semopenalex.org/work/W3020423550', 'https://semopenalex.org/work/W4389692495', 'https://semopenalex.org/work/W2052206457', 'https://semopenalex.org/work/W2081488658', 'https://semopenalex.org/work/W2900379070', 'https://semopenalex.org/work/W2143818732', 'https://semopenalex.org/work/W2998591860', 'https://semopenalex.org/work/W2904413102', 'https://semopenalex.org/work/W4288039534', 'https://semopenalex.org/work/W3205428400', 'https://semopenalex.org/work/W4313291203', 'https://semopenalex.org/work/W4360901644', 'https://semopenalex.org/work/W2373453410', 'https://semopenalex.org/work/W2095529201', 'https://semopenalex.org/work/W2566566708', 'https://semopenalex.org/work/W2022326160', 'https://semopenalex.org/work/W2149743901', 'https://semopenalex.org/work/W2949306598', 'https://semopenalex.org/work/W4393174751', 'https://semopenalex.org/work/W4320068529', 'https://semopenalex.org/work/W2995016007', 'https://semopenalex.org/work/W2473454588', 'https://semopenalex.org/work/W2892268308', 'https://semopenalex.org/work/W4328012044', 'https://semopenalex.org/work/W4402835717', 'https://semopenalex.org/work/W2144892219', 'https://semopenalex.org/work/W3143088633', 'https://semopenalex.org/work/W3140868540', 'https://semopenalex.org/work/W4392573792', 'https://semopenalex.org/work/W4295046603', 'https://semopenalex.org/work/W2027931215', 'https://semopenalex.org/work/W2805010740', 'https://semopenalex.org/work/W2047610380', 'https://semopenalex.org/work/W4323644072', 'https://semopenalex.org/work/W3089077757', 'https://semopenalex.org/work/W2134725794', 'https://semopenalex.org/work/W1525424336', 'https://semopenalex.org/work/W2188557470', 'https://semopenalex.org/work/W3152870376', 'https://semopenalex.org/work/W2327416585', 'https://semopenalex.org/work/W2538882601', 'https://semopenalex.org/work/W4388213914', 'https://semopenalex.org/work/W4213097356', 'https://semopenalex.org/work/W2115836030', 'https://semopenalex.org/work/W2539966993', 'https://semopenalex.org/work/W2624719059', 'https://semopenalex.org/work/W2966881022', 'https://semopenalex.org/work/W4379034010', 'https://semopenalex.org/work/W4289203223', 'https://semopenalex.org/work/W4403233403', 'https://semopenalex.org/work/W4399910027', 'https://semopenalex.org/work/W2124863572', 'https://semopenalex.org/work/W2613801228', 'https://semopenalex.org/work/W2556760577', 'https://semopenalex.org/work/W2782998407', 'https://semopenalex.org/work/W4389317944', 'https://semopenalex.org/work/W3112944858', 'https://semopenalex.org/work/W3110950550', 'https://semopenalex.org/work/W2591061174', 'https://semopenalex.org/work/W2906372377', 'https://semopenalex.org/work/W2999941952', 'https://semopenalex.org/work/W2018860951', 'https://semopenalex.org/work/W2115198688', 'https://semopenalex.org/work/W2174090751', 'https://semopenalex.org/work/W4401990766', 'https://semopenalex.org/work/W2013087313', 'https://semopenalex.org/work/W2887046167', 'https://semopenalex.org/work/W4404979988', 'https://semopenalex.org/work/W2113578263', 'https://semopenalex.org/work/W4224994268', 'https://semopenalex.org/work/W2737288996', 'https://semopenalex.org/work/W4387319244', 'https://semopenalex.org/work/W4312265249', 'https://semopenalex.org/work/W2964541684', 'https://semopenalex.org/work/W4385826750', 'https://semopenalex.org/work/W4382119833', 'https://semopenalex.org/work/W1981489703', 'https://semopenalex.org/work/W2017487069', 'https://semopenalex.org/work/W4387697022', 'https://semopenalex.org/work/W2073648968', 'https://semopenalex.org/work/W176895944', 'https://semopenalex.org/work/W3141789341', 'https://semopenalex.org/work/W3085844533', 'https://semopenalex.org/work/W2085741604', 'https://semopenalex.org/work/W4296441394', 'https://semopenalex.org/work/W3167125565', 'https://semopenalex.org/work/W4313534837', 'https://semopenalex.org/work/W2529348703', 'https://semopenalex.org/work/W2921446145', 'https://semopenalex.org/work/W2793708954', 'https://semopenalex.org/work/W1489929835', 'https://semopenalex.org/work/W3018428182', 'https://semopenalex.org/work/W2928810931', 'https://semopenalex.org/work/W3017282193', 'https://semopenalex.org/work/W2782839007', 'https://semopenalex.org/work/W3004954023', 'https://semopenalex.org/work/W2289787480', 'https://semopenalex.org/work/W2530101013', 'https://semopenalex.org/work/W2100819606', 'https://semopenalex.org/work/W2901482574', 'https://semopenalex.org/work/W2977054173', 'https://semopenalex.org/work/W3041302202', 'https://semopenalex.org/work/W4387322936', 'https://semopenalex.org/work/W2810470829', 'https://semopenalex.org/work/W2138141935', 'https://semopenalex.org/work/W2139900006', 'https://semopenalex.org/work/W2334282167', 'https://semopenalex.org/work/W2168624747', 'https://semopenalex.org/work/W1968665462', 'https://semopenalex.org/work/W4226219986', 'https://semopenalex.org/work/W2042556111', 'https://semopenalex.org/work/W2883689704', 'https://semopenalex.org/work/W4388837994', 'https://semopenalex.org/work/W2518984475', 'https://semopenalex.org/work/W3199993893', 'https://semopenalex.org/work/W4313306257', 'https://semopenalex.org/work/W4404576824', 'https://semopenalex.org/work/W4402978247', 'https://semopenalex.org/work/W3133565115', 'https://semopenalex.org/work/W4405937034', 'https://semopenalex.org/work/W4391072497', 'https://semopenalex.org/work/W2593161952', 'https://semopenalex.org/work/W4392024074', 'https://semopenalex.org/work/W4367663134', 'https://semopenalex.org/work/W2903850618', 'https://semopenalex.org/work/W4295127425', 'https://semopenalex.org/work/W2804348493', 'https://semopenalex.org/work/W2037720083', 'https://semopenalex.org/work/W2052995625', 'https://semopenalex.org/work/W3213939512', 'https://semopenalex.org/work/W2351972364', 'https://semopenalex.org/work/W2783829353', 'https://semopenalex.org/work/W4402836042', 'https://semopenalex.org/work/W2804263862', 'https://semopenalex.org/work/W2768917932', 'https://semopenalex.org/work/W2891934018', 'https://semopenalex.org/work/W3133842302', 'https://semopenalex.org/work/W2803338056', 'https://semopenalex.org/work/W4402834371', 'https://semopenalex.org/work/W2045885650', 'https://semopenalex.org/work/W4392607874', 'https://semopenalex.org/work/W2089235671', 'https://semopenalex.org/work/W3196195396', 'https://semopenalex.org/work/W2413354569', 'https://semopenalex.org/work/W2023195652', 'https://semopenalex.org/work/W976487463', 'https://semopenalex.org/work/W2292434057', 'https://semopenalex.org/work/W2393603173', 'https://semopenalex.org/work/W4390777144', 'https://semopenalex.org/work/W3125270863', 'https://semopenalex.org/work/W4401210873', 'https://semopenalex.org/work/W4312643037', 'https://semopenalex.org/work/W4388551259', 'https://semopenalex.org/work/W2181697561', 'https://semopenalex.org/work/W2566656454', 'https://semopenalex.org/work/W2624040609', 'https://semopenalex.org/work/W2077093994', 'https://semopenalex.org/work/W2904825736', 'https://semopenalex.org/work/W2151517333', 'https://semopenalex.org/work/W3088595531', 'https://semopenalex.org/work/W2395017188', 'https://semopenalex.org/work/W4376142881', 'https://semopenalex.org/work/W2473050328', 'https://semopenalex.org/work/W3145628585', 'https://semopenalex.org/work/W2145337100', 'https://semopenalex.org/work/W4328027566', 'https://semopenalex.org/work/W4391326572', 'https://semopenalex.org/work/W2549420274', 'https://semopenalex.org/work/W4282826154', 'https://semopenalex.org/work/W2566503827', 'https://semopenalex.org/work/W4405270053', 'https://semopenalex.org/work/W4210569910', 'https://semopenalex.org/work/W4388953015', 'https://semopenalex.org/work/W4289821472', 'https://semopenalex.org/work/W2258995161', 'https://semopenalex.org/work/W2055837742', 'https://semopenalex.org/work/W4312161546', 'https://semopenalex.org/work/W3090262174', 'https://semopenalex.org/work/W2135168342', 'https://semopenalex.org/work/W2029284131', 'https://semopenalex.org/work/W2298711843', 'https://semopenalex.org/work/W4389076217', 'https://semopenalex.org/work/W2004984354', 'https://semopenalex.org/work/W3001204101', 'https://semopenalex.org/work/W4367148398', 'https://semopenalex.org/work/W2804410540', 'https://semopenalex.org/work/W4282825011', 'https://semopenalex.org/work/W3127926476', 'https://semopenalex.org/work/W2000486418', 'https://semopenalex.org/work/W3186776699', 'https://semopenalex.org/work/W4306793569', 'https://semopenalex.org/work/W4386790563', 'https://semopenalex.org/work/W1990457279', 'https://semopenalex.org/work/W4285207151', 'https://semopenalex.org/work/W2910852288', 'https://semopenalex.org/work/W2779973510', 'https://semopenalex.org/work/W2060045560', 'https://semopenalex.org/work/W4404958656', 'https://semopenalex.org/work/W3193875369', 'https://semopenalex.org/work/W2535129896', 'https://semopenalex.org/work/W2522766745', 'https://semopenalex.org/work/W4367147664', 'https://semopenalex.org/work/W3152943384', 'https://semopenalex.org/work/W2476848331', 'https://semopenalex.org/work/W2066271829', 'https://semopenalex.org/work/W2051236310', 'https://semopenalex.org/work/W2533270794', 'https://semopenalex.org/work/W4288391286', 'https://semopenalex.org/work/W4393252675', 'https://semopenalex.org/work/W3080639911', 'https://semopenalex.org/work/W2911885303', 'https://semopenalex.org/work/W2167929182', 'https://semopenalex.org/work/W2511146638', 'https://semopenalex.org/work/W2389323797', 'https://semopenalex.org/work/W2800613805', 'https://semopenalex.org/work/W2078714953', 'https://semopenalex.org/work/W4388519971', 'https://semopenalex.org/work/W2289776346', 'https://semopenalex.org/work/W4402466985', 'https://semopenalex.org/work/W2997612014', 'https://semopenalex.org/work/W2905049939', 'https://semopenalex.org/work/W2291708615', 'https://semopenalex.org/work/W4400515993', 'https://semopenalex.org/work/W4390763328', 'https://semopenalex.org/work/W4313244937', 'https://semopenalex.org/work/W2915318915', 'https://semopenalex.org/work/W4388675409', 'https://semopenalex.org/work/W4388145646', 'https://semopenalex.org/work/W4379983689', 'https://semopenalex.org/work/W2799485966', 'https://semopenalex.org/work/W4387886204', 'https://semopenalex.org/work/W4226107162', 'https://semopenalex.org/work/W2727836510', 'https://semopenalex.org/work/W2517312722', 'https://semopenalex.org/work/W2035601794', 'https://semopenalex.org/work/W2103606916', 'https://semopenalex.org/work/W2971778528', 'https://semopenalex.org/work/W1781921775', 'https://semopenalex.org/work/W1991274348', 'https://semopenalex.org/work/W2292837460', 'https://semopenalex.org/work/W4386494434', 'https://semopenalex.org/work/W4387714561', 'https://semopenalex.org/work/W2520379429', 'https://semopenalex.org/work/W1967335608', 'https://semopenalex.org/work/W2785923962', 'https://semopenalex.org/work/W3047065943', 'https://semopenalex.org/work/W2109392297', 'https://semopenalex.org/work/W2969688740', 'https://semopenalex.org/work/W4386307089', 'https://semopenalex.org/work/W2920565953', 'https://semopenalex.org/work/W2905616463', 'https://semopenalex.org/work/W2792002389', 'https://semopenalex.org/work/W2289770078', 'https://semopenalex.org/work/W2967537836', 'https://semopenalex.org/work/W3156800857', 'https://semopenalex.org/work/W4225826211', 'https://semopenalex.org/work/W2313795635', 'https://semopenalex.org/work/W4386249920', 'https://semopenalex.org/work/W3129170312', 'https://semopenalex.org/work/W2570577251', 'https://semopenalex.org/work/W2920325736', 'https://semopenalex.org/work/W4213068964', 'https://semopenalex.org/work/W4285211669', 'https://semopenalex.org/work/W2154039139', 'https://semopenalex.org/work/W3147589610', 'https://semopenalex.org/work/W4213429388', 'https://semopenalex.org/work/W2171432711', 'https://semopenalex.org/work/W2118451262', 'https://semopenalex.org/work/W2887358166', 'https://semopenalex.org/work/W4318603270', 'https://semopenalex.org/work/W4387715010', 'https://semopenalex.org/work/W4213269113', 'https://semopenalex.org/work/W2383025629', 'https://semopenalex.org/work/W2794180747', 'https://semopenalex.org/work/W4393034258', 'https://semopenalex.org/work/W3197269278', 'https://semopenalex.org/work/W2118701267', 'https://semopenalex.org/work/W4317555541', 'https://semopenalex.org/work/W4386920013', 'https://semopenalex.org/work/W2986174999', 'https://semopenalex.org/work/W4396783549', 'https://semopenalex.org/work/W2473242321', 'https://semopenalex.org/work/W1968455523', 'https://semopenalex.org/work/W4323663048', 'https://semopenalex.org/work/W3197793222', 'https://semopenalex.org/work/W1978699422', 'https://semopenalex.org/work/W4394858588', 'https://semopenalex.org/work/W2556195709', 'https://semopenalex.org/work/W4205838995', 'https://semopenalex.org/work/W2887838626', 'https://semopenalex.org/work/W2077753966', 'https://semopenalex.org/work/W4210326058', 'https://semopenalex.org/work/W2129096944', 'https://semopenalex.org/work/W4282837228', 'https://semopenalex.org/work/W2151584377', 'https://semopenalex.org/work/W3176567159', 'https://semopenalex.org/work/W2743477693', 'https://semopenalex.org/work/W2290066430', 'https://semopenalex.org/work/W4307405043', 'https://semopenalex.org/work/W2991588661', 'https://semopenalex.org/work/W3016347687', 'https://semopenalex.org/work/W3086256320', 'https://semopenalex.org/work/W4389879531', 'https://semopenalex.org/work/W4285122724', 'https://semopenalex.org/work/W2069882645', 'https://semopenalex.org/work/W1980855612', 'https://semopenalex.org/work/W4386766558', 'https://semopenalex.org/work/W2548217541', 'https://semopenalex.org/work/W4392096060', 'https://semopenalex.org/work/W4312837885', 'https://semopenalex.org/work/W2011087369', 'https://semopenalex.org/work/W2115497161', 'https://semopenalex.org/work/W3134664381', 'https://semopenalex.org/work/W4312427776', 'https://semopenalex.org/work/W4366987396', 'https://semopenalex.org/work/W2972948959', 'https://semopenalex.org/work/W2495190596', 'https://semopenalex.org/work/W2604384156', 'https://semopenalex.org/work/W1963528679', 'https://semopenalex.org/work/W4396604650', 'https://semopenalex.org/work/W4365808277', 'https://semopenalex.org/work/W4406355769', 'https://semopenalex.org/work/W3134544950', 'https://semopenalex.org/work/W4396817519', 'https://semopenalex.org/work/W2719102196', 'https://semopenalex.org/work/W3034006897', 'https://semopenalex.org/work/W4404480496', 'https://semopenalex.org/work/W4296916443', 'https://semopenalex.org/work/W3210281673', 'https://semopenalex.org/work/W1991497382', 'https://semopenalex.org/work/W4386918403', 'https://semopenalex.org/work/W4220782062', 'https://semopenalex.org/work/W2909902231', 'https://semopenalex.org/work/W2024504253', 'https://semopenalex.org/work/W2152003934', 'https://semopenalex.org/work/W4224321673', 'https://semopenalex.org/work/W4285251260', 'https://semopenalex.org/work/W3005600351', 'https://semopenalex.org/work/W2783173327', 'https://semopenalex.org/work/W2141441280', 'https://semopenalex.org/work/W4385214694', 'https://semopenalex.org/work/W2055657753', 'https://semopenalex.org/work/W2167210003', 'https://semopenalex.org/work/W2291553515', 'https://semopenalex.org/work/W3201511537', 'https://semopenalex.org/work/W4285055114', 'https://semopenalex.org/work/W2990735505', 'https://semopenalex.org/work/W4200533036', 'https://semopenalex.org/work/W2912634456', 'https://semopenalex.org/work/W4404459004', 'https://semopenalex.org/work/W3215103574', 'https://semopenalex.org/work/W4391770026', 'https://semopenalex.org/work/W4212902180', 'https://semopenalex.org/work/W2059373588', 'https://semopenalex.org/work/W4401806242', 'https://semopenalex.org/work/W3033096606', 'https://semopenalex.org/work/W3040766658', 'https://semopenalex.org/work/W2518181354', 'https://semopenalex.org/work/W3006413083', 'https://semopenalex.org/work/W2605389968', 'https://semopenalex.org/work/W3142830832', 'https://semopenalex.org/work/W2903985815', 'https://semopenalex.org/work/W2797561181', 'https://semopenalex.org/work/W2023637192', 'https://semopenalex.org/work/W131277285', 'https://semopenalex.org/work/W2519882343', 'https://semopenalex.org/work/W2210737596', 'https://semopenalex.org/work/W4296912939', 'https://semopenalex.org/work/W4213143207', 'https://semopenalex.org/work/W2786607830', 'https://semopenalex.org/work/W3199970339', 'https://semopenalex.org/work/W4312614504', 'https://semopenalex.org/work/W1505692277', 'https://semopenalex.org/work/W2060658651', 'https://semopenalex.org/work/W1964959731', 'https://semopenalex.org/work/W2996592540', 'https://semopenalex.org/work/W2156848415', 'https://semopenalex.org/work/W4367148405', 'https://semopenalex.org/work/W4282831232', 'https://semopenalex.org/work/W2085645466', 'https://semopenalex.org/work/W3200805258', 'https://semopenalex.org/work/W4387023949', 'https://semopenalex.org/work/W2901539986', 'https://semopenalex.org/work/W4386249995', 'https://semopenalex.org/work/W2967954306', 'https://semopenalex.org/work/W2016629668', 'https://semopenalex.org/work/W43217051', 'https://semopenalex.org/work/W3040063675', 'https://semopenalex.org/work/W2964463995', 'https://semopenalex.org/work/W2547677547', 'https://semopenalex.org/work/W2792380105', 'https://semopenalex.org/work/W2891734979', 'https://semopenalex.org/work/W2139368697', 'https://semopenalex.org/work/W4386352842', 'https://semopenalex.org/work/W4318603823', 'https://semopenalex.org/work/W2901820813', 'https://semopenalex.org/work/W3105144424', 'https://semopenalex.org/work/W1972594074', 'https://semopenalex.org/work/W2538847865', 'https://semopenalex.org/work/W2291494764', 'https://semopenalex.org/work/W4392460796', 'https://semopenalex.org/work/W3176436409', 'https://semopenalex.org/work/W3115725655', 'https://semopenalex.org/work/W2101911810', 'https://semopenalex.org/work/W4282836627', 'https://semopenalex.org/work/W4367146924', 'https://semopenalex.org/work/W4386260739', 'https://semopenalex.org/work/W3005715390', 'https://semopenalex.org/work/W2137422967', 'https://semopenalex.org/work/W2737405495', 'https://semopenalex.org/work/W2145101624', 'https://semopenalex.org/work/W4213124543', 'https://semopenalex.org/work/W1966645219', 'https://semopenalex.org/work/W4308342707', 'https://semopenalex.org/work/W2034325389', 'https://semopenalex.org/work/W2076438760', 'https://semopenalex.org/work/W4304203349', 'https://semopenalex.org/work/W3213340154', 'https://semopenalex.org/work/W2344052410', 'https://semopenalex.org/work/W2277015358', 'https://semopenalex.org/work/W2068489330', 'https://semopenalex.org/work/W4387714613', 'https://semopenalex.org/work/W3076344446', 'https://semopenalex.org/work/W2808159133', 'https://semopenalex.org/work/W4393034150', 'https://semopenalex.org/work/W4312235824', 'https://semopenalex.org/work/W4392207726', 'https://semopenalex.org/work/W4388666963', 'https://semopenalex.org/work/W4367148109', 'https://semopenalex.org/work/W2947280819', 'https://semopenalex.org/work/W2100586747', 'https://semopenalex.org/work/W4386361261', 'https://semopenalex.org/work/W4396505344', 'https://semopenalex.org/work/W2119212601', 'https://semopenalex.org/work/W4378805022', 'https://semopenalex.org/work/W4285548139', 'https://semopenalex.org/work/W2528857590', 'https://semopenalex.org/work/W2419608502', 'https://semopenalex.org/work/W4318601869', 'https://semopenalex.org/work/W2533548130', 'https://semopenalex.org/work/W2919497189', 'https://semopenalex.org/work/W4360907566', 'https://semopenalex.org/work/W2168645783', 'https://semopenalex.org/work/W2051784811', 'https://semopenalex.org/work/W2072045292', 'https://semopenalex.org/work/W2551664773', 'https://semopenalex.org/work/W2332928857', 'https://semopenalex.org/work/W2001792450', 'https://semopenalex.org/work/W4229028795', 'https://semopenalex.org/work/W4389471415', 'https://semopenalex.org/work/W2039365023', 'https://semopenalex.org/work/W4392939659', 'https://semopenalex.org/work/W4402834678', 'https://semopenalex.org/work/W2095857057', 'https://semopenalex.org/work/W4393033575', 'https://semopenalex.org/work/W2271825901', 'https://semopenalex.org/work/W2085023162', 'https://semopenalex.org/work/W2118051735', 'https://semopenalex.org/work/W2782853409', 'https://semopenalex.org/work/W2349466730', 'https://semopenalex.org/work/W4212865190', 'https://semopenalex.org/work/W3023366540', 'https://semopenalex.org/work/W2888258411', 'https://semopenalex.org/work/W4401069975', 'https://semopenalex.org/work/W2573269249', 'https://semopenalex.org/work/W2554849750', 'https://semopenalex.org/work/W2114540871', 'https://semopenalex.org/work/W2528623020', 'https://semopenalex.org/work/W4312466007', 'https://semopenalex.org/work/W3144172827', 'https://semopenalex.org/work/W4294690843', 'https://semopenalex.org/work/W4399881765', 'https://semopenalex.org/work/W2753440200', 'https://semopenalex.org/work/W2561275332', 'https://semopenalex.org/work/W4401548819', 'https://semopenalex.org/work/W2757377912', 'https://semopenalex.org/work/W2540006586', 'https://semopenalex.org/work/W2551309437', 'https://semopenalex.org/work/W4391877334', 'https://semopenalex.org/work/W2559992739', 'https://semopenalex.org/work/W4312387367', 'https://semopenalex.org/work/W4388133782', 'https://semopenalex.org/work/W3135039935', 'https://semopenalex.org/work/W4390778218', 'https://semopenalex.org/work/W3156877779', 'https://semopenalex.org/work/W1971957085', 'https://semopenalex.org/work/W4387714660', 'https://semopenalex.org/work/W3214254401', 'https://semopenalex.org/work/W4403646133', 'https://semopenalex.org/work/W2289803878', 'https://semopenalex.org/work/W2109565528', 'https://semopenalex.org/work/W2137563824', 'https://semopenalex.org/work/W2729083427', 'https://semopenalex.org/work/W3005571193', 'https://semopenalex.org/work/W4390204058', 'https://semopenalex.org/work/W4386920758', 'https://semopenalex.org/work/W3006046181', 'https://semopenalex.org/work/W2768420153', 'https://semopenalex.org/work/W3040466764', 'https://semopenalex.org/work/W2028756273', 'https://semopenalex.org/work/W2137121156', 'https://semopenalex.org/work/W4312363564', 'https://semopenalex.org/work/W2076890843', 'https://semopenalex.org/work/W4387714810', 'https://semopenalex.org/work/W4392175577', 'https://semopenalex.org/work/W2321042880', 'https://semopenalex.org/work/W2800408116', 'https://semopenalex.org/work/W2547271336', 'https://semopenalex.org/work/W2130027208', 'https://semopenalex.org/work/W2120904939', 'https://semopenalex.org/work/W4385832244', 'https://semopenalex.org/work/W2104385531', 'https://semopenalex.org/work/W1978499995', 'https://semopenalex.org/work/W1035642985', 'https://semopenalex.org/work/W2759469946', 'https://semopenalex.org/work/W1485445045', 'https://semopenalex.org/work/W2898562797', 'https://semopenalex.org/work/W3094268044', 'https://semopenalex.org/work/W4403724277', 'https://semopenalex.org/work/W2128477511', 'https://semopenalex.org/work/W4311533450', 'https://semopenalex.org/work/W2096177399']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W4226484154', 'https://semopenalex.org/work/W3100717519', 'https://semopenalex.org/work/W4402904139', 'https://semopenalex.org/work/W4390874790', 'https://semopenalex.org/work/W3161716357', 'https://semopenalex.org/work/W4200628991', 'https://semopenalex.org/work/W3013912585', 'https://semopenalex.org/work/W4286911846', 'https://semopenalex.org/work/W3153883354', 'https://semopenalex.org/work/W4385714105', 'https://semopenalex.org/work/W3103017991', 'https://semopenalex.org/work/W4298544123', 'https://semopenalex.org/work/W4394948053', 'https://semopenalex.org/work/W4297748315', 'https://semopenalex.org/work/W4287081849', 'https://semopenalex.org/work/W3215869014', 'https://semopenalex.org/work/W4385002722', 'https://semopenalex.org/work/W4285563099', 'https://semopenalex.org/work/W4287081323', 'https://semopenalex.org/work/W3120808211', 'https://semopenalex.org/work/W2962689474', 'https://semopenalex.org/work/W4385764233', 'https://semopenalex.org/work/W4400527591', 'https://semopenalex.org/work/W4286783899', 'https://semopenalex.org/work/W3212725128', 'https://semopenalex.org/work/W3013080309', 'https://semopenalex.org/work/W2983383098', 'https://semopenalex.org/work/W4200024628', 'https://semopenalex.org/work/W4385484931', 'https://semopenalex.org/work/W3014613652', 'https://semopenalex.org/work/W4394647969', 'https://semopenalex.org/work/W4302012844', 'https://semopenalex.org/work/W4386044088', 'https://semopenalex.org/work/W3209714413', 'https://semopenalex.org/work/W4287854900', 'https://semopenalex.org/work/W4287679359', 'https://semopenalex.org/work/W4252150734', 'https://semopenalex.org/work/W4293585133', 'https://semopenalex.org/work/W4287990567', 'https://semopenalex.org/work/W3022437633', 'https://semopenalex.org/work/W2976881356', 'https://semopenalex.org/work/W4312987540', 'https://semopenalex.org/work/W4312705355', 'https://semopenalex.org/work/W2895638065', 'https://semopenalex.org/work/W4288864169', 'https://semopenalex.org/work/W3126451397', 'https://semopenalex.org/work/W4237531552', 'https://semopenalex.org/work/W3000280594', 'https://semopenalex.org/work/W4320009753', 'https://semopenalex.org/work/W3015075688', 'https://semopenalex.org/work/W4390874573', 'https://semopenalex.org/work/W4400527813', 'https://semopenalex.org/work/W4361807104', 'https://semopenalex.org/work/W2781902187', 'https://semopenalex.org/work/W4394948067', 'https://semopenalex.org/work/W3158336705', 'https://semopenalex.org/work/W3081562204', 'https://semopenalex.org/work/W4200560875', 'https://semopenalex.org/work/W3185096436', 'https://semopenalex.org/work/W3205150709', 'https://semopenalex.org/work/W4391630218', 'https://semopenalex.org/work/W3101597364', 'https://semopenalex.org/work/W4384807954', 'https://semopenalex.org/work/W3185989052', 'https://semopenalex.org/work/W3088160891', 'https://semopenalex.org/work/W4306178227', 'https://semopenalex.org/work/W4395687580', 'https://semopenalex.org/work/W3021881370', 'https://semopenalex.org/work/W4288853838', 'https://semopenalex.org/work/W4391980038', 'https://semopenalex.org/work/W3120604548', 'https://semopenalex.org/work/W4287659757', 'https://semopenalex.org/work/W4289785280', 'https://semopenalex.org/work/W4400527808', 'https://semopenalex.org/work/W4287205368', 'https://semopenalex.org/work/W4312262410', 'https://semopenalex.org/work/W4312541592', 'https://semopenalex.org/work/W3136988982', 'https://semopenalex.org/work/W4396913892', 'https://semopenalex.org/work/W2799020610', 'https://semopenalex.org/work/W4385489024', 'https://semopenalex.org/work/W4398156585', 'https://semopenalex.org/work/W4392488099', 'https://semopenalex.org/work/W4287070342', 'https://semopenalex.org/work/W3195437714', 'https://semopenalex.org/work/W4401415202', 'https://semopenalex.org/work/W3204322065', 'https://semopenalex.org/work/W2996574577', 'https://semopenalex.org/work/W4287208746', 'https://semopenalex.org/work/W4288854368', 'https://semopenalex.org/work/W3008209689', 'https://semopenalex.org/work/W4385801394', 'https://semopenalex.org/work/W3046138787', 'https://semopenalex.org/work/W3158615621', 'https://semopenalex.org/work/W3126473778', 'https://semopenalex.org/work/W3114189270', 'https://semopenalex.org/work/W2913466142', 'https://semopenalex.org/work/W3170528657', 'https://semopenalex.org/work/W4288897652', 'https://semopenalex.org/work/W3175370919', 'https://semopenalex.org/work/W3107972479', 'https://semopenalex.org/work/W3089582082', 'https://semopenalex.org/work/W2995697759', 'https://semopenalex.org/work/W3182129567', 'https://semopenalex.org/work/W3007894033', 'https://semopenalex.org/work/W4392971989', 'https://semopenalex.org/work/W4320036968', 'https://semopenalex.org/work/W4230527737', 'https://semopenalex.org/work/W3209110530', 'https://semopenalex.org/work/W2888163892', 'https://semopenalex.org/work/W4366198559', 'https://semopenalex.org/work/W3210107892', 'https://semopenalex.org/work/W4312903731', 'https://semopenalex.org/work/W4283695942', 'https://semopenalex.org/work/W4287263991', 'https://semopenalex.org/work/W4287864395', 'https://semopenalex.org/work/W4287141413', 'https://semopenalex.org/work/W4287822736', 'https://semopenalex.org/work/W4319336332', 'https://semopenalex.org/work/W4406524575', 'https://semopenalex.org/work/W4224014834', 'https://semopenalex.org/work/W4287271714', 'https://semopenalex.org/work/W2972050850', 'https://semopenalex.org/work/W4287822968', 'https://semopenalex.org/work/W4386044022', 'https://semopenalex.org/work/W3193694068', 'https://semopenalex.org/work/W4289550833', 'https://semopenalex.org/work/W4312293932', 'https://semopenalex.org/work/W2969182950', 'https://semopenalex.org/work/W3139116348', 'https://semopenalex.org/work/W4226112052', 'https://semopenalex.org/work/W4390189793', 'https://semopenalex.org/work/W3136579074', 'https://semopenalex.org/work/W4404988180', 'https://semopenalex.org/work/W4221162127', 'https://semopenalex.org/work/W3013092573', 'https://semopenalex.org/work/W2787117880', 'https://semopenalex.org/work/W2997573805', 'https://semopenalex.org/work/W2937532208', 'https://semopenalex.org/work/W4386114434', 'https://semopenalex.org/work/W4292829106', 'https://semopenalex.org/work/W4301131967', 'https://semopenalex.org/work/W4309873272', 'https://semopenalex.org/work/W3188528620', 'https://semopenalex.org/work/W3156185860', 'https://semopenalex.org/work/W4287068220', 'https://semopenalex.org/work/W4396814528', 'https://semopenalex.org/work/W3139499926', 'https://semopenalex.org/work/W4297823196', 'https://semopenalex.org/work/W2941870244', 'https://semopenalex.org/work/W4200338016', 'https://semopenalex.org/work/W3181073899', 'https://semopenalex.org/work/W3034765865', 'https://semopenalex.org/work/W3207776446', 'https://semopenalex.org/work/W3133932964', 'https://semopenalex.org/work/W3203158837', 'https://semopenalex.org/work/W4287822940', 'https://semopenalex.org/work/W3184989806', 'https://semopenalex.org/work/W3178180605', 'https://semopenalex.org/work/W4390190325', 'https://semopenalex.org/work/W3034875137', 'https://semopenalex.org/work/W4390190222', 'https://semopenalex.org/work/W3187413453', 'https://semopenalex.org/work/W4293161686', 'https://semopenalex.org/work/W3035684383', 'https://semopenalex.org/work/W3137123492', 'https://semopenalex.org/work/W4288023982', 'https://semopenalex.org/work/W4389519214', 'https://semopenalex.org/work/W3035434014', 'https://semopenalex.org/work/W3195626503', 'https://semopenalex.org/work/W4224928639', 'https://semopenalex.org/work/W4386069017', 'https://semopenalex.org/work/W4221139182', 'https://semopenalex.org/work/W2986822919', 'https://semopenalex.org/work/W4251566388', 'https://semopenalex.org/work/W2972424355', 'https://semopenalex.org/work/W4402502660', 'https://semopenalex.org/work/W4400527492', 'https://semopenalex.org/work/W3161569725', 'https://semopenalex.org/work/W3128169604', 'https://semopenalex.org/work/W4392933323']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W4224295260', 'https://semopenalex.org/work/W3158973558', 'https://semopenalex.org/work/W4281670064', 'https://semopenalex.org/work/W3172648176', 'https://semopenalex.org/work/W4200494113', 'https://semopenalex.org/work/W4392473011', 'https://semopenalex.org/work/W4213455810', 'https://semopenalex.org/work/W4399991068']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W4403094633', 'https://semopenalex.org/work/W4390604119', 'https://semopenalex.org/work/W4386065896', 'https://semopenalex.org/work/W4312804251']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W4391680987', 'https://semopenalex.org/work/W4404849982', 'https://semopenalex.org/work/W4391903798', 'https://semopenalex.org/work/W4406802119', 'https://semopenalex.org/work/W4405564152', 'https://semopenalex.org/work/W4396509789', 'https://semopenalex.org/work/W4404839780', 'https://semopenalex.org/work/W4401879044', 'https://semopenalex.org/work/W4405643736', 'https://semopenalex.org/work/W4405718129', 'https://semopenalex.org/work/W4392180008', 'https://semopenalex.org/work/W4406620652']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W4391928869', 'https://semopenalex.org/work/W4400410989', 'https://semopenalex.org/work/W4400410445', 'https://semopenalex.org/work/W4391010236', 'https://semopenalex.org/work/W4399070942', 'https://semopenalex.org/work/W4396787938']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W3108935870', 'https://semopenalex.org/work/W3140085153', 'https://semopenalex.org/work/W3008842679', 'https://semopenalex.org/work/W4376171783', 'https://semopenalex.org/work/W3095401597', 'https://semopenalex.org/work/W4362502510', 'https://semopenalex.org/work/W4321503169', 'https://semopenalex.org/work/W4321230650', 'https://semopenalex.org/work/W4283322066', 'https://semopenalex.org/work/W4283320724', 'https://semopenalex.org/work/W4376210033', 'https://semopenalex.org/work/W4362464600', 'https://semopenalex.org/work/W4362464651']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/source/S4306525036', 'https://semopenalex.org/source/S4306400562', 'https://semopenalex.org/source/S4210219776', 'https://semopenalex.org/source/S4306419921', 'https://semopenalex.org/source/S37879656', 'https://semopenalex.org/source/S2738664114', 'https://semopenalex.org/source/S4306417857', 'https://semopenalex.org/source/S4210191760', 'https://semopenalex.org/source/S60711021', 'https://semopenalex.org/source/S4306402641', 'https://semopenalex.org/source/S2764435056', 'https://semopenalex.org/source/S4210170441', 'https://semopenalex.org/source/S85375271', 'https://semopenalex.org/source/S4210177346', 'https://semopenalex.org/source/S157146593', 'https://semopenalex.org/source/S86192639', 'https://semopenalex.org/source/S4210175514', 'https://semopenalex.org/source/S63392143', 'https://semopenalex.org/source/S4210177502', 'https://semopenalex.org/source/S158797327', 'https://semopenalex.org/source/S11065456', 'https://semopenalex.org/source/S4306421051', 'https://semopenalex.org/source/S120348307', 'https://semopenalex.org/source/S64245694', 'https://semopenalex.org/source/S4210174798', 'https://semopenalex.org/source/S1250476', 'https://semopenalex.org/source/S34838331', 'https://semopenalex.org/source/S4306418113', 'https://semopenalex.org/source/S4306420911', 'https://semopenalex.org/source/S153984684', 'https://semopenalex.org/source/S4363605881', 'https://semopenalex.org/source/S207090427', 'https://semopenalex.org/source/S4210184905', 'https://semopenalex.org/source/S4306419875', 'https://semopenalex.org/source/S4306419550', 'https://semopenalex.org/source/S157921468', 'https://semopenalex.org/source/S4306400194', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S4210175912', 'https://semopenalex.org/source/S4306401280', 'https://semopenalex.org/source/S96783963', 'https://semopenalex.org/source/S101949793', 'https://semopenalex.org/source/S4210197804', 'https://semopenalex.org/source/S4306463937', 'https://semopenalex.org/source/S4210194901', 'https://semopenalex.org/source/S58563349', 'https://semopenalex.org/source/S129236917', 'https://semopenalex.org/source/S4306418564', 'https://semopenalex.org/source/S106296714', 'https://semopenalex.org/source/S4210233398', 'https://semopenalex.org/source/S4210177528', 'https://semopenalex.org/source/S116972989', 'https://semopenalex.org/source/S52395412', 'https://semopenalex.org/source/S4210187899', 'https://semopenalex.org/source/S4363608934', 'https://semopenalex.org/source/S115004586', 'https://semopenalex.org/source/S4210187232', 'https://semopenalex.org/source/S4306524001', 'https://semopenalex.org/source/S97833917', 'https://semopenalex.org/source/S126644992', 'https://semopenalex.org/source/S4306417563', 'https://semopenalex.org/source/S36560696', 'https://semopenalex.org/source/S4306400483', 'https://semopenalex.org/source/S30128005', 'https://semopenalex.org/source/S4306400349', 'https://semopenalex.org/source/S4306402512', 'https://semopenalex.org/source/S2764455111', 'https://semopenalex.org/source/S186357190', 'https://semopenalex.org/source/S4306402450', 'https://semopenalex.org/source/S136993123', 'https://semopenalex.org/source/S4306421096', 'https://semopenalex.org/source/S147790641', 'https://semopenalex.org/source/S140982614', 'https://semopenalex.org/source/S106148199', 'https://semopenalex.org/source/S157670870', 'https://semopenalex.org/source/S2485537415']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/source/S4306400562', 'https://semopenalex.org/source/S4306419152', 'https://semopenalex.org/source/S4306532718', 'https://semopenalex.org/source/S4210173311', 'https://semopenalex.org/source/S4306420780', 'https://semopenalex.org/source/S4306400662', 'https://semopenalex.org/source/S4377196258', 'https://semopenalex.org/source/S18088403', 'https://semopenalex.org/source/S4306530687', 'https://semopenalex.org/source/S2764905038', 'https://semopenalex.org/source/S139930977', 'https://semopenalex.org/source/S106296714', 'https://semopenalex.org/source/S4306420436', 'https://semopenalex.org/source/S4306402512', 'https://semopenalex.org/source/S2764696622', 'https://semopenalex.org/source/S4210185096', 'https://semopenalex.org/source/S4210239725', 'https://semopenalex.org/source/S4210226000', 'https://semopenalex.org/source/S4210235676', 'https://semopenalex.org/source/S4306400194', 'https://semopenalex.org/source/S4306418416', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S4306535130']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/source/S4306525036', 'https://semopenalex.org/source/S107964287', 'https://semopenalex.org/source/S4210211936', 'https://semopenalex.org/source/S4363608199', 'https://semopenalex.org/source/S21313077', 'https://semopenalex.org/source/S144091109', 'https://semopenalex.org/source/S4210212400', 'https://semopenalex.org/source/S137468011', 'https://semopenalex.org/source/S4210224236', 'https://semopenalex.org/source/S201921491', 'https://semopenalex.org/source/S178916657', 'https://semopenalex.org/source/S2764900261', 'https://semopenalex.org/source/S62507282', 'https://semopenalex.org/source/S185008460', 'https://semopenalex.org/source/S179591353', 'https://semopenalex.org/source/S4363607828', 'https://semopenalex.org/source/S4306464320', 'https://semopenalex.org/source/S84339699', 'https://semopenalex.org/source/S68719679', 'https://semopenalex.org/source/S91329792', 'https://semopenalex.org/source/S4306400385', 'https://semopenalex.org/source/S34730769', 'https://semopenalex.org/source/S170217976', 'https://semopenalex.org/source/S41486457', 'https://semopenalex.org/source/S202381698', 'https://semopenalex.org/source/S4306417879', 'https://semopenalex.org/source/S4306462995', 'https://semopenalex.org/source/S45696439', 'https://semopenalex.org/source/S4210195248', 'https://semopenalex.org/source/S2495878607', 'https://semopenalex.org/source/S104717114', 'https://semopenalex.org/source/S4306401722', 'https://semopenalex.org/source/S4210191458', 'https://semopenalex.org/source/S4306462788', 'https://semopenalex.org/source/S2764905038', 'https://semopenalex.org/source/S2764696622', 'https://semopenalex.org/source/S4210171255', 'https://semopenalex.org/source/S4210214825', 'https://semopenalex.org/source/S4306400194', 'https://semopenalex.org/source/S4363608034', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S52732750', 'https://semopenalex.org/source/S4210212310', 'https://semopenalex.org/source/S4306401280', 'https://semopenalex.org/source/S45281609', 'https://semopenalex.org/source/S4210213674', 'https://semopenalex.org/source/S4363608116', 'https://semopenalex.org/source/S4306463937', 'https://semopenalex.org/source/S4210211086', 'https://semopenalex.org/source/S4210212235', 'https://semopenalex.org/source/S4210205812', 'https://semopenalex.org/source/S4363607702', 'https://semopenalex.org/source/S4306463687', 'https://semopenalex.org/source/S2764763012', 'https://semopenalex.org/source/S11296630', 'https://semopenalex.org/source/S4363608918', 'https://semopenalex.org/source/S195488530', 'https://semopenalex.org/source/S4363607712', 'https://semopenalex.org/source/S4210240769', 'https://semopenalex.org/source/S4306463409', 'https://semopenalex.org/source/S4306463708', 'https://semopenalex.org/source/S4306533995', 'https://semopenalex.org/source/S4306419250', 'https://semopenalex.org/source/S106296714', 'https://semopenalex.org/source/S4306402118', 'https://semopenalex.org/source/S4210169774', 'https://semopenalex.org/source/S975621743', 'https://semopenalex.org/source/S4363607734', 'https://semopenalex.org/source/S4363608837', 'https://semopenalex.org/source/S4306419999', 'https://semopenalex.org/source/S15952048', 'https://semopenalex.org/source/S4210179954', 'https://semopenalex.org/source/S4210226272', 'https://semopenalex.org/source/S4306400806', 'https://semopenalex.org/source/S4306402651', 'https://semopenalex.org/source/S4363607711', 'https://semopenalex.org/source/S131145815', 'https://semopenalex.org/source/S4210233094', 'https://semopenalex.org/source/S56112914', 'https://semopenalex.org/source/S124503262', 'https://semopenalex.org/source/S116420536', 'https://semopenalex.org/source/S131921510', 'https://semopenalex.org/source/S4363607705', 'https://semopenalex.org/source/S4363608614', 'https://semopenalex.org/source/S4306400349', 'https://semopenalex.org/source/S183492911', 'https://semopenalex.org/source/S4363607759', 'https://semopenalex.org/source/S2595095599', 'https://semopenalex.org/source/S4306497580', 'https://semopenalex.org/source/S2764455111', 'https://semopenalex.org/source/S58778951', 'https://semopenalex.org/source/S76152103', 'https://semopenalex.org/source/S133768115', 'https://semopenalex.org/source/S157664362', 'https://semopenalex.org/source/S177430994', 'https://semopenalex.org/source/S92163612', 'https://semopenalex.org/source/S111927887']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W2535846100', 'https://semopenalex.org/work/W2917509290', 'https://semopenalex.org/work/W2903327589', 'https://semopenalex.org/work/W2952648029', 'https://semopenalex.org/work/W2789779636', 'https://semopenalex.org/work/W2973574727', 'https://semopenalex.org/work/W2579543964', 'https://semopenalex.org/work/W2797304630', 'https://semopenalex.org/work/W3037554454', 'https://semopenalex.org/work/W4230018104', 'https://semopenalex.org/work/W2901496061', 'https://semopenalex.org/work/W2793980407', 'https://semopenalex.org/work/W3022089151', 'https://semopenalex.org/work/W2770068518']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W2398987174', 'https://semopenalex.org/work/W2001181659', 'https://semopenalex.org/work/W1815020819', 'https://semopenalex.org/work/W1591196343', 'https://semopenalex.org/work/W2155878381', 'https://semopenalex.org/work/W61308258', 'https://semopenalex.org/work/W177260087', 'https://semopenalex.org/work/W2055897235', 'https://semopenalex.org/work/W4236474819', 'https://semopenalex.org/work/W1482090313', 'https://semopenalex.org/work/W4292013335', 'https://semopenalex.org/work/W116884602', 'https://semopenalex.org/work/W2100356383', 'https://semopenalex.org/work/W1510701494', 'https://semopenalex.org/work/W2501927875', 'https://semopenalex.org/work/W1555904986', 'https://semopenalex.org/work/W2768865949', 'https://semopenalex.org/work/W2056596857', 'https://semopenalex.org/work/W2402284853', 'https://semopenalex.org/work/W1536752040', 'https://semopenalex.org/work/W1575252762', 'https://semopenalex.org/work/W1576645054', 'https://semopenalex.org/work/W2157877717', 'https://semopenalex.org/work/W1528198126', 'https://semopenalex.org/work/W1971453213', 'https://semopenalex.org/work/W2126729622', 'https://semopenalex.org/work/W1582766542', 'https://semopenalex.org/work/W2241306549', 'https://semopenalex.org/work/W1481479141', 'https://semopenalex.org/work/W2322381474', 'https://semopenalex.org/work/W2497935614', 'https://semopenalex.org/work/W2258785380', 'https://semopenalex.org/work/W1533819156', 'https://semopenalex.org/work/W2159677278', 'https://semopenalex.org/work/W1976471311', 'https://semopenalex.org/work/W2023461062', 'https://semopenalex.org/work/W2087682696', 'https://semopenalex.org/work/W1489802521', 'https://semopenalex.org/work/W2113401317', 'https://semopenalex.org/work/W2274048031', 'https://semopenalex.org/work/W1584905179', 'https://semopenalex.org/work/W2146830885', 'https://semopenalex.org/work/W1504849558', 'https://semopenalex.org/work/W1575176919', 'https://semopenalex.org/work/W2912169901']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W1984905848', 'https://semopenalex.org/work/W2084452057', 'https://semopenalex.org/work/W1522292253', 'https://semopenalex.org/work/W2029593259', 'https://semopenalex.org/work/W2077395955', 'https://semopenalex.org/work/W1912917402', 'https://semopenalex.org/work/W1978468648', 'https://semopenalex.org/work/W2058758829', 'https://semopenalex.org/work/W2014659753', 'https://semopenalex.org/work/W2147427359', 'https://semopenalex.org/work/W2102195169', 'https://semopenalex.org/work/W2057938070', 'https://semopenalex.org/work/W2146661121', 'https://semopenalex.org/work/W1967044695', 'https://semopenalex.org/work/W2032444227', 'https://semopenalex.org/work/W2005155776', 'https://semopenalex.org/work/W1500154637', 'https://semopenalex.org/work/W1983778833', 'https://semopenalex.org/work/W2114233612', 'https://semopenalex.org/work/W3146442409']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/author/A5101619735', 'https://semopenalex.org/author/A5051642217', 'https://semopenalex.org/author/A5078921853', 'https://semopenalex.org/author/A5112907430', 'https://semopenalex.org/author/A5092106609', 'https://semopenalex.org/author/A5017353478', 'https://semopenalex.org/author/A5044578275', 'https://semopenalex.org/author/A5034037954', 'https://semopenalex.org/author/A5089362779', 'https://semopenalex.org/author/A5086346640', 'https://semopenalex.org/author/A5062261441', 'https://semopenalex.org/author/A5086787573', 'https://semopenalex.org/author/A5090529701', 'https://semopenalex.org/author/A5013421545', 'https://semopenalex.org/author/A5004507308', 'https://semopenalex.org/author/A5078555911', 'https://semopenalex.org/author/A5111252081', 'https://semopenalex.org/author/A5084373522', 'https://semopenalex.org/author/A5028395580', 'https://semopenalex.org/author/A5093495936', 'https://semopenalex.org/author/A5040925885', 'https://semopenalex.org/author/A5102720885', 'https://semopenalex.org/author/A5071109276', 'https://semopenalex.org/author/A5089983554', 'https://semopenalex.org/author/A5062553581', 'https://semopenalex.org/author/A5025631312', 'https://semopenalex.org/author/A5020939308', 'https://semopenalex.org/author/A5038581932', 'https://semopenalex.org/author/A5012375687', 'https://semopenalex.org/author/A5101845418', 'https://semopenalex.org/author/A5028750310', 'https://semopenalex.org/author/A5108988435', 'https://semopenalex.org/author/A5075061218', 'https://semopenalex.org/author/A5035247809', 'https://semopenalex.org/author/A5092276800', 'https://semopenalex.org/author/A5031601776', 'https://semopenalex.org/author/A5112596472', 'https://semopenalex.org/author/A5048521450', 'https://semopenalex.org/author/A5078461261', 'https://semopenalex.org/author/A5061675674', 'https://semopenalex.org/author/A5112900377', 'https://semopenalex.org/author/A5093415912', 'https://semopenalex.org/author/A5074316484', 'https://semopenalex.org/author/A5091453565', 'https://semopenalex.org/author/A5015144665', 'https://semopenalex.org/author/A5080374319', 'https://semopenalex.org/author/A5027096307', 'https://semopenalex.org/author/A5023645490', 'https://semopenalex.org/author/A5074486298', 'https://semopenalex.org/author/A5025632720', 'https://semopenalex.org/author/A5024581040', 'https://semopenalex.org/author/A5069922587', 'https://semopenalex.org/author/A5024584252', 'https://semopenalex.org/author/A5042413456', 'https://semopenalex.org/author/A5043204400', 'https://semopenalex.org/author/A5089914165', 'https://semopenalex.org/author/A5092276801', 'https://semopenalex.org/author/A5084631861', 'https://semopenalex.org/author/A5064387363', 'https://semopenalex.org/author/A5001454735', 'https://semopenalex.org/author/A5015356632', 'https://semopenalex.org/author/A5093413149', 'https://semopenalex.org/author/A5091298748', 'https://semopenalex.org/author/A5014205279', 'https://semopenalex.org/author/A5106808077', 'https://semopenalex.org/author/A5006430488', 'https://semopenalex.org/author/A5064622877', 'https://semopenalex.org/author/A5112387040', 'https://semopenalex.org/author/A5114057383', 'https://semopenalex.org/author/A5060768396', 'https://semopenalex.org/author/A5082863339', 'https://semopenalex.org/author/A5051221846', 'https://semopenalex.org/author/A5074393288']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/author/A5044628664', 'https://semopenalex.org/author/A5069815943', 'https://semopenalex.org/author/A5113723639', 'https://semopenalex.org/author/A5074589032', 'https://semopenalex.org/author/A5046366918', 'https://semopenalex.org/author/A5104053258', 'https://semopenalex.org/author/A5040926780', 'https://semopenalex.org/author/A5101223282', 'https://semopenalex.org/author/A5058321053', 'https://semopenalex.org/author/A5041069081', 'https://semopenalex.org/author/A5090735746', 'https://semopenalex.org/author/A5029196810', 'https://semopenalex.org/author/A5055129023', 'https://semopenalex.org/author/A5110867527', 'https://semopenalex.org/author/A5075050367', 'https://semopenalex.org/author/A5081627591', 'https://semopenalex.org/author/A5077656562', 'https://semopenalex.org/author/A5114257544', 'https://semopenalex.org/author/A5111299292', 'https://semopenalex.org/author/A5065215412', 'https://semopenalex.org/author/A5054436767', 'https://semopenalex.org/author/A5074074791', 'https://semopenalex.org/author/A5094966959', 'https://semopenalex.org/author/A5109894548', 'https://semopenalex.org/author/A5072570670', 'https://semopenalex.org/author/A5078249187', 'https://semopenalex.org/author/A5109056620', 'https://semopenalex.org/author/A5025851255', 'https://semopenalex.org/author/A5080362727', 'https://semopenalex.org/author/A5054239026', 'https://semopenalex.org/author/A5073739308', 'https://semopenalex.org/author/A5111957985', 'https://semopenalex.org/author/A5065662869', 'https://semopenalex.org/author/A5057006392', 'https://semopenalex.org/author/A5018309977', 'https://semopenalex.org/author/A5110293736', 'https://semopenalex.org/author/A5101815353', 'https://semopenalex.org/author/A5027434411', 'https://semopenalex.org/author/A5070430119', 'https://semopenalex.org/author/A5088742299', 'https://semopenalex.org/author/A5011271066', 'https://semopenalex.org/author/A5005290550', 'https://semopenalex.org/author/A5028489255', 'https://semopenalex.org/author/A5042185262', 'https://semopenalex.org/author/A5113979090', 'https://semopenalex.org/author/A5045348077', 'https://semopenalex.org/author/A5057833118', 'https://semopenalex.org/author/A5026576007', 'https://semopenalex.org/author/A5040481275', 'https://semopenalex.org/author/A5075748306', 'https://semopenalex.org/author/A5002964350', 'https://semopenalex.org/author/A5040682720', 'https://semopenalex.org/author/A5110244736', 'https://semopenalex.org/author/A5015977158', 'https://semopenalex.org/author/A5113669589', 'https://semopenalex.org/author/A5073803240', 'https://semopenalex.org/author/A5086297102', 'https://semopenalex.org/author/A5094850550', 'https://semopenalex.org/author/A5032040667', 'https://semopenalex.org/author/A5031914716', 'https://semopenalex.org/author/A5027650657', 'https://semopenalex.org/author/A5101843778', 'https://semopenalex.org/author/A5035006986', 'https://semopenalex.org/author/A5006842195', 'https://semopenalex.org/author/A5074567046', 'https://semopenalex.org/author/A5073749152', 'https://semopenalex.org/author/A5007832994', 'https://semopenalex.org/author/A5039203221', 'https://semopenalex.org/author/A5020701887', 'https://semopenalex.org/author/A5062087243', 'https://semopenalex.org/author/A5088803193', 'https://semopenalex.org/author/A5013806560', 'https://semopenalex.org/author/A5015192494', 'https://semopenalex.org/author/A5052558062', 'https://semopenalex.org/author/A5029995660', 'https://semopenalex.org/author/A5035328623', 'https://semopenalex.org/author/A5046291387', 'https://semopenalex.org/author/A5030697774', 'https://semopenalex.org/author/A5072916330', 'https://semopenalex.org/author/A5101159426', 'https://semopenalex.org/author/A5074598788', 'https://semopenalex.org/author/A5011208990', 'https://semopenalex.org/author/A5110879810', 'https://semopenalex.org/author/A5100428572', 'https://semopenalex.org/author/A5077947231', 'https://semopenalex.org/author/A5094850553', 'https://semopenalex.org/author/A5021139451', 'https://semopenalex.org/author/A5088935199', 'https://semopenalex.org/author/A5081846222', 'https://semopenalex.org/author/A5067111142', 'https://semopenalex.org/author/A5004978878', 'https://semopenalex.org/author/A5092591629', 'https://semopenalex.org/author/A5050603750', 'https://semopenalex.org/author/A5042981767', 'https://semopenalex.org/author/A5047034022', 'https://semopenalex.org/author/A5088805136', 'https://semopenalex.org/author/A5035241917', 'https://semopenalex.org/author/A5013164571', 'https://semopenalex.org/author/A5083067976', 'https://semopenalex.org/author/A5004095672', 'https://semopenalex.org/author/A5012057735', 'https://semopenalex.org/author/A5030954130', 'https://semopenalex.org/author/A5005357612', 'https://semopenalex.org/author/A5102845298', 'https://semopenalex.org/author/A5005645577', 'https://semopenalex.org/author/A5091888698', 'https://semopenalex.org/author/A5076209207', 'https://semopenalex.org/author/A5034842369', 'https://semopenalex.org/author/A5100563292', 'https://semopenalex.org/author/A5036018560', 'https://semopenalex.org/author/A5081380385', 'https://semopenalex.org/author/A5026923870', 'https://semopenalex.org/author/A5040457891', 'https://semopenalex.org/author/A5061493594', 'https://semopenalex.org/author/A5004693243', 'https://semopenalex.org/author/A5023532428', 'https://semopenalex.org/author/A5088083982', 'https://semopenalex.org/author/A5100436760', 'https://semopenalex.org/author/A5072444030', 'https://semopenalex.org/author/A5073513391', 'https://semopenalex.org/author/A5019810478', 'https://semopenalex.org/author/A5057143288', 'https://semopenalex.org/author/A5053876673', 'https://semopenalex.org/author/A5046196600', 'https://semopenalex.org/author/A5038024446', 'https://semopenalex.org/author/A5007943091', 'https://semopenalex.org/author/A5057963205', 'https://semopenalex.org/author/A5110866135', 'https://semopenalex.org/author/A5057579122', 'https://semopenalex.org/author/A5073410087', 'https://semopenalex.org/author/A5001240699', 'https://semopenalex.org/author/A5049495092', 'https://semopenalex.org/author/A5057685487', 'https://semopenalex.org/author/A5108609396', 'https://semopenalex.org/author/A5057083638', 'https://semopenalex.org/author/A5039301079', 'https://semopenalex.org/author/A5065466432', 'https://semopenalex.org/author/A5069815367', 'https://semopenalex.org/author/A5030785463', 'https://semopenalex.org/author/A5094850559', 'https://semopenalex.org/author/A5110360335', 'https://semopenalex.org/author/A5094850560', 'https://semopenalex.org/author/A5010169168', 'https://semopenalex.org/author/A5031522111', 'https://semopenalex.org/author/A5009578658', 'https://semopenalex.org/author/A5112770923', 'https://semopenalex.org/author/A5013828217', 'https://semopenalex.org/author/A5003443602', 'https://semopenalex.org/author/A5079894695', 'https://semopenalex.org/author/A5069695344', 'https://semopenalex.org/author/A5072902302', 'https://semopenalex.org/author/A5102146502', 'https://semopenalex.org/author/A5058422878', 'https://semopenalex.org/author/A5100458893', 'https://semopenalex.org/author/A5000563459', 'https://semopenalex.org/author/A5112705691', 'https://semopenalex.org/author/A5100425978', 'https://semopenalex.org/author/A5085424530', 'https://semopenalex.org/author/A5034690905', 'https://semopenalex.org/author/A5002266542', 'https://semopenalex.org/author/A5021792918', 'https://semopenalex.org/author/A5017841368', 'https://semopenalex.org/author/A5009498321', 'https://semopenalex.org/author/A5070309541', 'https://semopenalex.org/author/A5002874750', 'https://semopenalex.org/author/A5013031003', 'https://semopenalex.org/author/A5110568866', 'https://semopenalex.org/author/A5110866136', 'https://semopenalex.org/author/A5067291755', 'https://semopenalex.org/author/A5040530849', 'https://semopenalex.org/author/A5103726315', 'https://semopenalex.org/author/A5062882537', 'https://semopenalex.org/author/A5040540194', 'https://semopenalex.org/author/A5069829960', 'https://semopenalex.org/author/A5061625295', 'https://semopenalex.org/author/A5070478103', 'https://semopenalex.org/author/A5094966948', 'https://semopenalex.org/author/A5042070270', 'https://semopenalex.org/author/A5100928778', 'https://semopenalex.org/author/A5083967897', 'https://semopenalex.org/author/A5063515034', 'https://semopenalex.org/author/A5010466931', 'https://semopenalex.org/author/A5015400278', 'https://semopenalex.org/author/A5054875158', 'https://semopenalex.org/author/A5025012438', 'https://semopenalex.org/author/A5079309664', 'https://semopenalex.org/author/A5110126701', 'https://semopenalex.org/author/A5053715191', 'https://semopenalex.org/author/A5070045696', 'https://semopenalex.org/author/A5083053651', 'https://semopenalex.org/author/A5059675637', 'https://semopenalex.org/author/A5004548068', 'https://semopenalex.org/author/A5029732249', 'https://semopenalex.org/author/A5083689259', 'https://semopenalex.org/author/A5090610271', 'https://semopenalex.org/author/A5032586796', 'https://semopenalex.org/author/A5102135372', 'https://semopenalex.org/author/A5067664620', 'https://semopenalex.org/author/A5113750346', 'https://semopenalex.org/author/A5036580072', 'https://semopenalex.org/author/A5029543403', 'https://semopenalex.org/author/A5063043381', 'https://semopenalex.org/author/A5049348869', 'https://semopenalex.org/author/A5082652832', 'https://semopenalex.org/author/A5084563184', 'https://semopenalex.org/author/A5020223949', 'https://semopenalex.org/author/A5019863108', 'https://semopenalex.org/author/A5109550727', 'https://semopenalex.org/author/A5110970351', 'https://semopenalex.org/author/A5000889165', 'https://semopenalex.org/author/A5087685351', 'https://semopenalex.org/author/A5065516130', 'https://semopenalex.org/author/A5039368373', 'https://semopenalex.org/author/A5049244926', 'https://semopenalex.org/author/A5047925616', 'https://semopenalex.org/author/A5084114117', 'https://semopenalex.org/author/A5086046410', 'https://semopenalex.org/author/A5056612861', 'https://semopenalex.org/author/A5112789076', 'https://semopenalex.org/author/A5054904146', 'https://semopenalex.org/author/A5102775803', 'https://semopenalex.org/author/A5013975143', 'https://semopenalex.org/author/A5100418957', 'https://semopenalex.org/author/A5072028806', 'https://semopenalex.org/author/A5090335855', 'https://semopenalex.org/author/A5094966946', 'https://semopenalex.org/author/A5026619574', 'https://semopenalex.org/author/A5026731126', 'https://semopenalex.org/author/A5082559019', 'https://semopenalex.org/author/A5058658281', 'https://semopenalex.org/author/A5051949776', 'https://semopenalex.org/author/A5101159425', 'https://semopenalex.org/author/A5100426981', 'https://semopenalex.org/author/A5113653050', 'https://semopenalex.org/author/A5113667088', 'https://semopenalex.org/author/A5021496374', 'https://semopenalex.org/author/A5000203614', 'https://semopenalex.org/author/A5111874391', 'https://semopenalex.org/author/A5094966960', 'https://semopenalex.org/author/A5087206674', 'https://semopenalex.org/author/A5052396894', 'https://semopenalex.org/author/A5075931954', 'https://semopenalex.org/author/A5094966957', 'https://semopenalex.org/author/A5112014544', 'https://semopenalex.org/author/A5109232422', 'https://semopenalex.org/author/A5000285989', 'https://semopenalex.org/author/A5032060363', 'https://semopenalex.org/author/A5101159424', 'https://semopenalex.org/author/A5065634430', 'https://semopenalex.org/author/A5063943061', 'https://semopenalex.org/author/A5088120976', 'https://semopenalex.org/author/A5082617098', 'https://semopenalex.org/author/A5005503619', 'https://semopenalex.org/author/A5094966950', 'https://semopenalex.org/author/A5051435891', 'https://semopenalex.org/author/A5100353446', 'https://semopenalex.org/author/A5011147039', 'https://semopenalex.org/author/A5066794150', 'https://semopenalex.org/author/A5054687162', 'https://semopenalex.org/author/A5006412870', 'https://semopenalex.org/author/A5089148668', 'https://semopenalex.org/author/A5109550728', 'https://semopenalex.org/author/A5113716037', 'https://semopenalex.org/author/A5027495637', 'https://semopenalex.org/author/A5021519204', 'https://semopenalex.org/author/A5094966956', 'https://semopenalex.org/author/A5061791546', 'https://semopenalex.org/author/A5047487369', 'https://semopenalex.org/author/A5100678452', 'https://semopenalex.org/author/A5035713595', 'https://semopenalex.org/author/A5113537073', 'https://semopenalex.org/author/A5000527699', 'https://semopenalex.org/author/A5109401743', 'https://semopenalex.org/author/A5035879340', 'https://semopenalex.org/author/A5073590393', 'https://semopenalex.org/author/A5052771319', 'https://semopenalex.org/author/A5001888075', 'https://semopenalex.org/author/A5074596026', 'https://semopenalex.org/author/A5015415192', 'https://semopenalex.org/author/A5051259649', 'https://semopenalex.org/author/A5033142925', 'https://semopenalex.org/author/A5058048101', 'https://semopenalex.org/author/A5060375005', 'https://semopenalex.org/author/A5109557605', 'https://semopenalex.org/author/A5034482692', 'https://semopenalex.org/author/A5065946530', 'https://semopenalex.org/author/A5108112356', 'https://semopenalex.org/author/A5037590981', 'https://semopenalex.org/author/A5075602267', 'https://semopenalex.org/author/A5059726739', 'https://semopenalex.org/author/A5041758250', 'https://semopenalex.org/author/A5094966947', 'https://semopenalex.org/author/A5013290328', 'https://semopenalex.org/author/A5115595642', 'https://semopenalex.org/author/A5025298438', 'https://semopenalex.org/author/A5027345703', 'https://semopenalex.org/author/A5101164166', 'https://semopenalex.org/author/A5033358586', 'https://semopenalex.org/author/A5080593862', 'https://semopenalex.org/author/A5064864099', 'https://semopenalex.org/author/A5025025481', 'https://semopenalex.org/author/A5059663464', 'https://semopenalex.org/author/A5030396947', 'https://semopenalex.org/author/A5103176355', 'https://semopenalex.org/author/A5027994157', 'https://semopenalex.org/author/A5033806544', 'https://semopenalex.org/author/A5052111753', 'https://semopenalex.org/author/A5106680720', 'https://semopenalex.org/author/A5014584767', 'https://semopenalex.org/author/A5024892754', 'https://semopenalex.org/author/A5025998224', 'https://semopenalex.org/author/A5094850554', 'https://semopenalex.org/author/A5111877855', 'https://semopenalex.org/author/A5109550726', 'https://semopenalex.org/author/A5075933702', 'https://semopenalex.org/author/A5042669324', 'https://semopenalex.org/author/A5112770924', 'https://semopenalex.org/author/A5072234007', 'https://semopenalex.org/author/A5050785938', 'https://semopenalex.org/author/A5052097686', 'https://semopenalex.org/author/A5110225216', 'https://semopenalex.org/author/A5031092968', 'https://semopenalex.org/author/A5067216808', 'https://semopenalex.org/author/A5068502658', 'https://semopenalex.org/author/A5012860343', 'https://semopenalex.org/author/A5031002895', 'https://semopenalex.org/author/A5040815520', 'https://semopenalex.org/author/A5038742643', 'https://semopenalex.org/author/A5112318312', 'https://semopenalex.org/author/A5100698896', 'https://semopenalex.org/author/A5069460336', 'https://semopenalex.org/author/A5016900185', 'https://semopenalex.org/author/A5062073470', 'https://semopenalex.org/author/A5088969714', 'https://semopenalex.org/author/A5044848288', 'https://semopenalex.org/author/A5038114517', 'https://semopenalex.org/author/A5076724937', 'https://semopenalex.org/author/A5077149145', 'https://semopenalex.org/author/A5049158387', 'https://semopenalex.org/author/A5070025348', 'https://semopenalex.org/author/A5040178908', 'https://semopenalex.org/author/A5090198878', 'https://semopenalex.org/author/A5013152760', 'https://semopenalex.org/author/A5042204813', 'https://semopenalex.org/author/A5100732392', 'https://semopenalex.org/author/A5069065883', 'https://semopenalex.org/author/A5100390687', 'https://semopenalex.org/author/A5109550729', 'https://semopenalex.org/author/A5100760216', 'https://semopenalex.org/author/A5033256132', 'https://semopenalex.org/author/A5054694688', 'https://semopenalex.org/author/A5101525412', 'https://semopenalex.org/author/A5048205587', 'https://semopenalex.org/author/A5089085275', 'https://semopenalex.org/author/A5008144788', 'https://semopenalex.org/author/A5033517451', 'https://semopenalex.org/author/A5103256649', 'https://semopenalex.org/author/A5091752605', 'https://semopenalex.org/author/A5082861248', 'https://semopenalex.org/author/A5057416433', 'https://semopenalex.org/author/A5035534381', 'https://semopenalex.org/author/A5108866418', 'https://semopenalex.org/author/A5052057125', 'https://semopenalex.org/author/A5037317771', 'https://semopenalex.org/author/A5010873632', 'https://semopenalex.org/author/A5064540278', 'https://semopenalex.org/author/A5113926166', 'https://semopenalex.org/author/A5077182059', 'https://semopenalex.org/author/A5100613030', 'https://semopenalex.org/author/A5014845685', 'https://semopenalex.org/author/A5112385471', 'https://semopenalex.org/author/A5011383988', 'https://semopenalex.org/author/A5062953965', 'https://semopenalex.org/author/A5065938167', 'https://semopenalex.org/author/A5048011759', 'https://semopenalex.org/author/A5108166978', 'https://semopenalex.org/author/A5102756198', 'https://semopenalex.org/author/A5030803226', 'https://semopenalex.org/author/A5000830051', 'https://semopenalex.org/author/A5019071895', 'https://semopenalex.org/author/A5051357966', 'https://semopenalex.org/author/A5058288079', 'https://semopenalex.org/author/A5084014359', 'https://semopenalex.org/author/A5080136207', 'https://semopenalex.org/author/A5102455066', 'https://semopenalex.org/author/A5028279714', 'https://semopenalex.org/author/A5006986556', 'https://semopenalex.org/author/A5057228007', 'https://semopenalex.org/author/A5011958240', 'https://semopenalex.org/author/A5058021734', 'https://semopenalex.org/author/A5040920032', 'https://semopenalex.org/author/A5014053775', 'https://semopenalex.org/author/A5100350849', 'https://semopenalex.org/author/A5044500644', 'https://semopenalex.org/author/A5003775830', 'https://semopenalex.org/author/A5017945484', 'https://semopenalex.org/author/A5050409448', 'https://semopenalex.org/author/A5112307831', 'https://semopenalex.org/author/A5030807574', 'https://semopenalex.org/author/A5038743559', 'https://semopenalex.org/author/A5010413083', 'https://semopenalex.org/author/A5094850562', 'https://semopenalex.org/author/A5064138452', 'https://semopenalex.org/author/A5003399501', 'https://semopenalex.org/author/A5023475606', 'https://semopenalex.org/author/A5064932423', 'https://semopenalex.org/author/A5009197679', 'https://semopenalex.org/author/A5016460678', 'https://semopenalex.org/author/A5112789074', 'https://semopenalex.org/author/A5088485570', 'https://semopenalex.org/author/A5031841696', 'https://semopenalex.org/author/A5082724929', 'https://semopenalex.org/author/A5113502195', 'https://semopenalex.org/author/A5023277983', 'https://semopenalex.org/author/A5062066146', 'https://semopenalex.org/author/A5104016331', 'https://semopenalex.org/author/A5008094693', 'https://semopenalex.org/author/A5058899219', 'https://semopenalex.org/author/A5077839667', 'https://semopenalex.org/author/A5019451172', 'https://semopenalex.org/author/A5044367354', 'https://semopenalex.org/author/A5024594245', 'https://semopenalex.org/author/A5102185302', 'https://semopenalex.org/author/A5081277076', 'https://semopenalex.org/author/A5000810401', 'https://semopenalex.org/author/A5058766860', 'https://semopenalex.org/author/A5091863156', 'https://semopenalex.org/author/A5100329846', 'https://semopenalex.org/author/A5069481232', 'https://semopenalex.org/author/A5035044634', 'https://semopenalex.org/author/A5032514888', 'https://semopenalex.org/author/A5020549462', 'https://semopenalex.org/author/A5047735602', 'https://semopenalex.org/author/A5101725214', 'https://semopenalex.org/author/A5087781429', 'https://semopenalex.org/author/A5101835251', 'https://semopenalex.org/author/A5039019367', 'https://semopenalex.org/author/A5094966954', 'https://semopenalex.org/author/A5013719267', 'https://semopenalex.org/author/A5010139814', 'https://semopenalex.org/author/A5058506527', 'https://semopenalex.org/author/A5101754929', 'https://semopenalex.org/author/A5066368261', 'https://semopenalex.org/author/A5102722569', 'https://semopenalex.org/author/A5044745609', 'https://semopenalex.org/author/A5054677861', 'https://semopenalex.org/author/A5113619301', 'https://semopenalex.org/author/A5094966958', 'https://semopenalex.org/author/A5087025037', 'https://semopenalex.org/author/A5022655755', 'https://semopenalex.org/author/A5094966949', 'https://semopenalex.org/author/A5000045142', 'https://semopenalex.org/author/A5101729519', 'https://semopenalex.org/author/A5043857690', 'https://semopenalex.org/author/A5083755757', 'https://semopenalex.org/author/A5080481085', 'https://semopenalex.org/author/A5025747170', 'https://semopenalex.org/author/A5074788841', 'https://semopenalex.org/author/A5065638410', 'https://semopenalex.org/author/A5102461996', 'https://semopenalex.org/author/A5086959491', 'https://semopenalex.org/author/A5071892402', 'https://semopenalex.org/author/A5108795667', 'https://semopenalex.org/author/A5080195917', 'https://semopenalex.org/author/A5100866986', 'https://semopenalex.org/author/A5040341362', 'https://semopenalex.org/author/A5109618877', 'https://semopenalex.org/author/A5003335464', 'https://semopenalex.org/author/A5100439502', 'https://semopenalex.org/author/A5026925615', 'https://semopenalex.org/author/A5088560930', 'https://semopenalex.org/author/A5101080554', 'https://semopenalex.org/author/A5072728622', 'https://semopenalex.org/author/A5063071825', 'https://semopenalex.org/author/A5100389568', 'https://semopenalex.org/author/A5109040569', 'https://semopenalex.org/author/A5006214623', 'https://semopenalex.org/author/A5087315126', 'https://semopenalex.org/author/A5073780213', 'https://semopenalex.org/author/A5064358069', 'https://semopenalex.org/author/A5023770864', 'https://semopenalex.org/author/A5100308761', 'https://semopenalex.org/author/A5055669214', 'https://semopenalex.org/author/A5062356522', 'https://semopenalex.org/author/A5104808391', 'https://semopenalex.org/author/A5094850563', 'https://semopenalex.org/author/A5056480200', 'https://semopenalex.org/author/A5021385837', 'https://semopenalex.org/author/A5048567127', 'https://semopenalex.org/author/A5111965782', 'https://semopenalex.org/author/A5019114258', 'https://semopenalex.org/author/A5069616469', 'https://semopenalex.org/author/A5020890252', 'https://semopenalex.org/author/A5021976057', 'https://semopenalex.org/author/A5090533480', 'https://semopenalex.org/author/A5032948315', 'https://semopenalex.org/author/A5033778949', 'https://semopenalex.org/author/A5090185743', 'https://semopenalex.org/author/A5046114637', 'https://semopenalex.org/author/A5041359027', 'https://semopenalex.org/author/A5082932410', 'https://semopenalex.org/author/A5108754601', 'https://semopenalex.org/author/A5088731092', 'https://semopenalex.org/author/A5101159427', 'https://semopenalex.org/author/A5010667155', 'https://semopenalex.org/author/A5034996813', 'https://semopenalex.org/author/A5088694364', 'https://semopenalex.org/author/A5077352940', 'https://semopenalex.org/author/A5083932343', 'https://semopenalex.org/author/A5029808771', 'https://semopenalex.org/author/A5028142123', 'https://semopenalex.org/author/A5108795666', 'https://semopenalex.org/author/A5103860234', 'https://semopenalex.org/author/A5016341376', 'https://semopenalex.org/author/A5100531979', 'https://semopenalex.org/author/A5001078030', 'https://semopenalex.org/author/A5107204848', 'https://semopenalex.org/author/A5027348774', 'https://semopenalex.org/author/A5110468084', 'https://semopenalex.org/author/A5083965446', 'https://semopenalex.org/author/A5100382191', 'https://semopenalex.org/author/A5102461997', 'https://semopenalex.org/author/A5001699131', 'https://semopenalex.org/author/A5110866134', 'https://semopenalex.org/author/A5043740841', 'https://semopenalex.org/author/A5050624359', 'https://semopenalex.org/author/A5066279170', 'https://semopenalex.org/author/A5026707758', 'https://semopenalex.org/author/A5094850561', 'https://semopenalex.org/author/A5110432474', 'https://semopenalex.org/author/A5069142363', 'https://semopenalex.org/author/A5111745917', 'https://semopenalex.org/author/A5106121692', 'https://semopenalex.org/author/A5078310286', 'https://semopenalex.org/author/A5112796516', 'https://semopenalex.org/author/A5112770927', 'https://semopenalex.org/author/A5113491971', 'https://semopenalex.org/author/A5033908021', 'https://semopenalex.org/author/A5085413987', 'https://semopenalex.org/author/A5007690829', 'https://semopenalex.org/author/A5084544975', 'https://semopenalex.org/author/A5057391353', 'https://semopenalex.org/author/A5009296051', 'https://semopenalex.org/author/A5028655113', 'https://semopenalex.org/author/A5062058930', 'https://semopenalex.org/author/A5013993834', 'https://semopenalex.org/author/A5054624012', 'https://semopenalex.org/author/A5067334214', 'https://semopenalex.org/author/A5052937413', 'https://semopenalex.org/author/A5070309508', 'https://semopenalex.org/author/A5112789075', 'https://semopenalex.org/author/A5033607252', 'https://semopenalex.org/author/A5076181565', 'https://semopenalex.org/author/A5114085404', 'https://semopenalex.org/author/A5059112151', 'https://semopenalex.org/author/A5075449266', 'https://semopenalex.org/author/A5100307045', 'https://semopenalex.org/author/A5054833334', 'https://semopenalex.org/author/A5056986371', 'https://semopenalex.org/author/A5049740030', 'https://semopenalex.org/author/A5046691620', 'https://semopenalex.org/author/A5048006075', 'https://semopenalex.org/author/A5038398097', 'https://semopenalex.org/author/A5083759644', 'https://semopenalex.org/author/A5027703220', 'https://semopenalex.org/author/A5094966955', 'https://semopenalex.org/author/A5058940849', 'https://semopenalex.org/author/A5020293284', 'https://semopenalex.org/author/A5046907740', 'https://semopenalex.org/author/A5071699360', 'https://semopenalex.org/author/A5061668006', 'https://semopenalex.org/author/A5108134868', 'https://semopenalex.org/author/A5012514876', 'https://semopenalex.org/author/A5103447072', 'https://semopenalex.org/author/A5021964111', 'https://semopenalex.org/author/A5044651647', 'https://semopenalex.org/author/A5074969316', 'https://semopenalex.org/author/A5108854968', 'https://semopenalex.org/author/A5102676712', 'https://semopenalex.org/author/A5081082953', 'https://semopenalex.org/author/A5002400587', 'https://semopenalex.org/author/A5108322148', 'https://semopenalex.org/author/A5032959229', 'https://semopenalex.org/author/A5094850557', 'https://semopenalex.org/author/A5037435544', 'https://semopenalex.org/author/A5014706612', 'https://semopenalex.org/author/A5100681023', 'https://semopenalex.org/author/A5015406329', 'https://semopenalex.org/author/A5011886931', 'https://semopenalex.org/author/A5102836787', 'https://semopenalex.org/author/A5105408906', 'https://semopenalex.org/author/A5065892913', 'https://semopenalex.org/author/A5076222775', 'https://semopenalex.org/author/A5111408885', 'https://semopenalex.org/author/A5054944358', 'https://semopenalex.org/author/A5053204071', 'https://semopenalex.org/author/A5009940583', 'https://semopenalex.org/author/A5112194416', 'https://semopenalex.org/author/A5009982918', 'https://semopenalex.org/author/A5011287069', 'https://semopenalex.org/author/A5100437036', 'https://semopenalex.org/author/A5072385590', 'https://semopenalex.org/author/A5059992565', 'https://semopenalex.org/author/A5108450184', 'https://semopenalex.org/author/A5094850558', 'https://semopenalex.org/author/A5017534073', 'https://semopenalex.org/author/A5028602300', 'https://semopenalex.org/author/A5113164291', 'https://semopenalex.org/author/A5039508234', 'https://semopenalex.org/author/A5011092157', 'https://semopenalex.org/author/A5065844089', 'https://semopenalex.org/author/A5089847337', 'https://semopenalex.org/author/A5005192499', 'https://semopenalex.org/author/A5106691602', 'https://semopenalex.org/author/A5045601109', 'https://semopenalex.org/author/A5112770925', 'https://semopenalex.org/author/A5021047347', 'https://semopenalex.org/author/A5043574831', 'https://semopenalex.org/author/A5055164211', 'https://semopenalex.org/author/A5094850549', 'https://semopenalex.org/author/A5058644115', 'https://semopenalex.org/author/A5017549278', 'https://semopenalex.org/author/A5032100463', 'https://semopenalex.org/author/A5002366144', 'https://semopenalex.org/author/A5076828229', 'https://semopenalex.org/author/A5031901931', 'https://semopenalex.org/author/A5042189562', 'https://semopenalex.org/author/A5100421943', 'https://semopenalex.org/author/A5061880585', 'https://semopenalex.org/author/A5049314735', 'https://semopenalex.org/author/A5029701178', 'https://semopenalex.org/author/A5101535147', 'https://semopenalex.org/author/A5111747866', 'https://semopenalex.org/author/A5100353457', 'https://semopenalex.org/author/A5026800235', 'https://semopenalex.org/author/A5045614803', 'https://semopenalex.org/author/A5006074944', 'https://semopenalex.org/author/A5009158005', 'https://semopenalex.org/author/A5101558388', 'https://semopenalex.org/author/A5050944699', 'https://semopenalex.org/author/A5049803081', 'https://semopenalex.org/author/A5072837074', 'https://semopenalex.org/author/A5087961115', 'https://semopenalex.org/author/A5055397205', 'https://semopenalex.org/author/A5021741380', 'https://semopenalex.org/author/A5020905436', 'https://semopenalex.org/author/A5057180938', 'https://semopenalex.org/author/A5044086454', 'https://semopenalex.org/author/A5059045306', 'https://semopenalex.org/author/A5088241324', 'https://semopenalex.org/author/A5079760641', 'https://semopenalex.org/author/A5103141604', 'https://semopenalex.org/author/A5041317074', 'https://semopenalex.org/author/A5013759413', 'https://semopenalex.org/author/A5075283583', 'https://semopenalex.org/author/A5063124631', 'https://semopenalex.org/author/A5112770926', 'https://semopenalex.org/author/A5112433524', 'https://semopenalex.org/author/A5022809952', 'https://semopenalex.org/author/A5110866138', 'https://semopenalex.org/author/A5078631705', 'https://semopenalex.org/author/A5094966944', 'https://semopenalex.org/author/A5083460317', 'https://semopenalex.org/author/A5103267619', 'https://semopenalex.org/author/A5101941642', 'https://semopenalex.org/author/A5035731144', 'https://semopenalex.org/author/A5049144743', 'https://semopenalex.org/author/A5015181699', 'https://semopenalex.org/author/A5006284497', 'https://semopenalex.org/author/A5086794491', 'https://semopenalex.org/author/A5094966952', 'https://semopenalex.org/author/A5003817085', 'https://semopenalex.org/author/A5039281963', 'https://semopenalex.org/author/A5083002157', 'https://semopenalex.org/author/A5020691490', 'https://semopenalex.org/author/A5007728844', 'https://semopenalex.org/author/A5091510633', 'https://semopenalex.org/author/A5009425558', 'https://semopenalex.org/author/A5074308388', 'https://semopenalex.org/author/A5031513518', 'https://semopenalex.org/author/A5044014333', 'https://semopenalex.org/author/A5029000917', 'https://semopenalex.org/author/A5019187849', 'https://semopenalex.org/author/A5101505215', 'https://semopenalex.org/author/A5039946576', 'https://semopenalex.org/author/A5090679545', 'https://semopenalex.org/author/A5044990862', 'https://semopenalex.org/author/A5087123689', 'https://semopenalex.org/author/A5018037913', 'https://semopenalex.org/author/A5035030619', 'https://semopenalex.org/author/A5021090586', 'https://semopenalex.org/author/A5047323924', 'https://semopenalex.org/author/A5111920218', 'https://semopenalex.org/author/A5091820260', 'https://semopenalex.org/author/A5102832962', 'https://semopenalex.org/author/A5010793783', 'https://semopenalex.org/author/A5100695007', 'https://semopenalex.org/author/A5058473639', 'https://semopenalex.org/author/A5075544010', 'https://semopenalex.org/author/A5094850552', 'https://semopenalex.org/author/A5021048076', 'https://semopenalex.org/author/A5062934322', 'https://semopenalex.org/author/A5044657641', 'https://semopenalex.org/author/A5000004709', 'https://semopenalex.org/author/A5053913249', 'https://semopenalex.org/author/A5057173697', 'https://semopenalex.org/author/A5111246205', 'https://semopenalex.org/author/A5016330520', 'https://semopenalex.org/author/A5010063800', 'https://semopenalex.org/author/A5093323203', 'https://semopenalex.org/author/A5013796744', 'https://semopenalex.org/author/A5001294898', 'https://semop</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/author/A5103223639', 'https://semopenalex.org/author/A5081340873', 'https://semopenalex.org/author/A5066916130', 'https://semopenalex.org/author/A5101194950', 'https://semopenalex.org/author/A5100388627', 'https://semopenalex.org/author/A5085611398', 'https://semopenalex.org/author/A5070152860', 'https://semopenalex.org/author/A5089294104', 'https://semopenalex.org/author/A5049076146', 'https://semopenalex.org/author/A5103047914', 'https://semopenalex.org/author/A5081650066', 'https://semopenalex.org/author/A5049622460', 'https://semopenalex.org/author/A5050308989', 'https://semopenalex.org/author/A5041073042', 'https://semopenalex.org/author/A5023155310', 'https://semopenalex.org/author/A5101601497', 'https://semopenalex.org/author/A5079729956', 'https://semopenalex.org/author/A5100301259', 'https://semopenalex.org/author/A5072002680', 'https://semopenalex.org/author/A5002503342', 'https://semopenalex.org/author/A5032068969', 'https://semopenalex.org/author/A5072432956', 'https://semopenalex.org/author/A5074540830', 'https://semopenalex.org/author/A5040987266', 'https://semopenalex.org/author/A5101011726', 'https://semopenalex.org/author/A5100386104', 'https://semopenalex.org/author/A5102204689', 'https://semopenalex.org/author/A5047271595', 'https://semopenalex.org/author/A5110161847', 'https://semopenalex.org/author/A5076516205', 'https://semopenalex.org/author/A5086338440', 'https://semopenalex.org/author/A5100385498', 'https://semopenalex.org/author/A5101852647', 'https://semopenalex.org/author/A5056526226', 'https://semopenalex.org/author/A5012621594', 'https://semopenalex.org/author/A5100458045', 'https://semopenalex.org/author/A5100405159', 'https://semopenalex.org/author/A5100447531', 'https://semopenalex.org/author/A5081145634', 'https://semopenalex.org/author/A5077008083', 'https://semopenalex.org/author/A5100365555', 'https://semopenalex.org/author/A5053084752', 'https://semopenalex.org/author/A5101468661', 'https://semopenalex.org/author/A5000582109', 'https://semopenalex.org/author/A5100299966', 'https://semopenalex.org/author/A5102020713', 'https://semopenalex.org/author/A5045500611', 'https://semopenalex.org/author/A5006357713', 'https://semopenalex.org/author/A5018128809', 'https://semopenalex.org/author/A5103233342', 'https://semopenalex.org/author/A5061863093', 'https://semopenalex.org/author/A5101637945', 'https://semopenalex.org/author/A5051192643', 'https://semopenalex.org/author/A5100361984', 'https://semopenalex.org/author/A5059396373', 'https://semopenalex.org/author/A5100322125', 'https://semopenalex.org/author/A5040272202', 'https://semopenalex.org/author/A5059555100', 'https://semopenalex.org/author/A5087587101', 'https://semopenalex.org/author/A5085666756', 'https://semopenalex.org/author/A5103286574', 'https://semopenalex.org/author/A5101966381', 'https://semopenalex.org/author/A5102900280', 'https://semopenalex.org/author/A5081036622', 'https://semopenalex.org/author/A5101614814', 'https://semopenalex.org/author/A5027206285', 'https://semopenalex.org/author/A5101983121', 'https://semopenalex.org/author/A5100388609', 'https://semopenalex.org/author/A5085247180', 'https://semopenalex.org/author/A5000019783', 'https://semopenalex.org/author/A5113115887', 'https://semopenalex.org/author/A5005639930', 'https://semopenalex.org/author/A5011667547', 'https://semopenalex.org/author/A5050748634', 'https://semopenalex.org/author/A5100385507', 'https://semopenalex.org/author/A5030490896', 'https://semopenalex.org/author/A5100638997', 'https://semopenalex.org/author/A5039326697', 'https://semopenalex.org/author/A5101812436', 'https://semopenalex.org/author/A5102858698', 'https://semopenalex.org/author/A5100639062', 'https://semopenalex.org/author/A5102014459', 'https://semopenalex.org/author/A5056980315', 'https://semopenalex.org/author/A5101261545', 'https://semopenalex.org/author/A5021631329', 'https://semopenalex.org/author/A5026939932', 'https://semopenalex.org/author/A5056755949', 'https://semopenalex.org/author/A5022905724', 'https://semopenalex.org/author/A5054115813', 'https://semopenalex.org/author/A5101655978', 'https://semopenalex.org/author/A5100633784', 'https://semopenalex.org/author/A5102859232', 'https://semopenalex.org/author/A5088498790', 'https://semopenalex.org/author/A5081449581', 'https://semopenalex.org/author/A5101636662', 'https://semopenalex.org/author/A5000845080', 'https://semopenalex.org/author/A5040203716', 'https://semopenalex.org/author/A5058828089', 'https://semopenalex.org/author/A5100375823', 'https://semopenalex.org/author/A5019450472', 'https://semopenalex.org/author/A5103205784', 'https://semopenalex.org/author/A5036986396', 'https://semopenalex.org/author/A5013325392', 'https://semopenalex.org/author/A5025099559', 'https://semopenalex.org/author/A5101555891', 'https://semopenalex.org/author/A5101617703', 'https://semopenalex.org/author/A5060364305', 'https://semopenalex.org/author/A5100388599', 'https://semopenalex.org/author/A5091706559', 'https://semopenalex.org/author/A5000645139', 'https://semopenalex.org/author/A5110172698', 'https://semopenalex.org/author/A5100753039', 'https://semopenalex.org/author/A5077658936', 'https://semopenalex.org/author/A5100779597', 'https://semopenalex.org/author/A5069809962', 'https://semopenalex.org/author/A5010958113', 'https://semopenalex.org/author/A5068122240', 'https://semopenalex.org/author/A5042235813', 'https://semopenalex.org/author/A5102987690', 'https://semopenalex.org/author/A5011367069', 'https://semopenalex.org/author/A5072456187', 'https://semopenalex.org/author/A5107864790', 'https://semopenalex.org/author/A5100388597', 'https://semopenalex.org/author/A5102717988', 'https://semopenalex.org/author/A5100388716', 'https://semopenalex.org/author/A5100758675', 'https://semopenalex.org/author/A5100608460', 'https://semopenalex.org/author/A5100665833', 'https://semopenalex.org/author/A5081886276', 'https://semopenalex.org/author/A5016401353', 'https://semopenalex.org/author/A5024073253', 'https://semopenalex.org/author/A5021179945', 'https://semopenalex.org/author/A5054753279', 'https://semopenalex.org/author/A5074075949', 'https://semopenalex.org/author/A5048118068', 'https://semopenalex.org/author/A5024456332', 'https://semopenalex.org/author/A5039037722', 'https://semopenalex.org/author/A5073947585', 'https://semopenalex.org/author/A5012561478', 'https://semopenalex.org/author/A5015967363', 'https://semopenalex.org/author/A5100376204', 'https://semopenalex.org/author/A5049142567', 'https://semopenalex.org/author/A5013438083', 'https://semopenalex.org/author/A5042986574', 'https://semopenalex.org/author/A5047965752', 'https://semopenalex.org/author/A5036039721', 'https://semopenalex.org/author/A5006669765', 'https://semopenalex.org/author/A5005604635', 'https://semopenalex.org/author/A5101660937', 'https://semopenalex.org/author/A5109297018', 'https://semopenalex.org/author/A5100738974', 'https://semopenalex.org/author/A5023035566', 'https://semopenalex.org/author/A5100440010', 'https://semopenalex.org/author/A5114213934', 'https://semopenalex.org/author/A5064776947', 'https://semopenalex.org/author/A5025292884', 'https://semopenalex.org/author/A5043546718', 'https://semopenalex.org/author/A5065120715', 'https://semopenalex.org/author/A5044689090', 'https://semopenalex.org/author/A5003031253', 'https://semopenalex.org/author/A5010181158', 'https://semopenalex.org/author/A5068340305', 'https://semopenalex.org/author/A5017334961', 'https://semopenalex.org/author/A5100439996', 'https://semopenalex.org/author/A5028716858', 'https://semopenalex.org/author/A5084868951', 'https://semopenalex.org/author/A5100408010', 'https://semopenalex.org/author/A5007043113', 'https://semopenalex.org/author/A5011086593', 'https://semopenalex.org/author/A5108459503', 'https://semopenalex.org/author/A5101540631', 'https://semopenalex.org/author/A5077610917', 'https://semopenalex.org/author/A5034057959', 'https://semopenalex.org/author/A5019525050', 'https://semopenalex.org/author/A5101308414', 'https://semopenalex.org/author/A5101289775', 'https://semopenalex.org/author/A5015836405', 'https://semopenalex.org/author/A5100388581', 'https://semopenalex.org/author/A5100438174', 'https://semopenalex.org/author/A5100458090', 'https://semopenalex.org/author/A5101264794', 'https://semopenalex.org/author/A5100426931', 'https://semopenalex.org/author/A5076444296', 'https://semopenalex.org/author/A5100610450', 'https://semopenalex.org/author/A5033111691', 'https://semopenalex.org/author/A5075273130', 'https://semopenalex.org/author/A5103234102', 'https://semopenalex.org/author/A5043798385', 'https://semopenalex.org/author/A5115595561', 'https://semopenalex.org/author/A5032062525', 'https://semopenalex.org/author/A5032194564', 'https://semopenalex.org/author/A5101612059', 'https://semopenalex.org/author/A5114778131', 'https://semopenalex.org/author/A5058164381', 'https://semopenalex.org/author/A5100738977', 'https://semopenalex.org/author/A5081420063', 'https://semopenalex.org/author/A5046237164', 'https://semopenalex.org/author/A5084735407', 'https://semopenalex.org/author/A5100409885', 'https://semopenalex.org/author/A5100388576', 'https://semopenalex.org/author/A5100447682', 'https://semopenalex.org/author/A5102222159', 'https://semopenalex.org/author/A5100676331', 'https://semopenalex.org/author/A5030626281', 'https://semopenalex.org/author/A5009071576', 'https://semopenalex.org/author/A5100429004', 'https://semopenalex.org/author/A5050080938', 'https://semopenalex.org/author/A5087492388', 'https://semopenalex.org/author/A5043801432', 'https://semopenalex.org/author/A5002594574', 'https://semopenalex.org/author/A5049100391', 'https://semopenalex.org/author/A5077424533', 'https://semopenalex.org/author/A5100772234', 'https://semopenalex.org/author/A5101556258', 'https://semopenalex.org/author/A5004490190', 'https://semopenalex.org/author/A5009435651', 'https://semopenalex.org/author/A5024821632', 'https://semopenalex.org/author/A5077138780', 'https://semopenalex.org/author/A5100459874', 'https://semopenalex.org/author/A5067163535', 'https://semopenalex.org/author/A5052249316', 'https://semopenalex.org/author/A5002289161', 'https://semopenalex.org/author/A5100327487', 'https://semopenalex.org/author/A5102928967', 'https://semopenalex.org/author/A5074307489', 'https://semopenalex.org/author/A5045087569', 'https://semopenalex.org/author/A5065293581', 'https://semopenalex.org/author/A5090671359', 'https://semopenalex.org/author/A5021222755', 'https://semopenalex.org/author/A5100408160', 'https://semopenalex.org/author/A5009455568', 'https://semopenalex.org/author/A5100367807', 'https://semopenalex.org/author/A5058738211', 'https://semopenalex.org/author/A5100738980', 'https://semopenalex.org/author/A5018031899', 'https://semopenalex.org/author/A5100753041', 'https://semopenalex.org/author/A5084874990', 'https://semopenalex.org/author/A5026927053', 'https://semopenalex.org/author/A5027084532', 'https://semopenalex.org/author/A5000381434', 'https://semopenalex.org/author/A5013103539', 'https://semopenalex.org/author/A5059065212', 'https://semopenalex.org/author/A5103761162', 'https://semopenalex.org/author/A5088725475', 'https://semopenalex.org/author/A5067467896', 'https://semopenalex.org/author/A5041961808', 'https://semopenalex.org/author/A5023093639', 'https://semopenalex.org/author/A5100388617', 'https://semopenalex.org/author/A5100331488', 'https://semopenalex.org/author/A5022677467', 'https://semopenalex.org/author/A5073965511', 'https://semopenalex.org/author/A5100349346', 'https://semopenalex.org/author/A5100523187', 'https://semopenalex.org/author/A5038017715', 'https://semopenalex.org/author/A5100361632', 'https://semopenalex.org/author/A5012469172', 'https://semopenalex.org/author/A5040850915', 'https://semopenalex.org/author/A5100367825', 'https://semopenalex.org/author/A5067395122', 'https://semopenalex.org/author/A5060115298', 'https://semopenalex.org/author/A5100445622', 'https://semopenalex.org/author/A5055149708', 'https://semopenalex.org/author/A5103073505', 'https://semopenalex.org/author/A5107006112', 'https://semopenalex.org/author/A5052981404', 'https://semopenalex.org/author/A5103205468', 'https://semopenalex.org/author/A5075929099', 'https://semopenalex.org/author/A5100443727', 'https://semopenalex.org/author/A5111956187', 'https://semopenalex.org/author/A5069596903', 'https://semopenalex.org/author/A5034794084', 'https://semopenalex.org/author/A5101558050', 'https://semopenalex.org/author/A5043476448', 'https://semopenalex.org/author/A5055422837', 'https://semopenalex.org/author/A5088708850', 'https://semopenalex.org/author/A5052199638', 'https://semopenalex.org/author/A5077984014', 'https://semopenalex.org/author/A5035089987', 'https://semopenalex.org/author/A5058258996', 'https://semopenalex.org/author/A5035359666', 'https://semopenalex.org/author/A5100388644', 'https://semopenalex.org/author/A5100401412', 'https://semopenalex.org/author/A5036120394', 'https://semopenalex.org/author/A5113160035', 'https://semopenalex.org/author/A5033164669', 'https://semopenalex.org/author/A5100394129', 'https://semopenalex.org/author/A5115590096', 'https://semopenalex.org/author/A5069621751', 'https://semopenalex.org/author/A5100447691', 'https://semopenalex.org/author/A5100677820', 'https://semopenalex.org/author/A5052404451', 'https://semopenalex.org/author/A5009487151', 'https://semopenalex.org/author/A5085393851', 'https://semopenalex.org/author/A5065848808', 'https://semopenalex.org/author/A5090627608', 'https://semopenalex.org/author/A5025977354', 'https://semopenalex.org/author/A5100697624', 'https://semopenalex.org/author/A5033163346', 'https://semopenalex.org/author/A5079431306', 'https://semopenalex.org/author/A5005007374', 'https://semopenalex.org/author/A5058257080', 'https://semopenalex.org/author/A5100412598', 'https://semopenalex.org/author/A5088646345', 'https://semopenalex.org/author/A5100349343', 'https://semopenalex.org/author/A5048041198', 'https://semopenalex.org/author/A5025839857', 'https://semopenalex.org/author/A5030997313', 'https://semopenalex.org/author/A5033542967']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W2056938644', '2020', 'https://semopenalex.org/work/W4200567986', '2009', 'https://semopenalex.org/work/W3081722247', 'https://semopenalex.org/work/W1538014482', 'https://semopenalex.org/work/W4229332766', 'https://semopenalex.org/work/W1497260915', 'https://semopenalex.org/work/W3042971551', 'https://semopenalex.org/work/W2132176043', 'https://semopenalex.org/work/W1992481796', 'https://semopenalex.org/work/W2259681201', '2008', 'https://semopenalex.org/work/W4312466951', 'https://semopenalex.org/work/W2166474382', 'https://semopenalex.org/work/W2460327056', 'https://semopenalex.org/work/W4283727356', 'https://semopenalex.org/work/W4389542639', 'https://semopenalex.org/work/W2948842040', 'https://semopenalex.org/work/W2883605426', 'https://semopenalex.org/work/W2574426197', 'https://semopenalex.org/work/W2984980523', 'https://semopenalex.org/work/W2002565472', '2019', 'https://semopenalex.org/work/W1975460851', 'https://semopenalex.org/work/W2517469201', 'https://semopenalex.org/work/W2469358968', 'https://semopenalex.org/work/W2729358317', 'https://semopenalex.org/work/W2198531583', 'https://semopenalex.org/work/W4283719869', 'https://semopenalex.org/work/W1500793049', 'https://semopenalex.org/work/W2188075483', 'https://semopenalex.org/work/W2948301006', 'https://semopenalex.org/work/W3119942460', 'https://semopenalex.org/work/W2040041660', 'https://semopenalex.org/work/W4396774950', 'https://semopenalex.org/work/W2906936538', 'https://semopenalex.org/work/W2080778070', 'https://semopenalex.org/work/W2559459321', 'https://semopenalex.org/work/W3094530900', 'https://semopenalex.org/work/W1642534804', 'https://semopenalex.org/work/W4402111012', 'https://semopenalex.org/work/W2201795542', 'https://semopenalex.org/work/W2912718446', 'https://semopenalex.org/work/W2979306097', 'https://semopenalex.org/work/W2895960982', 'https://semopenalex.org/work/W2768867910', 'https://semopenalex.org/work/W2810777165', 'https://semopenalex.org/work/W2980909386', 'https://semopenalex.org/work/W1966638294', 'https://semopenalex.org/work/W577437274', 'https://semopenalex.org/work/W2742357289', 'https://semopenalex.org/work/W4200171350', 'https://semopenalex.org/work/W4405721239', 'https://semopenalex.org/work/W4388442457', 'https://semopenalex.org/work/W3020102474', 'https://semopenalex.org/work/W1990881389', 'https://semopenalex.org/work/W4225665789', '2012', 'https://semopenalex.org/work/W2786699184', '2014', '2013', '2010', 'https://semopenalex.org/work/W2146499289', 'https://semopenalex.org/work/W2916024294', 'https://semopenalex.org/work/W1517780295', '2022', 'https://semopenalex.org/work/W2160324252', '2021', '2016', 'https://semopenalex.org/work/W2509319904', 'https://semopenalex.org/work/W3216430907', '2011', 'https://semopenalex.org/work/W4205142910', '2017', 'https://semopenalex.org/work/W2064795090', 'https://semopenalex.org/work/W2781983165', 'https://semopenalex.org/work/W2080816360', 'https://semopenalex.org/work/W2943023300', 'https://semopenalex.org/work/W2525447956', 'https://semopenalex.org/work/W2898652465', 'https://semopenalex.org/work/W4312342218', 'https://semopenalex.org/work/W2056876297', 'https://semopenalex.org/work/W2108772193', 'https://semopenalex.org/work/W2948077456', 'https://semopenalex.org/work/W2767279489', 'https://semopenalex.org/work/W1970969056', 'https://semopenalex.org/work/W2137973352', 'https://semopenalex.org/work/W2905245385', '2015', '2007', 'https://semopenalex.org/work/W2103141465', 'https://semopenalex.org/work/W2139123718', 'https://semopenalex.org/work/W2898517899', 'https://semopenalex.org/work/W12409091', 'https://semopenalex.org/work/W4386658225', 'https://semopenalex.org/work/W1524855866', 'https://semopenalex.org/work/W2066797554', 'https://semopenalex.org/work/W2102571324', 'https://semopenalex.org/work/W3196969850', 'https://semopenalex.org/work/W3146074607', 'https://semopenalex.org/work/W1997556505', '2018', 'https://semopenalex.org/work/W4389542588', 'https://semopenalex.org/work/W2140663815', '2024', 'https://semopenalex.org/work/W2600317709', 'https://semopenalex.org/work/W4394843643', 'https://semopenalex.org/work/W2974391363', 'https://semopenalex.org/work/W2066079643', 'https://semopenalex.org/work/W2773748254', '2023', 'https://semopenalex.org/work/W2614777946', 'https://semopenalex.org/work/W2013683587', 'https://semopenalex.org/work/W3183223328', 'https://semopenalex.org/work/W2062582789', 'https://semopenalex.org/work/W3003315047', 'https://semopenalex.org/work/W4200300839']</t>
+  </si>
+  <si>
+    <t>['2006', '2020', '2009', 'https://semopenalex.org/work/W2734683486', 'https://semopenalex.org/work/W3036594918', '2004', 'https://semopenalex.org/work/W3123633695', 'https://semopenalex.org/work/W2319667788', 'https://semopenalex.org/work/W1527780249', '2008', 'https://semopenalex.org/work/W84099738', 'https://semopenalex.org/work/W2955996770', 'https://semopenalex.org/work/W4390951576', 'https://semopenalex.org/work/W2996424405', 'https://semopenalex.org/work/W4285585511', 'https://semopenalex.org/work/W4285149163', 'https://semopenalex.org/work/W2610903992', '2019', 'https://semopenalex.org/work/W4220866607', 'https://semopenalex.org/work/W2894658205', 'https://semopenalex.org/work/W2550600565', 'https://semopenalex.org/work/W1109050', 'https://semopenalex.org/work/W4229365934', 'https://semopenalex.org/work/W579278758', 'https://semopenalex.org/work/W2171009049', 'https://semopenalex.org/work/W4245961146', 'https://semopenalex.org/work/W2246115839', 'https://semopenalex.org/work/W4321792691', 'https://semopenalex.org/work/W2754831193', 'https://semopenalex.org/work/W4400851484', 'https://semopenalex.org/work/W2258710106', 'https://semopenalex.org/work/W4287876838', '2005', 'https://semopenalex.org/work/W3111209168', 'https://semopenalex.org/work/W2130875118', 'https://semopenalex.org/work/W2343633423', 'https://semopenalex.org/work/W2058003955', 'https://semopenalex.org/work/W4213054152', 'https://semopenalex.org/work/W3007487359', 'https://semopenalex.org/work/W1971349525', 'https://semopenalex.org/work/W1756002337', 'https://semopenalex.org/work/W2970509049', 'https://semopenalex.org/work/W3010786249', 'https://semopenalex.org/work/W3187488983', 'https://semopenalex.org/work/W2790216340', 'https://semopenalex.org/work/W2794346483', 'https://semopenalex.org/work/W2142335546', 'https://semopenalex.org/work/W1961387618', 'https://semopenalex.org/work/W3069035240', 'https://semopenalex.org/work/W4376878797', '1994', 'https://semopenalex.org/work/W2783561900', 'https://semopenalex.org/work/W3170390068', '2025', 'https://semopenalex.org/work/W4232171693', 'https://semopenalex.org/work/W3207358793', 'https://semopenalex.org/work/W2010105821', 'https://semopenalex.org/work/W2794552363', '1991', 'https://semopenalex.org/work/W2118255469', 'https://semopenalex.org/work/W2586196676', 'https://semopenalex.org/work/W4394351286', '2012', 'https://semopenalex.org/work/W644371662', 'https://semopenalex.org/work/W2086291403', '2014', '2010', '2013', 'https://semopenalex.org/work/W3129198752', 'https://semopenalex.org/work/W2059263765', 'https://semopenalex.org/work/W333159667', 'https://semopenalex.org/work/W2072306533', '2022', 'https://semopenalex.org/work/W4239059882', '2021', '2016', 'https://semopenalex.org/work/W1549914272', '2011', '2017', 'https://semopenalex.org/work/W4200295656', 'https://semopenalex.org/work/W2947887973', 'https://semopenalex.org/work/W2923244310', 'https://semopenalex.org/work/W4229334755', 'https://semopenalex.org/work/W4300809016', 'https://semopenalex.org/work/W3018966866', 'https://semopenalex.org/work/W2761369579', 'https://semopenalex.org/work/W3205969438', 'https://semopenalex.org/work/W4403148167', 'https://semopenalex.org/work/W2737958970', 'https://semopenalex.org/work/W2124884294', 'https://semopenalex.org/work/W2140290607', '1983', 'https://semopenalex.org/work/W2893305614', '2015', 'https://semopenalex.org/work/W2067220443', 'https://semopenalex.org/work/W103992416', 'https://semopenalex.org/work/W4406613231', 'https://semopenalex.org/work/W4214922121', '2007', 'https://semopenalex.org/work/W1986447757', 'https://semopenalex.org/work/W2069403900', 'https://semopenalex.org/work/W2004089424', 'https://semopenalex.org/work/W4239020865', 'https://semopenalex.org/work/W3120867123', 'https://semopenalex.org/work/W3009651427', 'https://semopenalex.org/work/W2004860585', 'https://semopenalex.org/work/W3047226873', 'https://semopenalex.org/work/W2623352630', 'https://semopenalex.org/work/W4292377875', 'https://semopenalex.org/work/W3001208788', 'https://semopenalex.org/work/W4221004647', '2018', 'https://semopenalex.org/work/W2980431486', '2024', 'https://semopenalex.org/work/W2997254714', 'https://semopenalex.org/work/W2122737845', 'https://semopenalex.org/work/W4292378819', 'https://semopenalex.org/work/W3193926349', 'https://semopenalex.org/work/W3003870406', 'https://semopenalex.org/work/W4321105981', 'https://semopenalex.org/work/W1842188952', 'https://semopenalex.org/work/W4300970433', '2023', 'https://semopenalex.org/work/W2151014511', 'https://semopenalex.org/work/W2165467091', 'https://semopenalex.org/work/W3113261051']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W2791275386', '2006', 'https://semopenalex.org/work/W2481729578', 'https://semopenalex.org/work/W4200635145', '2020', 'https://semopenalex.org/work/W4322732827', 'https://semopenalex.org/work/W176670434', 'https://semopenalex.org/work/W2136188588', 'https://semopenalex.org/work/W4402548755', 'https://semopenalex.org/work/W2402441967', 'https://semopenalex.org/work/W4391011167', 'https://semopenalex.org/work/W2246393841', '2004', 'https://semopenalex.org/work/W4296902974', 'https://semopenalex.org/work/W4253642683', 'https://semopenalex.org/work/W2282010801', 'https://semopenalex.org/work/W2786772600', 'https://semopenalex.org/work/W2396037699', '2008', 'https://semopenalex.org/work/W2205191101', 'https://semopenalex.org/work/W1964676816', 'https://semopenalex.org/work/W201066287', 'https://semopenalex.org/work/W4287199679', 'https://semopenalex.org/work/W2921556996', 'https://semopenalex.org/work/W2400864908', '2003', 'https://semopenalex.org/work/W57476147', 'https://semopenalex.org/work/W3026162943', 'https://semopenalex.org/work/W2980624012', 'https://semopenalex.org/work/W4302377316', 'https://semopenalex.org/work/W4400169339', '2019', 'https://semopenalex.org/work/W4375869296', 'https://semopenalex.org/work/W2736149122', 'https://semopenalex.org/work/W1984877205', 'https://semopenalex.org/work/W4311721661', 'https://semopenalex.org/work/W4392903219', 'https://semopenalex.org/work/W110984805', 'https://semopenalex.org/work/W1616031638', 'https://semopenalex.org/work/W4396819389', '2005', 'https://semopenalex.org/work/W2127936745', 'https://semopenalex.org/work/W2508726376', 'https://semopenalex.org/work/W4361193366', 'https://semopenalex.org/work/W4392188516', 'https://semopenalex.org/work/W4280542824', 'https://semopenalex.org/work/W3168497289', 'https://semopenalex.org/work/W2021438034', 'https://semopenalex.org/work/W4400165275', 'https://semopenalex.org/work/W2617659622', 'https://semopenalex.org/work/W4386406820', 'https://semopenalex.org/work/W3005127776', 'https://semopenalex.org/work/W2098962393', 'https://semopenalex.org/work/W3048280215', 'https://semopenalex.org/work/W4404609477', 'https://semopenalex.org/work/W1729130926', 'https://semopenalex.org/work/W4399992019', 'https://semopenalex.org/work/W3009280029', 'https://semopenalex.org/work/W4399991973', 'https://semopenalex.org/work/W4391589175', 'https://semopenalex.org/work/W3031195982', 'https://semopenalex.org/work/W3006009898', 'https://semopenalex.org/work/W4206891293', 'https://semopenalex.org/work/W2095962821', 'https://semopenalex.org/work/W2735097653', '2001', 'https://semopenalex.org/work/W3200101073', 'https://semopenalex.org/work/W341170223', 'https://semopenalex.org/work/W3049587051', 'https://semopenalex.org/work/W2141047835', 'https://semopenalex.org/work/W4406492175', 'https://semopenalex.org/work/W1603914949', 'https://semopenalex.org/work/W3037451085', 'https://semopenalex.org/work/W3135916968', 'https://semopenalex.org/work/W4317487766', 'https://semopenalex.org/work/W2622265924', 'https://semopenalex.org/work/W2918054698', 'https://semopenalex.org/work/W2787015518', 'https://semopenalex.org/work/W2734345462', 'https://semopenalex.org/work/W4206844749', 'https://semopenalex.org/work/W2171302802', 'https://semopenalex.org/work/W4392931449', 'https://semopenalex.org/work/W4401978390', 'https://semopenalex.org/work/W4386439320', '2012', '2014', '2013', 'https://semopenalex.org/work/W4309564724', 'https://semopenalex.org/work/W3037369523', '2010', 'https://semopenalex.org/work/W2261240196', '2002', '2022', 'https://semopenalex.org/work/W4391940378', 'https://semopenalex.org/work/W2538817717', '2021', '2016', 'https://semopenalex.org/work/W2340829226', '2011', '2017', 'https://semopenalex.org/work/W4282823283', 'https://semopenalex.org/work/W4293229595', 'https://semopenalex.org/work/W3089124902', 'https://semopenalex.org/work/W2097450352', 'https://semopenalex.org/work/W2621391193', 'https://semopenalex.org/work/W65353647', 'https://semopenalex.org/work/W2002383345', 'https://semopenalex.org/work/W2498298891', 'https://semopenalex.org/work/W2990368351', 'https://semopenalex.org/work/W2987987546', 'https://semopenalex.org/work/W4360764206', 'https://semopenalex.org/work/W4399985329', 'https://semopenalex.org/work/W4399991937', 'https://semopenalex.org/work/W2056981644', 'https://semopenalex.org/work/W844598165', '2015', 'https://semopenalex.org/work/W4206887950', 'https://semopenalex.org/work/W4312690141', '2007', 'https://semopenalex.org/work/W4386096501', 'https://semopenalex.org/work/W4298259748', 'https://semopenalex.org/work/W4292536319', 'https://semopenalex.org/work/W4385822382', 'https://semopenalex.org/work/W2922616702', 'https://semopenalex.org/work/W4319776757', 'https://semopenalex.org/work/W4255342101', 'https://semopenalex.org/work/W4205871850', 'https://semopenalex.org/work/W4402148308', 'https://semopenalex.org/work/W2613217108', 'https://semopenalex.org/work/W172033102', '2018', 'https://semopenalex.org/work/W3088081769', 'https://semopenalex.org/work/W4400169194', 'https://semopenalex.org/work/W2736540096', '2024', 'https://semopenalex.org/work/W3198527244', 'https://semopenalex.org/work/W4280560758', 'https://semopenalex.org/work/W2123872165', 'https://semopenalex.org/work/W4404569657', '2023', 'https://semopenalex.org/work/W4401568144']</t>
+  </si>
+  <si>
+    <t>['2020', 'https://semopenalex.org/work/W1710751537', 'https://semopenalex.org/work/W2078770126', 'https://semopenalex.org/work/W1997210046', 'https://semopenalex.org/work/W2103982927', 'https://semopenalex.org/work/W2061236588', 'https://semopenalex.org/work/W4385473607', 'https://semopenalex.org/work/W4391272934', 'https://semopenalex.org/work/W2015180219', 'https://semopenalex.org/work/W1517590008', 'https://semopenalex.org/work/W1975513208', 'https://semopenalex.org/work/W1775494561', 'https://semopenalex.org/work/W2980176182', '2008', 'https://semopenalex.org/work/W2129825950', '2000', 'https://semopenalex.org/work/W2085609918', 'https://semopenalex.org/work/W2915945450', 'https://semopenalex.org/work/W2915030750', '2003', 'https://semopenalex.org/work/W4402442861', 'https://semopenalex.org/work/W1991332789', 'https://semopenalex.org/work/W3195402331', 'https://semopenalex.org/work/W1579677221', '2019', 'https://semopenalex.org/work/W2127281178', 'https://semopenalex.org/work/W4296041368', 'https://semopenalex.org/work/W1531484838', 'https://semopenalex.org/work/W2525118715', '1999', '1800', 'https://semopenalex.org/work/W4312240104', 'https://semopenalex.org/work/W2806131721', 'https://semopenalex.org/work/W4313563519', 'https://semopenalex.org/work/W2515946176', '2005', 'https://semopenalex.org/work/W3092639686', 'https://semopenalex.org/work/W2809114684', 'https://semopenalex.org/work/W2953255159', 'https://semopenalex.org/work/W2949504704', 'https://semopenalex.org/work/W2206340513', 'https://semopenalex.org/work/W1556803451', '1993', 'https://semopenalex.org/work/W2123904236', 'https://semopenalex.org/work/W2952092732', 'https://semopenalex.org/work/W4384155490', 'https://semopenalex.org/work/W2077394967', 'https://semopenalex.org/work/W1987557201', 'https://semopenalex.org/work/W1495962746', 'https://semopenalex.org/work/W1994977110', 'https://semopenalex.org/work/W2734789924', 'https://semopenalex.org/work/W4238210800', 'https://semopenalex.org/work/W2132574120', '1997', 'https://semopenalex.org/work/W2122811495', 'https://semopenalex.org/work/W36371468', 'https://semopenalex.org/work/W2171326679', 'https://semopenalex.org/work/W1511466363', 'https://semopenalex.org/work/W1537902892', 'https://semopenalex.org/work/W2523177018', 'https://semopenalex.org/work/W2139525797', '2012', 'https://semopenalex.org/work/W2008078972', '2010', 'https://semopenalex.org/work/W4324007121', 'https://semopenalex.org/work/W2522928308', '2002', 'https://semopenalex.org/work/W3138989164', 'https://semopenalex.org/work/W139130934', '2016', 'https://semopenalex.org/work/W2400762887', 'https://semopenalex.org/work/W2754252703', 'https://semopenalex.org/work/W3136236837', 'https://semopenalex.org/work/W1595761884', '1995', 'https://semopenalex.org/work/W4253646682', 'https://semopenalex.org/work/W4404057326', 'https://semopenalex.org/work/W1792464322', 'https://semopenalex.org/work/W1588297513', 'https://semopenalex.org/work/W2751928463', 'https://semopenalex.org/work/W2123889292', 'https://semopenalex.org/work/W144935353', 'https://semopenalex.org/work/W2173733616', 'https://semopenalex.org/work/W147488175', 'https://semopenalex.org/work/W1811359278', 'https://semopenalex.org/work/W2899402023', 'https://semopenalex.org/work/W1774324140', 'https://semopenalex.org/work/W3158293305', 'https://semopenalex.org/work/W1253240651', 'https://semopenalex.org/work/W2125383988', 'https://semopenalex.org/work/W48558007', 'https://semopenalex.org/work/W4393474997', 'https://semopenalex.org/work/W2115447277', 'https://semopenalex.org/work/W2581324891', 'https://semopenalex.org/work/W1975908943', 'https://semopenalex.org/work/W1475955015', 'https://semopenalex.org/work/W1798073562', 'https://semopenalex.org/work/W2520217242', 'https://semopenalex.org/work/W2008732772', 'https://semopenalex.org/work/W3137115172', 'https://semopenalex.org/work/W1579914521', '2023', 'https://semopenalex.org/work/W2104421582', 'https://semopenalex.org/work/W2778798134', 'https://semopenalex.org/work/W1679509962', 'https://semopenalex.org/work/W2747419197', 'https://semopenalex.org/work/W2047400318', 'https://semopenalex.org/work/W2520300422', 'https://semopenalex.org/work/W2103704182', 'https://semopenalex.org/work/W2778029444', 'https://semopenalex.org/work/W2779900466', '2006', 'https://semopenalex.org/work/W2101874499', '2009', 'https://semopenalex.org/work/W2094034408', '2004', 'https://semopenalex.org/work/W1550675824', 'https://semopenalex.org/work/W1978640117', 'https://semopenalex.org/work/W2912433096', 'https://semopenalex.org/work/W3108668383', 'https://semopenalex.org/work/W2012114748', 'https://semopenalex.org/work/W2008606555', 'https://semopenalex.org/work/W2612371455', 'https://semopenalex.org/work/W2044926733', 'https://semopenalex.org/work/W2039085252', 'https://semopenalex.org/work/W2181042156', 'https://semopenalex.org/work/W2011170798', 'https://semopenalex.org/work/W4387755431', 'https://semopenalex.org/work/W2130495724', 'https://semopenalex.org/work/W2071433880', 'https://semopenalex.org/work/W1593317697', 'https://semopenalex.org/work/W991450633', 'https://semopenalex.org/work/W1595752763', 'https://semopenalex.org/work/W2028893723', 'https://semopenalex.org/work/W2915009967', 'https://semopenalex.org/work/W4398191656', 'https://semopenalex.org/work/W1520649080', 'https://semopenalex.org/work/W3028360334', 'https://semopenalex.org/work/W2921648886', 'https://semopenalex.org/work/W4237909807', 'https://semopenalex.org/work/W2109952361', 'https://semopenalex.org/work/W1996454760', 'https://semopenalex.org/work/W1592700375', 'https://semopenalex.org/work/W1588734579', 'https://semopenalex.org/work/W2734788368', 'https://semopenalex.org/work/W2041544991', 'https://semopenalex.org/work/W2088263927', 'https://semopenalex.org/work/W1572167134', 'https://semopenalex.org/work/W1633377437', 'https://semopenalex.org/work/W2091478774', 'https://semopenalex.org/work/W4403628532', 'https://semopenalex.org/work/W4242041539', 'https://semopenalex.org/work/W4282583221', 'https://semopenalex.org/work/W2154282221', 'https://semopenalex.org/work/W3033698111', 'https://semopenalex.org/work/W2014199531', 'https://semopenalex.org/work/W115310691', 'https://semopenalex.org/work/W173156922', '2001', 'https://semopenalex.org/work/W1574950491', 'https://semopenalex.org/work/W52260594', 'https://semopenalex.org/work/W2189085557', '1994', 'https://semopenalex.org/work/W2928532935', 'https://semopenalex.org/work/W2466104094', 'https://semopenalex.org/work/W4406859981', 'https://semopenalex.org/work/W3009455989', 'https://semopenalex.org/work/W4249900482', 'https://semopenalex.org/work/W2949106240', 'https://semopenalex.org/work/W2963855145', 'https://semopenalex.org/work/W4298063358', 'https://semopenalex.org/work/W2400182190', 'https://semopenalex.org/work/W2123344956', '2014', 'https://semopenalex.org/work/W4242436304', '2013', 'https://semopenalex.org/work/W2118889869', 'https://semopenalex.org/work/W4292761028', 'https://semopenalex.org/work/W1570916159', 'https://semopenalex.org/work/W156157953', 'https://semopenalex.org/work/W2152544235', '2022', '2021', 'https://semopenalex.org/work/W2632860668', 'https://semopenalex.org/work/W3183165251', '2011', 'https://semopenalex.org/work/W2132155852', '2017', 'https://semopenalex.org/work/W2008620714', 'https://semopenalex.org/work/W371525118', 'https://semopenalex.org/work/W89291972', 'https://semopenalex.org/work/W4400976691', '1996', 'https://semopenalex.org/work/W4393943425', 'https://semopenalex.org/work/W2527377534', 'https://semopenalex.org/work/W2098211566', 'https://semopenalex.org/work/W2145761885', 'https://semopenalex.org/work/W2128127301', 'https://semopenalex.org/work/W2112609211', 'https://semopenalex.org/work/W2153339030', 'https://semopenalex.org/work/W2525395252', '2015', 'https://semopenalex.org/work/W2747898780', 'https://semopenalex.org/work/W2087840232', 'https://semopenalex.org/work/W2592423893', 'https://semopenalex.org/work/W2401057219', 'https://semopenalex.org/work/W4394555057', '2007', 'https://semopenalex.org/work/W1978847709', 'https://semopenalex.org/work/W1971941065', 'https://semopenalex.org/work/W2155935413', 'https://semopenalex.org/work/W2166938786', 'https://semopenalex.org/work/W1719093023', 'https://semopenalex.org/work/W1908231796', 'https://semopenalex.org/work/W2739356170', 'https://semopenalex.org/work/W2049801349', 'https://semopenalex.org/work/W2017269495', '2018', 'https://semopenalex.org/work/W3116695505', '2024', 'https://semopenalex.org/work/W1560854026', 'https://semopenalex.org/work/W4400939550', 'https://semopenalex.org/work/W2612962685', 'https://semopenalex.org/work/W2794546965', 'https://semopenalex.org/work/W4282576055', 'https://semopenalex.org/work/W1573454147', 'https://semopenalex.org/work/W205920923', 'https://semopenalex.org/work/W3216444132', '1998', 'https://semopenalex.org/work/W2055963247', 'https://semopenalex.org/work/W2958694015', 'https://semopenalex.org/work/W4393670548', 'https://semopenalex.org/work/W2609404595', 'https://semopenalex.org/work/W1501840263']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/source/S4306525036', 'Minimum variance power spectrum based calibration for improved clutter suppression in PCL on moving platforms', '&amp;lt;title&amp;gt;Passive radar prototypes for multifrequency target detection&amp;lt;/title&amp;gt;', 'Dual Channel Adaptive Antenna Nulling with Auxiliary Selection for Spaceborne Radar', 'Advanced Processing Methods for Passive Bistatic Radar Systems', 'https://semopenalex.org/source/S4306531480', 'Polarimetric Detection Scheme for Passive Radar based on a 2D Auto-Regressive Disturbance Model', 'Security enhancement in small private airports through active and passive radar sensors', 'Antenna Sidelobes Level Control in Transmit Subaperturing MIMO Radar', 'https://semopenalex.org/source/S10936095', 'DVB-T based Passive Bistatic Radar for maritime surveillance', 'Experimental results of polarimetric detection schemes for DVB‐T‐based passive radar', 'https://semopenalex.org/source/S4306418371', 'Forward-Looking Passive Radar With Non-Uniform Linear Array for Automotive Applications', 'VHF Cross-Range Profiling of Aerial Targets Via Passive ISAR: Signal Processing Schemes and Experimental Results', 'On the Use of Reciprocal Filter Against WiFi Packets for Passive Radar', 'Passive Radar: A Challenge Where Resourcefulness Is the Key to Success', 'Passive Radar STAP Detection and DoA Estimation Under Antenna Calibration Errors', 'Eco-friendly dual-band AULOS® passive radar for air and maritime surveillance applications', 'An apodization approach for passive GMTI Radar with Non-Uniform Linear Arrays', 'Exploiting Polarization together with Space-Time Adaptive Processing for GMTI in high resolution SAR images', 'Quasi-Monostatic Versus Near Forward Scatter Geometry in WiFi-Based Passive Radar Sensors', 'Fusing Measurements from Wi-Fi Emission-Based and Passive Radar Sensors for Short-Range Surveillance', 'Lagrange-Polynomial-Interpolation-Based Keystone Transform for a Passive Radar', 'Multi-carrier Adaptive Detection in Polarimetric Passive Radars', 'Performance Prediction of the Loaded Reciprocal Filter for OFDM-based Passive Radar', 'Experimental results for OFDM WiFi-based passive bistatic radar', 'https://semopenalex.org/source/S4306498246', 'https://semopenalex.org/source/S4306418812', '[Front matter]', 'Passive Radar: Past, Present, and Future Challenges', 'A Survey on Fundamental Limits of Integrated Sensing and Communication', 'Threshold Region Performance of Multicarrier Maximum Likelihood Direction of Arrival Estimator', 'Inside front cover', 'A spectral slope-based approach for mitigating bistatic STAP clutter dispersion', 'https://semopenalex.org/source/S4306400194', 'A fast disturbance cancellation scheme for orthogonal frequency division multiplexing‐based passive radar exploiting reciprocal filter', 'Optimization of multistatic passive radar geometry based on CRLB with uncertain observations', 'Exploiting long coherent integration times in DVB-T based passive radar systems', 'Outlier Rejection Approach for Direction of Arrival Estimation in Low SNR Conditions', 'https://semopenalex.org/source/S4306401280', 'https://semopenalex.org/source/S111326731', 'From the expected scientific applications to the functional specifications, products and performance of the SABRINA missions', 'A two-stage approach for direct signal and clutter cancellation in passive radar on moving platforms', 'Exploiting polarimetric diversity in passive radar', 'Facing channel calibration issues affecting passive radar DPCA and STAP for GMTI', 'Foreword to the Special Section on Innovations in Radar Spectrum', 'Passive radar components of ARGUS 3D', 'WiFi-Based Passive Bistatic Radar: Data Processing Schemes and Experimental Results', 'Autoregressive Model Based Polarimetric Adaptive Detection Scheme Part II: Performance Assessment Under Spectral Model Mismatch', 'Polarimetric Passive Radar: A Practical Approach to Parametric Adaptive Detection', 'https://semopenalex.org/source/S189694085', 'https://semopenalex.org/source/S3569471', 'Detection performance assessment of the FM-based AULOS® Passive Radar for air surveillance applications', 'Parasitic Exploitation of Wi-Fi Signals for Indoor Radar Surveillance', 'https://semopenalex.org/source/S4306463440', 'Experimental results for passive bistatic radar based on DVB-T signals', 'Tackling the different target dynamics issues in counter drone operations using passive radar', 'DVB-T-based passive radar for silent surveillance of drones', 'Autoregressive Model Based Polarimetric Adaptive Detection Scheme Part I: Theoretical Derivation and Performance Analysis', 'Range sidelobes reduction filters for WiFi-based passive bistatic radar', 'Experimental evaluation of Supervised Reciprocal Filter Strategies for OFDM-radar signal processing', 'Automatic vehicles classification approaches for WiFi-based Passive Forward Scatter Radar', 'PBR activity at INFOCOM: Adaptive processing techniques and experimental results', 'https://semopenalex.org/source/S4306400806', 'Exploiting polarimetric diversity to mitigate the effect of interferences in FM-based passive radar', 'Preliminary experimental results of polarimetric detection schemes for DVB-T based passive radar', 'https://semopenalex.org/source/S4387286330', 'https://semopenalex.org/source/S4306400024', 'Passive radar for GMTI', 'Exploitation of Long Coherent Integration Times to Improve Drone Detection in DVB-S based Passive Radar', 'Supervised DPCA Scheme Based on Reciprocal Filter for Clutter Cancellation From Moving OFDM Radar', 'Conclusion', 'https://semopenalex.org/source/S153794155', 'Passive radar detection of drones with staring illuminators of opportunity', 'A simple NULA design strategy for target detection and DoA estimation in mobile passive radar', 'Exploiting polarimetric diversity in FM-based PCL', 'Polarimetric passive coherent location', '2D Localization with WiFi Passive Radar and Device-Based Techniques: An Analysis of Target Measurements Accuracy', 'Potentialities and challenges of WiFi-based passive radar', 'https://semopenalex.org/source/S4363608355', 'Foreword to the Special Section on Fully Digital Arrays for Radar', 'Multifrequency integration in FM radio-based passive bistatic radar. Part II: Direction of arrival estimation', "This Month's Covers....", 'WiFi emission-based vs passive radar localization of human targets', 'Polarimetric diversity in reference-free amplitude-based Wi-Fi sensing', 'IEEE aerospace &amp;amp; electronic systems society organization 2019', 'From the EiC: The IEEE Radar Journal is Born', 'Dual Cancelled Channel STAP for Target Detection and DOA Estimation in Passive Radar', 'Cramér‐Rao lower bound with &lt;i&gt;P&lt;/i&gt; &lt;sub&gt;d&lt;/sub&gt; &amp;lt; 1 for target localisation accuracy in multistatic passive radar', 'Passive Detection Using a Staring Radar Illuminator of Opportunity', 'Reference-free Amplitude-based WiFi Passive Sensing', 'Two‐dimensional location of moving targets within local areas using WiFi‐based multistatic passive radar', 'Impact of Beacon Interval on the performance of WiFi-based passive radar against human targets', 'https://semopenalex.org/source/S23688054', 'Spectral slope-based approach for mitigating bistatic space-time adaptive processing clutter dispersion', 'https://semopenalex.org/source/S4210215198', 'Multistatic passive radar geometry optimization for target 3D positioning accuracy', 'Ambiguity Function analysis of WiMAX transmissions for passive radar', 'Passive Radar DPCA Schemes With Adaptive Channel Calibration', 'https://semopenalex.org/source/S4306420046', 'DVB-T based Forward Scatter Radar for Small Target Surveillance', 'https://semopenalex.org/source/S4306402478', 'Enhanced WiFi-based passive ISAR for indoor and outdoor surveillance', 'https://semopenalex.org/source/S4377196266', 'https://semopenalex.org/source/S161080992', 'A Flexible Design Strategy for Three-Element Non-Uniform Linear Arrays', 'Passive Bistatic Radar based on mixed DSSS and OFDM WiFi transmissions', 'DVB‐T based passive radar for simultaneous counter‐drone operations and civil air traffic surveillance', 'Non-linear and adaptive two-dimensional FIR filters for STAP theory and experimental results', 'Computationally effective range migration compensation in PCL systems for maritime surveillance', 'Reduced Order Jammer Cancellation Scheme Based on Double Adaptivity', 'First experimental results for a WiFi-based passive forward scatter radar', 'Performance analysis of a multi-frequency FM based Passive Bistatic Radar', 'Monitoring and surveillance potentialities obtained by splitting the antenna of the COSMO-SkyMed SAR into multiple sub-apertures', 'Passive STAP approaches for GMTI', 'A reduced order jammer cancellation scheme based on double adaptivity', 'A procedure for effective receiver positioning in multistatic passive radar', 'https://semopenalex.org/source/S4306420045', 'Direction of arrival estimation performance comparison of dual cancelled channels space–time adaptive processing techniques', 'Sliding extensive cancellation algorithm for disturbance removal in passive radar', 'Effect of Apodization on SAR Image Understanding', 'A new approach for DVB-T Cross-Ambiguity Function evaluation', 'WiFi-based passive ISAR for high resolution cross-range profiling of moving targets', 'Integrated clutter cancellation and high-resolution imaging of moving targets in Multi-channel SAR', 'EuMW 2022 Special Issue', 'OFDM based WiFi Passive Sensing: a reference-free non-coherent approach', 'https://semopenalex.org/source/S4210193624', 'https://semopenalex.org/source/S141761900', 'https://semopenalex.org/source/S4363608562', 'Exploiting the Properties of Reciprocal Filter in Low-Complexity OFDM Radar Signal Processing Architectures', 'Space-based passive radar enabled by the new generation of geostationary broadcast satellites', 'https://semopenalex.org/source/S4306418573', 'Multi-frequency polarimetric target detection in FM-based passive radar', 'Enabling DPCA via Supervised Reciprocal Filter in OFDM Radar Onboard Moving Platforms', 'https://semopenalex.org/source/S4363608006', 'Passive radar in the high frequency band', 'A Multistage Processing Algorithm for Disturbance Removal and Target Detection in Passive Bistatic Radar', 'WiFi-Based Passive ISAR for High-Resolution Cross-Range Profiling of Moving Targets', 'Space–time constant modulus algorithm for multipath removal on the reference signal exploited by passive bistatic radar', 'Analysis and Emulation of FM Radio Signals for Passive Radar', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S101949793', 'Multi‐carrier and multi‐polarimetric model based adaptive target detector for passive radar systems', 'Disturbance removal in passive radar via sliding extensive cancellation algorithm (ECA-S)', 'Efficient Detection and Imaging of Moving Targets in SAR Images Based on Chirp Scaling', 'Antenna Array for Passive Radar: Configuration Design and Adaptive Approaches to Disturbance Cancellation', 'Localization and tracking of moving targets with WiFi-based passive radar', 'https://semopenalex.org/source/S4404663355', 'Target DoA estimation in passive radar using non-uniform linear arrays and multiple frequency channels', 'Reducing the computational complexity of WiFi-based passive radar processing', 'Ambiguity Function Analysis of Wireless LAN Transmissions for Passive Radar', 'Low-cost solutions for mobile passive radar based on multichannel DPCA and NULA configurations', 'Adaptive beamforming for high-frequency over-the-horizon passive radar', 'Microphone array based classification for security monitoring in unstructured environments', 'https://semopenalex.org/source/S4210171417', 'https://semopenalex.org/source/S4377196107', 'Multiband passive radar for drones detection and localization', 'A simple clutter suppression approach for OFDM-based passive radar exploiting reciprocal filter', 'https://semopenalex.org/source/S193624734', 'Passive radar concept for automotive applications', 'Exploiting the joint distribution of amplitude and monopulse ratio for chi-square fluctuating targets for target DOA estimation', 'Short-range passive radar for small private airports surveillance', 'A practical approach to polarimetric adaptive target detection in Passive Radar', 'Reciprocal-Filter-Based STAP for Passive Radar on Moving Platforms', 'Multifrequency integration in FM radio-based passive bistatic radar. Part I: Target detection', 'Clutter Suppression Using Thresholded Reciprocal Filter in OFDM Radar', 'https://semopenalex.org/source/S153101029', 'Maritime surveillance via multi-frequency DVB-T based passive radar', 'Stand-alone WiFi-based Passive Forward Scatter Radar sensor for vehicles classification', 'Comparing reference‐free WiFi radar sensing approaches for monitoring people and drones', 'Using real data for the implementation of multistatic passive radar geometry optimization procedure', 'DVB-S based Passive Radar for Short Range Security Application', 'Supervised Reciprocal Filter for OFDM Radar Signal Processing', 'Loaded Reciprocal Filter for OFDM-based Passive Radar Signal Processing', 'DVB-T-Based Passive Forward Scatter Radar: Inherent Limitations and Enabling Solutions', 'https://semopenalex.org/source/S183492911', 'Foreword to the Special section on Advances in Radar Imaging', 'A Study for a Space-Based Passive Multi-Channel SAR', 'https://semopenalex.org/source/S4306402512', 'Multi-Frequency Target Detection Techniques for DVB-T Based Passive Radar Sensors', 'https://semopenalex.org/source/S2764455111', 'Parasitic Surveillance Potentialities Based on a GEO-SAR Illuminator', 'Short-range passive radar potentialities', 'https://semopenalex.org/source/S4210172892', 'Non‐coherent adaptive detection in passive radar exploiting polarimetric and frequency diversity', 'Comparison of Clutter and Multipath Cancellation Techniques for Passive Radar', 'Dual adaptive channel STAP: Theory and experimental results', 'Simultaneous short and long range surveillance of drones and aircrafts with DVB-T based Passive Radar', 'https://semopenalex.org/source/S43295729', 'Impact of synchronization on the ambiguity function shape for PBR based on DVB-T signals', 'WiFi-based PCL for monitoring private airfields', 'Detection and 3D localization of ultralight aircrafts and drones with a WiFi-based Passive Radar', 'Comparing phase-locked and non-phase-locked architectures for dual-channel DVB-S passive radar', 'High resolution cross-range profiling with Passive Radar via ISAR processing', 'DVB-T Signal Ambiguity Function Control for Passive Radars', 'A Three-Stage Inter-Channel Calibration Approach for Passive Radar on Moving Platforms Exploiting the Minimum Variance Power Spectrum']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/source/S4306525036', 'https://semopenalex.org/source/S147316732', 'A Globally Optimal Energy-Efficient Power Control Framework and Its Efficient Implementation in Wireless Interference Networks', 'https://semopenalex.org/source/S4306400562', 'https://semopenalex.org/source/S4363608593', 'https://semopenalex.org/source/S173102057', 'Multi-User Frequency Assignment for Ultra-Reliable mmWave Two-Ray Channels', 'https://semopenalex.org/source/S4210214273', 'Bounds on the Outage Probability in Dependent Rayleigh Fading Channels', 'Neural Network Wiretap Code Design for Multi-Mode Fiber Optical Channels', 'https://semopenalex.org/source/S63459445', 'Bounds on the Ergodic Secret-Key Capacity for Dependent Fading Channels.', 'Building Resilience in Wireless Communication Systems With a Secret-Key  Budget', 'Non-Convex Optimization of Energy Efficient Power Control in Interference Networks via Machine Learning', 'On Fading Channel Dependency Structures with a Positive Zero-Outage Capacity', 'Reinforcement Learning Based Dynamic Power Control for UAV Mobility Management', 'https://semopenalex.org/source/S4363608623', 'A Simple Frequency Diversity Scheme for Ultra-Reliable Communications in Ground Reflection Scenarios', 'Frequency Diversity for Ultra-Reliable and Secure Communications in Sub-THz Two-Ray Scenarios', 'Hierarchical Multi-Agent DRL Based Dynamic Cluster Reconfiguration for  UAV Mobility Management', 'QMKPy: A Python Testbed for the Quadratic Multiple Knapsack Problem', 'Artificial Fast Fading from Reconfigurable Surfaces Enables Ultra-Reliable Communications', 'On Fading Channel Dependency Structures With a Positive Zero-Outage Capacity', 'Bounds on the Secrecy Outage Probability for Dependent Fading Channels', 'Deep Learning Based Resource Allocation: How Much Training Data is Needed?', 'Calculation of Bounds on the Ergodic Capacity for Fading Channels with Dependency Uncertainty', 'https://semopenalex.org/source/S4210218516', 'Flexible Design of Finite Blocklength Wiretap Codes by Autoencoders', 'Learning Based Dynamic Cluster Reconfiguration for UAV Mobility Management with 3D Beamforming', 'https://semopenalex.org/source/S4306400194', 'On the Zero-Outage Secrecy-Capacity of Dependent Fading Wiretap Channels', 'Machine Learning Assisted Wiretapping', 'Reconfigurable Intelligent Surface Phase Hopping for Ultra-Reliable Communications', 'Reliable Communications Over Dependent Fading Wireless Channels.', 'https://semopenalex.org/source/S4393179698', 'https://semopenalex.org/source/S4306401280', 'Measurements of Wiretap Encoded Image Transmissions over Multi-Mode Fibers', 'Reliability Bounds for Dependent Fading Wireless Channels', 'https://semopenalex.org/source/S195231649', 'Reliability and Latency Analysis for Wireless Communication Systems with a Secret-Key Budget', 'https://semopenalex.org/source/S4363607702', 'Achievable Physical-Layer Secrecy in Multi-Mode Fiber Channels using Artificial Noise', 'An efficient frequency diversity scheme for ultra-reliable communications in two-path fading channels', 'Distributed Combinatorial Optimization of Downlink User Assignment in  mmWave Cell-free Massive MIMO Using Graph Neural Networks', 'https://semopenalex.org/source/S4306534978', 'RISnet: A Domain-Knowledge Driven Neural Network Architecture for RIS  Optimization with Mutual Coupling and Partial CSI', 'Approaching Globally Optimal Energy Efficiency in Interference Networks via Machine Learning', 'Securing Data in Multimode Fibers by Exploiting Mode-Dependent Light Propagation Effects', 'https://semopenalex.org/source/S4363607711', 'Reliability and Latency Analysis for Wireless Communication Systems With a Secret-Key Budget', 'Optimal Resource Allocation for Loss-Tolerant Multicast Video Streaming', 'https://semopenalex.org/source/S61310614', 'Reinforcement Learning-Based Global Programming for Energy Efficiency in Multi-Cell Interference Networks', 'https://semopenalex.org/source/S4363607705', 'RISnet: A Scalable Approach for Reconfigurable Intelligent Surface Optimization with Partial CSI', 'Learning Based Dynamic Cluster Reconfiguration for UAV Mobility  Management with 3D Beamforming', 'Copula-Based Bounds for Multi-User Communications–Part I: Average Performance', 'https://semopenalex.org/source/S2764455111', 'Wiretap Code Design by Neural Network Autoencoders', 'https://semopenalex.org/source/S196647941', 'https://semopenalex.org/source/S4306402636', 'https://semopenalex.org/source/S168680287', 'Outage Probability Calculation for Two-Ray Ground Reflection Scenarios with Frequency Diversity', 'https://semopenalex.org/source/S4306402617', 'On the Set of Joint Rayleigh Fading Distributions Achieving Positive Zero-Outage Capacities', 'Copula-Based Bounds for Multi-User Communications–Part II: Outage Performance', 'Reliability and Latency of Wireless Communication Systems with a Secret-Key Budget']</t>
+  </si>
+  <si>
+    <t>['A self-equilibrium Friedman-like urn via stochastic approximation', 'https://semopenalex.org/source/S985303', 'Age statistics in the Moran population model', 'The size of random bucket trees via urn models', 'Some properties of exponential trees', 'https://semopenalex.org/source/S4210186879', 'Analytic variations on bucket selection and sorting', 'Survivors in leader election algorithms', 'Distances in random digital search trees', 'The Department of Statistics at The George Washington University', 'Imbalance in Random Digital Trees', 'On the Most Probable Shape of a Search Tree Grown from a Random Permutation', 'On the joint distribution of the insertion path length and the number of comparisons in search trees', 'Degrees in random $m$-ary hooking networks', 'Probabilistic Analysis of MULTIPLE QUICK SELECT', 'A stochastic model for solitons', 'A Limit Law for Outputs in Random Recursive Circuits', 'Random sprouts as internet models, and P�lya processes', 'https://semopenalex.org/source/S164906323', 'The Power of Choice in the Construction of Recursive Trees', 'https://semopenalex.org/source/S4210182901', 'Limit laws for the Randić index of random binary tree models', 'Polya Urn Models', 'The class of tenable zero-balanced Pólya urns with an initially dominant subset of colors', 'Insertion depth in power-weight trees', 'Egorychev Method: A Hidden Treasure', 'https://semopenalex.org/source/S165473669', 'https://semopenalex.org/source/S44643521', 'ON THE COMBINATORICS OF BINARY SERIES-PARALLEL GRAPHS', 'https://semopenalex.org/source/S4306417669', 'Degrees in random self-similar bipolar networks', 'Winning a Tournament According to Bradley-Terry Probability Model', 'On nodes of small degrees and degree profile in preferential dynamic attachment circuits', 'Two-color balanced affine urn models with multiple drawings II: large-index and triangular urns', 'On generalized Pólya urn models', 'https://semopenalex.org/source/S2765029694', 'Probabilistic analysis of maximal gap and total accumulated length in interval division', 'https://semopenalex.org/source/S4306400194', 'Distribution of the size of random hash trees, pebbled hash trees and N-trees', 'Exact Covariances and Refined Asymptotics in Dichromatic Tenable Balanced Polya Urn Schemes', 'https://semopenalex.org/source/S9093621', 'Analysis of a generalized Friedman’s urn with multiple drawings', 'https://semopenalex.org/source/S84409463', 'An Efficiency Robust Nonparametric Test for Scale Change for Data from a Gamma Distribution', 'https://semopenalex.org/source/S4306401280', 'Asymptotic Properties of Protected Nodes in Random Recursive Trees', 'https://semopenalex.org/source/S4210234901', 'Balancing m-ary search trees with compressions on the fringe', 'Average-Case Analysis of Cousins in m-ary Tries', 'Covariances in Pólya urn schemes', 'The continuous-time triangular Pólya process', 'EXTREMAL WEIGHTED PATH LENGTHS IN RANDOM BINARY SEARCH TREES', 'Distributions in a class of Poissonized urns with an application to Apollonian networks', 'Asymptotic distribution of two-protected nodes in random binary search trees', 'https://semopenalex.org/source/S4306402264', 'https://semopenalex.org/source/S4306463075', 'Distribution of inter-node distances in digital trees', 'Exact Covariances and Refined Asymptotics in Dichromatic Tenable Balanced Pólya Urn Schemes', 'مدلهای آوند پولیاگونه با برداشتهای چندگانه', 'On rotations in fringe-balanced binary trees', 'Throughput analysis in wireless networks with multiple users and multiple channels', 'Affine Diminishing Urns', 'https://semopenalex.org/source/S59667848', 'Degrees in random &lt;mml:math xmlns:mml=http://www.w3.org/1998/Math/MathML&gt;&lt;mml:mi&gt;m&lt;/mml:mi&gt;&lt;/mml:math&gt;-ary hooking networks', 'Pólya urns: Probabilistic analysis and statistical questions', 'The joint distribution of the three types of nodes in uniform binary trees', 'https://semopenalex.org/source/S4306463019', 'Polya Urn Models and Connections to Ran- dom Trees: A Review', 'https://semopenalex.org/source/S4306402042', 'Polya-Type Urn Models with Multiple Drawings', 'The Class of Tenable Zero-Balanced Pólya Urn Schemes: Characterization and Gaussian Phases', 'Analysis of quickselect : an algorithm for order statistics', 'Local and global degree profiles of randomly grown self-similar hooking networks under uniform and preferential attachment', 'The Expected Distribution of Degrees in Random Binary Search Trees', 'https://semopenalex.org/source/S200334879', 'https://semopenalex.org/source/S4306463230', 'JISC: Adaptive stream processing using just-in-time state completion?', 'https://semopenalex.org/source/S160779208', 'https://semopenalex.org/source/S23873141', 'The Sackin index and depth of leaves in generalized Schröder trees', 'On the Variety of Shapes on the Fringe of a Random Recursive Tree', 'Toward a Formal Derivation of the Expected Behavior of Prefix &lt;i&gt;B&lt;/i&gt;-Trees', 'An Urn Model for Population Mixing and the Phases Within', 'Distributions in the constant-differentials Pólya process', 'ON CLIMBING TRIES', 'Distribution of distances in random binary search trees', 'Profile of Random Exponential Recursive Trees', 'https://semopenalex.org/source/S4386872458', 'The containment profile of hyperrecursive trees', 'Phases in the two-color tenable zero-balanced Pólya process', 'One-sided variations on binary search trees', 'https://semopenalex.org/source/S6941720', 'https://semopenalex.org/source/S4210224136', 'Analysis of Quickselect Under Yaroslavskiy’s Dual-Pivoting Algorithm', 'Dynamic Pólya–Eggenberger urns', 'Oツリー,Bツリー,接頭Bツリーのストレージのオーバーヘッド 比較分析', 'DEGREE PROFILE OF HIERARCHICAL LATTICE NETWORKS', 'Phase Changes in Subtree Varieties in Random Recursive and Binary Search Trees', 'BUILDING RANDOM TREES FROM BLOCKS', 'A Strong Law for the Height of Random Binary Pyramids', 'Some empirical and theoretical attributes of random multi-hooking networks', 'DEGREE PROFILE OF &lt;i&gt;m&lt;/i&gt;-ARY SEARCH TREES: A VEHICLE FOR DATA STRUCTURE COMPRESSION', 'Correction to: Egorychev Method: A Hidden Treasure', 'Exact and limiting distributions in diagonal Pólya processes', 'On the distribution for the duration of a randomized leader election algorithm', 'Bivariate Issues in Leader Election Algorithms with Marshall-Olkin Limit Distribution', 'Profile of Random Exponential Binary Trees', 'Asymptotic Properties of a Leader Election Algorithm', 'Analysis of swaps in radix selection', 'https://semopenalex.org/source/S989097277', 'Random networks grown by fusing edges via urns', 'Exact and Limiting Distributions in Diagonal Pólya Processes', 'On the variety of shapes in digital trees', 'Two-colour balanced affine urn models with multiple drawings I: central limit theorems', 'Asymptotic Joint Normality of Outdegrees of Nodes in Random Recursive Trees', 'https://semopenalex.org/source/S156280010', 'The degree profile and weight in Apollonian networks and &lt;i&gt;k&lt;/i&gt;-trees', 'https://semopenalex.org/source/S18902827', 'The continuum Pólya-like random walk', 'BERNOULLI CONVOLUTION OF THE DEPTH OF NODES IN RECURSIVE TREES WITH GENERAL AFFINITIES', 'Phases in the Diffusion of Gases via the Ehrenfest URN Modelx', 'Affine diminishing urns', 'DRAWING MULTISETS OF BALLS FROM TENABLE BALANCED LINEAR URNS', 'https://semopenalex.org/source/S180803011', 'A multivariate view of random bucket digital search trees', 'Problems and Solutions', 'Characterization and Enumeration of Certain Classes of Tenable Pólya Urns Grown by Drawing Multisets of Balls', 'Average measures in polymer graphs', 'https://semopenalex.org/source/S2530642067', 'One-sided Variations on Tries: Path Imbalance, Climbing, and Key Sampling', 'Limiting Distributions for Path Lengths in Recursive Trees', 'The Degree Profile in Some Classes of Random Graphs that Generalize Recursive Trees', 'Random multi-hooking networks', 'On the structure of random plane‐oriented recursive trees and their branches', 'On affine multi-color urns grown under multiple drawing', 'The Gini index of random trees with an application to caterpillars', 'https://semopenalex.org/source/S94688346', 'https://semopenalex.org/source/S4393179698', 'The Joint Distribution of Elastic Buckets in Multiway Search Trees', 'Statistical Inequalities', 'https://semopenalex.org/source/S117679221', 'The Degree Gini Index of Several Classes of Random Trees and Their Poissonized Counterparts�Evidence for Duality', 'Asymptotic Joint Normality of Counts of Uncorrelated Motifs in Recursive Trees', 'On the average internal path length of m-ary search trees', 'The oscillatory distribution of distances in random tries', 'https://semopenalex.org/source/S4306463937', 'https://semopenalex.org/source/S4306418406', 'An index for betting with examples from games and sports', 'On the Distribution of Leaves in Rooted Subtrees of Recursive Trees', 'On the internal structure of random recursive circuits', 'https://semopenalex.org/source/S153560523', 'The class of tenable zero-balanced Pólya urn schemes: characterization and Gaussian phases', 'https://semopenalex.org/source/S7571225', 'Algorithmics of Nonuniformity', 'On the Variety of Shapes in Digital Trees', 'https://semopenalex.org/source/S147953040', 'https://semopenalex.org/source/S2764830807', 'https://semopenalex.org/source/S110520077', 'SOME NODE DEGREE PROPERTIES OF SERIES–PARALLEL GRAPHS EVOLVING UNDER A STOCHASTIC GROWTH MODEL', 'Explicit characterization of moments of balanced triangular Pólya urns by an elementary approach', 'Corrigendum', 'STORAGE OVERHEAD OF O-TREES, B-TREES AND PREFIX B-TREES: A COMPARATIVE ANALYSIS', 'Paths in &lt;mml:math xmlns:mml=http://www.w3.org/1998/Math/MathML altimg=si2.gif overflow=scroll&gt;&lt;mml:mi&gt;m&lt;/mml:mi&gt;&lt;/mml:math&gt;-ary interval trees', 'Exactly Solvable Balanced Tenable Urns with Random Entries via the Analytic Methodology', "Mixed distributions in Sattolo's algorithm for cyclic permutations via randomization and derandomization", 'https://semopenalex.org/source/S90727058', 'Two-color balanced affine urn models with multiple drawings', 'Analysis of an Algorithm for Random Sampling', 'https://semopenalex.org/source/S68047077', 'Distances in random plane-oriented recursive trees', 'Bar Bets and Generating Functions: The Distribution of the Separation of Two Distinct Card Ranks', 'Analysis of Boyer-Moore-Horspool string-matching heuristic', 'Limit laws for terminal nodes in random circuits with restricted fan-out: a family of graphs generalizing binary search trees', 'An Efficiency Robust Nonparametric Test for Scale Change for Data From a Gamma Distribution', 'https://semopenalex.org/source/S9424914', 'https://semopenalex.org/source/S203441484', 'https://semopenalex.org/source/S4210191297', 'Sorting 1-away permutations with underlying Fibonacci convolutions', 'https://semopenalex.org/source/S171741597', 'Distributions in the Ehrenfest process', 'https://semopenalex.org/source/S128350725', 'DEGREE-BASED GINI INDEX FOR GRAPHS', 'https://semopenalex.org/source/S2764412775', 'Probabilistic analysis of bucket recursive trees', 'https://semopenalex.org/source/S193011845', 'Average-case analysis of multiple Quickselect: An algorithm for finding order statistics', 'On the Joint Behavior of Types of Coupons in Generalized Coupon Collection', 'The containment profile of hyper-recursive trees', 'https://semopenalex.org/source/S4306536558', 'https://semopenalex.org/source/S89324355', 'On tree-growing search strategies', 'Trees grown under young-age preferential attachment', 'On Nodes of Small Degrees and Degree Profile in Preferential Dynamic Attachment Circuits', 'A SPECTRUM OF SERIES–PARALLEL GRAPHS WITH MULTIPLE EDGE EVOLUTION', 'Limit distribution of distances in biased random tries', 'A model for the spreading of fake news', 'https://semopenalex.org/source/S4306400349', 'https://semopenalex.org/source/S4210215866', 'Analysis of the space of search trees under the random insertion algorithm', 'https://semopenalex.org/source/S4306400744', 'https://semopenalex.org/source/S4306402441', 'https://semopenalex.org/source/S4306402512', 'Distributional analysis of swaps in Quick Select', 'https://semopenalex.org/source/S150892397', 'Estimating the Pólya process', 'One-sided variations on interval trees', 'https://semopenalex.org/source/S177771411', 'Gaussian phases in generalized coupon collection', 'https://semopenalex.org/source/S4210172589', 'https://semopenalex.org/source/S170765028', 'SOME PROPERTIES OF BINARY SERIES-PARALLEL GRAPHS', 'The degree Gini index of several classes of random trees and their poissonized counterparts---an evidence for a duality theory', 'Perpetuities in Fair Leader Election Algorithms', 'https://semopenalex.org/source/S4377196372', 'On affine multicolor urns grown under multiple drawing', 'Depths in hooking networks']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/source/S4210179225', 'https://semopenalex.org/source/S4306525036', 'Technology for societal change: Evaluating a mobile app addressing the emotional needs of people experiencing homelessness', 'Using a digital personal recovery resource in routine mental health practice: feasibility, acceptability and outcomes', 'https://semopenalex.org/source/S4210211086', 'https://semopenalex.org/source/S112414500', 'https://semopenalex.org/source/S34944277', 'https://semopenalex.org/source/S4210212400', 'Motivational models for validating agile requirements in Software Engineering subjects', 'Understanding Confidence of Older Adults for Embracing Mobile Technologies', 'https://semopenalex.org/source/S4306402621', 'https://semopenalex.org/source/S4306401600', 'https://semopenalex.org/source/S4306463409', 'Evaluating Engagement in Technology-Supported Social Interaction by People Living with Dementia in Residential Care', 'Interdisciplinary Design Teams Translating Ethnographic Field Data Into Design Models', 'https://semopenalex.org/source/S4306400572', 'Editorial: Designing Technology for Emotions to Improve Mental Health and Wellbeing', 'Using Motivational Modelling With an App Designed to Increase Student Performance and Retention', 'https://semopenalex.org/source/S201800618', 'Weisst Du wieviel Sternlein stehen? – Building older adults’ confidence in technology use through co-designing digital storytelling', 'Designing Meaningful, Beneficial and Positive Human Robot Interactions with Older Adults for Increased Wellbeing During Care Activities', 'Emotional Factors for Teleaudiology', 'https://semopenalex.org/source/S89276529', 'https://semopenalex.org/source/S4306400194', 'Adding Emotions to Models in a Viewpoint Modelling Framework From Agent-Oriented Software Engineering', 'https://semopenalex.org/source/S4393179698', 'Brainstorm', 'A Co-design Approach for Developing and Implementing Smart Health Technologies and Services']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/source/S4306525036', 'https://semopenalex.org/source/S4363604921', 'Freezing of gait in Parkinson’s disease: Classification using computational intelligence', 'Evolutionary Computation', 'https://semopenalex.org/source/S4210218191', 'Dungeons, Dragons, and Data Breaches: Analyzing AI Attacks on Various Network Configurations', 'AI Versus Epidemics', 'https://semopenalex.org/source/S4210216571', 'All lockdowns are not equal: Reducing epidemic impact through evolutionary computation', 'Network Induction Issues', 'What Drives Evolution of Self-Driving Automata?', 'Network Induction', 'Conference Report on 2022 IEEE Conference on Computational Intelligence in Bioinformatics and Computational Biology (IEEE CIBCB 2022) [Conference Report]', '2022 IEEE conference on computational intelligence in bioinformatics and computational biology (IEEE CIBCB, 2022)', 'https://semopenalex.org/source/S4363605353', 'https://semopenalex.org/source/S99347777', 'https://semopenalex.org/source/S104797584', 'Vaccine Distribution', 'A multi-objective genetic algorithm for compression of weighted graphs to simplify epidemic analysis', 'Promoting Diversity in the Evolution of Biological Sequence Data', 'Graph Compression', 'https://semopenalex.org/source/S140556538', 'Introduction']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/source/S4306525036', 'https://semopenalex.org/source/S2764607890', 'https://semopenalex.org/source/S4306401629', 'https://semopenalex.org/source/S4210183703', 'Rancang Bangun Purwarupa Pemilah Sampah Pintar Berbasis Deep Learning', 'Effect of CLAHE-based Enhancement on Bean Leaf Disease Classification through Explainable AI', 'https://semopenalex.org/source/S4210205812', 'https://semopenalex.org/source/S4210196574', 'https://semopenalex.org/source/S4210187594', 'Augmentation of Additional Arabic Dataset for Jawi Writing and Classification Using Deep Learning', 'Moving Object Detection for Complex Scenes by Merging BG Modeling and Deep Learning Method', 'Performance Evaluation of Binary Classification of Diabetic Retinopathy through Deep Learning Techniques using Texture Feature', 'Pendeteksian Septoria pada Tanaman Tomat dengan Metode Deep Learning berbasis Raspberry Pi', 'Performance Evaluation of Hardhat Image Classification Using Deep Learning and Grad-CAM', 'Comparison Study of Corn Leaf Disease Detection based on Deep Learning YOLO-v5 and YOLO-v8', 'Comparative analysis of deep learning models for detecting face mask', 'An Edge AI-Powered Defect Coffee Detector Using Streamlit Web App', 'https://semopenalex.org/source/S4363607821', 'Performance Evaluation And Analysis of LBP Utilization In Face Spoofing Detection With Deep Learning', 'Embedded-based Tomato Septoria Leaf Detection with Intel Movidius Neural Compute Stick', 'Substraksi Latar Menggunakan Nilai Mean Untuk Klasifikasi Kendaraan Bergerak Berbasis Deep Learning', 'https://semopenalex.org/source/S4210179954', 'Improved Classification of Handwritten Jawi Script Based on Main Part of Script Body', 'Web-App based Melanoma Skin Cancer Classification through Streamlit and Deep Learning', 'https://semopenalex.org/source/S4306417765', 'Impact of Image Pre-Processing on Skin Cancer Classification Melanoma Through Deep Learning', 'A Deep Learning Method for Early Detection of Diabetic Foot Using Decision Fusion and Thermal Images', 'https://semopenalex.org/source/S4363606538', 'Identification of male and female nutmeg seeds based on the shape and texture features of leaf images using the learning vector quantization (LVQ)', 'https://semopenalex.org/source/S120348307', 'Moving Pedestrian Localization and Detection With Guided Filtering', 'Comparative Study of Deep Learning Methods through Improvement of Skin Image Quality of Basal Cell Carcinoma', 'https://semopenalex.org/source/S2737955091', 'Performance Evaluation of Binary Classification of Tuberculosis through Unsharp Masking and Deep Learning Technique', 'Perbandingan Kinerja Deep Learning Dalam Pendeteksian Kerusakan Biji Kopi', 'https://semopenalex.org/source/S30680879', 'Convolutional Network and Moving Object Analysis for Vehicle Detection in Highway Surveillance Videos', 'https://semopenalex.org/source/S4306498607', 'Image Enhancement for Tuberculosis Detection Using Deep Learning', 'Students’ emotion classification system through an ensemble approach', 'A Low-cost Raspberry Pi and Deep Learning System for Customer Analysis', 'https://semopenalex.org/source/S2764455111', 'Performance evaluation of hyper-parameter tuning automation in YOLOV8 and YOLO-NAS for corn leaf disease detection', 'Deep anomaly detection through visual attention in surveillance videos', 'Performance Evaluation of Coffee Bean Binary Classification Through Deep Learning Techniques', 'https://semopenalex.org/source/S4363607800', 'https://semopenalex.org/source/S4210223945', 'https://semopenalex.org/source/S4210230916', 'Streamlit Application for Helmet Detection Based on YOLOS: Case Study Indonesia', 'Utilizing Edge Device and Streamlit for Comparative Evaluation of CLAHE-Based Underwater Image Enhancement Techniques', 'https://semopenalex.org/source/S4210178035', 'Lightweight Pedestrian Detection through Guided Filtering and Deep Learning', 'Impact of CLAHE-based image enhancement for diabetic retinopathy classification through deep learning', 'https://semopenalex.org/source/S4210198570', 'https://semopenalex.org/source/S4306401280', 'Hybrid Models for Emotion Classification and Sentiment Analysis in Indonesian Language', 'https://semopenalex.org/source/S2485537415']</t>
+  </si>
+  <si>
+    <t>['W. R. OWENS, STUART SIM, AND DAVID WALKER, EDS. BUNYAN STUDIES: A JOURNAL OF REFORMATION AND NONCONFORMIST CULTURE. NUMBER 22. NORTHUMBRIA UNIVERSITY, 2018. PP. 164.', 'Rotten green tests in Java, Pharo and Python', 'https://semopenalex.org/source/S109852484', 'https://semopenalex.org/source/S4363604151', 'Pope and the Reformation of the Oral: The Iliad in the History of Mediation', 'Advances in monitoring carbon dioxide exchange between the atmosphere and mine waste derived from ultramafic-hosted mineral deposits; a pilot study at Cassiar, B.C.', 'The Secret History of HB-2: Bathroom Safety in the Eighteenth Century and Beyond', 'https://semopenalex.org/source/S73505065', 'https://semopenalex.org/source/S4306463865', 'https://semopenalex.org/source/S4210192127', 'Rotten Green Tests in Java, Pharo and Python', 'https://semopenalex.org/source/S4306402512', 'https://semopenalex.org/source/S4306462979', 'https://semopenalex.org/source/S4377196300', 'https://semopenalex.org/source/S4306402203', 'W. R. Owens, Stuart Sim, and David Walker, eds. Bunyan Studies: A Journal of Reformation and Nonconformist Culture']</t>
   </si>
   <si>
     <t>['true']</t>
   </si>
   <si>
-    <t>['https://semopenalex.org/work/W3029899401', 'https://semopenalex.org/work/W4324150573', 'https://semopenalex.org/work/W3193396842', 'https://semopenalex.org/work/W2736312195', 'https://semopenalex.org/work/W2752493326', 'https://semopenalex.org/work/W2790187313', 'https://semopenalex.org/work/W2913475584', 'https://semopenalex.org/work/W2131570437', 'https://semopenalex.org/work/W2899470128', 'https://semopenalex.org/work/W2752042616', 'https://semopenalex.org/work/W3028790862', 'https://semopenalex.org/work/W4401406766', 'https://semopenalex.org/work/W4400189062', 'https://semopenalex.org/work/W4396832885', 'https://semopenalex.org/work/W2519730427', 'https://semopenalex.org/work/W3003204379', 'https://semopenalex.org/work/W1710215999', 'https://semopenalex.org/work/W3024164567', 'https://semopenalex.org/work/W4224242333', 'https://semopenalex.org/work/W2024357873', 'https://semopenalex.org/work/W2775793881', 'https://semopenalex.org/work/W3190617503', 'https://semopenalex.org/work/W4393067390', 'https://semopenalex.org/work/W3188420011', 'https://semopenalex.org/work/W3163921267', 'https://semopenalex.org/work/W4324151651', 'https://semopenalex.org/work/W2899389394', 'https://semopenalex.org/work/W2940716241', 'https://semopenalex.org/work/W2899305210', 'https://semopenalex.org/work/W2897414246', 'https://semopenalex.org/work/W3028180736', 'https://semopenalex.org/work/W4256454723', 'https://semopenalex.org/work/W4213455276', 'https://semopenalex.org/work/W2068367136', 'https://semopenalex.org/work/W1985142918', 'https://semopenalex.org/work/W1877041815', 'https://semopenalex.org/work/W3163327897', 'https://semopenalex.org/work/W1985504739', 'https://semopenalex.org/work/W3094759305', 'https://semopenalex.org/work/W1993984611', 'https://semopenalex.org/work/W2972419497', 'https://semopenalex.org/work/W2725971658', 'https://semopenalex.org/work/W2885122621', 'https://semopenalex.org/work/W2067004171', 'https://semopenalex.org/work/W2753363725', 'https://semopenalex.org/work/W3163521409', 'https://semopenalex.org/work/W3121775658', 'https://semopenalex.org/work/W2461856634', 'https://semopenalex.org/work/W2929751249', 'https://semopenalex.org/work/W2119929248', 'https://semopenalex.org/work/W3142764819', 'https://semopenalex.org/work/W4404569483', 'https://semopenalex.org/work/W2075286904', 'https://semopenalex.org/work/W4324152586', 'https://semopenalex.org/work/W791468510', 'https://semopenalex.org/work/W4366583934', 'https://semopenalex.org/work/W4389891943', 'https://semopenalex.org/work/W2263778529', 'https://semopenalex.org/work/W2898820983', 'https://semopenalex.org/work/W2752490344', 'https://semopenalex.org/work/W2187647369', 'https://semopenalex.org/work/W4379033872', 'https://semopenalex.org/work/W4400430993', 'https://semopenalex.org/work/W4221065578', 'https://semopenalex.org/work/W2795581336', 'https://semopenalex.org/work/W4241289669', 'https://semopenalex.org/work/W4287071181', 'https://semopenalex.org/work/W2811468211', 'https://semopenalex.org/work/W3194688439', 'https://semopenalex.org/work/W3015284588', 'https://semopenalex.org/work/W4319452484', 'https://semopenalex.org/work/W3201213010', 'https://semopenalex.org/work/W1771936601', 'https://semopenalex.org/work/W2017727997', 'https://semopenalex.org/work/W3034123328', 'https://semopenalex.org/work/W2409578015', 'https://semopenalex.org/work/W3188766356', 'https://semopenalex.org/work/W3062298123', 'https://semopenalex.org/work/W1553133540', 'https://semopenalex.org/work/W2537880674', 'https://semopenalex.org/work/W4402722090', 'https://semopenalex.org/work/W2903417746', 'https://semopenalex.org/work/W2625122753', 'https://semopenalex.org/work/W3177151358', 'https://semopenalex.org/work/W4229043996', 'https://semopenalex.org/work/W4404915142', 'https://semopenalex.org/work/W2902563098', 'https://semopenalex.org/work/W2977979696', 'https://semopenalex.org/work/W4210768549', 'https://semopenalex.org/work/W1484203263', 'https://semopenalex.org/work/W4393877125', 'https://semopenalex.org/work/W2055070571', 'https://semopenalex.org/work/W4402722131', 'https://semopenalex.org/work/W2129488573', 'https://semopenalex.org/work/W3000816869', 'https://semopenalex.org/work/W4232727837', 'https://semopenalex.org/work/W2968293343', 'https://semopenalex.org/work/W4387421144', 'https://semopenalex.org/work/W4404977899', 'https://semopenalex.org/work/W2898627444', 'https://semopenalex.org/work/W2052607251', 'https://semopenalex.org/work/W2978280554', 'https://semopenalex.org/work/W2108512685', 'https://semopenalex.org/work/W4312572845', 'https://semopenalex.org/work/W3206712787', 'https://semopenalex.org/work/W4366549587', 'https://semopenalex.org/work/W2072697691', 'https://semopenalex.org/work/W862033376', 'https://semopenalex.org/work/W3201451193', 'https://semopenalex.org/work/W2088502162', 'https://semopenalex.org/work/W1568803211', 'https://semopenalex.org/work/W2293208404', 'https://semopenalex.org/work/W3193717464', 'https://semopenalex.org/work/W2973132733', 'https://semopenalex.org/work/W2519250278', 'https://semopenalex.org/work/W2567779880', 'https://semopenalex.org/work/W2346027641', 'https://semopenalex.org/work/W4404373433', 'https://semopenalex.org/work/W2102905932', 'https://semopenalex.org/work/W3033839905', 'https://semopenalex.org/work/W2591593006', 'https://semopenalex.org/work/W4310446060', 'https://semopenalex.org/work/W2080327955', 'https://semopenalex.org/work/W2976524236', 'https://semopenalex.org/work/W3110075456', 'https://semopenalex.org/work/W4324150147', 'https://semopenalex.org/work/W2072490274', 'https://semopenalex.org/work/W4233748389', 'https://semopenalex.org/work/W3215451397', 'https://semopenalex.org/work/W4366598255', 'https://semopenalex.org/work/W2898145840', 'https://semopenalex.org/work/W2978827769', 'https://semopenalex.org/work/W3160199101', 'https://semopenalex.org/work/W1834136374', 'https://semopenalex.org/work/W3197280612', 'https://semopenalex.org/work/W2256119246', 'https://semopenalex.org/work/W2611151946', 'https://semopenalex.org/work/W4393752214', 'https://semopenalex.org/work/W3119309106', 'https://semopenalex.org/work/W2057014910', 'https://semopenalex.org/work/W4309619903', 'https://semopenalex.org/work/W3043824623', 'https://semopenalex.org/work/W4394883037', 'https://semopenalex.org/work/W2972702127', 'https://semopenalex.org/work/W4225088745', 'https://semopenalex.org/work/W2294561329', 'https://semopenalex.org/work/W2149683870', 'https://semopenalex.org/work/W2921533080', 'https://semopenalex.org/work/W4404026276', 'https://semopenalex.org/work/W4391423303', 'https://semopenalex.org/work/W3183940262', 'https://semopenalex.org/work/W2165066165', 'https://semopenalex.org/work/W2962975962', 'https://semopenalex.org/work/W2019487042', 'https://semopenalex.org/work/W3035628382', 'https://semopenalex.org/work/W2795503716', 'https://semopenalex.org/work/W2008208122', 'https://semopenalex.org/work/W4391210282', 'https://semopenalex.org/work/W2602429360', 'https://semopenalex.org/work/W3162832522', 'https://semopenalex.org/work/W4389256452', 'https://semopenalex.org/work/W2598459295', 'https://semopenalex.org/work/W2774467220', 'https://semopenalex.org/work/W2942738233', 'https://semopenalex.org/work/W2942324097', 'https://semopenalex.org/work/W4287729941', 'https://semopenalex.org/work/W2754101670', 'https://semopenalex.org/work/W2079488626', 'https://semopenalex.org/work/W3095347735', 'https://semopenalex.org/work/W3143959337', 'https://semopenalex.org/work/W3032662532', 'https://semopenalex.org/work/W3032857618', 'https://semopenalex.org/work/W4393908582', 'https://semopenalex.org/work/W2966384546', 'https://semopenalex.org/work/W4239396382', 'https://semopenalex.org/work/W2753801751', 'https://semopenalex.org/work/W4238249729', 'https://semopenalex.org/work/W3091007149', 'https://semopenalex.org/work/W4211095911', 'https://semopenalex.org/work/W3196785132', 'https://semopenalex.org/work/W4377250056', 'https://semopenalex.org/work/W3121062173', 'https://semopenalex.org/work/W2605978692', 'https://semopenalex.org/work/W4292261957', 'https://semopenalex.org/work/W2089266363', 'https://semopenalex.org/work/W1246643588', 'https://semopenalex.org/work/W2977617583', 'https://semopenalex.org/work/W2909558410', 'https://semopenalex.org/work/W2177601947', 'https://semopenalex.org/work/W2528963299', 'https://semopenalex.org/work/W4214504130', 'https://semopenalex.org/work/W3206366132', 'https://semopenalex.org/work/W4393067517', 'https://semopenalex.org/work/W2752658305', 'https://semopenalex.org/work/W3160545975', 'https://semopenalex.org/work/W4308467568', 'https://semopenalex.org/work/W2007978709', 'https://semopenalex.org/work/W2156243282', 'https://semopenalex.org/work/W2012358521', 'https://semopenalex.org/work/W2751622533', 'https://semopenalex.org/work/W2973140914', 'https://semopenalex.org/work/W4224305168', 'https://semopenalex.org/work/W4241528240', 'https://semopenalex.org/work/W4211259494', 'https://semopenalex.org/work/W3005470382', 'https://semopenalex.org/work/W3112877194', 'https://semopenalex.org/work/W3161974712', 'https://semopenalex.org/work/W2410138785', 'https://semopenalex.org/work/W2033680836', 'https://semopenalex.org/work/W2903849727', 'https://semopenalex.org/work/W4200018492', 'https://semopenalex.org/work/W4366967286', 'https://semopenalex.org/work/W2898822823', 'https://semopenalex.org/work/W2576215493', 'https://semopenalex.org/work/W4307475355', 'https://semopenalex.org/work/W2946308339', 'https://semopenalex.org/work/W2519558346', 'https://semopenalex.org/work/W3162177365', 'https://semopenalex.org/work/W4366583171', 'https://semopenalex.org/work/W2895512277', 'https://semopenalex.org/work/W3095367321', 'https://semopenalex.org/work/W2110284634', 'https://semopenalex.org/work/W2087800309', 'https://semopenalex.org/work/W2752031858', 'https://semopenalex.org/work/W2978422619', 'https://semopenalex.org/work/W2092202628', 'https://semopenalex.org/work/W2973046614', 'https://semopenalex.org/work/W4392429145', 'https://semopenalex.org/work/W2520352456', 'https://semopenalex.org/work/W3030735111', 'https://semopenalex.org/work/W1704771702', 'https://semopenalex.org/work/W4220905243', 'https://semopenalex.org/work/W4389897704', 'https://semopenalex.org/work/W3200245219', 'https://semopenalex.org/work/W2888386951', 'https://semopenalex.org/work/W4224255688', 'https://semopenalex.org/work/W4200616097', 'https://semopenalex.org/work/W2753671526', 'https://semopenalex.org/work/W3112090964', 'https://semopenalex.org/work/W2762577600', 'https://semopenalex.org/work/W4242142265', 'https://semopenalex.org/work/W4387085789', 'https://semopenalex.org/work/W2977911811', 'https://semopenalex.org/work/W2133951180', 'https://semopenalex.org/work/W2610274107', 'https://semopenalex.org/work/W1982984133', 'https://semopenalex.org/work/W2288812598', 'https://semopenalex.org/work/W2054886944', 'https://semopenalex.org/work/W2921194733', 'https://semopenalex.org/work/W2791540051', 'https://semopenalex.org/work/W4251839844', 'https://semopenalex.org/work/W1510660243', 'https://semopenalex.org/work/W2273076933', 'https://semopenalex.org/work/W2602397751', 'https://semopenalex.org/work/W2768260654', 'https://semopenalex.org/work/W2078369692', 'https://semopenalex.org/work/W2975736083', 'https://semopenalex.org/work/W2610676428', 'https://semopenalex.org/work/W2519458229', 'https://semopenalex.org/work/W3095740806', 'https://semopenalex.org/work/W4230032809', 'https://semopenalex.org/work/W3030149602', 'https://semopenalex.org/work/W3047192924', 'https://semopenalex.org/work/W1976594634', 'https://semopenalex.org/work/W4366588423', 'https://semopenalex.org/work/W2972889118', 'https://semopenalex.org/work/W2548042282', 'https://semopenalex.org/work/W2088270376', 'https://semopenalex.org/work/W2033617925', 'https://semopenalex.org/work/W4210450354', 'https://semopenalex.org/work/W2968884122', 'https://semopenalex.org/work/W3009160614', 'https://semopenalex.org/work/W2091382943', 'https://semopenalex.org/work/W3161959528', 'https://semopenalex.org/work/W2751429127', 'https://semopenalex.org/work/W3117330688', 'https://semopenalex.org/work/W3033480106', 'https://semopenalex.org/work/W4387606708', 'https://semopenalex.org/work/W3165155612', 'https://semopenalex.org/work/W3126826400', 'https://semopenalex.org/work/W2037697732', 'https://semopenalex.org/work/W3033866035', 'https://semopenalex.org/work/W3096658838', 'https://semopenalex.org/work/W2551155618', 'https://semopenalex.org/work/W2904910662', 'https://semopenalex.org/work/W2755164339', 'https://semopenalex.org/work/W3163085734', 'https://semopenalex.org/work/W4404873047', 'https://semopenalex.org/work/W1981715407', 'https://semopenalex.org/work/W2896178739', 'https://semopenalex.org/work/W4225133274', 'https://semopenalex.org/work/W3161202338', 'https://semopenalex.org/work/W3203088685', 'https://semopenalex.org/work/W2344158693', 'https://semopenalex.org/work/W4406805368', 'https://semopenalex.org/work/W2793897377', 'https://semopenalex.org/work/W2789478762', 'https://semopenalex.org/work/W4379879736', 'https://semopenalex.org/work/W4283397308', 'https://semopenalex.org/work/W2755506150', 'https://semopenalex.org/work/W3028614762', 'https://semopenalex.org/work/W3141512745', 'https://semopenalex.org/work/W4361189030', 'https://semopenalex.org/work/W3036463368', 'https://semopenalex.org/work/W2465877051', 'https://semopenalex.org/work/W2159491375', 'https://semopenalex.org/work/W2977597077', 'https://semopenalex.org/work/W2121082751', 'https://semopenalex.org/work/W2520661109', 'https://semopenalex.org/work/W2090841027', 'https://semopenalex.org/work/W2901616108', 'https://semopenalex.org/work/W2913594206', 'https://semopenalex.org/work/W4315777028', 'https://semopenalex.org/work/W2136876773', 'https://semopenalex.org/work/W2557881781', 'https://semopenalex.org/work/W2513683703', 'https://semopenalex.org/work/W4200525013', 'https://semopenalex.org/work/W3110591323', 'https://semopenalex.org/work/W4225473762', 'https://semopenalex.org/work/W2102667737', 'https://semopenalex.org/work/W2518694405', 'https://semopenalex.org/work/W3198359754', 'https://semopenalex.org/work/W3202016550', 'https://semopenalex.org/work/W3171875220', 'https://semopenalex.org/work/W3031395001', 'https://semopenalex.org/work/W1998431265', 'https://semopenalex.org/work/W3090583924', 'https://semopenalex.org/work/W2139733095', 'https://semopenalex.org/work/W1993514406', 'https://semopenalex.org/work/W4385856456', 'https://semopenalex.org/work/W2108911539', 'https://semopenalex.org/work/W2169202944', 'https://semopenalex.org/work/W2515389026', 'https://semopenalex.org/work/W2613908791', 'https://semopenalex.org/work/W3178374478', 'https://semopenalex.org/work/W4312646439', 'https://semopenalex.org/work/W4214684069', 'https://semopenalex.org/work/W3130372017', 'https://semopenalex.org/work/W4399763801', 'https://semopenalex.org/work/W2519914856', 'https://semopenalex.org/work/W1522158218', 'https://semopenalex.org/work/W3184531492', 'https://semopenalex.org/work/W3186694431', 'https://semopenalex.org/work/W2798335699', 'https://semopenalex.org/work/W2899333601', 'https://semopenalex.org/work/W1975028026', 'https://semopenalex.org/work/W4214593503', 'https://semopenalex.org/work/W4393102879', 'https://semopenalex.org/work/W2610780371', 'https://semopenalex.org/work/W4312841490', 'https://semopenalex.org/work/W2063007215', 'https://semopenalex.org/work/W2944843734', 'https://semopenalex.org/work/W4324154015', 'https://semopenalex.org/work/W3022986551', 'https://semopenalex.org/work/W2561633795', 'https://semopenalex.org/work/W3182364466', 'https://semopenalex.org/work/W2611685970', 'https://semopenalex.org/work/W4224279084', 'https://semopenalex.org/work/W3030577208', 'https://semopenalex.org/work/W2294361658', 'https://semopenalex.org/work/W2082538501', 'https://semopenalex.org/work/W2810881717', 'https://semopenalex.org/work/W1524596993', 'https://semopenalex.org/work/W3135072684', 'https://semopenalex.org/work/W2972600126', 'https://semopenalex.org/work/W3035727063', 'https://semopenalex.org/work/W1965526182', 'https://semopenalex.org/work/W2346980133', 'https://semopenalex.org/work/W3181801907', 'https://semopenalex.org/work/W2920869031', 'https://semopenalex.org/work/W3196772354', 'https://semopenalex.org/work/W2152557601', 'https://semopenalex.org/work/W4312605566', 'https://semopenalex.org/work/W2346600598', 'https://semopenalex.org/work/W2520077052', 'https://semopenalex.org/work/W2401872729', 'https://semopenalex.org/work/W4307204790', 'https://semopenalex.org/work/W3037695612', 'https://semopenalex.org/work/W2921058600', 'https://semopenalex.org/work/W4386929049', 'https://semopenalex.org/work/W2902941289', 'https://semopenalex.org/work/W2060118520', 'https://semopenalex.org/work/W4230967253', 'https://semopenalex.org/work/W1860259465', 'https://semopenalex.org/work/W3204110051', 'https://semopenalex.org/work/W4312282153', 'https://semopenalex.org/work/W3011317564', 'https://semopenalex.org/work/W4394825420', 'https://semopenalex.org/work/W3003369003', 'https://semopenalex.org/work/W3204393727', 'https://semopenalex.org/work/W3163078982', 'https://semopenalex.org/work/W2737450254', 'https://semopenalex.org/work/W2752561456', 'https://semopenalex.org/work/W4366597679', 'https://semopenalex.org/work/W2114418543', 'https://semopenalex.org/work/W2061583538', 'https://semopenalex.org/work/W4383220643', 'https://semopenalex.org/work/W2318574332', 'https://semopenalex.org/work/W1751138515', 'https://semopenalex.org/work/W2986358413', 'https://semopenalex.org/work/W2898667062', 'https://semopenalex.org/work/W2137846113', 'https://semopenalex.org/work/W3033704563', 'https://semopenalex.org/work/W4386163788', 'https://semopenalex.org/work/W3007521088', 'https://semopenalex.org/work/W2154752229', 'https://semopenalex.org/work/W2972759039', 'https://semopenalex.org/work/W3084729599', 'https://semopenalex.org/work/W4366547357', 'https://semopenalex.org/work/W2981708234', 'https://semopenalex.org/work/W3096988350', 'https://semopenalex.org/work/W4245844025', 'https://semopenalex.org/work/W2738622408', 'https://semopenalex.org/work/W4399126764', 'https://semopenalex.org/work/W2750727230', 'https://semopenalex.org/work/W4294891921', 'https://semopenalex.org/work/W3161889270', 'https://semopenalex.org/work/W2973016298', 'https://semopenalex.org/work/W4234952088']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W1938912534', 'https://semopenalex.org/work/W3101678388', 'https://semopenalex.org/work/W2798444339', 'https://semopenalex.org/work/W10552456', 'https://semopenalex.org/work/W1481252923', 'https://semopenalex.org/work/W2167318748', 'https://semopenalex.org/work/W2344677227', 'https://semopenalex.org/work/W4405179263', 'https://semopenalex.org/work/W2502765568', 'https://semopenalex.org/work/W2071898607', 'https://semopenalex.org/work/W3204280976', 'https://semopenalex.org/work/W4387190940', 'https://semopenalex.org/work/W2088840086', 'https://semopenalex.org/work/W3200977970', 'https://semopenalex.org/work/W2250659747', 'https://semopenalex.org/work/W1581844963', 'https://semopenalex.org/work/W4386474911', 'https://semopenalex.org/work/W4312038601', 'https://semopenalex.org/work/W2896561783', 'https://semopenalex.org/work/W3097074140', 'https://semopenalex.org/work/W4402599958', 'https://semopenalex.org/work/W2794632798', 'https://semopenalex.org/work/W2068346480', 'https://semopenalex.org/work/W1600095712', 'https://semopenalex.org/work/W2990998351', 'https://semopenalex.org/work/W4391661476', 'https://semopenalex.org/work/W2557853356', 'https://semopenalex.org/work/W4362502008', 'https://semopenalex.org/work/W3110928664', 'https://semopenalex.org/work/W2915831115', 'https://semopenalex.org/work/W4388320652', 'https://semopenalex.org/work/W2017629483', 'https://semopenalex.org/work/W4243814040', 'https://semopenalex.org/work/W2612035199', 'https://semopenalex.org/work/W2052312648', 'https://semopenalex.org/work/W4384756284', 'https://semopenalex.org/work/W4362655741', 'https://semopenalex.org/work/W1496034358', 'https://semopenalex.org/work/W2427008665', 'https://semopenalex.org/work/W2150013559', 'https://semopenalex.org/work/W2053495332', 'https://semopenalex.org/work/W2905317998', 'https://semopenalex.org/work/W3003707605', 'https://semopenalex.org/work/W2554367017', 'https://semopenalex.org/work/W2040345481', 'https://semopenalex.org/work/W1493881734', 'https://semopenalex.org/work/W4389575826', 'https://semopenalex.org/work/W1753378771', 'https://semopenalex.org/work/W1565188338', 'https://semopenalex.org/work/W2051680663', 'https://semopenalex.org/work/W2909965602', 'https://semopenalex.org/work/W2003420345', 'https://semopenalex.org/work/W2097959755', 'https://semopenalex.org/work/W2808806636', 'https://semopenalex.org/work/W2059788348', 'https://semopenalex.org/work/W4379964950', 'https://semopenalex.org/work/W2468217693', 'https://semopenalex.org/work/W2086824798', 'https://semopenalex.org/work/W4226101170', 'https://semopenalex.org/work/W4406500025', 'https://semopenalex.org/work/W4389509728', 'https://semopenalex.org/work/W2422465781', 'https://semopenalex.org/work/W4401463259', 'https://semopenalex.org/work/W1702322733', 'https://semopenalex.org/work/W3140378604', 'https://semopenalex.org/work/W1508670223', 'https://semopenalex.org/work/W3116763688', 'https://semopenalex.org/work/W2594649443', 'https://semopenalex.org/work/W2084265221', 'https://semopenalex.org/work/W2804252553', 'https://semopenalex.org/work/W2063775187', 'https://semopenalex.org/work/W4287902628', 'https://semopenalex.org/work/W2898238060', 'https://semopenalex.org/work/W2167984494', 'https://semopenalex.org/work/W2916230113', 'https://semopenalex.org/work/W2479269651', 'https://semopenalex.org/work/W2087831714', 'https://semopenalex.org/work/W2613136061', 'https://semopenalex.org/work/W3066802614', 'https://semopenalex.org/work/W2511600948', 'https://semopenalex.org/work/W2032640310', 'https://semopenalex.org/work/W2901563117', 'https://semopenalex.org/work/W4389226119', 'https://semopenalex.org/work/W4252278539', 'https://semopenalex.org/work/W3045638492', 'https://semopenalex.org/work/W2809590475', 'https://semopenalex.org/work/W2899754551', 'https://semopenalex.org/work/W125254009', 'https://semopenalex.org/work/W4317640658', 'https://semopenalex.org/work/W4388040916', 'https://semopenalex.org/work/W2775115790', 'https://semopenalex.org/work/W2344504222', 'https://semopenalex.org/work/W4312911917', 'https://semopenalex.org/work/W4381855531', 'https://semopenalex.org/work/W104210143', 'https://semopenalex.org/work/W4230101435', 'https://semopenalex.org/work/W4401719068', 'https://semopenalex.org/work/W1720341833', 'https://semopenalex.org/work/W2912179439', 'https://semopenalex.org/work/W2092411821', 'https://semopenalex.org/work/W433641300', 'https://semopenalex.org/work/W4391248380', 'https://semopenalex.org/work/W1507165467', 'https://semopenalex.org/work/W4200400669', 'https://semopenalex.org/work/W2107915643', 'https://semopenalex.org/work/W3097918021', 'https://semopenalex.org/work/W1479774717', 'https://semopenalex.org/work/W4393969247', 'https://semopenalex.org/work/W2898587907', 'https://semopenalex.org/work/W3216694898', 'https://semopenalex.org/work/W3038546681', 'https://semopenalex.org/work/W2755922538', 'https://semopenalex.org/work/W2897073097', 'https://semopenalex.org/work/W4401110041', 'https://semopenalex.org/work/W139217162', 'https://semopenalex.org/work/W2506885748', 'https://semopenalex.org/work/W1988741859', 'https://semopenalex.org/work/W4317619163', 'https://semopenalex.org/work/W2025843016', 'https://semopenalex.org/work/W2198834745', 'https://semopenalex.org/work/W1974608646', 'https://semopenalex.org/work/W1566552779', 'https://semopenalex.org/work/W4323923480', 'https://semopenalex.org/work/W1507246359', 'https://semopenalex.org/work/W2005330588', 'https://semopenalex.org/work/W3190788066', 'https://semopenalex.org/work/W2735638814', 'https://semopenalex.org/work/W3122406465', 'https://semopenalex.org/work/W2422976594', 'https://semopenalex.org/work/W3035750004', 'https://semopenalex.org/work/W4399881333', 'https://semopenalex.org/work/W2986139096', 'https://semopenalex.org/work/W4294500063', 'https://semopenalex.org/work/W4289866493', 'https://semopenalex.org/work/W2030563576', 'https://semopenalex.org/work/W1827647151', 'https://semopenalex.org/work/W2125430046', 'https://semopenalex.org/work/W1984186194', 'https://semopenalex.org/work/W4404788249', 'https://semopenalex.org/work/W2284502685', 'https://semopenalex.org/work/W4391973940', 'https://semopenalex.org/work/W3138702399', 'https://semopenalex.org/work/W2515387399', 'https://semopenalex.org/work/W2296703446', 'https://semopenalex.org/work/W4402091088', 'https://semopenalex.org/work/W2775805395', 'https://semopenalex.org/work/W2770240327', 'https://semopenalex.org/work/W3030557354', 'https://semopenalex.org/work/W2467591515', 'https://semopenalex.org/work/W1498712689', 'https://semopenalex.org/work/W3023950320', 'https://semopenalex.org/work/W2733791027', 'https://semopenalex.org/work/W1608885791', 'https://semopenalex.org/work/W2795633027', 'https://semopenalex.org/work/W2610117056', 'https://semopenalex.org/work/W3004495293', 'https://semopenalex.org/work/W3124693625', 'https://semopenalex.org/work/W2032265428', 'https://semopenalex.org/work/W2700566289', 'https://semopenalex.org/work/W4246273094', 'https://semopenalex.org/work/W4376269693', 'https://semopenalex.org/work/W4312953992', 'https://semopenalex.org/work/W2017988065', 'https://semopenalex.org/work/W2920780560', 'https://semopenalex.org/work/W1980418511', 'https://semopenalex.org/work/W4406794085', 'https://semopenalex.org/work/W4220938834', 'https://semopenalex.org/work/W4380136543', 'https://semopenalex.org/work/W2951057438', 'https://semopenalex.org/work/W4394576023', 'https://semopenalex.org/work/W2990317423', 'https://semopenalex.org/work/W4400611446', 'https://semopenalex.org/work/W3026213155', 'https://semopenalex.org/work/W2404446956', 'https://semopenalex.org/work/W1688396929', 'https://semopenalex.org/work/W2150949003', 'https://semopenalex.org/work/W3208070608', 'https://semopenalex.org/work/W2084970449', 'https://semopenalex.org/work/W2141276288', 'https://semopenalex.org/work/W4292848294', 'https://semopenalex.org/work/W2791022910', 'https://semopenalex.org/work/W3024403368', 'https://semopenalex.org/work/W4406261609', 'https://semopenalex.org/work/W2426048753', 'https://semopenalex.org/work/W4289364680', 'https://semopenalex.org/work/W4297725807', 'https://semopenalex.org/work/W3176983082', 'https://semopenalex.org/work/W2920007056', 'https://semopenalex.org/work/W2984000149', 'https://semopenalex.org/work/W4401689701', 'https://semopenalex.org/work/W2076165157', 'https://semopenalex.org/work/W4223526958', 'https://semopenalex.org/work/W4226040560', 'https://semopenalex.org/work/W3111943635', 'https://semopenalex.org/work/W2185480307', 'https://semopenalex.org/work/W3157617328', 'https://semopenalex.org/work/W2149498440', 'https://semopenalex.org/work/W2251316727', 'https://semopenalex.org/work/W1608148813', 'https://semopenalex.org/work/W1664839614', 'https://semopenalex.org/work/W2735964774', 'https://semopenalex.org/work/W1985846348', 'https://semopenalex.org/work/W3098889210', 'https://semopenalex.org/work/W2329646465', 'https://semopenalex.org/work/W2808066670', 'https://semopenalex.org/work/W1507429943', 'https://semopenalex.org/work/W2092295977', 'https://semopenalex.org/work/W4406679155', 'https://semopenalex.org/work/W4388742679', 'https://semopenalex.org/work/W4232691833', 'https://semopenalex.org/work/W79646937', 'https://semopenalex.org/work/W2013042849', 'https://semopenalex.org/work/W2027402731', 'https://semopenalex.org/work/W2422116896', 'https://semopenalex.org/work/W2970882829', 'https://semopenalex.org/work/W1495063990', 'https://semopenalex.org/work/W4402538155', 'https://semopenalex.org/work/W4400812269', 'https://semopenalex.org/work/W2110495371', 'https://semopenalex.org/work/W2152979493', 'https://semopenalex.org/work/W4294707045', 'https://semopenalex.org/work/W2505162744', 'https://semopenalex.org/work/W3175986586', 'https://semopenalex.org/work/W2465409613', 'https://semopenalex.org/work/W4213388674', 'https://semopenalex.org/work/W4388972775', 'https://semopenalex.org/work/W2998494411', 'https://semopenalex.org/work/W2795298263', 'https://semopenalex.org/work/W4283365825', 'https://semopenalex.org/work/W2136344560', 'https://semopenalex.org/work/W2499168780', 'https://semopenalex.org/work/W4231180551', 'https://semopenalex.org/work/W2140346433', 'https://semopenalex.org/work/W4367682485', 'https://semopenalex.org/work/W2484289073', 'https://semopenalex.org/work/W2337491900', 'https://semopenalex.org/work/W4391673335', 'https://semopenalex.org/work/W4390137041', 'https://semopenalex.org/work/W2147228279', 'https://semopenalex.org/work/W2293638396', 'https://semopenalex.org/work/W2735732687', 'https://semopenalex.org/work/W2616473319', 'https://semopenalex.org/work/W1601136399', 'https://semopenalex.org/work/W4381549091', 'https://semopenalex.org/work/W4385285133', 'https://semopenalex.org/work/W3136943238', 'https://semopenalex.org/work/W2981705990', 'https://semopenalex.org/work/W2400388471', 'https://semopenalex.org/work/W4404464211', 'https://semopenalex.org/work/W192156609', 'https://semopenalex.org/work/W2016580264', 'https://semopenalex.org/work/W2330628472', 'https://semopenalex.org/work/W4319053914', 'https://semopenalex.org/work/W2584286364', 'https://semopenalex.org/work/W2615044227', 'https://semopenalex.org/work/W175358687', 'https://semopenalex.org/work/W4405522042', 'https://semopenalex.org/work/W4221002597', 'https://semopenalex.org/work/W2805393243', 'https://semopenalex.org/work/W2131164945', 'https://semopenalex.org/work/W2903414282', 'https://semopenalex.org/work/W4401719105', 'https://semopenalex.org/work/W4377099260', 'https://semopenalex.org/work/W1504659965', 'https://semopenalex.org/work/W4302306230', 'https://semopenalex.org/work/W4220657425', 'https://semopenalex.org/work/W2908443740', 'https://semopenalex.org/work/W4302859022', 'https://semopenalex.org/work/W4309647912', 'https://semopenalex.org/work/W2954580762', 'https://semopenalex.org/work/W4232799872', 'https://semopenalex.org/work/W1487391256', 'https://semopenalex.org/work/W1527508100', 'https://semopenalex.org/work/W2922408557', 'https://semopenalex.org/work/W3013272684', 'https://semopenalex.org/work/W4283718670', 'https://semopenalex.org/work/W4213121575', 'https://semopenalex.org/work/W4312262758', 'https://semopenalex.org/work/W2114238248', 'https://semopenalex.org/work/W4283643625', 'https://semopenalex.org/work/W2900798442', 'https://semopenalex.org/work/W2075258117', 'https://semopenalex.org/work/W4301486307', 'https://semopenalex.org/work/W3090908182', 'https://semopenalex.org/work/W3130665718', 'https://semopenalex.org/work/W4394048733', 'https://semopenalex.org/work/W2499947387', 'https://semopenalex.org/work/W2321758884', 'https://semopenalex.org/work/W4365205158', 'https://semopenalex.org/work/W2965941321', 'https://semopenalex.org/work/W2809627415', 'https://semopenalex.org/work/W3210789515', 'https://semopenalex.org/work/W3107101618', 'https://semopenalex.org/work/W3033848960', 'https://semopenalex.org/work/W2083708758', 'https://semopenalex.org/work/W4317438183', 'https://semopenalex.org/work/W4404788038', 'https://semopenalex.org/work/W3163303484', 'https://semopenalex.org/work/W2923319240', 'https://semopenalex.org/work/W2417471897', 'https://semopenalex.org/work/W1605123443', 'https://semopenalex.org/work/W3153444696', 'https://semopenalex.org/work/W2901915930', 'https://semopenalex.org/work/W2169290493', 'https://semopenalex.org/work/W4399118880', 'https://semopenalex.org/work/W32663231', 'https://semopenalex.org/work/W2550260459', 'https://semopenalex.org/work/W1990240966', 'https://semopenalex.org/work/W2008632807', 'https://semopenalex.org/work/W4401023469', 'https://semopenalex.org/work/W2942454712', 'https://semopenalex.org/work/W2795358293', 'https://semopenalex.org/work/W4400881052', 'https://semopenalex.org/work/W2901185014', 'https://semopenalex.org/work/W2172069600', 'https://semopenalex.org/work/W3211356533', 'https://semopenalex.org/work/W2163121311', 'https://semopenalex.org/work/W2066037774', 'https://semopenalex.org/work/W2587382914', 'https://semopenalex.org/work/W4244365690', 'https://semopenalex.org/work/W2009396504', 'https://semopenalex.org/work/W2796403873', 'https://semopenalex.org/work/W3010046448', 'https://semopenalex.org/work/W2902564735', 'https://semopenalex.org/work/W2050276970', 'https://semopenalex.org/work/W2500329317', 'https://semopenalex.org/work/W4389575859', 'https://semopenalex.org/work/W2048339977', 'https://semopenalex.org/work/W4390570315', 'https://semopenalex.org/work/W4281629096', 'https://semopenalex.org/work/W1660366533', 'https://semopenalex.org/work/W2608436687', 'https://semopenalex.org/work/W3134356917', 'https://semopenalex.org/work/W2998183977', 'https://semopenalex.org/work/W3140552826', 'https://semopenalex.org/work/W2991585802', 'https://semopenalex.org/work/W4385852291', 'https://semopenalex.org/work/W1793399427', 'https://semopenalex.org/work/W4287758300', 'https://semopenalex.org/work/W4402352406', 'https://semopenalex.org/work/W1934576426', 'https://semopenalex.org/work/W2124874701', 'https://semopenalex.org/work/W2138607828', 'https://semopenalex.org/work/W3149145084', 'https://semopenalex.org/work/W2165611534', 'https://semopenalex.org/work/W2065926303', 'https://semopenalex.org/work/W4229056530', 'https://semopenalex.org/work/W1581509591', 'https://semopenalex.org/work/W2953273686', 'https://semopenalex.org/work/W4402594156', 'https://semopenalex.org/work/W2900534295', 'https://semopenalex.org/work/W4399554294', 'https://semopenalex.org/work/W3112151564', 'https://semopenalex.org/work/W2146501308', 'https://semopenalex.org/work/W2778221989', 'https://semopenalex.org/work/W4250640589', 'https://semopenalex.org/work/W4309613628', 'https://semopenalex.org/work/W3066383670', 'https://semopenalex.org/work/W1992237536', 'https://semopenalex.org/work/W2489798131', 'https://semopenalex.org/work/W4309647894', 'https://semopenalex.org/work/W4316672181', 'https://semopenalex.org/work/W2119701885', 'https://semopenalex.org/work/W4402157005', 'https://semopenalex.org/work/W1971405342', 'https://semopenalex.org/work/W1983176793', 'https://semopenalex.org/work/W629466361', 'https://semopenalex.org/work/W4394867508', 'https://semopenalex.org/work/W2131027594', 'https://semopenalex.org/work/W2309229337', 'https://semopenalex.org/work/W2003561941', 'https://semopenalex.org/work/W3161264338', 'https://semopenalex.org/work/W2901968423', 'https://semopenalex.org/work/W1974446585', 'https://semopenalex.org/work/W4405828728', 'https://semopenalex.org/work/W2808185912', 'https://semopenalex.org/work/W3206119617', 'https://semopenalex.org/work/W1484038335', 'https://semopenalex.org/work/W4294578223', 'https://semopenalex.org/work/W4395064999', 'https://semopenalex.org/work/W3077087723', 'https://semopenalex.org/work/W2991082611', 'https://semopenalex.org/work/W4206564475', 'https://semopenalex.org/work/W2735379054', 'https://semopenalex.org/work/W4286794087', 'https://semopenalex.org/work/W2155277804', 'https://semopenalex.org/work/W2006918362', 'https://semopenalex.org/work/W1588641552', 'https://semopenalex.org/work/W1500858206', 'https://semopenalex.org/work/W1609271133', 'https://semopenalex.org/work/W610311842', 'https://semopenalex.org/work/W2915383148', 'https://semopenalex.org/work/W4404252082', 'https://semopenalex.org/work/W51883144', 'https://semopenalex.org/work/W4404037007', 'https://semopenalex.org/work/W2439110316', 'https://semopenalex.org/work/W4309325586', 'https://semopenalex.org/work/W2089975859', 'https://semopenalex.org/work/W2166042493', 'https://semopenalex.org/work/W2491619570', 'https://semopenalex.org/work/W3112593626', 'https://semopenalex.org/work/W2920517911', 'https://semopenalex.org/work/W4387293718', 'https://semopenalex.org/work/W4377234328', 'https://semopenalex.org/work/W4386486628', 'https://semopenalex.org/work/W1563606705', 'https://semopenalex.org/work/W4320909166', 'https://semopenalex.org/work/W4406118666', 'https://semopenalex.org/work/W4252774423', 'https://semopenalex.org/work/W4247657810', 'https://semopenalex.org/work/W2464669661', 'https://semopenalex.org/work/W3041363918', 'https://semopenalex.org/work/W2152170845', 'https://semopenalex.org/work/W4393748815', 'https://semopenalex.org/work/W4402710970', 'https://semopenalex.org/work/W4378768161', 'https://semopenalex.org/work/W4317042649', 'https://semopenalex.org/work/W4316116419', 'https://semopenalex.org/work/W2036885872', 'https://semopenalex.org/work/W2889404430', 'https://semopenalex.org/work/W2007985134', 'https://semopenalex.org/work/W2900517348', 'https://semopenalex.org/work/W2548544249', 'https://semopenalex.org/work/W4389880140', 'https://semopenalex.org/work/W171268263', 'https://semopenalex.org/work/W4309647909', 'https://semopenalex.org/work/W2013870117', 'https://semopenalex.org/work/W3008028280', 'https://semopenalex.org/work/W4221168020', 'https://semopenalex.org/work/W4255591746', 'https://semopenalex.org/work/W4233690695', 'https://semopenalex.org/work/W2515263588', 'https://semopenalex.org/work/W4226214859', 'https://semopenalex.org/work/W4402595291', 'https://semopenalex.org/work/W4389543458', 'https://semopenalex.org/work/W4402713726', 'https://semopenalex.org/work/W2792554287', 'https://semopenalex.org/work/W23340818', 'https://semopenalex.org/work/W4235399974', 'https://semopenalex.org/work/W4406729944', 'https://semopenalex.org/work/W1986302656', 'https://semopenalex.org/work/W2134387352', 'https://semopenalex.org/work/W2806499268', 'https://semopenalex.org/work/W4404411574', 'https://semopenalex.org/work/W2949762754', 'https://semopenalex.org/work/W112461364', 'https://semopenalex.org/work/W2804137108', 'https://semopenalex.org/work/W2612374761', 'https://semopenalex.org/work/W4376061047', 'https://semopenalex.org/work/W4396594158', 'https://semopenalex.org/work/W2359704875', 'https://semopenalex.org/work/W1497322082', 'https://semopenalex.org/work/W1524789227', 'https://semopenalex.org/work/W2296355030', 'https://semopenalex.org/work/W4405305567', 'https://semopenalex.org/work/W2060252439', 'https://semopenalex.org/work/W2551266388', 'https://semopenalex.org/work/W3167737483', 'https://semopenalex.org/work/W4400268996', 'https://semopenalex.org/work/W2805105531', 'https://semopenalex.org/work/W2085892029', 'https://semopenalex.org/work/W3162622638', 'https://semopenalex.org/work/W2165303722', 'https://semopenalex.org/work/W4390456266', 'https://semopenalex.org/work/W2130677504', 'https://semopenalex.org/work/W4404758113', 'https://semopenalex.org/work/W2143252268', 'https://semopenalex.org/work/W4403792402', 'https://semopenalex.org/work/W2950787737', 'https://semopenalex.org/work/W2991281508', 'https://semopenalex.org/work/W2756536429', 'https://semopenalex.org/work/W3082096159', 'https://semopenalex.org/work/W4313267141', 'https://semopenalex.org/work/W2098055383', 'https://semopenalex.org/work/W3121529680', 'https://semopenalex.org/work/W2953012688', 'https://semopenalex.org/work/W3173479430', 'https://semopenalex.org/work/W2730099201', 'https://semopenalex.org/work/W3126556715', 'https://semopenalex.org/work/W3179758589', 'https://semopenalex.org/work/W2077564315', 'https://semopenalex.org/work/W4312710991', 'https://semopenalex.org/work/W2746969608', 'https://semopenalex.org/work/W2908865778', 'https://semopenalex.org/work/W4233194301', 'https://semopenalex.org/work/W2584636165', 'https://semopenalex.org/work/W2924425593', 'https://semopenalex.org/work/W2494607466', 'https://semopenalex.org/work/W4226150381', 'https://semopenalex.org/work/W2052330128', 'https://semopenalex.org/work/W2738171721', 'https://semopenalex.org/work/W2063106869', 'https://semopenalex.org/work/W3176873809', 'https://semopenalex.org/work/W1980320703', 'https://semopenalex.org/work/W4237415699', 'https://semopenalex.org/work/W4288549248', 'https://semopenalex.org/work/W2623350311', 'https://semopenalex.org/work/W3203105904', 'https://semopenalex.org/work/W3139199248', 'https://semopenalex.org/work/W2041919000', 'https://semopenalex.org/work/W2594546957', 'https://semopenalex.org/work/W2045329305', 'https://semopenalex.org/work/W1510296842', 'https://semopenalex.org/work/W3106296980', 'https://semopenalex.org/work/W2919684758', 'https://semopenalex.org/work/W2054374338', 'https://semopenalex.org/work/W2557660464', 'https://semopenalex.org/work/W2990448760', 'https://semopenalex.org/work/W1517726756', 'https://semopenalex.org/work/W4400909999', 'https://semopenalex.org/work/W4287231113', 'https://semopenalex.org/work/W4312471121', 'https://semopenalex.org/work/W4386486604', 'https://semopenalex.org/work/W2118486116', 'https://semopenalex.org/work/W1554846139', 'https://semopenalex.org/work/W2052763829', 'https://semopenalex.org/work/W3001462578', 'https://semopenalex.org/work/W2918375401', 'https://semopenalex.org/work/W3200087552', 'https://semopenalex.org/work/W4392110461', 'https://semopenalex.org/work/W2748668979', 'https://semopenalex.org/work/W2156065383', 'https://semopenalex.org/work/W2000718212', 'https://semopenalex.org/work/W2138167749', 'https://semopenalex.org/work/W1492139710', 'https://semopenalex.org/work/W4380885381', 'https://semopenalex.org/work/W2065468011', 'https://semopenalex.org/work/W4386346214', 'https://semopenalex.org/work/W3015227276', 'https://semopenalex.org/work/W4385270466', 'https://semopenalex.org/work/W4291287572', 'https://semopenalex.org/work/W102169640', 'https://semopenalex.org/work/W2033132959', 'https://semopenalex.org/work/W2478525669', 'https://semopenalex.org/work/W2022462411', 'https://semopenalex.org/work/W2170735098', 'https://semopenalex.org/work/W2133544364', 'https://semopenalex.org/work/W4404735027', 'https://semopenalex.org/work/W3162065424', 'https://semopenalex.org/work/W1968925642', 'https://semopenalex.org/work/W2906612108', 'https://semopenalex.org/work/W2949205410', 'https://semopenalex.org/work/W4404180354', 'https://semopenalex.org/work/W4404370664', 'https://semopenalex.org/work/W2476253347', 'https://semopenalex.org/work/W4285292709', 'https://semopenalex.org/work/W4319792183', 'https://semopenalex.org/work/W4393144966', 'https://semopenalex.org/work/W3103436608', 'https://semopenalex.org/work/W4391766346', 'https://semopenalex.org/work/W2062482216', 'https://semopenalex.org/work/W2089906307', 'https://semopenalex.org/work/W2033368298', 'https://semopenalex.org/work/W206771271', 'https://semopenalex.org/work/W2117052376', 'https://semopenalex.org/work/W4250963083', 'https://semopenalex.org/work/W3177070127', 'https://semopenalex.org/work/W2919204815', 'https://semopenalex.org/work/W1715440516', 'https://semopenalex.org/work/W3012031786', 'https://semopenalex.org/work/W2116893958', 'https://semopenalex.org/work/W4255845198', 'https://semopenalex.org/work/W2089762145', 'https://semopenalex.org/work/W4387427541', 'https://semopenalex.org/work/W3056873248', 'https://semopenalex.org/work/W2903238830', 'https://semopenalex.org/work/W4239052734', 'https://semopenalex.org/work/W2945594129', 'https://semopenalex.org/work/W3124266007', 'https://semopenalex.org/work/W1971179860', 'https://semopenalex.org/work/W75044610', 'https://semopenalex.org/work/W1474354901', 'https://semopenalex.org/work/W4385270603', 'https://semopenalex.org/work/W4388989593', 'https://semopenalex.org/work/W4211034214', 'https://semopenalex.org/work/W2982576723', 'https://semopenalex.org/work/W4362501917', 'https://semopenalex.org/work/W1981719736', 'https://semopenalex.org/work/W4293105619', 'https://semopenalex.org/work/W2344152126', 'https://semopenalex.org/work/W4283121050', 'https://semopenalex.org/work/W3052245613', 'https://semopenalex.org/work/W4393635391', 'https://semopenalex.org/work/W4317438846', 'https://semopenalex.org/work/W4404350797', 'https://semopenalex.org/work/W2102773241', 'https://semopenalex.org/work/W3088922018', 'https://semopenalex.org/work/W2073549416', 'https://semopenalex.org/work/W1995310630', 'https://semopenalex.org/work/W4306706460', 'https://semopenalex.org/work/W2151186309', 'https://semopenalex.org/work/W4394049163', 'https://semopenalex.org/work/W2424120713', 'https://semopenalex.org/work/W4399117352', 'https://semopenalex.org/work/W2025036412', 'https://semopenalex.org/work/W22394099', 'https://semopenalex.org/work/W4403706502', 'https://semopenalex.org/work/W4396628099', 'https://semopenalex.org/work/W2990965235', 'https://semopenalex.org/work/W2184516195', 'https://semopenalex.org/work/W3153580448', 'https://semopenalex.org/work/W2041991478', 'https://semopenalex.org/work/W2046727875', 'https://semopenalex.org/work/W1974715273', 'https://semopenalex.org/work/W2106327888', 'https://semopenalex.org/work/W3122345191', 'https://semopenalex.org/work/W2080485692', 'https://semopenalex.org/work/W2793061613', 'https://semopenalex.org/work/W1892888926', 'https://semopenalex.org/work/W1546420109', 'https://semopenalex.org/work/W3174896615', 'https://semopenalex.org/work/W2912891501', 'https://semopenalex.org/work/W2772476628', 'https://semopenalex.org/work/W3159055025', 'https://semopenalex.org/work/W2440860577', 'https://semopenalex.org/work/W2772495508', 'https://semopenalex.org/work/W2077926445', 'https://semopenalex.org/work/W2126868220', 'https://semopenalex.org/work/W4283708463', 'https://semopenalex.org/work/W2950506233', 'https://semopenalex.org/work/W3012851928', 'https://semopenalex.org/work/W2122476743', 'https://semopenalex.org/work/W2077846458', 'https://semopenalex.org/work/W3105123138', 'https://semopenalex.org/work/W4380433250', 'https://semopenalex.org/work/W2951240690', 'https://semopenalex.org/work/W4404180533', 'https://semopenalex.org/work/W4200386693', 'https://semopenalex.org/work/W1579468036', 'https://semopenalex.org/work/W3214995238', 'https://semopenalex.org/work/W2951520541', 'https://semopenalex.org/work/W4232242059', 'https://semopenalex.org/work/W2734465187', 'https://semopenalex.org/work/W2557438307', 'https://semopenalex.org/work/W1594237328', 'https://semopenalex.org/work/W4306706940', 'https://semopenalex.org/work/W4313007851', 'https://semopenalex.org/work/W4375927790', 'https://semopenalex.org/work/W2020493833', 'https://semopenalex.org/work/W3114057505', 'https://semopenalex.org/work/W2487722436', 'https://semopenalex.org/work/W1984473368', 'https://semopenalex.org/work/W4237499061', 'https://semopenalex.org/work/W2067642869', 'https://semopenalex.org/work/W4285140876', 'https://semopenalex.org/work/W4390784356', 'https://semopenalex.org/work/W2766641608', 'https://semopenalex.org/work/W2773234510', 'https://semopenalex.org/work/W3125272485', 'https://semopenalex.org/work/W4239701257', 'https://semopenalex.org/work/W2901246026', 'https://semopenalex.org/work/W2507120666', 'https://semopenalex.org/work/W4405448580', 'https://semopenalex.org/work/W2021445484', 'https://semopenalex.org/work/W4302806', 'https://semopenalex.org/work/W4391892492', 'https://semopenalex.org/work/W53369794', 'https://semopenalex.org/work/W2036965066']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2759844371', 'https://semopenalex.org/work/W3171874410', 'https://semopenalex.org/work/W245480222', 'https://semopenalex.org/work/W2992326856', 'https://semopenalex.org/work/W2749915073', 'https://semopenalex.org/work/W2895365144', 'https://semopenalex.org/work/W1497133195', 'https://semopenalex.org/work/W2475234954', 'https://semopenalex.org/work/W2990740408', 'https://semopenalex.org/work/W3082423688', 'https://semopenalex.org/work/W2485827646', 'https://semopenalex.org/work/W2618538987', 'https://semopenalex.org/work/W2905528077', 'https://semopenalex.org/work/W1542554459', 'https://semopenalex.org/work/W2792530018', 'https://semopenalex.org/work/W2946816105', 'https://semopenalex.org/work/W2485416095', 'https://semopenalex.org/work/W110371783', 'https://semopenalex.org/work/W2768698326', 'https://semopenalex.org/work/W88942648', 'https://semopenalex.org/work/W2525511442', 'https://semopenalex.org/work/W4317743417', 'https://semopenalex.org/work/W3093904374', 'https://semopenalex.org/work/W3004959688', 'https://semopenalex.org/work/W17468934', 'https://semopenalex.org/work/W2521279915', 'https://semopenalex.org/work/W2972771325', 'https://semopenalex.org/work/W2499042039', 'https://semopenalex.org/work/W164245990', 'https://semopenalex.org/work/W1491368226', 'https://semopenalex.org/work/W2934430003', 'https://semopenalex.org/work/W2519725791', 'https://semopenalex.org/work/W2759156905', 'https://semopenalex.org/work/W2403056045', 'https://semopenalex.org/work/W2945130429', 'https://semopenalex.org/work/W4307540197', 'https://semopenalex.org/work/W369652278', 'https://semopenalex.org/work/W2800536240', 'https://semopenalex.org/work/W4402905786', 'https://semopenalex.org/work/W3145615144', 'https://semopenalex.org/work/W2471512599', 'https://semopenalex.org/work/W2618805771', 'https://semopenalex.org/work/W2945468257', 'https://semopenalex.org/work/W2338915076', 'https://semopenalex.org/work/W2751786971', 'https://semopenalex.org/work/W1554337061', 'https://semopenalex.org/work/W3163818535', 'https://semopenalex.org/work/W2620328864', 'https://semopenalex.org/work/W2341278403', 'https://semopenalex.org/work/W620578786', 'https://semopenalex.org/work/W3146451828', 'https://semopenalex.org/work/W2497589022', 'https://semopenalex.org/work/W2404426467', 'https://semopenalex.org/work/W2618579849', 'https://semopenalex.org/work/W2618660430', 'https://semopenalex.org/work/W3093823430', 'https://semopenalex.org/work/W2172124872', 'https://semopenalex.org/work/W2016390608', 'https://semopenalex.org/work/W3140161002', 'https://semopenalex.org/work/W2277087513', 'https://semopenalex.org/work/W2520607372', 'https://semopenalex.org/work/W82707212', 'https://semopenalex.org/work/W2282418302', 'https://semopenalex.org/work/W2995766444', 'https://semopenalex.org/work/W2801765505', 'https://semopenalex.org/work/W2495892083', 'https://semopenalex.org/work/W802645426', 'https://semopenalex.org/work/W4307456085', 'https://semopenalex.org/work/W2142245421', 'https://semopenalex.org/work/W2344732212', 'https://semopenalex.org/work/W4386696286', 'https://semopenalex.org/work/W3201935125', 'https://semopenalex.org/work/W991337960', 'https://semopenalex.org/work/W4388100645', 'https://semopenalex.org/work/W3217720994', 'https://semopenalex.org/work/W2503647715', 'https://semopenalex.org/work/W2277556528', 'https://semopenalex.org/work/W2219349787', 'https://semopenalex.org/work/W2141692554', 'https://semopenalex.org/work/W2502519563', 'https://semopenalex.org/work/W4386141724', 'https://semopenalex.org/work/W2978289855', 'https://semopenalex.org/work/W3032139222', 'https://semopenalex.org/work/W2336060370', 'https://semopenalex.org/work/W205286942', 'https://semopenalex.org/work/W2752853118']</t>
+    <t>['https://semopenalex.org/work/W862033376', 'https://semopenalex.org/work/W4242142265', 'https://semopenalex.org/work/W1484203263', 'https://semopenalex.org/work/W2977911811', 'https://semopenalex.org/work/W4393908582', 'https://semopenalex.org/work/W4404915142', 'https://semopenalex.org/work/W2811468211', 'https://semopenalex.org/work/W3029899401', 'https://semopenalex.org/work/W3143959337', 'https://semopenalex.org/work/W2929751249', 'https://semopenalex.org/work/W3190617503', 'https://semopenalex.org/work/W1985504739', 'https://semopenalex.org/work/W3095347735', 'https://semopenalex.org/work/W2610274107', 'https://semopenalex.org/work/W1834136374', 'https://semopenalex.org/work/W2753671526', 'https://semopenalex.org/work/W4386929049', 'https://semopenalex.org/work/W2102905932', 'https://semopenalex.org/work/W2751622533', 'https://semopenalex.org/work/W2940716241', 'https://semopenalex.org/work/W2898820983', 'https://semopenalex.org/work/W4225088745', 'https://semopenalex.org/work/W4312282153', 'https://semopenalex.org/work/W4211259494', 'https://semopenalex.org/work/W4391423303', 'https://semopenalex.org/work/W4245844025', 'https://semopenalex.org/work/W4324150147', 'https://semopenalex.org/work/W2904910662', 'https://semopenalex.org/work/W1751138515', 'https://semopenalex.org/work/W1710215999', 'https://semopenalex.org/work/W4213455276', 'https://semopenalex.org/work/W4214593503', 'https://semopenalex.org/work/W2751429127', 'https://semopenalex.org/work/W3090583924', 'https://semopenalex.org/work/W2898667062', 'https://semopenalex.org/work/W2033617925', 'https://semopenalex.org/work/W2899389394', 'https://semopenalex.org/work/W2752031858', 'https://semopenalex.org/work/W2075286904', 'https://semopenalex.org/work/W4404026276', 'https://semopenalex.org/work/W4389891943', 'https://semopenalex.org/work/W2513683703', 'https://semopenalex.org/work/W2079488626', 'https://semopenalex.org/work/W2898822823', 'https://semopenalex.org/work/W4287071181', 'https://semopenalex.org/work/W2520352456', 'https://semopenalex.org/work/W3000816869', 'https://semopenalex.org/work/W4404977899', 'https://semopenalex.org/work/W2913594206', 'https://semopenalex.org/work/W2089266363', 'https://semopenalex.org/work/W4389897704', 'https://semopenalex.org/work/W2088502162', 'https://semopenalex.org/work/W2019487042', 'https://semopenalex.org/work/W4393752214', 'https://semopenalex.org/work/W4387085789', 'https://semopenalex.org/work/W4392429145', 'https://semopenalex.org/work/W2605978692', 'https://semopenalex.org/work/W3204393727', 'https://semopenalex.org/work/W2346980133', 'https://semopenalex.org/work/W3037695612', 'https://semopenalex.org/work/W2902941289', 'https://semopenalex.org/work/W2090841027', 'https://semopenalex.org/work/W4256454723', 'https://semopenalex.org/work/W2519914856', 'https://semopenalex.org/work/W4211095911', 'https://semopenalex.org/work/W3035628382', 'https://semopenalex.org/work/W3126826400', 'https://semopenalex.org/work/W2409578015', 'https://semopenalex.org/work/W1981715407', 'https://semopenalex.org/work/W3160199101', 'https://semopenalex.org/work/W3188420011', 'https://semopenalex.org/work/W4307475355', 'https://semopenalex.org/work/W3007521088', 'https://semopenalex.org/work/W2752493326', 'https://semopenalex.org/work/W2465877051', 'https://semopenalex.org/work/W4406805368', 'https://semopenalex.org/work/W1976594634', 'https://semopenalex.org/work/W4315777028', 'https://semopenalex.org/work/W2973132733', 'https://semopenalex.org/work/W3030735111', 'https://semopenalex.org/work/W2088270376', 'https://semopenalex.org/work/W4308467568', 'https://semopenalex.org/work/W2037697732', 'https://semopenalex.org/work/W3110075456', 'https://semopenalex.org/work/W3196772354', 'https://semopenalex.org/work/W2774467220', 'https://semopenalex.org/work/W2791540051', 'https://semopenalex.org/work/W2133951180', 'https://semopenalex.org/work/W2318574332', 'https://semopenalex.org/work/W4396832885', 'https://semopenalex.org/work/W4383220643', 'https://semopenalex.org/work/W2518694405', 'https://semopenalex.org/work/W2072697691', 'https://semopenalex.org/work/W4324152586', 'https://semopenalex.org/work/W2114418543', 'https://semopenalex.org/work/W2110284634', 'https://semopenalex.org/work/W4287729941', 'https://semopenalex.org/work/W2187647369', 'https://semopenalex.org/work/W3204110051', 'https://semopenalex.org/work/W2972600126', 'https://semopenalex.org/work/W4324154015', 'https://semopenalex.org/work/W2121082751', 'https://semopenalex.org/work/W3181801907', 'https://semopenalex.org/work/W4319452484', 'https://semopenalex.org/work/W2888386951', 'https://semopenalex.org/work/W2288812598', 'https://semopenalex.org/work/W4387421144', 'https://semopenalex.org/work/W2520077052', 'https://semopenalex.org/work/W3117330688', 'https://semopenalex.org/work/W2008208122', 'https://semopenalex.org/work/W3163921267', 'https://semopenalex.org/work/W3033480106', 'https://semopenalex.org/work/W2613908791', 'https://semopenalex.org/work/W2177601947', 'https://semopenalex.org/work/W2977617583', 'https://semopenalex.org/work/W2752658305', 'https://semopenalex.org/work/W3161974712', 'https://semopenalex.org/work/W2975736083', 'https://semopenalex.org/work/W4404373433', 'https://semopenalex.org/work/W2981708234', 'https://semopenalex.org/work/W2986358413', 'https://semopenalex.org/work/W2154752229', 'https://semopenalex.org/work/W2972419497', 'https://semopenalex.org/work/W3033839905', 'https://semopenalex.org/work/W1877041815', 'https://semopenalex.org/work/W4200018492', 'https://semopenalex.org/work/W4389256452', 'https://semopenalex.org/work/W2515389026', 'https://semopenalex.org/work/W4283397308', 'https://semopenalex.org/work/W4366549587', 'https://semopenalex.org/work/W3165155612', 'https://semopenalex.org/work/W4394825420', 'https://semopenalex.org/work/W3200245219', 'https://semopenalex.org/work/W2795503716', 'https://semopenalex.org/work/W2611151946', 'https://semopenalex.org/work/W2789478762', 'https://semopenalex.org/work/W4366547357', 'https://semopenalex.org/work/W4324150573', 'https://semopenalex.org/work/W3177151358', 'https://semopenalex.org/work/W2977597077', 'https://semopenalex.org/work/W3171875220', 'https://semopenalex.org/work/W2942324097', 'https://semopenalex.org/work/W3160545975', 'https://semopenalex.org/work/W4377250056', 'https://semopenalex.org/work/W4224255688', 'https://semopenalex.org/work/W4230967253', 'https://semopenalex.org/work/W2978280554', 'https://semopenalex.org/work/W4312646439', 'https://semopenalex.org/work/W2738622408', 'https://semopenalex.org/work/W2754101670', 'https://semopenalex.org/work/W2898627444', 'https://semopenalex.org/work/W2007978709', 'https://semopenalex.org/work/W4386163788', 'https://semopenalex.org/work/W2557881781', 'https://semopenalex.org/work/W4241528240', 'https://semopenalex.org/work/W2899470128', 'https://semopenalex.org/work/W2790187313', 'https://semopenalex.org/work/W2611685970', 'https://semopenalex.org/work/W1246643588', 'https://semopenalex.org/work/W4292261957', 'https://semopenalex.org/work/W4294891921', 'https://semopenalex.org/work/W2131570437', 'https://semopenalex.org/work/W4224242333', 'https://semopenalex.org/work/W3096658838', 'https://semopenalex.org/work/W2598459295', 'https://semopenalex.org/work/W3030149602', 'https://semopenalex.org/work/W4404569483', 'https://semopenalex.org/work/W2344158693', 'https://semopenalex.org/work/W2156243282', 'https://semopenalex.org/work/W2057014910', 'https://semopenalex.org/work/W4399763801', 'https://semopenalex.org/work/W3188766356', 'https://semopenalex.org/work/W2108512685', 'https://semopenalex.org/work/W4220905243', 'https://semopenalex.org/work/W2902563098', 'https://semopenalex.org/work/W2017727997', 'https://semopenalex.org/work/W3028180736', 'https://semopenalex.org/work/W4210450354', 'https://semopenalex.org/work/W1985142918', 'https://semopenalex.org/work/W3033866035', 'https://semopenalex.org/work/W4379879736', 'https://semopenalex.org/work/W3112090964', 'https://semopenalex.org/work/W4366583934', 'https://semopenalex.org/work/W2012358521', 'https://semopenalex.org/work/W3036463368', 'https://semopenalex.org/work/W3162177365', 'https://semopenalex.org/work/W2273076933', 'https://semopenalex.org/work/W3084729599', 'https://semopenalex.org/work/W3194688439', 'https://semopenalex.org/work/W2294361658', 'https://semopenalex.org/work/W2810881717', 'https://semopenalex.org/work/W2901616108', 'https://semopenalex.org/work/W1568803211', 'https://semopenalex.org/work/W2561633795', 'https://semopenalex.org/work/W2256119246', 'https://semopenalex.org/work/W4366583171', 'https://semopenalex.org/work/W4310446060', 'https://semopenalex.org/work/W2921058600', 'https://semopenalex.org/work/W2755164339', 'https://semopenalex.org/work/W2159491375', 'https://semopenalex.org/work/W4366597679', 'https://semopenalex.org/work/W1510660243', 'https://semopenalex.org/work/W2775793881', 'https://semopenalex.org/work/W2903849727', 'https://semopenalex.org/work/W1704771702', 'https://semopenalex.org/work/W4241289669', 'https://semopenalex.org/work/W2913475584', 'https://semopenalex.org/work/W3141512745', 'https://semopenalex.org/work/W3094759305', 'https://semopenalex.org/work/W2033680836', 'https://semopenalex.org/work/W4391210282', 'https://semopenalex.org/work/W2294561329', 'https://semopenalex.org/work/W1522158218', 'https://semopenalex.org/work/W1965526182', 'https://semopenalex.org/work/W2078369692', 'https://semopenalex.org/work/W2897414246', 'https://semopenalex.org/work/W4312572845', 'https://semopenalex.org/work/W3196785132', 'https://semopenalex.org/work/W2793897377', 'https://semopenalex.org/work/W1982984133', 'https://semopenalex.org/work/W2942738233', 'https://semopenalex.org/work/W3203088685', 'https://semopenalex.org/work/W4312841490', 'https://semopenalex.org/work/W4239396382', 'https://semopenalex.org/work/W4230032809', 'https://semopenalex.org/work/W3121062173', 'https://semopenalex.org/work/W4233748389', 'https://semopenalex.org/work/W2102667737', 'https://semopenalex.org/work/W3163521409', 'https://semopenalex.org/work/W3197280612', 'https://semopenalex.org/work/W3215451397', 'https://semopenalex.org/work/W3201213010', 'https://semopenalex.org/work/W2978422619', 'https://semopenalex.org/work/W3034123328', 'https://semopenalex.org/work/W2346027641', 'https://semopenalex.org/work/W2576215493', 'https://semopenalex.org/work/W4224305168', 'https://semopenalex.org/work/W4394883037', 'https://semopenalex.org/work/W2973016298', 'https://semopenalex.org/work/W3003204379', 'https://semopenalex.org/work/W2752561456', 'https://semopenalex.org/work/W2762577600', 'https://semopenalex.org/work/W2896178739', 'https://semopenalex.org/work/W2063007215', 'https://semopenalex.org/work/W4234952088', 'https://semopenalex.org/work/W2903417746', 'https://semopenalex.org/work/W4214504130', 'https://semopenalex.org/work/W2972889118', 'https://semopenalex.org/work/W3186694431', 'https://semopenalex.org/work/W2519458229', 'https://semopenalex.org/work/W3119309106', 'https://semopenalex.org/work/W2977979696', 'https://semopenalex.org/work/W2519730427', 'https://semopenalex.org/work/W3135072684', 'https://semopenalex.org/work/W3015284588', 'https://semopenalex.org/work/W2461856634', 'https://semopenalex.org/work/W2962975962', 'https://semopenalex.org/work/W3182364466', 'https://semopenalex.org/work/W3202016550', 'https://semopenalex.org/work/W4401406766', 'https://semopenalex.org/work/W3162832522', 'https://semopenalex.org/work/W3009160614', 'https://semopenalex.org/work/W3022986551', 'https://semopenalex.org/work/W3033704563', 'https://semopenalex.org/work/W4312605566', 'https://semopenalex.org/work/W2885122621', 'https://semopenalex.org/work/W2602397751', 'https://semopenalex.org/work/W4214684069', 'https://semopenalex.org/work/W2055070571', 'https://semopenalex.org/work/W4229043996', 'https://semopenalex.org/work/W2129488573', 'https://semopenalex.org/work/W2768260654', 'https://semopenalex.org/work/W2752042616', 'https://semopenalex.org/work/W2737450254', 'https://semopenalex.org/work/W2725971658', 'https://semopenalex.org/work/W2108911539', 'https://semopenalex.org/work/W4402722090', 'https://semopenalex.org/work/W3163327897', 'https://semopenalex.org/work/W3178374478', 'https://semopenalex.org/work/W2973140914', 'https://semopenalex.org/work/W1998431265', 'https://semopenalex.org/work/W3035727063', 'https://semopenalex.org/work/W4404873047', 'https://semopenalex.org/work/W3163085734', 'https://semopenalex.org/work/W3096988350', 'https://semopenalex.org/work/W4366967286', 'https://semopenalex.org/work/W2052607251', 'https://semopenalex.org/work/W4379033872', 'https://semopenalex.org/work/W3142764819', 'https://semopenalex.org/work/W3024164567', 'https://semopenalex.org/work/W2087800309', 'https://semopenalex.org/work/W2263778529', 'https://semopenalex.org/work/W2519558346', 'https://semopenalex.org/work/W4366598255', 'https://semopenalex.org/work/W791468510', 'https://semopenalex.org/work/W2567779880', 'https://semopenalex.org/work/W2091382943', 'https://semopenalex.org/work/W3028614762', 'https://semopenalex.org/work/W3193396842', 'https://semopenalex.org/work/W2798335699', 'https://semopenalex.org/work/W2520661109', 'https://semopenalex.org/work/W2548042282', 'https://semopenalex.org/work/W2551155618', 'https://semopenalex.org/work/W4393067390', 'https://semopenalex.org/work/W3201451193', 'https://semopenalex.org/work/W3184531492', 'https://semopenalex.org/work/W3206366132', 'https://semopenalex.org/work/W3206712787', 'https://semopenalex.org/work/W2061583538', 'https://semopenalex.org/work/W4400430993', 'https://semopenalex.org/work/W2909558410', 'https://semopenalex.org/work/W2625122753', 'https://semopenalex.org/work/W3032857618', 'https://semopenalex.org/work/W3003369003', 'https://semopenalex.org/work/W2602429360', 'https://semopenalex.org/work/W3161889270', 'https://semopenalex.org/work/W3011317564', 'https://semopenalex.org/work/W1975028026', 'https://semopenalex.org/work/W2067004171', 'https://semopenalex.org/work/W4200616097', 'https://semopenalex.org/work/W2898145840', 'https://semopenalex.org/work/W2024357873', 'https://semopenalex.org/work/W2968293343', 'https://semopenalex.org/work/W3183940262', 'https://semopenalex.org/work/W2795581336', 'https://semopenalex.org/work/W4309619903', 'https://semopenalex.org/work/W4238249729', 'https://semopenalex.org/work/W2060118520', 'https://semopenalex.org/work/W3047192924', 'https://semopenalex.org/work/W2139733095', 'https://semopenalex.org/work/W2968884122', 'https://semopenalex.org/work/W4251839844', 'https://semopenalex.org/work/W2899333601', 'https://semopenalex.org/work/W2920869031', 'https://semopenalex.org/work/W3032662532', 'https://semopenalex.org/work/W2753801751', 'https://semopenalex.org/work/W3028790862', 'https://semopenalex.org/work/W2054886944', 'https://semopenalex.org/work/W2169202944', 'https://semopenalex.org/work/W2537880674', 'https://semopenalex.org/work/W2137846113', 'https://semopenalex.org/work/W2119929248', 'https://semopenalex.org/work/W3062298123', 'https://semopenalex.org/work/W2895512277', 'https://semopenalex.org/work/W1860259465', 'https://semopenalex.org/work/W2293208404', 'https://semopenalex.org/work/W2899305210', 'https://semopenalex.org/work/W4210768549', 'https://semopenalex.org/work/W2978827769', 'https://semopenalex.org/work/W4400189062', 'https://semopenalex.org/work/W3193717464', 'https://semopenalex.org/work/W4361189030', 'https://semopenalex.org/work/W4399126764', 'https://semopenalex.org/work/W2591593006', 'https://semopenalex.org/work/W3091007149', 'https://semopenalex.org/work/W4225133274', 'https://semopenalex.org/work/W2519250278', 'https://semopenalex.org/work/W2149683870', 'https://semopenalex.org/work/W4387606708', 'https://semopenalex.org/work/W2136876773', 'https://semopenalex.org/work/W4225473762', 'https://semopenalex.org/work/W3031395001', 'https://semopenalex.org/work/W4385856456', 'https://semopenalex.org/work/W2410138785', 'https://semopenalex.org/work/W4324151651', 'https://semopenalex.org/work/W2082538501', 'https://semopenalex.org/work/W2755506150', 'https://semopenalex.org/work/W2165066165', 'https://semopenalex.org/work/W2092202628', 'https://semopenalex.org/work/W2753363725', 'https://semopenalex.org/work/W3110591323', 'https://semopenalex.org/work/W4402722131', 'https://semopenalex.org/work/W2068367136', 'https://semopenalex.org/work/W3095367321', 'https://semopenalex.org/work/W1993984611', 'https://semopenalex.org/work/W2976524236', 'https://semopenalex.org/work/W3112877194', 'https://semopenalex.org/work/W3095740806', 'https://semopenalex.org/work/W4224279084', 'https://semopenalex.org/work/W2972759039', 'https://semopenalex.org/work/W4200525013', 'https://semopenalex.org/work/W2346600598', 'https://semopenalex.org/work/W1553133540', 'https://semopenalex.org/work/W3198359754', 'https://semopenalex.org/work/W3121775658', 'https://semopenalex.org/work/W1993514406', 'https://semopenalex.org/work/W2944843734', 'https://semopenalex.org/work/W3130372017', 'https://semopenalex.org/work/W2152557601', 'https://semopenalex.org/work/W2080327955', 'https://semopenalex.org/work/W2921194733', 'https://semopenalex.org/work/W2972702127', 'https://semopenalex.org/work/W2921533080', 'https://semopenalex.org/work/W4232727837', 'https://semopenalex.org/work/W1771936601', 'https://semopenalex.org/work/W1524596993', 'https://semopenalex.org/work/W2752490344', 'https://semopenalex.org/work/W4393067517', 'https://semopenalex.org/work/W4221065578', 'https://semopenalex.org/work/W2401872729', 'https://semopenalex.org/work/W2750727230', 'https://semopenalex.org/work/W2946308339', 'https://semopenalex.org/work/W2528963299', 'https://semopenalex.org/work/W2973046614', 'https://semopenalex.org/work/W3161959528', 'https://semopenalex.org/work/W2072490274', 'https://semopenalex.org/work/W4366588423', 'https://semopenalex.org/work/W3005470382', 'https://semopenalex.org/work/W4307204790', 'https://semopenalex.org/work/W2610780371', 'https://semopenalex.org/work/W2966384546', 'https://semopenalex.org/work/W3161202338', 'https://semopenalex.org/work/W3163078982', 'https://semopenalex.org/work/W4393102879', 'https://semopenalex.org/work/W3030577208', 'https://semopenalex.org/work/W3043824623', 'https://semopenalex.org/work/W2736312195', 'https://semopenalex.org/work/W2610676428', 'https://semopenalex.org/work/W4393877125']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W4404180354', 'https://semopenalex.org/work/W2805393243', 'https://semopenalex.org/work/W2149498440', 'https://semopenalex.org/work/W3121529680', 'https://semopenalex.org/work/W22394099', 'https://semopenalex.org/work/W1479774717', 'https://semopenalex.org/work/W4400268996', 'https://semopenalex.org/work/W4388742679', 'https://semopenalex.org/work/W3077087723', 'https://semopenalex.org/work/W75044610', 'https://semopenalex.org/work/W2610117056', 'https://semopenalex.org/work/W4309613628', 'https://semopenalex.org/work/W2916230113', 'https://semopenalex.org/work/W2155277804', 'https://semopenalex.org/work/W4402599958', 'https://semopenalex.org/work/W2152979493', 'https://semopenalex.org/work/W139217162', 'https://semopenalex.org/work/W4400881052', 'https://semopenalex.org/work/W2073549416', 'https://semopenalex.org/work/W4404788249', 'https://semopenalex.org/work/W2919684758', 'https://semopenalex.org/work/W610311842', 'https://semopenalex.org/work/W1565188338', 'https://semopenalex.org/work/W2793061613', 'https://semopenalex.org/work/W4388989593', 'https://semopenalex.org/work/W3045638492', 'https://semopenalex.org/work/W2796403873', 'https://semopenalex.org/work/W2901246026', 'https://semopenalex.org/work/W2122476743', 'https://semopenalex.org/work/W4394048733', 'https://semopenalex.org/work/W2951057438', 'https://semopenalex.org/work/W4394576023', 'https://semopenalex.org/work/W4255591746', 'https://semopenalex.org/work/W4309647912', 'https://semopenalex.org/work/W2422116896', 'https://semopenalex.org/work/W4405828728', 'https://semopenalex.org/work/W2915383148', 'https://semopenalex.org/work/W3001462578', 'https://semopenalex.org/work/W4387293718', 'https://semopenalex.org/work/W2809590475', 'https://semopenalex.org/work/W4213388674', 'https://semopenalex.org/work/W4401110041', 'https://semopenalex.org/work/W2131027594', 'https://semopenalex.org/work/W2479269651', 'https://semopenalex.org/work/W2052330128', 'https://semopenalex.org/work/W4232799872', 'https://semopenalex.org/work/W1660366533', 'https://semopenalex.org/work/W1974446585', 'https://semopenalex.org/work/W2008632807', 'https://semopenalex.org/work/W2046727875', 'https://semopenalex.org/work/W2920007056', 'https://semopenalex.org/work/W3124693625', 'https://semopenalex.org/work/W1988741859', 'https://semopenalex.org/work/W4395064999', 'https://semopenalex.org/work/W4283708463', 'https://semopenalex.org/work/W4294578223', 'https://semopenalex.org/work/W2138607828', 'https://semopenalex.org/work/W4385270466', 'https://semopenalex.org/work/W2156065383', 'https://semopenalex.org/work/W1566552779', 'https://semopenalex.org/work/W4389880140', 'https://semopenalex.org/work/W2770240327', 'https://semopenalex.org/work/W1493881734', 'https://semopenalex.org/work/W2140346433', 'https://semopenalex.org/work/W4380136543', 'https://semopenalex.org/work/W4288549248', 'https://semopenalex.org/work/W3175986586', 'https://semopenalex.org/work/W4226040560', 'https://semopenalex.org/work/W2478525669', 'https://semopenalex.org/work/W2033132959', 'https://semopenalex.org/work/W3088922018', 'https://semopenalex.org/work/W3066802614', 'https://semopenalex.org/work/W2009396504', 'https://semopenalex.org/work/W2808185912', 'https://semopenalex.org/work/W4400611446', 'https://semopenalex.org/work/W4309325586', 'https://semopenalex.org/work/W4390570315', 'https://semopenalex.org/work/W2036885872', 'https://semopenalex.org/work/W3153580448', 'https://semopenalex.org/work/W2476253347', 'https://semopenalex.org/work/W3110928664', 'https://semopenalex.org/work/W2900798442', 'https://semopenalex.org/work/W1938912534', 'https://semopenalex.org/work/W2778221989', 'https://semopenalex.org/work/W2901185014', 'https://semopenalex.org/work/W4252278539', 'https://semopenalex.org/work/W2136344560', 'https://semopenalex.org/work/W2915831115', 'https://semopenalex.org/work/W2092295977', 'https://semopenalex.org/work/W4289364680', 'https://semopenalex.org/work/W3159055025', 'https://semopenalex.org/work/W1500858206', 'https://semopenalex.org/work/W2908443740', 'https://semopenalex.org/work/W4200386693', 'https://semopenalex.org/work/W3097074140', 'https://semopenalex.org/work/W2616473319', 'https://semopenalex.org/work/W4405522042', 'https://semopenalex.org/work/W2165611534', 'https://semopenalex.org/work/W4403792402', 'https://semopenalex.org/work/W1507246359', 'https://semopenalex.org/work/W2003420345', 'https://semopenalex.org/work/W4391973940', 'https://semopenalex.org/work/W3082096159', 'https://semopenalex.org/work/W2184516195', 'https://semopenalex.org/work/W4293105619', 'https://semopenalex.org/work/W2321758884', 'https://semopenalex.org/work/W3052245613', 'https://semopenalex.org/work/W2117052376', 'https://semopenalex.org/work/W2040345481', 'https://semopenalex.org/work/W2296355030', 'https://semopenalex.org/work/W2198834745', 'https://semopenalex.org/work/W2551266388', 'https://semopenalex.org/work/W4406261609', 'https://semopenalex.org/work/W4362501917', 'https://semopenalex.org/work/W1581509591', 'https://semopenalex.org/work/W2422465781', 'https://semopenalex.org/work/W2116893958', 'https://semopenalex.org/work/W4213121575', 'https://semopenalex.org/work/W2075258117', 'https://semopenalex.org/work/W2901563117', 'https://semopenalex.org/work/W206771271', 'https://semopenalex.org/work/W2912179439', 'https://semopenalex.org/work/W2775115790', 'https://semopenalex.org/work/W2805105531', 'https://semopenalex.org/work/W4231180551', 'https://semopenalex.org/work/W3162065424', 'https://semopenalex.org/work/W2439110316', 'https://semopenalex.org/work/W4401719105', 'https://semopenalex.org/work/W4386474911', 'https://semopenalex.org/work/W3105123138', 'https://semopenalex.org/work/W1601136399', 'https://semopenalex.org/work/W3140378604', 'https://semopenalex.org/work/W2170735098', 'https://semopenalex.org/work/W3103436608', 'https://semopenalex.org/work/W4226150381', 'https://semopenalex.org/work/W4378768161', 'https://semopenalex.org/work/W3177070127', 'https://semopenalex.org/work/W3098889210', 'https://semopenalex.org/work/W2126868220', 'https://semopenalex.org/work/W4393748815', 'https://semopenalex.org/work/W4226214859', 'https://semopenalex.org/work/W4393635391', 'https://semopenalex.org/work/W2068346480', 'https://semopenalex.org/work/W2515387399', 'https://semopenalex.org/work/W1546420109', 'https://semopenalex.org/work/W1702322733', 'https://semopenalex.org/work/W2791022910', 'https://semopenalex.org/work/W4306706940', 'https://semopenalex.org/work/W4393969247', 'https://semopenalex.org/work/W2918375401', 'https://semopenalex.org/work/W1980320703', 'https://semopenalex.org/work/W1974608646', 'https://semopenalex.org/work/W2905317998', 'https://semopenalex.org/work/W2344677227', 'https://semopenalex.org/work/W2991281508', 'https://semopenalex.org/work/W2048339977', 'https://semopenalex.org/work/W4392110461', 'https://semopenalex.org/work/W2484289073', 'https://semopenalex.org/work/W4406729944', 'https://semopenalex.org/work/W3013272684', 'https://semopenalex.org/work/W1985846348', 'https://semopenalex.org/work/W192156609', 'https://semopenalex.org/work/W3140552826', 'https://semopenalex.org/work/W2756536429', 'https://semopenalex.org/work/W4250963083', 'https://semopenalex.org/work/W4316672181', 'https://semopenalex.org/work/W4389509728', 'https://semopenalex.org/work/W4211034214', 'https://semopenalex.org/work/W2920780560', 'https://semopenalex.org/work/W4391248380', 'https://semopenalex.org/work/W3200087552', 'https://semopenalex.org/work/W2772476628', 'https://semopenalex.org/work/W2795633027', 'https://semopenalex.org/work/W4380433250', 'https://semopenalex.org/work/W2151186309', 'https://semopenalex.org/work/W2991585802', 'https://semopenalex.org/work/W4391661476', 'https://semopenalex.org/work/W2041919000', 'https://semopenalex.org/work/W4399554294', 'https://semopenalex.org/work/W2953012688', 'https://semopenalex.org/work/W4316116419', 'https://semopenalex.org/work/W3216694898', 'https://semopenalex.org/work/W2612035199', 'https://semopenalex.org/work/W1984186194', 'https://semopenalex.org/work/W3010046448', 'https://semopenalex.org/work/W4312911917', 'https://semopenalex.org/work/W1983176793', 'https://semopenalex.org/work/W2507120666', 'https://semopenalex.org/work/W4283643625', 'https://semopenalex.org/work/W23340818', 'https://semopenalex.org/work/W3004495293', 'https://semopenalex.org/work/W3112151564', 'https://semopenalex.org/work/W2912891501', 'https://semopenalex.org/work/W4286794087', 'https://semopenalex.org/work/W2118486116', 'https://semopenalex.org/work/W4365205158', 'https://semopenalex.org/work/W125254009', 'https://semopenalex.org/work/W2990448760', 'https://semopenalex.org/work/W3149145084', 'https://semopenalex.org/work/W2505162744', 'https://semopenalex.org/work/W1481252923', 'https://semopenalex.org/work/W2548544249', 'https://semopenalex.org/work/W2125430046', 'https://semopenalex.org/work/W2030563576', 'https://semopenalex.org/work/W1492139710', 'https://semopenalex.org/work/W2076165157', 'https://semopenalex.org/work/W4232691833', 'https://semopenalex.org/work/W2087831714', 'https://semopenalex.org/work/W2746969608', 'https://semopenalex.org/work/W2766641608', 'https://semopenalex.org/work/W4391892492', 'https://semopenalex.org/work/W2467591515', 'https://semopenalex.org/work/W1720341833', 'https://semopenalex.org/work/W4221168020', 'https://semopenalex.org/work/W3038546681', 'https://semopenalex.org/work/W4381855531', 'https://semopenalex.org/work/W4405305567', 'https://semopenalex.org/work/W1496034358', 'https://semopenalex.org/work/W2097959755', 'https://semopenalex.org/work/W2584286364', 'https://semopenalex.org/work/W2134387352', 'https://semopenalex.org/work/W4221002597', 'https://semopenalex.org/work/W2623350311', 'https://semopenalex.org/work/W4362502008', 'https://semopenalex.org/work/W2329646465', 'https://semopenalex.org/work/W3203105904', 'https://semopenalex.org/work/W1986302656', 'https://semopenalex.org/work/W2738171721', 'https://semopenalex.org/work/W2899754551', 'https://semopenalex.org/work/W2990965235', 'https://semopenalex.org/work/W2124874701', 'https://semopenalex.org/work/W4302806', 'https://semopenalex.org/work/W3114057505', 'https://semopenalex.org/work/W4381549091', 'https://semopenalex.org/work/W2098055383', 'https://semopenalex.org/work/W3122406465', 'https://semopenalex.org/work/W4402594156', 'https://semopenalex.org/work/W2146501308', 'https://semopenalex.org/work/W3174896615', 'https://semopenalex.org/work/W4396594158', 'https://semopenalex.org/work/W2080485692', 'https://semopenalex.org/work/W3116763688', 'https://semopenalex.org/work/W4317438183', 'https://semopenalex.org/work/W3214995238', 'https://semopenalex.org/work/W4294707045', 'https://semopenalex.org/work/W2506885748', 'https://semopenalex.org/work/W3162622638', 'https://semopenalex.org/work/W2086824798', 'https://semopenalex.org/work/W4289866493', 'https://semopenalex.org/work/W2051680663', 'https://semopenalex.org/work/W3090908182', 'https://semopenalex.org/work/W2284502685', 'https://semopenalex.org/work/W2748668979', 'https://semopenalex.org/work/W79646937', 'https://semopenalex.org/work/W1984473368', 'https://semopenalex.org/work/W4404252082', 'https://semopenalex.org/work/W1563606705', 'https://semopenalex.org/work/W1517726756', 'https://semopenalex.org/work/W1981719736', 'https://semopenalex.org/work/W2898587907', 'https://semopenalex.org/work/W1495063990', 'https://semopenalex.org/work/W2468217693', 'https://semopenalex.org/work/W3066383670', 'https://semopenalex.org/work/W3126556715', 'https://semopenalex.org/work/W2735732687', 'https://semopenalex.org/work/W4401023469', 'https://semopenalex.org/work/W2795298263', 'https://semopenalex.org/work/W2502765568', 'https://semopenalex.org/work/W3210789515', 'https://semopenalex.org/work/W2515263588', 'https://semopenalex.org/work/W2033368298', 'https://semopenalex.org/work/W2511600948', 'https://semopenalex.org/work/W2077564315', 'https://semopenalex.org/work/W3124266007', 'https://semopenalex.org/work/W4404350797', 'https://semopenalex.org/work/W4404370664', 'https://semopenalex.org/work/W10552456', 'https://semopenalex.org/work/W4402595291', 'https://semopenalex.org/work/W4367682485', 'https://semopenalex.org/work/W3008028280', 'https://semopenalex.org/work/W2141276288', 'https://semopenalex.org/work/W2464669661', 'https://semopenalex.org/work/W4312471121', 'https://semopenalex.org/work/W4313007851', 'https://semopenalex.org/work/W4396628099', 'https://semopenalex.org/work/W4400812269', 'https://semopenalex.org/work/W1664839614', 'https://semopenalex.org/work/W2089975859', 'https://semopenalex.org/work/W4406794085', 'https://semopenalex.org/work/W2337491900', 'https://semopenalex.org/work/W2990317423', 'https://semopenalex.org/work/W3176873809', 'https://semopenalex.org/work/W1484038335', 'https://semopenalex.org/work/W2500329317', 'https://semopenalex.org/work/W2792554287', 'https://semopenalex.org/work/W4391673335', 'https://semopenalex.org/work/W2032640310', 'https://semopenalex.org/work/W4323923480', 'https://semopenalex.org/work/W4244365690', 'https://semopenalex.org/work/W1600095712', 'https://semopenalex.org/work/W2013870117', 'https://semopenalex.org/work/W2615044227', 'https://semopenalex.org/work/W2772495508', 'https://semopenalex.org/work/W2902564735', 'https://semopenalex.org/work/W4220938834', 'https://semopenalex.org/work/W2000718212', 'https://semopenalex.org/work/W2036965066', 'https://semopenalex.org/work/W4319792183', 'https://semopenalex.org/work/W3024403368', 'https://semopenalex.org/work/W2133544364', 'https://semopenalex.org/work/W4386346214', 'https://semopenalex.org/work/W2798444339', 'https://semopenalex.org/work/W4380885381', 'https://semopenalex.org/work/W2991082611', 'https://semopenalex.org/work/W2017629483', 'https://semopenalex.org/work/W4317619163', 'https://semopenalex.org/work/W2901968423', 'https://semopenalex.org/work/W3130665718', 'https://semopenalex.org/work/W2951240690', 'https://semopenalex.org/work/W2889404430', 'https://semopenalex.org/work/W1507429943', 'https://semopenalex.org/work/W2584636165', 'https://semopenalex.org/work/W4291287572', 'https://semopenalex.org/work/W3012851928', 'https://semopenalex.org/work/W2900534295', 'https://semopenalex.org/work/W4402538155', 'https://semopenalex.org/work/W2906612108', 'https://semopenalex.org/work/W2981705990', 'https://semopenalex.org/work/W4389226119', 'https://semopenalex.org/work/W4285292709', 'https://semopenalex.org/work/W1990240966', 'https://semopenalex.org/work/W4399117352', 'https://semopenalex.org/work/W4394049163', 'https://semopenalex.org/work/W1474354901', 'https://semopenalex.org/work/W3173479430', 'https://semopenalex.org/work/W4232242059', 'https://semopenalex.org/work/W2150949003', 'https://semopenalex.org/work/W3041363918', 'https://semopenalex.org/work/W4379964950', 'https://semopenalex.org/work/W2808806636', 'https://semopenalex.org/work/W4229056530', 'https://semopenalex.org/work/W2050276970', 'https://semopenalex.org/work/W3161264338', 'https://semopenalex.org/work/W2896561783', 'https://semopenalex.org/work/W1581844963', 'https://semopenalex.org/work/W1504659965', 'https://semopenalex.org/work/W2102773241', 'https://semopenalex.org/work/W1487391256', 'https://semopenalex.org/work/W2487722436', 'https://semopenalex.org/work/W3111943635', 'https://semopenalex.org/work/W4393144966', 'https://semopenalex.org/work/W4247657810', 'https://semopenalex.org/work/W4237499061', 'https://semopenalex.org/work/W1605123443', 'https://semopenalex.org/work/W2804252553', 'https://semopenalex.org/work/W4243814040', 'https://semopenalex.org/work/W2903414282', 'https://semopenalex.org/work/W2489798131', 'https://semopenalex.org/work/W2169290493', 'https://semopenalex.org/work/W3190788066', 'https://semopenalex.org/work/W2083708758', 'https://semopenalex.org/work/W2084970449', 'https://semopenalex.org/work/W2950506233', 'https://semopenalex.org/work/W2143252268', 'https://semopenalex.org/work/W4302859022', 'https://semopenalex.org/work/W2949205410', 'https://semopenalex.org/work/W4306706460', 'https://semopenalex.org/work/W2808066670', 'https://semopenalex.org/work/W629466361', 'https://semopenalex.org/work/W2359704875', 'https://semopenalex.org/work/W4200400669', 'https://semopenalex.org/work/W4309647909', 'https://semopenalex.org/work/W3030557354', 'https://semopenalex.org/work/W2806499268', 'https://semopenalex.org/work/W3153444696', 'https://semopenalex.org/work/W4250640589', 'https://semopenalex.org/work/W4388972775', 'https://semopenalex.org/work/W4389575859', 'https://semopenalex.org/work/W4404037007', 'https://semopenalex.org/work/W2773234510', 'https://semopenalex.org/work/W4283365825', 'https://semopenalex.org/work/W4402710970', 'https://semopenalex.org/work/W2440860577', 'https://semopenalex.org/work/W2755922538', 'https://semopenalex.org/work/W3134356917', 'https://semopenalex.org/work/W2733791027', 'https://semopenalex.org/work/W2119701885', 'https://semopenalex.org/work/W2945594129', 'https://semopenalex.org/work/W2172069600', 'https://semopenalex.org/work/W2417471897', 'https://semopenalex.org/work/W2150013559', 'https://semopenalex.org/work/W3176983082', 'https://semopenalex.org/work/W4220657425', 'https://semopenalex.org/work/W3026213155', 'https://semopenalex.org/work/W3211356533', 'https://semopenalex.org/work/W2059788348', 'https://semopenalex.org/work/W2138167749', 'https://semopenalex.org/work/W2809627415', 'https://semopenalex.org/work/W4283718670', 'https://semopenalex.org/work/W4387190940', 'https://semopenalex.org/work/W1974715273', 'https://semopenalex.org/work/W2006918362', 'https://semopenalex.org/work/W3033848960', 'https://semopenalex.org/work/W2185480307', 'https://semopenalex.org/work/W4389575826', 'https://semopenalex.org/work/W4312953992', 'https://semopenalex.org/work/W3139199248', 'https://semopenalex.org/work/W2898238060', 'https://semopenalex.org/work/W2984000149', 'https://semopenalex.org/work/W4401463259', 'https://semopenalex.org/work/W4377234328', 'https://semopenalex.org/work/W2499168780', 'https://semopenalex.org/work/W2250659747', 'https://semopenalex.org/work/W4246273094', 'https://semopenalex.org/work/W4294500063', 'https://semopenalex.org/work/W4319053914', 'https://semopenalex.org/work/W1588641552', 'https://semopenalex.org/work/W4401719068', 'https://semopenalex.org/work/W2330628472', 'https://semopenalex.org/work/W4239701257', 'https://semopenalex.org/work/W2923319240', 'https://semopenalex.org/work/W3056873248', 'https://semopenalex.org/work/W2062482216', 'https://semopenalex.org/work/W2071898607', 'https://semopenalex.org/work/W4406500025', 'https://semopenalex.org/work/W2296703446', 'https://semopenalex.org/work/W3208070608', 'https://semopenalex.org/work/W2053495332', 'https://semopenalex.org/work/W4226101170', 'https://semopenalex.org/work/W3138702399', 'https://semopenalex.org/work/W1507165467', 'https://semopenalex.org/work/W4386486628', 'https://semopenalex.org/work/W2041991478', 'https://semopenalex.org/work/W2065468011', 'https://semopenalex.org/work/W4285140876', 'https://semopenalex.org/work/W2130677504', 'https://semopenalex.org/work/W2900517348', 'https://semopenalex.org/work/W2114238248', 'https://semopenalex.org/work/W2954580762', 'https://semopenalex.org/work/W2942454712', 'https://semopenalex.org/work/W175358687', 'https://semopenalex.org/work/W2400388471', 'https://semopenalex.org/work/W2021445484', 'https://semopenalex.org/work/W4377099260', 'https://semopenalex.org/work/W2775805395', 'https://semopenalex.org/work/W2901915930', 'https://semopenalex.org/work/W1971179860', 'https://semopenalex.org/work/W4387427541', 'https://semopenalex.org/work/W4385285133', 'https://semopenalex.org/work/W2166042493', 'https://semopenalex.org/work/W2344152126', 'https://semopenalex.org/work/W2608436687', 'https://semopenalex.org/work/W4302306230', 'https://semopenalex.org/work/W2965941321', 'https://semopenalex.org/work/W3206119617', 'https://semopenalex.org/work/W2067642869', 'https://semopenalex.org/work/W2089762145', 'https://semopenalex.org/work/W2017988065', 'https://semopenalex.org/work/W4297725807', 'https://semopenalex.org/work/W4404411574', 'https://semopenalex.org/work/W53369794', 'https://semopenalex.org/work/W1608885791', 'https://semopenalex.org/work/W51883144', 'https://semopenalex.org/work/W2970882829', 'https://semopenalex.org/work/W2998494411', 'https://semopenalex.org/work/W2344504222', 'https://semopenalex.org/work/W4404788038', 'https://semopenalex.org/work/W4281629096', 'https://semopenalex.org/work/W2013042849', 'https://semopenalex.org/work/W2990998351', 'https://semopenalex.org/work/W4394867508', 'https://semopenalex.org/work/W3204280976', 'https://semopenalex.org/work/W2924425593', 'https://semopenalex.org/work/W2465409613', 'https://semopenalex.org/work/W4401689701', 'https://semopenalex.org/work/W1497322082', 'https://semopenalex.org/work/W4206564475', 'https://semopenalex.org/work/W2077846458', 'https://semopenalex.org/work/W4312710991', 'https://semopenalex.org/work/W4405448580', 'https://semopenalex.org/work/W1992237536', 'https://semopenalex.org/work/W3106296980', 'https://semopenalex.org/work/W2005330588', 'https://semopenalex.org/work/W2613136061', 'https://semopenalex.org/work/W4255845198', 'https://semopenalex.org/work/W2066037774', 'https://semopenalex.org/work/W1892888926', 'https://semopenalex.org/work/W1971405342', 'https://semopenalex.org/work/W2550260459', 'https://semopenalex.org/work/W4376269693', 'https://semopenalex.org/work/W4292848294', 'https://semopenalex.org/work/W4402091088', 'https://semopenalex.org/work/W4402157005', 'https://semopenalex.org/work/W1608148813', 'https://semopenalex.org/work/W2152170845', 'https://semopenalex.org/work/W2052312648', 'https://semopenalex.org/work/W1527508100', 'https://semopenalex.org/work/W4406118666', 'https://semopenalex.org/work/W2594546957', 'https://semopenalex.org/work/W1980418511', 'https://semopenalex.org/work/W1995310630', 'https://semopenalex.org/work/W2949762754', 'https://semopenalex.org/work/W4237415699', 'https://semopenalex.org/work/W2293638396', 'https://semopenalex.org/work/W3012031786', 'https://semopenalex.org/work/W4388320652', 'https://semopenalex.org/work/W4385852291', 'https://semopenalex.org/work/W4404464211', 'https://semopenalex.org/work/W2084265221', 'https://semopenalex.org/work/W4287758300', 'https://semopenalex.org/work/W2986139096', 'https://semopenalex.org/work/W3101678388', 'https://semopenalex.org/work/W2422976594', 'https://semopenalex.org/work/W171268263', 'https://semopenalex.org/work/W2309229337', 'https://semopenalex.org/work/W4283121050', 'https://semopenalex.org/work/W1508670223', 'https://semopenalex.org/work/W4312262758', 'https://semopenalex.org/work/W3003707605', 'https://semopenalex.org/work/W4390137041', 'https://semopenalex.org/work/W4235399974', 'https://semopenalex.org/work/W3136943238', 'https://semopenalex.org/work/W112461364', 'https://semopenalex.org/work/W2165303722', 'https://semopenalex.org/work/W2735379054', 'https://semopenalex.org/work/W1579468036', 'https://semopenalex.org/work/W2982576723', 'https://semopenalex.org/work/W4385270603', 'https://semopenalex.org/work/W1609271133', 'https://semopenalex.org/work/W2022462411', 'https://semopenalex.org/work/W4404180533', 'https://semopenalex.org/work/W4309647894', 'https://semopenalex.org/work/W2052763829', 'https://semopenalex.org/work/W2700566289', 'https://semopenalex.org/work/W1753378771', 'https://semopenalex.org/work/W2804137108', 'https://semopenalex.org/work/W3125272485', 'https://semopenalex.org/work/W2499947387', 'https://semopenalex.org/work/W2951520541', 'https://semopenalex.org/work/W2734465187', 'https://semopenalex.org/work/W2735638814', 'https://semopenalex.org/work/W4313267141', 'https://semopenalex.org/work/W2427008665', 'https://semopenalex.org/work/W2953273686', 'https://semopenalex.org/work/W2085892029', 'https://semopenalex.org/work/W2077926445', 'https://semopenalex.org/work/W2426048753', 'https://semopenalex.org/work/W2594649443', 'https://semopenalex.org/work/W32663231', 'https://semopenalex.org/work/W2131164945', 'https://semopenalex.org/work/W2016580264', 'https://semopenalex.org/work/W2919204815', 'https://semopenalex.org/work/W3035750004', 'https://semopenalex.org/work/W4390456266', 'https://semopenalex.org/work/W2950787737', 'https://semopenalex.org/work/W4239052734', 'https://semopenalex.org/work/W4317438846', 'https://semopenalex.org/work/W4389543458', 'https://semopenalex.org/work/W2107915643', 'https://semopenalex.org/work/W2163121311', 'https://semopenalex.org/work/W2612374761', 'https://semopenalex.org/work/W1827647151', 'https://semopenalex.org/work/W2054374338', 'https://semopenalex.org/work/W4400909999', 'https://semopenalex.org/work/W1498712689', 'https://semopenalex.org/work/W4362655741', 'https://semopenalex.org/work/W4388040916', 'https://semopenalex.org/work/W433641300', 'https://semopenalex.org/work/W3015227276', 'https://semopenalex.org/work/W2922408557', 'https://semopenalex.org/work/W2909965602', 'https://semopenalex.org/work/W2903238830', 'https://semopenalex.org/work/W3200977970', 'https://semopenalex.org/work/W4301486307', 'https://semopenalex.org/work/W3167737483', 'https://semopenalex.org/work/W2730099201', 'https://semopenalex.org/work/W4376061047', 'https://semopenalex.org/work/W2557853356', 'https://semopenalex.org/work/W4287231113', 'https://semopenalex.org/work/W4287902628', 'https://semopenalex.org/work/W4230101435', 'https://semopenalex.org/work/W1594237328', 'https://semopenalex.org/work/W1934576426', 'https://semopenalex.org/work/W2089906307', 'https://semopenalex.org/work/W4404735027', 'https://semopenalex.org/work/W3157617328', 'https://semopenalex.org/work/W2920517911', 'https://semopenalex.org/work/W1524789227', 'https://semopenalex.org/work/W4317640658', 'https://semopenalex.org/work/W2025036412', 'https://semopenalex.org/work/W4233690695', 'https://semopenalex.org/work/W2735964774', 'https://semopenalex.org/work/W2007985134', 'https://semopenalex.org/work/W2110495371', 'https://semopenalex.org/work/W3122345191', 'https://semopenalex.org/work/W2897073097', 'https://semopenalex.org/work/W1968925642', 'https://semopenalex.org/work/W2003561941', 'https://semopenalex.org/work/W2557438307', 'https://semopenalex.org/work/W3097918021', 'https://semopenalex.org/work/W4402352406', 'https://semopenalex.org/work/W4402713726', 'https://semopenalex.org/work/W2020493833', 'https://semopenalex.org/work/W1554846139', 'https://semopenalex.org/work/W4223526958', 'https://semopenalex.org/work/W1793399427', 'https://semopenalex.org/work/W2998183977', 'https://semopenalex.org/work/W3179758589', 'https://semopenalex.org/work/W3107101618', 'https://semopenalex.org/work/W2063106869', 'https://semopenalex.org/work/W2045329305', 'https://semopenalex.org/work/W4404758113', 'https://semopenalex.org/work/W4406679155', 'https://semopenalex.org/work/W4405179263', 'https://semopenalex.org/work/W2167984494', 'https://semopenalex.org/work/W2025843016', 'https://semopenalex.org/work/W2167318748', 'https://semopenalex.org/work/W2908865778', 'https://semopenalex.org/work/W4233194301', 'https://semopenalex.org/work/W4317042649', 'https://semopenalex.org/work/W1715440516', 'https://semopenalex.org/work/W2424120713', 'https://semopenalex.org/work/W2587382914', 'https://semopenalex.org/work/W2106327888', 'https://semopenalex.org/work/W3112593626', 'https://semopenalex.org/work/W4399118880', 'https://semopenalex.org/work/W4252774423', 'https://semopenalex.org/work/W3163303484', 'https://semopenalex.org/work/W2147228279', 'https://semopenalex.org/work/W4399881333', 'https://semopenalex.org/work/W4390784356', 'https://semopenalex.org/work/W2092411821', 'https://semopenalex.org/work/W1688396929', 'https://semopenalex.org/work/W4312038601', 'https://semopenalex.org/work/W4391766346', 'https://semopenalex.org/work/W2027402731', 'https://semopenalex.org/work/W2088840086', 'https://semopenalex.org/work/W2404446956', 'https://semopenalex.org/work/W4403706502', 'https://semopenalex.org/work/W4375927790', 'https://semopenalex.org/work/W2065926303', 'https://semopenalex.org/work/W2494607466', 'https://semopenalex.org/work/W2063775187', 'https://semopenalex.org/work/W4386486604', 'https://semopenalex.org/work/W2794632798', 'https://semopenalex.org/work/W2557660464', 'https://semopenalex.org/work/W3023950320', 'https://semopenalex.org/work/W2032265428', 'https://semopenalex.org/work/W2491619570', 'https://semopenalex.org/work/W2251316727', 'https://semopenalex.org/work/W4320909166', 'https://semopenalex.org/work/W1510296842', 'https://semopenalex.org/work/W2795358293', 'https://semopenalex.org/work/W2554367017', 'https://semopenalex.org/work/W104210143', 'https://semopenalex.org/work/W4384756284', 'https://semopenalex.org/work/W102169640', 'https://semopenalex.org/work/W2060252439']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W2945130429', 'https://semopenalex.org/work/W3145615144', 'https://semopenalex.org/work/W1497133195', 'https://semopenalex.org/work/W2751786971', 'https://semopenalex.org/work/W2485416095', 'https://semopenalex.org/work/W620578786', 'https://semopenalex.org/work/W2945468257', 'https://semopenalex.org/work/W4386696286', 'https://semopenalex.org/work/W3217720994', 'https://semopenalex.org/work/W802645426', 'https://semopenalex.org/work/W205286942', 'https://semopenalex.org/work/W3140161002', 'https://semopenalex.org/work/W3201935125', 'https://semopenalex.org/work/W3093823430', 'https://semopenalex.org/work/W1554337061', 'https://semopenalex.org/work/W2992326856', 'https://semopenalex.org/work/W2471512599', 'https://semopenalex.org/work/W4402905786', 'https://semopenalex.org/work/W2344732212', 'https://semopenalex.org/work/W2338915076', 'https://semopenalex.org/work/W2759156905', 'https://semopenalex.org/work/W2618538987', 'https://semopenalex.org/work/W2499042039', 'https://semopenalex.org/work/W2475234954', 'https://semopenalex.org/work/W3004959688', 'https://semopenalex.org/work/W2521279915', 'https://semopenalex.org/work/W3163818535', 'https://semopenalex.org/work/W2995766444', 'https://semopenalex.org/work/W4307540197', 'https://semopenalex.org/work/W17468934', 'https://semopenalex.org/work/W2277087513', 'https://semopenalex.org/work/W4386141724', 'https://semopenalex.org/work/W2934430003', 'https://semopenalex.org/work/W3082423688', 'https://semopenalex.org/work/W1491368226', 'https://semopenalex.org/work/W2502519563', 'https://semopenalex.org/work/W1542554459', 'https://semopenalex.org/work/W2525511442', 'https://semopenalex.org/work/W2759844371', 'https://semopenalex.org/work/W2172124872', 'https://semopenalex.org/work/W3146451828', 'https://semopenalex.org/work/W2341278403', 'https://semopenalex.org/work/W2142245421', 'https://semopenalex.org/work/W2404426467', 'https://semopenalex.org/work/W2336060370', 'https://semopenalex.org/work/W2497589022', 'https://semopenalex.org/work/W4307456085', 'https://semopenalex.org/work/W3093904374', 'https://semopenalex.org/work/W2768698326', 'https://semopenalex.org/work/W369652278', 'https://semopenalex.org/work/W2618579849', 'https://semopenalex.org/work/W2503647715', 'https://semopenalex.org/work/W2519725791', 'https://semopenalex.org/work/W4317743417', 'https://semopenalex.org/work/W2618660430', 'https://semopenalex.org/work/W2620328864', 'https://semopenalex.org/work/W2219349787', 'https://semopenalex.org/work/W2618805771', 'https://semopenalex.org/work/W88942648', 'https://semopenalex.org/work/W3171874410', 'https://semopenalex.org/work/W2800536240', 'https://semopenalex.org/work/W2520607372', 'https://semopenalex.org/work/W82707212', 'https://semopenalex.org/work/W164245990', 'https://semopenalex.org/work/W2403056045', 'https://semopenalex.org/work/W2946816105', 'https://semopenalex.org/work/W2016390608', 'https://semopenalex.org/work/W4388100645', 'https://semopenalex.org/work/W2282418302', 'https://semopenalex.org/work/W3032139222', 'https://semopenalex.org/work/W2277556528', 'https://semopenalex.org/work/W2485827646', 'https://semopenalex.org/work/W2141692554', 'https://semopenalex.org/work/W2978289855', 'https://semopenalex.org/work/W2990740408', 'https://semopenalex.org/work/W2792530018', 'https://semopenalex.org/work/W2895365144', 'https://semopenalex.org/work/W2495892083', 'https://semopenalex.org/work/W991337960', 'https://semopenalex.org/work/W245480222', 'https://semopenalex.org/work/W110371783', 'https://semopenalex.org/work/W2801765505', 'https://semopenalex.org/work/W2752853118', 'https://semopenalex.org/work/W2749915073', 'https://semopenalex.org/work/W2905528077', 'https://semopenalex.org/work/W2972771325']</t>
   </si>
   <si>
     <t>['3.228571428571428571428571']</t>
@@ -403,34 +403,34 @@
     <t>['https://semopenalex.org/author/A5081106289']</t>
   </si>
   <si>
-    <t>['https://semopenalex.org/work/W2996252512', 'https://semopenalex.org/work/W2809300184', 'https://semopenalex.org/author/A5074307489', 'https://semopenalex.org/work/W2103797968', 'https://semopenalex.org/author/A5052249316', 'https://semopenalex.org/author/A5100638997', 'https://semopenalex.org/author/A5101601497', 'https://semopenalex.org/author/A5070152860', 'https://semopenalex.org/author/A5050308989', 'https://semopenalex.org/author/A5102928967', 'https://semopenalex.org/work/W2772902362', 'https://semopenalex.org/author/A5041073042', 'https://semopenalex.org/author/A5018128809', 'https://semopenalex.org/work/W3205352458', 'https://semopenalex.org/author/A5101617703', 'https://semopenalex.org/author/A5040987266', 'https://semopenalex.org/author/A5002594574', 'https://semopenalex.org/author/A5010181158', 'https://semopenalex.org/author/A5073947585', 'https://semopenalex.org/author/A5101637945', 'https://semopenalex.org/work/W3120745352', 'https://semopenalex.org/author/A5101812436', 'https://semopenalex.org/author/A5100412598', 'https://semopenalex.org/work/W3142314132', 'https://semopenalex.org/author/A5005639930', 'https://semopenalex.org/work/W3011348248', 'https://semopenalex.org/author/A5024456332', 'https://semopenalex.org/work/W2089461653', 'https://semopenalex.org/work/W2950530129', 'https://semopenalex.org/work/W2901813505', 'https://semopenalex.org/work/W2136556709', 'https://semopenalex.org/author/A5021631329', 'https://semopenalex.org/author/A5101558050', 'https://semopenalex.org/work/W3169424470', 'https://semopenalex.org/work/W2068742710', 'https://semopenalex.org/author/A5013325392', 'https://semopenalex.org/author/A5072002680', 'https://semopenalex.org/author/A5058828089', 'https://semopenalex.org/author/A5012621594', 'https://semopenalex.org/author/A5033163346', 'https://semopenalex.org/work/W2577451492', 'https://semopenalex.org/author/A5068340305', 'https://semopenalex.org/author/A5100375823', 'https://semopenalex.org/work/W3108350045', 'https://semopenalex.org/author/A5115595561', 'https://semopenalex.org/author/A5077138780', 'https://semopenalex.org/author/A5065848808', 'https://semopenalex.org/author/A5100409885', 'https://semopenalex.org/author/A5103205468', 'https://semopenalex.org/work/W2951595269', 'https://semopenalex.org/author/A5081145634', 'https://semopenalex.org/work/W2973153063', 'https://semopenalex.org/author/A5019525050', 'https://semopenalex.org/author/A5081420063', 'https://semopenalex.org/author/A5051192643', 'https://semopenalex.org/author/A5044689090', 'https://semopenalex.org/work/W3092116317', 'https://semopenalex.org/author/A5030997313', 'https://semopenalex.org/work/W2963868406', 'https://semopenalex.org/author/A5005007374', 'https://semopenalex.org/author/A5047271595', 'https://semopenalex.org/work/W1976529112', 'https://semopenalex.org/author/A5100408010', 'https://semopenalex.org/author/A5103047914', 'https://semopenalex.org/author/A5100738980', 'https://semopenalex.org/author/A5025839857', 'https://semopenalex.org/author/A5101468661', 'https://semopenalex.org/work/W4284675318', 'https://semopenalex.org/author/A5100439996', 'https://semopenalex.org/author/A5100386104', 'https://semopenalex.org/author/A5101264794', 'https://semopenalex.org/author/A5100440010', 'https://semopenalex.org/author/A5107006112', 'https://semopenalex.org/work/W4253460413', 'https://semopenalex.org/author/A5049142567', 'https://semopenalex.org/work/W3175529320', 'https://semopenalex.org/author/A5017334961', 'https://semopenalex.org/author/A5026927053', 'https://semopenalex.org/author/A5088725475', 'https://semopenalex.org/author/A5049076146', 'https://semopenalex.org/author/A5103205784', 'https://semopenalex.org/work/W2116175419', 'https://semopenalex.org/work/W2850992922', 'https://semopenalex.org/author/A5069596903', 'https://semopenalex.org/author/A5109297018', 'https://semopenalex.org/work/W1971292095', 'https://semopenalex.org/author/A5050080938', 'https://semopenalex.org/author/A5101660937', 'https://semopenalex.org/work/W2788767656', 'https://semopenalex.org/author/A5110172698', 'https://semopenalex.org/author/A5033542967', 'https://semopenalex.org/work/W4391272793', 'https://semopenalex.org/work/W4307887474', 'https://semopenalex.org/author/A5100301259', 'https://semopenalex.org/work/W4391840543', 'https://semopenalex.org/work/W4362677137', 'https://semopenalex.org/author/A5007043113', 'https://semopenalex.org/work/W2611416225', 'https://semopenalex.org/author/A5102717988', 'https://semopenalex.org/author/A5052199638', 'https://semopenalex.org/author/A5000845080', 'https://semopenalex.org/work/W3212642516', 'https://semopenalex.org/author/A5100772234', 'https://semopenalex.org/author/A5100349343', 'https://semopenalex.org/author/A5000645139', 'https://semopenalex.org/work/W2062987337', 'https://semopenalex.org/work/W3180719646', 'https://semopenalex.org/work/W2323936395', 'https://semopenalex.org/author/A5032068969', 'https://semopenalex.org/work/W2066421240', 'https://semopenalex.org/author/A5103761162', 'https://semopenalex.org/author/A5067163535', 'https://semopenalex.org/author/A5100385498', 'https://semopenalex.org/author/A5100758675', 'https://semopenalex.org/work/W4405767877', 'https://semopenalex.org/work/W2137544679', 'https://semopenalex.org/author/A5103286574', 'https://semopenalex.org/author/A5103073505', 'https://semopenalex.org/author/A5101636662', 'https://semopenalex.org/work/W2431508043', 'https://semopenalex.org/author/A5101261545', 'https://semopenalex.org/author/A5077610917', 'https://semopenalex.org/work/W3048759314', 'https://semopenalex.org/work/W3017303867', 'https://semopenalex.org/work/W2596236679', 'https://semopenalex.org/author/A5043798385', 'https://semopenalex.org/author/A5086338440', 'https://semopenalex.org/work/W4393509326', 'https://semopenalex.org/author/A5081036622', 'https://semopenalex.org/author/A5046237164', 'https://semopenalex.org/author/A5100429004', 'https://semopenalex.org/work/W3158787061', 'https://semopenalex.org/work/W4375957525', 'https://semopenalex.org/author/A5084735407', 'https://semopenalex.org/author/A5058738211', 'https://semopenalex.org/work/W2990448925', 'https://semopenalex.org/work/W4239675110', 'https://semopenalex.org/work/W3044975328', 'https://semopenalex.org/author/A5011367069', 'https://semopenalex.org/author/A5101289775', 'https://semopenalex.org/work/W3007855180', 'https://semopenalex.org/work/W1982483659', 'https://semopenalex.org/author/A5114778131', 'https://semopenalex.org/author/A5100639062', 'https://semopenalex.org/author/A5033111691', 'https://semopenalex.org/work/W3166897865', 'https://semopenalex.org/work/W2617809069', 'https://semopenalex.org/author/A5024821632', 'https://semopenalex.org/work/W2790436343', 'https://semopenalex.org/work/W2048733335', 'https://semopenalex.org/author/A5100405159', 'https://semopenalex.org/author/A5015967363', 'https://semopenalex.org/author/A5022677467', 'https://semopenalex.org/author/A5032062525', 'https://semopenalex.org/work/W1993418924', 'https://semopenalex.org/author/A5012561478', 'https://semopenalex.org/author/A5103233342', 'https://semopenalex.org/author/A5039037722', 'https://semopenalex.org/author/A5060115298', 'https://semopenalex.org/work/W4388483786', 'https://semopenalex.org/work/W4402455271', 'https://semopenalex.org/author/A5113160035', 'https://semopenalex.org/work/W1980313439', 'https://semopenalex.org/work/W4388482995', 'https://semopenalex.org/work/W4405706648', 'https://semopenalex.org/author/A5026939932', 'https://semopenalex.org/work/W4384345709', 'https://semopenalex.org/author/A5101983121', 'https://semopenalex.org/author/A5101655978', 'https://semopenalex.org/work/W1991633729', 'https://semopenalex.org/author/A5009435651', 'https://semopenalex.org/author/A5087492388', 'https://semopenalex.org/author/A5100365555', 'https://semopenalex.org/work/W4250349204', 'https://semopenalex.org/author/A5067467896', 'https://semopenalex.org/author/A5077984014', 'https://semopenalex.org/author/A5107864790', 'https://semopenalex.org/author/A5058164381', 'https://semopenalex.org/work/W2547684973', 'https://semopenalex.org/work/W4391341613', 'https://semopenalex.org/work/W116531637', 'https://semopenalex.org/work/W2081871567', 'https://semopenalex.org/author/A5069621751', 'https://semopenalex.org/work/W4394028313', 'https://semopenalex.org/work/W3126104791', 'https://semopenalex.org/author/A5100610450', 'https://semopenalex.org/author/A5043801432', 'https://semopenalex.org/work/W3196137381', 'https://semopenalex.org/author/A5049100391', 'https://semopenalex.org/work/W2131346202', 'https://semopenalex.org/author/A5101556258', 'https://semopenalex.org/author/A5102900280', 'https://semopenalex.org/author/A5100349346', 'https://semopenalex.org/work/W3005774991', 'https://semopenalex.org/author/A5108459503', 'https://semopenalex.org/author/A5085666756', 'https://semopenalex.org/author/A5072432956', 'https://semopenalex.org/work/W3014659028', 'https://semopenalex.org/author/A5015836405', 'https://semopenalex.org/author/A5058258996', 'https://semopenalex.org/author/A5100388597', 'https://semopenalex.org/work/W4393258623', 'https://semopenalex.org/work/W2107351452', 'https://semopenalex.org/author/A5100401412', 'https://semopenalex.org/author/A5114213934', 'https://semopenalex.org/author/A5000019783', 'https://semopenalex.org/author/A5040272202', 'https://semopenalex.org/work/W2147571062', 'https://semopenalex.org/author/A5075929099', 'https://semopenalex.org/author/A5022905724', 'https://semopenalex.org/work/W2187270832', 'https://semopenalex.org/work/W4237256801', 'https://semopenalex.org/author/A5076516205', 'https://semopenalex.org/work/W2999892205', 'https://semopenalex.org/work/W2163581369', 'https://semopenalex.org/author/A5077658936', 'https://semopenalex.org/author/A5100388576', 'https://semopenalex.org/author/A5100426931', 'https://semopenalex.org/author/A5100676331', 'https://semopenalex.org/author/A5101011726', 'https://semopenalex.org/author/A5025292884', 'https://semopenalex.org/author/A5009487151', 'https://semopenalex.org/author/A5100385507', 'https://semopenalex.org/author/A5000381434', 'https://semopenalex.org/work/W4205415629', 'https://semopenalex.org/author/A5084874990', 'https://semopenalex.org/work/W2000778992', 'https://semopenalex.org/work/W4234850770', 'https://semopenalex.org/author/A5100447691', 'https://semopenalex.org/author/A5013438083', 'https://semopenalex.org/work/W3016797157', 'https://semopenalex.org/work/W4285602996', 'https://semopenalex.org/author/A5056526226', 'https://semopenalex.org/author/A5100633784', 'https://semopenalex.org/author/A5091706559', 'https://semopenalex.org/author/A5065293581', 'https://semopenalex.org/author/A5102222159', 'https://semopenalex.org/work/W4394769313', 'https://semopenalex.org/author/A5101555891', 'https://semopenalex.org/work/W2905627582', 'https://semopenalex.org/work/W2039325426', 'https://semopenalex.org/author/A5023155310', 'https://semopenalex.org/author/A5100361984', 'https://semopenalex.org/author/A5035359666', 'https://semopenalex.org/author/A5035089987', 'https://semopenalex.org/work/W3086623952', 'https://semopenalex.org/author/A5027206285', 'https://semopenalex.org/work/W4400484371', 'https://semopenalex.org/author/A5009455568', 'https://semopenalex.org/work/W2952920225', 'https://semopenalex.org/work/W4285605736', 'https://semopenalex.org/work/W4399553914', 'https://semopenalex.org/author/A5075273130', 'https://semopenalex.org/author/A5040203716', 'https://semopenalex.org/author/A5055422837', 'https://semopenalex.org/author/A5036120394', 'https://semopenalex.org/author/A5002289161', 'https://semopenalex.org/work/W4284702776', 'https://semopenalex.org/author/A5034057959', 'https://semopenalex.org/author/A5064776947', 'https://semopenalex.org/author/A5090671359', 'https://semopenalex.org/author/A5073965511', 'https://semopenalex.org/author/A5077008083', 'https://semopenalex.org/author/A5047965752', 'https://semopenalex.org/author/A5045087569', 'https://semopenalex.org/author/A5100299966', 'https://semopenalex.org/work/W3159230003', 'https://semopenalex.org/work/W2884327322', 'https://semopenalex.org/author/A5048118068', 'https://semopenalex.org/author/A5100388609', 'https://semopenalex.org/author/A5027084532', 'https://semopenalex.org/author/A5100458045', 'https://semopenalex.org/author/A5023035566', 'https://semopenalex.org/work/W4399851061', 'https://semopenalex.org/author/A5023093639', 'https://semopenalex.org/author/A5100779597', 'https://semopenalex.org/author/A5055149708', 'https://semopenalex.org/work/W4246723161', 'https://semopenalex.org/author/A5049622460', 'https://semopenalex.org/author/A5110161847', 'https://semopenalex.org/author/A5054115813', 'https://semopenalex.org/work/W2473476112', 'https://semopenalex.org/author/A5065120715', 'https://semopenalex.org/author/A5100367825', 'https://semopenalex.org/work/W2566570636', 'https://semopenalex.org/author/A5032194564', 'https://semopenalex.org/author/A5000582109', 'https://semopenalex.org/author/A5090627608', 'https://semopenalex.org/author/A5100523187', 'https://semopenalex.org/author/A5081340873', 'https://semopenalex.org/work/W2006579687', 'https://semopenalex.org/author/A5088708850', 'https://semopenalex.org/author/A5033164669', 'https://semopenalex.org/author/A5053084752', 'https://semopenalex.org/work/W4388212297', 'https://semopenalex.org/work/W2952675117', 'https://semopenalex.org/work/W2552981188', 'https://semopenalex.org/author/A5102858698', 'https://semopenalex.org/author/A5039326697', 'https://semopenalex.org/author/A5100388581', 'https://semopenalex.org/author/A5024073253', 'https://semopenalex.org/author/A5058257080', 'https://semopenalex.org/author/A5038017715', 'https://semopenalex.org/author/A5052404451', 'https://semopenalex.org/work/W2370472429', 'https://semopenalex.org/work/W2506015293', 'https://semopenalex.org/author/A5056980315', 'https://semopenalex.org/author/A5025977354', 'https://semopenalex.org/author/A5009071576', 'https://semopenalex.org/work/W2969773072', 'https://semopenalex.org/work/W4245733707', 'https://semopenalex.org/author/A5050748634', 'https://semopenalex.org/work/W2973149860', 'https://semopenalex.org/author/A5100608460', 'https://semopenalex.org/author/A5077424533', 'https://semopenalex.org/work/W2091170821', 'https://semopenalex.org/author/A5102014459', 'https://semopenalex.org/work/W3129269689', 'https://semopenalex.org/author/A5003031253', 'https://semopenalex.org/author/A5101614814', 'https://semopenalex.org/work/W2246822044', 'https://semopenalex.org/work/W2590137773', 'https://semopenalex.org/work/W4220884961', 'https://semopenalex.org/work/W2794806827', 'https://semopenalex.org/author/A5102859232', 'https://semopenalex.org/author/A5059065212', 'https://semopenalex.org/work/W1578028529', 'https://semopenalex.org/author/A5079431306', 'https://semopenalex.org/work/W2867448323', 'https://semopenalex.org/author/A5042235813', 'https://semopenalex.org/author/A5011086593', 'https://semopenalex.org/author/A5103234102', 'https://semopenalex.org/work/W2362205694', 'https://semopenalex.org/author/A5074540830', 'https://semopenalex.org/author/A5048041198', 'https://semopenalex.org/author/A5089294104', 'https://semopenalex.org/author/A5102987690', 'https://semopenalex.org/work/W4381053704', 'https://semopenalex.org/author/A5085247180', 'https://semopenalex.org/author/A5101966381', 'https://semopenalex.org/work/W1977393187', 'https://semopenalex.org/author/A5088498790', 'https://semopenalex.org/work/W2076676096', 'https://semopenalex.org/author/A5004490190', 'https://semopenalex.org/author/A5100388599', 'https://semopenalex.org/author/A5100447531', 'https://semopenalex.org/author/A5081650066', 'https://semopenalex.org/author/A5100738977', 'https://semopenalex.org/author/A5100408160', 'https://semopenalex.org/author/A5021179945', 'https://semopenalex.org/author/A5100665833', 'https://semopenalex.org/work/W3193682477', 'https://semopenalex.org/author/A5030490896', 'https://semopenalex.org/author/A5100388617', 'https://semopenalex.org/author/A5042986574', 'https://semopenalex.org/author/A5100458090', 'https://semopenalex.org/author/A5088646345', 'https://semopenalex.org/author/A5006357713', 'https://semopenalex.org/author/A5019450472', 'https://semopenalex.org/author/A5028716858', 'https://semopenalex.org/author/A5069809962', 'https://semopenalex.org/work/W2518136680', 'https://semopenalex.org/author/A5100443727', 'https://semopenalex.org/author/A5100331488', 'https://semopenalex.org/work/W2051945152', 'https://semopenalex.org/author/A5100367807', 'https://semopenalex.org/author/A5101308414', 'https://semopenalex.org/author/A5079729956', 'https://semopenalex.org/author/A5059555100', 'https://semopenalex.org/author/A5034794084', 'https://semopenalex.org/work/W2046104010', 'https://semopenalex.org/author/A5100388627', 'https://semopenalex.org/author/A5102204689', 'https://semopenalex.org/work/W3033481405', 'https://semopenalex.org/work/W2151320737', 'https://semopenalex.org/author/A5052981404', 'https://semopenalex.org/author/A5043476448', 'https://semopenalex.org/author/A5100322125', 'https://semopenalex.org/author/A5100394129', 'https://semopenalex.org/author/A5100753041', 'https://semopenalex.org/work/W2093107900', 'https://semopenalex.org/author/A5100445622', 'https://semopenalex.org/author/A5100447682', 'https://semopenalex.org/author/A5030626281', 'https://semopenalex.org/author/A5101194950', 'https://semopenalex.org/author/A5040850915', 'https://semopenalex.org/author/A5074075949', 'https://semopenalex.org/author/A5102020713', 'https://semopenalex.org/author/A5100459874', 'https://semopenalex.org/author/A5103223639', 'https://semopenalex.org/work/W3110369458', 'https://semopenalex.org/author/A5100677820', 'https://semopenalex.org/work/W3035746743', 'https://semopenalex.org/author/A5085393851', 'https://semopenalex.org/work/W3000636126', 'https://semopenalex.org/author/A5012469172', 'https://semopenalex.org/work/W2962715466', 'https://semopenalex.org/work/W2612190612', 'https://semopenalex.org/author/A5100438174', 'https://semopenalex.org/work/W2997847174', 'https://semopenalex.org/author/A5101540631', 'https://semopenalex.org/author/A5056755949', 'https://semopenalex.org/work/W2759005765', 'https://semopenalex.org/author/A5100376204', 'https://semopenalex.org/author/A5068122240', 'https://semopenalex.org/author/A5025099559', 'https://semopenalex.org/author/A5010958113', 'https://semopenalex.org/author/A5100753039', 'https://semopenalex.org/work/W3109004940', 'https://semopenalex.org/work/W3000410628', 'https://semopenalex.org/work/W3215130818', 'https://semopenalex.org/author/A5100697624', 'https://semopenalex.org/author/A5016401353', 'https://semopenalex.org/work/W2397328687', 'https://semopenalex.org/author/A5072456187', 'https://semopenalex.org/author/A5100388716', 'https://semopenalex.org/author/A5101852647', 'https://semopenalex.org/author/A5081886276', 'https://semopenalex.org/author/A5005604635', 'https://semopenalex.org/author/A5067395122', 'https://semopenalex.org/author/A5054753279', 'https://semopenalex.org/author/A5076444296', 'https://semopenalex.org/work/W1505288849', 'https://semopenalex.org/work/W4387674150', 'https://semopenalex.org/author/A5021222755', 'https://semopenalex.org/work/W2962858219', 'https://semopenalex.org/author/A5101612059', 'https://semopenalex.org/author/A5059396373', 'https://semopenalex.org/work/W2112857338', 'https://semopenalex.org/work/W3193977407', 'https://semopenalex.org/author/A5045500611', 'https://semopenalex.org/work/W4404317069', 'https://semopenalex.org/author/A5036986396', 'https://semopenalex.org/author/A5100327487', 'https://semopenalex.org/author/A5061863093', 'https://semopenalex.org/author/A5041961808', 'https://semopenalex.org/author/A5113115887', 'https://semopenalex.org/author/A5100361632', 'https://semopenalex.org/author/A5111956187', 'https://semopenalex.org/work/W3131838314', 'https://semopenalex.org/work/W4246206803', 'https://semopenalex.org/author/A5060364305', 'https://semopenalex.org/work/W2351461473', 'https://semopenalex.org/work/W1966337472', 'https://semopenalex.org/author/A5115590096', 'https://semopenalex.org/author/A5085611398', 'https://semopenalex.org/work/W4313563577', 'https://semopenalex.org/author/A5036039721', 'https://semopenalex.org/author/A5011667547', 'https://semopenalex.org/author/A5081449581', 'https://semopenalex.org/author/A5006669765', 'https://semopenalex.org/author/A5066916130', 'https://semopenalex.org/work/W4393891665', 'https://semopenalex.org/author/A5084868951', 'https://semopenalex.org/author/A5100388644', 'https://semopenalex.org/author/A5100738974', 'https://semopenalex.org/author/A5002503342', 'https://semopenalex.org/author/A5018031899', 'https://semopenalex.org/author/A5043546718', 'https://semopenalex.org/work/W1986191662', 'https://semopenalex.org/work/W2168668632', 'https://semopenalex.org/author/A5013103539', 'https://semopenalex.org/work/W2794957215', 'https://semopenalex.org/author/A5087587101', 'https://semopenalex.org/work/W2005680430', 'https://semopenalex.org/work/W3205951184']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2132574120', 'https://semopenalex.org/work/W2915009967', 'https://semopenalex.org/work/W173156922', 'https://semopenalex.org/work/W2011170798', 'https://semopenalex.org/work/W1991332789', 'https://semopenalex.org/work/W1997210046', 'https://semopenalex.org/work/W2154282221', 'https://semopenalex.org/work/W2806131721', 'https://semopenalex.org/work/W2129825950', 'https://semopenalex.org/work/W4398191656', 'https://semopenalex.org/work/W2915030750', 'https://semopenalex.org/work/W1574950491', 'https://semopenalex.org/work/W3138989164', 'https://semopenalex.org/work/W1579677221', 'https://semopenalex.org/work/W1550675824', 'https://semopenalex.org/work/W4384155490', 'https://semopenalex.org/work/W4400939550', 'https://semopenalex.org/work/W3216444132', 'https://semopenalex.org/work/W1475955015', 'https://semopenalex.org/work/W2921648886', 'https://semopenalex.org/work/W1679509962', 'https://semopenalex.org/work/W2008620714', 'https://semopenalex.org/work/W2012114748', 'https://semopenalex.org/work/W2400762887', 'https://semopenalex.org/work/W4324007121', 'https://semopenalex.org/work/W4394555057', 'https://semopenalex.org/work/W2189085557', 'https://semopenalex.org/work/W2014199531', 'https://semopenalex.org/work/W1560854026', 'https://semopenalex.org/work/W4393474997', 'https://semopenalex.org/work/W2949504704', 'https://semopenalex.org/work/W991450633', 'https://semopenalex.org/work/W2123904236', 'https://semopenalex.org/work/W2103704182', 'https://semopenalex.org/work/W2206340513', 'https://semopenalex.org/work/W2953255159', 'https://semopenalex.org/work/W4406859981', 'https://semopenalex.org/work/W4253646682', 'https://semopenalex.org/work/W2754252703', 'https://semopenalex.org/work/W2779900466', 'https://semopenalex.org/work/W2522928308', 'https://semopenalex.org/work/W4298063358', 'https://semopenalex.org/work/W1579914521', 'https://semopenalex.org/work/W1792464322', 'https://semopenalex.org/work/W2739356170', 'https://semopenalex.org/work/W2055963247', 'https://semopenalex.org/work/W2044926733', 'https://semopenalex.org/work/W2125383988', 'https://semopenalex.org/work/W3033698111', 'https://semopenalex.org/work/W2523177018', 'https://semopenalex.org/work/W2008732772', 'https://semopenalex.org/work/W2103982927', 'https://semopenalex.org/work/W1811359278', 'https://semopenalex.org/work/W1994977110', 'https://semopenalex.org/work/W2085609918', 'https://semopenalex.org/work/W4393943425', 'https://semopenalex.org/work/W1595752763', 'https://semopenalex.org/work/W4400976691', 'https://semopenalex.org/work/W2525118715', 'https://semopenalex.org/work/W2078770126', 'https://semopenalex.org/work/W2915945450', 'https://semopenalex.org/work/W52260594', 'https://semopenalex.org/work/W2632860668', 'https://semopenalex.org/work/W4282576055', 'https://semopenalex.org/work/W1719093023', 'https://semopenalex.org/work/W2008606555', 'https://semopenalex.org/work/W2008078972', 'https://semopenalex.org/work/W1710751537', 'https://semopenalex.org/work/W1978847709', 'https://semopenalex.org/work/W2520217242', 'https://semopenalex.org/work/W1572167134', 'https://semopenalex.org/work/W2747419197', 'https://semopenalex.org/work/W2166938786', 'https://semopenalex.org/work/W1573454147', 'https://semopenalex.org/work/W3158293305', 'https://semopenalex.org/work/W2747898780', 'https://semopenalex.org/work/W1588734579', 'https://semopenalex.org/work/W2061236588', 'https://semopenalex.org/work/W3116695505', 'https://semopenalex.org/work/W36371468', 'https://semopenalex.org/work/W1987557201', 'https://semopenalex.org/work/W2139525797', 'https://semopenalex.org/work/W1975908943', 'https://semopenalex.org/work/W2118889869', 'https://semopenalex.org/work/W1253240651', 'https://semopenalex.org/work/W2612371455', 'https://semopenalex.org/work/W2527377534', 'https://semopenalex.org/work/W2899402023', 'https://semopenalex.org/work/W2400182190', 'https://semopenalex.org/work/W2123344956', 'https://semopenalex.org/work/W2912433096', 'https://semopenalex.org/work/W89291972', 'https://semopenalex.org/work/W4282583221', 'https://semopenalex.org/work/W2041544991', 'https://semopenalex.org/work/W2612962685', 'https://semopenalex.org/work/W4385473607', 'https://semopenalex.org/work/W1537902892', 'https://semopenalex.org/work/W2958694015', 'https://semopenalex.org/work/W115310691', 'https://semopenalex.org/work/W2515946176', 'https://semopenalex.org/work/W2128127301', 'https://semopenalex.org/work/W2525395252', 'https://semopenalex.org/work/W2401057219', 'https://semopenalex.org/work/W1978640117', 'https://semopenalex.org/work/W3137115172', 'https://semopenalex.org/work/W1570916159', 'https://semopenalex.org/work/W2963855145', 'https://semopenalex.org/work/W1517590008', 'https://semopenalex.org/work/W2115447277', 'https://semopenalex.org/work/W1975513208', 'https://semopenalex.org/work/W2171326679', 'https://semopenalex.org/work/W1556803451', 'https://semopenalex.org/work/W2155935413', 'https://semopenalex.org/work/W1511466363', 'https://semopenalex.org/work/W205920923', 'https://semopenalex.org/work/W4249900482', 'https://semopenalex.org/work/W1908231796', 'https://semopenalex.org/work/W2098211566', 'https://semopenalex.org/work/W3108668383', 'https://semopenalex.org/work/W4242436304', 'https://semopenalex.org/work/W1520649080', 'https://semopenalex.org/work/W2127281178', 'https://semopenalex.org/work/W4242041539', 'https://semopenalex.org/work/W2520300422', 'https://semopenalex.org/work/W1971941065', 'https://semopenalex.org/work/W2091478774', 'https://semopenalex.org/work/W2039085252', 'https://semopenalex.org/work/W2466104094', 'https://semopenalex.org/work/W4391272934', 'https://semopenalex.org/work/W2047400318', 'https://semopenalex.org/work/W2794546965', 'https://semopenalex.org/work/W2778029444', 'https://semopenalex.org/work/W2153339030', 'https://semopenalex.org/work/W2181042156', 'https://semopenalex.org/work/W1588297513', 'https://semopenalex.org/work/W2015180219', 'https://semopenalex.org/work/W2980176182', 'https://semopenalex.org/work/W1495962746', 'https://semopenalex.org/work/W2152544235', 'https://semopenalex.org/work/W2122811495', 'https://semopenalex.org/work/W139130934', 'https://semopenalex.org/work/W4238210800', 'https://semopenalex.org/work/W1595761884', 'https://semopenalex.org/work/W2123889292', 'https://semopenalex.org/work/W2087840232', 'https://semopenalex.org/work/W2017269495', 'https://semopenalex.org/work/W2949106240', 'https://semopenalex.org/work/W4404057326', 'https://semopenalex.org/work/W2751928463', 'https://semopenalex.org/work/W4296041368', 'https://semopenalex.org/work/W2071433880', 'https://semopenalex.org/work/W3136236837', 'https://semopenalex.org/work/W2094034408', 'https://semopenalex.org/work/W2112609211', 'https://semopenalex.org/work/W2734788368', 'https://semopenalex.org/work/W4387755431', 'https://semopenalex.org/work/W2104421582', 'https://semopenalex.org/work/W3195402331', 'https://semopenalex.org/work/W4402442861', 'https://semopenalex.org/work/W48558007', 'https://semopenalex.org/work/W1593317697', 'https://semopenalex.org/work/W2592423893', 'https://semopenalex.org/work/W2109952361', 'https://semopenalex.org/work/W2132155852', 'https://semopenalex.org/work/W2952092732', 'https://semopenalex.org/work/W1798073562', 'https://semopenalex.org/work/W4237909807', 'https://semopenalex.org/work/W156157953', 'https://semopenalex.org/work/W1592700375', 'https://semopenalex.org/work/W1775494561', 'https://semopenalex.org/work/W2088263927', 'https://semopenalex.org/work/W4313563519', 'https://semopenalex.org/work/W2077394967', 'https://semopenalex.org/work/W147488175', 'https://semopenalex.org/work/W1633377437', 'https://semopenalex.org/work/W2173733616', 'https://semopenalex.org/work/W2734789924', 'https://semopenalex.org/work/W4403628532', 'https://semopenalex.org/work/W2130495724', 'https://semopenalex.org/work/W4292761028', 'https://semopenalex.org/work/W2145761885', 'https://semopenalex.org/work/W4393670548', 'https://semopenalex.org/work/W2028893723', 'https://semopenalex.org/work/W371525118', 'https://semopenalex.org/work/W3009455989', 'https://semopenalex.org/work/W2928532935', 'https://semopenalex.org/work/W3092639686', 'https://semopenalex.org/work/W1996454760', 'https://semopenalex.org/work/W1501840263', 'https://semopenalex.org/work/W2049801349', 'https://semopenalex.org/work/W2609404595', 'https://semopenalex.org/work/W3183165251', 'https://semopenalex.org/work/W3028360334', 'https://semopenalex.org/work/W144935353', 'https://semopenalex.org/work/W2809114684', 'https://semopenalex.org/work/W2778798134', 'https://semopenalex.org/work/W4312240104', 'https://semopenalex.org/work/W1531484838', 'https://semopenalex.org/work/W2101874499', 'https://semopenalex.org/work/W2581324891', 'https://semopenalex.org/work/W1774324140']</t>
-  </si>
-  <si>
-    <t>['Rotten Green Tests in Java, Pharo and Python', 'https://semopenalex.org/source/S4210192127', 'W. R. Owens, Stuart Sim, and David Walker, eds. Bunyan Studies: A Journal of Reformation and Nonconformist Culture', 'https://semopenalex.org/source/S73505065', 'https://semopenalex.org/source/S4377196300', 'W. R. OWENS, STUART SIM, AND DAVID WALKER, EDS. BUNYAN STUDIES: A JOURNAL OF REFORMATION AND NONCONFORMIST CULTURE. NUMBER 22. NORTHUMBRIA UNIVERSITY, 2018. PP. 164.', 'Rotten green tests in Java, Pharo and Python', 'https://semopenalex.org/work/W4287005120', 'https://semopenalex.org/work/W4224210536', 'https://semopenalex.org/work/W4294273680', 'https://semopenalex.org/source/S4363604151', 'The Secret History of HB-2: Bathroom Safety in the Eighteenth Century and Beyond', 'https://semopenalex.org/source/S4306402203', 'https://semopenalex.org/source/S109852484', 'https://semopenalex.org/work/W4312279131', 'https://semopenalex.org/work/W3202264790', 'https://semopenalex.org/source/S4306402512', 'https://semopenalex.org/source/S4306463865', 'Pope and the Reformation of the Oral: The Iliad in the History of Mediation', 'Advances in monitoring carbon dioxide exchange between the atmosphere and mine waste derived from ultramafic-hosted mineral deposits; a pilot study at Cassiar, B.C.', 'https://semopenalex.org/work/W4322392796', 'https://semopenalex.org/work/W4309899403', 'https://semopenalex.org/source/S4306462979']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W4400950811', 'https://semopenalex.org/work/W4399748832', 'https://semopenalex.org/work/W4323660310', 'https://semopenalex.org/work/W2947077169', 'https://semopenalex.org/work/W2952261671', 'https://semopenalex.org/work/W3099917237', 'https://semopenalex.org/work/W4210579963', 'https://semopenalex.org/work/W2805958446', 'https://semopenalex.org/work/W2567325662', 'https://semopenalex.org/work/W2112043190', 'https://semopenalex.org/work/W3217353773', 'https://semopenalex.org/work/W616114729', 'https://semopenalex.org/work/W4403612127', 'https://semopenalex.org/work/W2995007313', 'https://semopenalex.org/work/W2404155628', 'https://semopenalex.org/work/W2161672839', 'https://semopenalex.org/work/W4404660380', 'https://semopenalex.org/work/W2786034148', 'https://semopenalex.org/work/W2977439887', 'https://semopenalex.org/work/W4294328862', 'https://semopenalex.org/work/W1970619397', 'https://semopenalex.org/work/W2906756016', 'https://semopenalex.org/work/W2158980502', 'https://semopenalex.org/work/W2613478558', 'https://semopenalex.org/work/W4300606001']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2768137799', 'https://semopenalex.org/work/W2534209856', 'https://semopenalex.org/work/W4285228284', 'https://semopenalex.org/work/W2538728777', 'https://semopenalex.org/work/W2535112844', 'https://semopenalex.org/work/W2770615292', 'https://semopenalex.org/work/W4210437323', 'https://semopenalex.org/work/W2295752281', 'https://semopenalex.org/work/W2907903092', 'https://semopenalex.org/work/W2344766906', 'https://semopenalex.org/work/W2770896033', 'https://semopenalex.org/work/W2912223386']</t>
+    <t>['https://semopenalex.org/author/A5103223639', 'https://semopenalex.org/work/W2046104010', 'https://semopenalex.org/author/A5081340873', 'https://semopenalex.org/work/W2103797968', 'https://semopenalex.org/author/A5066916130', 'https://semopenalex.org/work/W2990448925', 'https://semopenalex.org/work/W2772902362', 'https://semopenalex.org/author/A5101194950', 'https://semopenalex.org/author/A5100388627', 'https://semopenalex.org/author/A5085611398', 'https://semopenalex.org/work/W3016797157', 'https://semopenalex.org/author/A5070152860', 'https://semopenalex.org/author/A5089294104', 'https://semopenalex.org/work/W2905627582', 'https://semopenalex.org/author/A5049076146', 'https://semopenalex.org/author/A5103047914', 'https://semopenalex.org/work/W4285605736', 'https://semopenalex.org/work/W3158787061', 'https://semopenalex.org/work/W2867448323', 'https://semopenalex.org/author/A5081650066', 'https://semopenalex.org/author/A5049622460', 'https://semopenalex.org/work/W2006579687', 'https://semopenalex.org/author/A5050308989', 'https://semopenalex.org/work/W2362205694', 'https://semopenalex.org/work/W4285602996', 'https://semopenalex.org/author/A5041073042', 'https://semopenalex.org/work/W4388482995', 'https://semopenalex.org/work/W2973149860', 'https://semopenalex.org/work/W3205951184', 'https://semopenalex.org/author/A5023155310', 'https://semopenalex.org/author/A5101601497', 'https://semopenalex.org/work/W3131838314', 'https://semopenalex.org/author/A5079729956', 'https://semopenalex.org/author/A5100301259', 'https://semopenalex.org/author/A5072002680', 'https://semopenalex.org/work/W3169424470', 'https://semopenalex.org/author/A5002503342', 'https://semopenalex.org/author/A5032068969', 'https://semopenalex.org/author/A5072432956', 'https://semopenalex.org/work/W2147571062', 'https://semopenalex.org/author/A5074540830', 'https://semopenalex.org/author/A5040987266', 'https://semopenalex.org/author/A5101011726', 'https://semopenalex.org/work/W4393509326', 'https://semopenalex.org/author/A5100386104', 'https://semopenalex.org/work/W2962715466', 'https://semopenalex.org/work/W2952675117', 'https://semopenalex.org/work/W2323936395', 'https://semopenalex.org/work/W2048733335', 'https://semopenalex.org/author/A5102204689', 'https://semopenalex.org/author/A5047271595', 'https://semopenalex.org/work/W3011348248', 'https://semopenalex.org/work/W2962858219', 'https://semopenalex.org/work/W4381053704', 'https://semopenalex.org/author/A5110161847', 'https://semopenalex.org/work/W2187270832', 'https://semopenalex.org/author/A5076516205', 'https://semopenalex.org/author/A5086338440', 'https://semopenalex.org/author/A5100385498', 'https://semopenalex.org/author/A5101852647', 'https://semopenalex.org/author/A5056526226', 'https://semopenalex.org/work/W2163581369', 'https://semopenalex.org/work/W3212642516', 'https://semopenalex.org/author/A5012621594', 'https://semopenalex.org/author/A5100458045', 'https://semopenalex.org/author/A5100405159', 'https://semopenalex.org/author/A5100447531', 'https://semopenalex.org/author/A5081145634', 'https://semopenalex.org/work/W3014659028', 'https://semopenalex.org/work/W3193977407', 'https://semopenalex.org/author/A5077008083', 'https://semopenalex.org/author/A5100365555', 'https://semopenalex.org/author/A5053084752', 'https://semopenalex.org/work/W2473476112', 'https://semopenalex.org/work/W4393891665', 'https://semopenalex.org/author/A5101468661', 'https://semopenalex.org/author/A5000582109', 'https://semopenalex.org/work/W4387674150', 'https://semopenalex.org/author/A5100299966', 'https://semopenalex.org/work/W3005774991', 'https://semopenalex.org/work/W4400484371', 'https://semopenalex.org/author/A5102020713', 'https://semopenalex.org/author/A5045500611', 'https://semopenalex.org/author/A5006357713', 'https://semopenalex.org/author/A5018128809', 'https://semopenalex.org/work/W3180719646', 'https://semopenalex.org/author/A5103233342', 'https://semopenalex.org/author/A5061863093', 'https://semopenalex.org/author/A5101637945', 'https://semopenalex.org/work/W3033481405', 'https://semopenalex.org/author/A5051192643', 'https://semopenalex.org/work/W4393258623', 'https://semopenalex.org/author/A5100361984', 'https://semopenalex.org/author/A5059396373', 'https://semopenalex.org/author/A5100322125', 'https://semopenalex.org/author/A5040272202', 'https://semopenalex.org/author/A5059555100', 'https://semopenalex.org/work/W3035746743', 'https://semopenalex.org/author/A5087587101', 'https://semopenalex.org/work/W1505288849', 'https://semopenalex.org/author/A5085666756', 'https://semopenalex.org/work/W4405767877', 'https://semopenalex.org/author/A5103286574', 'https://semopenalex.org/author/A5101966381', 'https://semopenalex.org/author/A5102900280', 'https://semopenalex.org/author/A5081036622', 'https://semopenalex.org/author/A5101614814', 'https://semopenalex.org/author/A5027206285', 'https://semopenalex.org/work/W2081871567', 'https://semopenalex.org/work/W2547684973', 'https://semopenalex.org/author/A5101983121', 'https://semopenalex.org/author/A5100388609', 'https://semopenalex.org/work/W2068742710', 'https://semopenalex.org/work/W2107351452', 'https://semopenalex.org/author/A5085247180', 'https://semopenalex.org/author/A5000019783', 'https://semopenalex.org/author/A5113115887', 'https://semopenalex.org/author/A5005639930', 'https://semopenalex.org/author/A5011667547', 'https://semopenalex.org/author/A5050748634', 'https://semopenalex.org/author/A5100385507', 'https://semopenalex.org/author/A5030490896', 'https://semopenalex.org/author/A5100638997', 'https://semopenalex.org/work/W3215130818', 'https://semopenalex.org/work/W2552981188', 'https://semopenalex.org/work/W2973153063', 'https://semopenalex.org/author/A5039326697', 'https://semopenalex.org/author/A5101812436', 'https://semopenalex.org/work/W4220884961', 'https://semopenalex.org/author/A5102858698', 'https://semopenalex.org/author/A5100639062', 'https://semopenalex.org/author/A5102014459', 'https://semopenalex.org/author/A5056980315', 'https://semopenalex.org/author/A5101261545', 'https://semopenalex.org/author/A5021631329', 'https://semopenalex.org/author/A5026939932', 'https://semopenalex.org/author/A5056755949', 'https://semopenalex.org/author/A5022905724', 'https://semopenalex.org/work/W2590137773', 'https://semopenalex.org/author/A5054115813', 'https://semopenalex.org/author/A5101655978', 'https://semopenalex.org/author/A5100633784', 'https://semopenalex.org/work/W3017303867', 'https://semopenalex.org/author/A5102859232', 'https://semopenalex.org/work/W2151320737', 'https://semopenalex.org/author/A5088498790', 'https://semopenalex.org/author/A5081449581', 'https://semopenalex.org/work/W2005680430', 'https://semopenalex.org/author/A5101636662', 'https://semopenalex.org/author/A5000845080', 'https://semopenalex.org/work/W2611416225', 'https://semopenalex.org/author/A5040203716', 'https://semopenalex.org/work/W2999892205', 'https://semopenalex.org/work/W2951595269', 'https://semopenalex.org/author/A5058828089', 'https://semopenalex.org/author/A5100375823', 'https://semopenalex.org/author/A5019450472', 'https://semopenalex.org/author/A5103205784', 'https://semopenalex.org/work/W2617809069', 'https://semopenalex.org/work/W4239675110', 'https://semopenalex.org/work/W4234850770', 'https://semopenalex.org/author/A5025099559', 'https://semopenalex.org/author/A5036986396', 'https://semopenalex.org/author/A5013325392', 'https://semopenalex.org/author/A5101555891', 'https://semopenalex.org/work/W3048759314', 'https://semopenalex.org/work/W2612190612', 'https://semopenalex.org/author/A5101617703', 'https://semopenalex.org/work/W1986191662', 'https://semopenalex.org/author/A5060364305', 'https://semopenalex.org/author/A5100388599', 'https://semopenalex.org/author/A5091706559', 'https://semopenalex.org/author/A5000645139', 'https://semopenalex.org/author/A5110172698', 'https://semopenalex.org/author/A5100753039', 'https://semopenalex.org/author/A5077658936', 'https://semopenalex.org/author/A5100779597', 'https://semopenalex.org/work/W2062987337', 'https://semopenalex.org/author/A5069809962', 'https://semopenalex.org/author/A5010958113', 'https://semopenalex.org/author/A5068122240', 'https://semopenalex.org/author/A5042235813', 'https://semopenalex.org/work/W4237256801', 'https://semopenalex.org/author/A5102987690', 'https://semopenalex.org/work/W2952920225', 'https://semopenalex.org/work/W4388483786', 'https://semopenalex.org/work/W2370472429', 'https://semopenalex.org/author/A5011367069', 'https://semopenalex.org/author/A5072456187', 'https://semopenalex.org/work/W3159230003', 'https://semopenalex.org/work/W3007855180', 'https://semopenalex.org/author/A5107864790', 'https://semopenalex.org/author/A5100388597', 'https://semopenalex.org/work/W4284702776', 'https://semopenalex.org/author/A5102717988', 'https://semopenalex.org/author/A5100388716', 'https://semopenalex.org/work/W4284675318', 'https://semopenalex.org/author/A5100758675', 'https://semopenalex.org/author/A5100608460', 'https://semopenalex.org/work/W2051945152', 'https://semopenalex.org/work/W1991633729', 'https://semopenalex.org/author/A5100665833', 'https://semopenalex.org/author/A5081886276', 'https://semopenalex.org/author/A5016401353', 'https://semopenalex.org/work/W2790436343', 'https://semopenalex.org/author/A5024073253', 'https://semopenalex.org/work/W3000636126', 'https://semopenalex.org/author/A5021179945', 'https://semopenalex.org/author/A5054753279', 'https://semopenalex.org/author/A5074075949', 'https://semopenalex.org/work/W2091170821', 'https://semopenalex.org/author/A5048118068', 'https://semopenalex.org/author/A5024456332', 'https://semopenalex.org/author/A5039037722', 'https://semopenalex.org/work/W3129269689', 'https://semopenalex.org/author/A5073947585', 'https://semopenalex.org/author/A5012561478', 'https://semopenalex.org/work/W2076676096', 'https://semopenalex.org/work/W3175529320', 'https://semopenalex.org/work/W4394769313', 'https://semopenalex.org/author/A5015967363', 'https://semopenalex.org/work/W2794957215', 'https://semopenalex.org/author/A5100376204', 'https://semopenalex.org/work/W4404317069', 'https://semopenalex.org/work/W4246206803', 'https://semopenalex.org/author/A5049142567', 'https://semopenalex.org/author/A5013438083', 'https://semopenalex.org/author/A5042986574', 'https://semopenalex.org/author/A5047965752', 'https://semopenalex.org/author/A5036039721', 'https://semopenalex.org/author/A5006669765', 'https://semopenalex.org/author/A5005604635', 'https://semopenalex.org/author/A5101660937', 'https://semopenalex.org/author/A5109297018', 'https://semopenalex.org/author/A5100738974', 'https://semopenalex.org/author/A5023035566', 'https://semopenalex.org/author/A5100440010', 'https://semopenalex.org/work/W4394028313', 'https://semopenalex.org/work/W4307887474', 'https://semopenalex.org/work/W4402455271', 'https://semopenalex.org/author/A5114213934', 'https://semopenalex.org/work/W2577451492', 'https://semopenalex.org/work/W4313563577', 'https://semopenalex.org/author/A5064776947', 'https://semopenalex.org/author/A5025292884', 'https://semopenalex.org/author/A5043546718', 'https://semopenalex.org/author/A5065120715', 'https://semopenalex.org/work/W2759005765', 'https://semopenalex.org/author/A5044689090', 'https://semopenalex.org/work/W2431508043', 'https://semopenalex.org/author/A5003031253', 'https://semopenalex.org/author/A5010181158', 'https://semopenalex.org/author/A5068340305', 'https://semopenalex.org/author/A5017334961', 'https://semopenalex.org/author/A5100439996', 'https://semopenalex.org/author/A5028716858', 'https://semopenalex.org/work/W2137544679', 'https://semopenalex.org/work/W1578028529', 'https://semopenalex.org/author/A5084868951', 'https://semopenalex.org/author/A5100408010', 'https://semopenalex.org/work/W2997847174', 'https://semopenalex.org/author/A5007043113', 'https://semopenalex.org/author/A5011086593', 'https://semopenalex.org/author/A5108459503', 'https://semopenalex.org/work/W2788767656', 'https://semopenalex.org/author/A5101540631', 'https://semopenalex.org/author/A5077610917', 'https://semopenalex.org/author/A5034057959', 'https://semopenalex.org/author/A5019525050', 'https://semopenalex.org/work/W4246723161', 'https://semopenalex.org/author/A5101308414', 'https://semopenalex.org/author/A5101289775', 'https://semopenalex.org/author/A5015836405', 'https://semopenalex.org/work/W2566570636', 'https://semopenalex.org/author/A5100388581', 'https://semopenalex.org/author/A5100438174', 'https://semopenalex.org/author/A5100458090', 'https://semopenalex.org/author/A5101264794', 'https://semopenalex.org/author/A5100426931', 'https://semopenalex.org/work/W2884327322', 'https://semopenalex.org/author/A5076444296', 'https://semopenalex.org/author/A5100610450', 'https://semopenalex.org/author/A5033111691', 'https://semopenalex.org/work/W2112857338', 'https://semopenalex.org/work/W2506015293', 'https://semopenalex.org/author/A5075273130', 'https://semopenalex.org/work/W2351461473', 'https://semopenalex.org/author/A5103234102', 'https://semopenalex.org/author/A5043798385', 'https://semopenalex.org/work/W4362677137', 'https://semopenalex.org/work/W2116175419', 'https://semopenalex.org/author/A5115595561', 'https://semopenalex.org/author/A5032062525', 'https://semopenalex.org/author/A5032194564', 'https://semopenalex.org/author/A5101612059', 'https://semopenalex.org/work/W2136556709', 'https://semopenalex.org/author/A5114778131', 'https://semopenalex.org/work/W3086623952', 'https://semopenalex.org/work/W1966337472', 'https://semopenalex.org/author/A5058164381', 'https://semopenalex.org/author/A5100738977', 'https://semopenalex.org/work/W2066421240', 'https://semopenalex.org/author/A5081420063', 'https://semopenalex.org/author/A5046237164', 'https://semopenalex.org/work/W4405706648', 'https://semopenalex.org/author/A5084735407', 'https://semopenalex.org/author/A5100409885', 'https://semopenalex.org/author/A5100388576', 'https://semopenalex.org/author/A5100447682', 'https://semopenalex.org/work/W2996252512', 'https://semopenalex.org/work/W3092116317', 'https://semopenalex.org/author/A5102222159', 'https://semopenalex.org/author/A5100676331', 'https://semopenalex.org/author/A5030626281', 'https://semopenalex.org/author/A5009071576', 'https://semopenalex.org/author/A5100429004', 'https://semopenalex.org/author/A5050080938', 'https://semopenalex.org/author/A5087492388', 'https://semopenalex.org/author/A5043801432', 'https://semopenalex.org/author/A5002594574', 'https://semopenalex.org/work/W3166897865', 'https://semopenalex.org/work/W3110369458', 'https://semopenalex.org/author/A5049100391', 'https://semopenalex.org/work/W3109004940', 'https://semopenalex.org/author/A5077424533', 'https://semopenalex.org/author/A5100772234', 'https://semopenalex.org/author/A5101556258', 'https://semopenalex.org/work/W2089461653', 'https://semopenalex.org/work/W4205415629', 'https://semopenalex.org/author/A5004490190', 'https://semopenalex.org/work/W2809300184', 'https://semopenalex.org/author/A5009435651', 'https://semopenalex.org/author/A5024821632', 'https://semopenalex.org/author/A5077138780', 'https://semopenalex.org/author/A5100459874', 'https://semopenalex.org/work/W4391272793', 'https://semopenalex.org/author/A5067163535', 'https://semopenalex.org/work/W3108350045', 'https://semopenalex.org/author/A5052249316', 'https://semopenalex.org/work/W2794806827', 'https://semopenalex.org/author/A5002289161', 'https://semopenalex.org/author/A5100327487', 'https://semopenalex.org/author/A5102928967', 'https://semopenalex.org/author/A5074307489', 'https://semopenalex.org/author/A5045087569', 'https://semopenalex.org/author/A5065293581', 'https://semopenalex.org/author/A5090671359', 'https://semopenalex.org/author/A5021222755', 'https://semopenalex.org/author/A5100408160', 'https://semopenalex.org/author/A5009455568', 'https://semopenalex.org/author/A5100367807', 'https://semopenalex.org/author/A5058738211', 'https://semopenalex.org/author/A5100738980', 'https://semopenalex.org/author/A5018031899', 'https://semopenalex.org/author/A5100753041', 'https://semopenalex.org/work/W2168668632', 'https://semopenalex.org/author/A5084874990', 'https://semopenalex.org/author/A5026927053', 'https://semopenalex.org/author/A5027084532', 'https://semopenalex.org/author/A5000381434', 'https://semopenalex.org/work/W2518136680', 'https://semopenalex.org/author/A5013103539', 'https://semopenalex.org/work/W3193682477', 'https://semopenalex.org/work/W4388212297', 'https://semopenalex.org/author/A5059065212', 'https://semopenalex.org/author/A5103761162', 'https://semopenalex.org/author/A5088725475', 'https://semopenalex.org/author/A5067467896', 'https://semopenalex.org/work/W1982483659', 'https://semopenalex.org/work/W3044975328', 'https://semopenalex.org/work/W1980313439', 'https://semopenalex.org/author/A5041961808', 'https://semopenalex.org/author/A5023093639', 'https://semopenalex.org/author/A5100388617', 'https://semopenalex.org/author/A5100331488', 'https://semopenalex.org/author/A5022677467', 'https://semopenalex.org/work/W3126104791', 'https://semopenalex.org/author/A5073965511', 'https://semopenalex.org/author/A5100349346', 'https://semopenalex.org/author/A5100523187', 'https://semopenalex.org/work/W2850992922', 'https://semopenalex.org/author/A5038017715', 'https://semopenalex.org/work/W4391341613', 'https://semopenalex.org/author/A5100361632', 'https://semopenalex.org/author/A5012469172', 'https://semopenalex.org/work/W2246822044', 'https://semopenalex.org/author/A5040850915', 'https://semopenalex.org/work/W4250349204', 'https://semopenalex.org/author/A5100367825', 'https://semopenalex.org/author/A5067395122', 'https://semopenalex.org/author/A5060115298', 'https://semopenalex.org/work/W3196137381', 'https://semopenalex.org/author/A5100445622', 'https://semopenalex.org/author/A5055149708', 'https://semopenalex.org/author/A5103073505', 'https://semopenalex.org/work/W2000778992', 'https://semopenalex.org/work/W1971292095', 'https://semopenalex.org/author/A5107006112', 'https://semopenalex.org/work/W116531637', 'https://semopenalex.org/author/A5052981404', 'https://semopenalex.org/author/A5103205468', 'https://semopenalex.org/work/W2901813505', 'https://semopenalex.org/work/W4384345709', 'https://semopenalex.org/author/A5075929099', 'https://semopenalex.org/author/A5100443727', 'https://semopenalex.org/work/W1993418924', 'https://semopenalex.org/work/W2131346202', 'https://semopenalex.org/author/A5111956187', 'https://semopenalex.org/author/A5069596903', 'https://semopenalex.org/author/A5034794084', 'https://semopenalex.org/author/A5101558050', 'https://semopenalex.org/work/W2963868406', 'https://semopenalex.org/author/A5043476448', 'https://semopenalex.org/author/A5055422837', 'https://semopenalex.org/author/A5088708850', 'https://semopenalex.org/author/A5052199638', 'https://semopenalex.org/work/W3000410628', 'https://semopenalex.org/work/W4399553914', 'https://semopenalex.org/author/A5077984014', 'https://semopenalex.org/author/A5035089987', 'https://semopenalex.org/author/A5058258996', 'https://semopenalex.org/work/W4375957525', 'https://semopenalex.org/author/A5035359666', 'https://semopenalex.org/author/A5100388644', 'https://semopenalex.org/author/A5100401412', 'https://semopenalex.org/work/W3120745352', 'https://semopenalex.org/author/A5036120394', 'https://semopenalex.org/author/A5113160035', 'https://semopenalex.org/work/W2093107900', 'https://semopenalex.org/work/W3142314132', 'https://semopenalex.org/author/A5033164669', 'https://semopenalex.org/author/A5100394129', 'https://semopenalex.org/author/A5115590096', 'https://semopenalex.org/work/W2950530129', 'https://semopenalex.org/author/A5069621751', 'https://semopenalex.org/author/A5100447691', 'https://semopenalex.org/author/A5100677820', 'https://semopenalex.org/author/A5052404451', 'https://semopenalex.org/work/W3205352458', 'https://semopenalex.org/work/W4245733707', 'https://semopenalex.org/work/W1976529112', 'https://semopenalex.org/author/A5009487151', 'https://semopenalex.org/author/A5025977354', 'https://semopenalex.org/author/A5085393851', 'https://semopenalex.org/author/A5090627608', 'https://semopenalex.org/author/A5065848808', 'https://semopenalex.org/work/W4391840543', 'https://semopenalex.org/author/A5100697624', 'https://semopenalex.org/author/A5033163346', 'https://semopenalex.org/author/A5079431306', 'https://semopenalex.org/author/A5005007374', 'https://semopenalex.org/work/W2397328687', 'https://semopenalex.org/author/A5058257080', 'https://semopenalex.org/author/A5100412598', 'https://semopenalex.org/author/A5088646345', 'https://semopenalex.org/author/A5100349343', 'https://semopenalex.org/work/W2596236679', 'https://semopenalex.org/author/A5048041198', 'https://semopenalex.org/work/W4399851061', 'https://semopenalex.org/work/W4253460413', 'https://semopenalex.org/author/A5025839857', 'https://semopenalex.org/author/A5030997313', 'https://semopenalex.org/author/A5033542967', 'https://semopenalex.org/work/W2969773072', 'https://semopenalex.org/work/W2039325426', 'https://semopenalex.org/work/W1977393187']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W1710751537', 'https://semopenalex.org/work/W2078770126', 'https://semopenalex.org/work/W1997210046', 'https://semopenalex.org/work/W2103982927', 'https://semopenalex.org/work/W2061236588', 'https://semopenalex.org/work/W4385473607', 'https://semopenalex.org/work/W4391272934', 'https://semopenalex.org/work/W2015180219', 'https://semopenalex.org/work/W1517590008', 'https://semopenalex.org/work/W1975513208', 'https://semopenalex.org/work/W1775494561', 'https://semopenalex.org/work/W2980176182', 'https://semopenalex.org/work/W2129825950', 'https://semopenalex.org/work/W2085609918', 'https://semopenalex.org/work/W2915945450', 'https://semopenalex.org/work/W2915030750', 'https://semopenalex.org/work/W4402442861', 'https://semopenalex.org/work/W1991332789', 'https://semopenalex.org/work/W3195402331', 'https://semopenalex.org/work/W1579677221', 'https://semopenalex.org/work/W2127281178', 'https://semopenalex.org/work/W4296041368', 'https://semopenalex.org/work/W1531484838', 'https://semopenalex.org/work/W2525118715', 'https://semopenalex.org/work/W4312240104', 'https://semopenalex.org/work/W2806131721', 'https://semopenalex.org/work/W4313563519', 'https://semopenalex.org/work/W2515946176', 'https://semopenalex.org/work/W3092639686', 'https://semopenalex.org/work/W2809114684', 'https://semopenalex.org/work/W2953255159', 'https://semopenalex.org/work/W2949504704', 'https://semopenalex.org/work/W2206340513', 'https://semopenalex.org/work/W1556803451', 'https://semopenalex.org/work/W2123904236', 'https://semopenalex.org/work/W2952092732', 'https://semopenalex.org/work/W4384155490', 'https://semopenalex.org/work/W2077394967', 'https://semopenalex.org/work/W1987557201', 'https://semopenalex.org/work/W1495962746', 'https://semopenalex.org/work/W1994977110', 'https://semopenalex.org/work/W2734789924', 'https://semopenalex.org/work/W4238210800', 'https://semopenalex.org/work/W2132574120', 'https://semopenalex.org/work/W2122811495', 'https://semopenalex.org/work/W36371468', 'https://semopenalex.org/work/W2171326679', 'https://semopenalex.org/work/W1511466363', 'https://semopenalex.org/work/W1537902892', 'https://semopenalex.org/work/W2523177018', 'https://semopenalex.org/work/W2139525797', 'https://semopenalex.org/work/W2008078972', 'https://semopenalex.org/work/W4324007121', 'https://semopenalex.org/work/W2522928308', 'https://semopenalex.org/work/W3138989164', 'https://semopenalex.org/work/W139130934', 'https://semopenalex.org/work/W2400762887', 'https://semopenalex.org/work/W2754252703', 'https://semopenalex.org/work/W3136236837', 'https://semopenalex.org/work/W1595761884', 'https://semopenalex.org/work/W4253646682', 'https://semopenalex.org/work/W4404057326', 'https://semopenalex.org/work/W1792464322', 'https://semopenalex.org/work/W1588297513', 'https://semopenalex.org/work/W2751928463', 'https://semopenalex.org/work/W2123889292', 'https://semopenalex.org/work/W144935353', 'https://semopenalex.org/work/W2173733616', 'https://semopenalex.org/work/W147488175', 'https://semopenalex.org/work/W1811359278', 'https://semopenalex.org/work/W2899402023', 'https://semopenalex.org/work/W1774324140', 'https://semopenalex.org/work/W3158293305', 'https://semopenalex.org/work/W1253240651', 'https://semopenalex.org/work/W2125383988', 'https://semopenalex.org/work/W48558007', 'https://semopenalex.org/work/W4393474997', 'https://semopenalex.org/work/W2115447277', 'https://semopenalex.org/work/W2581324891', 'https://semopenalex.org/work/W1975908943', 'https://semopenalex.org/work/W1475955015', 'https://semopenalex.org/work/W1798073562', 'https://semopenalex.org/work/W2520217242', 'https://semopenalex.org/work/W2008732772', 'https://semopenalex.org/work/W3137115172', 'https://semopenalex.org/work/W1579914521', 'https://semopenalex.org/work/W2104421582', 'https://semopenalex.org/work/W2778798134', 'https://semopenalex.org/work/W1679509962', 'https://semopenalex.org/work/W2747419197', 'https://semopenalex.org/work/W2047400318', 'https://semopenalex.org/work/W2520300422', 'https://semopenalex.org/work/W2103704182', 'https://semopenalex.org/work/W2778029444', 'https://semopenalex.org/work/W2779900466', 'https://semopenalex.org/work/W2101874499', 'https://semopenalex.org/work/W2094034408', 'https://semopenalex.org/work/W1550675824', 'https://semopenalex.org/work/W1978640117', 'https://semopenalex.org/work/W2912433096', 'https://semopenalex.org/work/W3108668383', 'https://semopenalex.org/work/W2012114748', 'https://semopenalex.org/work/W2008606555', 'https://semopenalex.org/work/W2612371455', 'https://semopenalex.org/work/W2044926733', 'https://semopenalex.org/work/W2039085252', 'https://semopenalex.org/work/W2181042156', 'https://semopenalex.org/work/W2011170798', 'https://semopenalex.org/work/W4387755431', 'https://semopenalex.org/work/W2130495724', 'https://semopenalex.org/work/W2071433880', 'https://semopenalex.org/work/W1593317697', 'https://semopenalex.org/work/W991450633', 'https://semopenalex.org/work/W1595752763', 'https://semopenalex.org/work/W2028893723', 'https://semopenalex.org/work/W2915009967', 'https://semopenalex.org/work/W4398191656', 'https://semopenalex.org/work/W1520649080', 'https://semopenalex.org/work/W3028360334', 'https://semopenalex.org/work/W2921648886', 'https://semopenalex.org/work/W4237909807', 'https://semopenalex.org/work/W2109952361', 'https://semopenalex.org/work/W1996454760', 'https://semopenalex.org/work/W1592700375', 'https://semopenalex.org/work/W1588734579', 'https://semopenalex.org/work/W2734788368', 'https://semopenalex.org/work/W2041544991', 'https://semopenalex.org/work/W2088263927', 'https://semopenalex.org/work/W1572167134', 'https://semopenalex.org/work/W1633377437', 'https://semopenalex.org/work/W2091478774', 'https://semopenalex.org/work/W4403628532', 'https://semopenalex.org/work/W4242041539', 'https://semopenalex.org/work/W4282583221', 'https://semopenalex.org/work/W2154282221', 'https://semopenalex.org/work/W3033698111', 'https://semopenalex.org/work/W2014199531', 'https://semopenalex.org/work/W115310691', 'https://semopenalex.org/work/W173156922', 'https://semopenalex.org/work/W1574950491', 'https://semopenalex.org/work/W52260594', 'https://semopenalex.org/work/W2189085557', 'https://semopenalex.org/work/W2928532935', 'https://semopenalex.org/work/W2466104094', 'https://semopenalex.org/work/W4406859981', 'https://semopenalex.org/work/W3009455989', 'https://semopenalex.org/work/W4249900482', 'https://semopenalex.org/work/W2949106240', 'https://semopenalex.org/work/W2963855145', 'https://semopenalex.org/work/W4298063358', 'https://semopenalex.org/work/W2400182190', 'https://semopenalex.org/work/W2123344956', 'https://semopenalex.org/work/W4242436304', 'https://semopenalex.org/work/W2118889869', 'https://semopenalex.org/work/W4292761028', 'https://semopenalex.org/work/W1570916159', 'https://semopenalex.org/work/W156157953', 'https://semopenalex.org/work/W2152544235', 'https://semopenalex.org/work/W2632860668', 'https://semopenalex.org/work/W3183165251', 'https://semopenalex.org/work/W2132155852', 'https://semopenalex.org/work/W2008620714', 'https://semopenalex.org/work/W371525118', 'https://semopenalex.org/work/W89291972', 'https://semopenalex.org/work/W4400976691', 'https://semopenalex.org/work/W4393943425', 'https://semopenalex.org/work/W2527377534', 'https://semopenalex.org/work/W2098211566', 'https://semopenalex.org/work/W2145761885', 'https://semopenalex.org/work/W2128127301', 'https://semopenalex.org/work/W2112609211', 'https://semopenalex.org/work/W2153339030', 'https://semopenalex.org/work/W2525395252', 'https://semopenalex.org/work/W2747898780', 'https://semopenalex.org/work/W2087840232', 'https://semopenalex.org/work/W2592423893', 'https://semopenalex.org/work/W2401057219', 'https://semopenalex.org/work/W4394555057', 'https://semopenalex.org/work/W1978847709', 'https://semopenalex.org/work/W1971941065', 'https://semopenalex.org/work/W2155935413', 'https://semopenalex.org/work/W2166938786', 'https://semopenalex.org/work/W1719093023', 'https://semopenalex.org/work/W1908231796', 'https://semopenalex.org/work/W2739356170', 'https://semopenalex.org/work/W2049801349', 'https://semopenalex.org/work/W2017269495', 'https://semopenalex.org/work/W3116695505', 'https://semopenalex.org/work/W1560854026', 'https://semopenalex.org/work/W4400939550', 'https://semopenalex.org/work/W2612962685', 'https://semopenalex.org/work/W2794546965', 'https://semopenalex.org/work/W4282576055', 'https://semopenalex.org/work/W1573454147', 'https://semopenalex.org/work/W205920923', 'https://semopenalex.org/work/W3216444132', 'https://semopenalex.org/work/W2055963247', 'https://semopenalex.org/work/W2958694015', 'https://semopenalex.org/work/W4393670548', 'https://semopenalex.org/work/W2609404595', 'https://semopenalex.org/work/W1501840263']</t>
+  </si>
+  <si>
+    <t>['W. R. OWENS, STUART SIM, AND DAVID WALKER, EDS. BUNYAN STUDIES: A JOURNAL OF REFORMATION AND NONCONFORMIST CULTURE. NUMBER 22. NORTHUMBRIA UNIVERSITY, 2018. PP. 164.', 'Rotten green tests in Java, Pharo and Python', 'https://semopenalex.org/source/S109852484', 'https://semopenalex.org/work/W4224210536', 'https://semopenalex.org/work/W4312279131', 'https://semopenalex.org/source/S4363604151', 'https://semopenalex.org/work/W4294273680', 'Pope and the Reformation of the Oral: The Iliad in the History of Mediation', 'Advances in monitoring carbon dioxide exchange between the atmosphere and mine waste derived from ultramafic-hosted mineral deposits; a pilot study at Cassiar, B.C.', 'The Secret History of HB-2: Bathroom Safety in the Eighteenth Century and Beyond', 'https://semopenalex.org/source/S73505065', 'https://semopenalex.org/source/S4306463865', 'W. R. Owens, Stuart Sim, and David Walker, eds. Bunyan Studies: A Journal of Reformation and Nonconformist Culture', 'https://semopenalex.org/source/S4210192127', 'Rotten Green Tests in Java, Pharo and Python', 'https://semopenalex.org/source/S4306402512', 'https://semopenalex.org/work/W4322392796', 'https://semopenalex.org/source/S4306462979', 'https://semopenalex.org/work/W4287005120', 'https://semopenalex.org/work/W4309899403', 'https://semopenalex.org/source/S4377196300', 'https://semopenalex.org/source/S4306402203', 'https://semopenalex.org/work/W3202264790']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W2906756016', 'https://semopenalex.org/work/W2947077169', 'https://semopenalex.org/work/W2613478558', 'https://semopenalex.org/work/W4404660380', 'https://semopenalex.org/work/W4323660310', 'https://semopenalex.org/work/W4210579963', 'https://semopenalex.org/work/W2161672839', 'https://semopenalex.org/work/W616114729', 'https://semopenalex.org/work/W2977439887', 'https://semopenalex.org/work/W3099917237', 'https://semopenalex.org/work/W4399748832', 'https://semopenalex.org/work/W4400950811', 'https://semopenalex.org/work/W2567325662', 'https://semopenalex.org/work/W2786034148', 'https://semopenalex.org/work/W4294328862', 'https://semopenalex.org/work/W2995007313', 'https://semopenalex.org/work/W1970619397', 'https://semopenalex.org/work/W2805958446', 'https://semopenalex.org/work/W4403612127', 'https://semopenalex.org/work/W2112043190', 'https://semopenalex.org/work/W2158980502', 'https://semopenalex.org/work/W2404155628', 'https://semopenalex.org/work/W2952261671', 'https://semopenalex.org/work/W3217353773', 'https://semopenalex.org/work/W4300606001']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W4285228284', 'https://semopenalex.org/work/W2538728777', 'https://semopenalex.org/work/W2770896033', 'https://semopenalex.org/work/W2907903092', 'https://semopenalex.org/work/W2534209856', 'https://semopenalex.org/work/W2912223386', 'https://semopenalex.org/work/W2535112844', 'https://semopenalex.org/work/W2770615292', 'https://semopenalex.org/work/W2295752281', 'https://semopenalex.org/work/W2768137799', 'https://semopenalex.org/work/W4210437323', 'https://semopenalex.org/work/W2344766906']</t>
   </si>
   <si>
     <t>['https://semopenalex.org/work/W2979411460']</t>
   </si>
   <si>
-    <t>['https://semopenalex.org/work/W4405522435', 'https://semopenalex.org/work/W2889152126', 'https://semopenalex.org/work/W3047549637', 'https://semopenalex.org/work/W2611425173', 'https://semopenalex.org/work/W4280535254', 'https://semopenalex.org/work/W1504851162', 'https://semopenalex.org/work/W1480251338', 'https://semopenalex.org/work/W2139884008', 'https://semopenalex.org/work/W4362480098', 'https://semopenalex.org/work/W2906279331', 'https://semopenalex.org/work/W4406614566', 'https://semopenalex.org/work/W2594567826', 'https://semopenalex.org/work/W3164215837', 'https://semopenalex.org/work/W3047187362', 'https://semopenalex.org/work/W3049077927', 'https://semopenalex.org/work/W277742567', 'https://semopenalex.org/work/W2467538262', 'https://semopenalex.org/work/W2197901163', 'https://semopenalex.org/work/W2893803239', 'https://semopenalex.org/work/W2908432809', 'https://semopenalex.org/work/W2900823847', 'https://semopenalex.org/work/W2294889963', 'https://semopenalex.org/work/W4403578243', 'https://semopenalex.org/work/W3021665866', 'https://semopenalex.org/work/W2029007624', 'https://semopenalex.org/work/W2750426793', 'https://semopenalex.org/work/W3019708749', 'https://semopenalex.org/work/W2218034962', 'https://semopenalex.org/work/W2549943073', 'https://semopenalex.org/work/W4380089170', 'https://semopenalex.org/work/W3213838697', 'https://semopenalex.org/work/W4380077038', 'https://semopenalex.org/work/W3022678954', 'https://semopenalex.org/work/W2609071468', 'https://semopenalex.org/work/W2891220991', 'https://semopenalex.org/work/W2796945618', 'https://semopenalex.org/work/W4386214602', 'https://semopenalex.org/work/W2900540570', 'https://semopenalex.org/work/W4300971360', 'https://semopenalex.org/work/W4286787675']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W3206712787', 'https://semopenalex.org/work/W2752493326', 'https://semopenalex.org/work/W4393752214', 'https://semopenalex.org/work/W2057014910', 'https://semopenalex.org/work/W4393908582', 'https://semopenalex.org/work/W4239396382', 'https://semopenalex.org/work/W2789478762', 'https://semopenalex.org/work/W2798335699', 'https://semopenalex.org/work/W4393877125', 'https://semopenalex.org/work/W2054886944', 'https://semopenalex.org/work/W2725971658', 'https://semopenalex.org/work/W2139733095', 'https://semopenalex.org/work/W2024357873', 'https://semopenalex.org/work/W2346600598', 'https://semopenalex.org/work/W2520077052', 'https://semopenalex.org/work/W2901616108', 'https://semopenalex.org/work/W2944843734', 'https://semopenalex.org/work/W2942324097']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W3116763688', 'https://semopenalex.org/work/W2089762145', 'https://semopenalex.org/work/W3066383670', 'https://semopenalex.org/work/W2906612108', 'https://semopenalex.org/work/W3111943635', 'https://semopenalex.org/work/W1688396929', 'https://semopenalex.org/work/W2734465187', 'https://semopenalex.org/work/W2808806636', 'https://semopenalex.org/work/W2557438307', 'https://semopenalex.org/work/W2735379054', 'https://semopenalex.org/work/W2623350311', 'https://semopenalex.org/work/W2902564735', 'https://semopenalex.org/work/W2922408557', 'https://semopenalex.org/work/W2511600948', 'https://semopenalex.org/work/W2809627415', 'https://semopenalex.org/work/W2775805395', 'https://semopenalex.org/work/W2427008665', 'https://semopenalex.org/work/W2808066670', 'https://semopenalex.org/work/W2772495508', 'https://semopenalex.org/work/W2594546957', 'https://semopenalex.org/work/W4402599958', 'https://semopenalex.org/work/W2507120666', 'https://semopenalex.org/work/W3041363918', 'https://semopenalex.org/work/W2422976594', 'https://semopenalex.org/work/W3153580448', 'https://semopenalex.org/work/W2901968423', 'https://semopenalex.org/work/W2808185912']</t>
-  </si>
-  <si>
-    <t>['https://semopenalex.org/work/W2905528077', 'https://semopenalex.org/work/W2485416095', 'https://semopenalex.org/work/W2277556528', 'https://semopenalex.org/work/W2219349787', 'https://semopenalex.org/work/W2016390608', 'https://semopenalex.org/work/W2620328864', 'https://semopenalex.org/work/W2800536240']</t>
+    <t>['https://semopenalex.org/work/W2796945618', 'https://semopenalex.org/work/W2900540570', 'https://semopenalex.org/work/W2029007624', 'https://semopenalex.org/work/W2139884008', 'https://semopenalex.org/work/W3164215837', 'https://semopenalex.org/work/W2549943073', 'https://semopenalex.org/work/W1504851162', 'https://semopenalex.org/work/W2893803239', 'https://semopenalex.org/work/W4403578243', 'https://semopenalex.org/work/W2594567826', 'https://semopenalex.org/work/W3213838697', 'https://semopenalex.org/work/W2294889963', 'https://semopenalex.org/work/W2609071468', 'https://semopenalex.org/work/W2611425173', 'https://semopenalex.org/work/W3047187362', 'https://semopenalex.org/work/W4300971360', 'https://semopenalex.org/work/W2900823847', 'https://semopenalex.org/work/W4286787675', 'https://semopenalex.org/work/W2889152126', 'https://semopenalex.org/work/W3022678954', 'https://semopenalex.org/work/W2906279331', 'https://semopenalex.org/work/W1480251338', 'https://semopenalex.org/work/W3049077927', 'https://semopenalex.org/work/W4405522435', 'https://semopenalex.org/work/W4380077038', 'https://semopenalex.org/work/W3021665866', 'https://semopenalex.org/work/W2197901163', 'https://semopenalex.org/work/W4362480098', 'https://semopenalex.org/work/W277742567', 'https://semopenalex.org/work/W2908432809', 'https://semopenalex.org/work/W2467538262', 'https://semopenalex.org/work/W4280535254', 'https://semopenalex.org/work/W3047549637', 'https://semopenalex.org/work/W2218034962', 'https://semopenalex.org/work/W4406614566', 'https://semopenalex.org/work/W4386214602', 'https://semopenalex.org/work/W3019708749', 'https://semopenalex.org/work/W2891220991', 'https://semopenalex.org/work/W4380089170', 'https://semopenalex.org/work/W2750426793']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W2789478762', 'https://semopenalex.org/work/W4393908582', 'https://semopenalex.org/work/W3206712787', 'https://semopenalex.org/work/W2520077052', 'https://semopenalex.org/work/W2725971658', 'https://semopenalex.org/work/W2901616108', 'https://semopenalex.org/work/W2942324097', 'https://semopenalex.org/work/W2139733095', 'https://semopenalex.org/work/W2346600598', 'https://semopenalex.org/work/W2057014910', 'https://semopenalex.org/work/W4239396382', 'https://semopenalex.org/work/W2944843734', 'https://semopenalex.org/work/W2054886944', 'https://semopenalex.org/work/W2024357873', 'https://semopenalex.org/work/W4393877125', 'https://semopenalex.org/work/W2752493326', 'https://semopenalex.org/work/W4393752214', 'https://semopenalex.org/work/W2798335699']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W2557438307', 'https://semopenalex.org/work/W3041363918', 'https://semopenalex.org/work/W2511600948', 'https://semopenalex.org/work/W2808806636', 'https://semopenalex.org/work/W2901968423', 'https://semopenalex.org/work/W2808066670', 'https://semopenalex.org/work/W2775805395', 'https://semopenalex.org/work/W2594546957', 'https://semopenalex.org/work/W2735379054', 'https://semopenalex.org/work/W2809627415', 'https://semopenalex.org/work/W2734465187', 'https://semopenalex.org/work/W2906612108', 'https://semopenalex.org/work/W2772495508', 'https://semopenalex.org/work/W3111943635', 'https://semopenalex.org/work/W2922408557', 'https://semopenalex.org/work/W4402599958', 'https://semopenalex.org/work/W2902564735', 'https://semopenalex.org/work/W1688396929', 'https://semopenalex.org/work/W2808185912', 'https://semopenalex.org/work/W2089762145', 'https://semopenalex.org/work/W3066383670', 'https://semopenalex.org/work/W2427008665', 'https://semopenalex.org/work/W2507120666', 'https://semopenalex.org/work/W2422976594', 'https://semopenalex.org/work/W3153580448', 'https://semopenalex.org/work/W3116763688', 'https://semopenalex.org/work/W2623350311']</t>
+  </si>
+  <si>
+    <t>['https://semopenalex.org/work/W2620328864', 'https://semopenalex.org/work/W2277556528', 'https://semopenalex.org/work/W2485416095', 'https://semopenalex.org/work/W2800536240', 'https://semopenalex.org/work/W2219349787', 'https://semopenalex.org/work/W2016390608', 'https://semopenalex.org/work/W2905528077']</t>
   </si>
   <si>
     <t>['1']</t>

</xml_diff>